<commit_message>
Improved processing mode (metastage) as Owner:Meta:stage
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -942,34 +942,34 @@
     <t>[release-name]</t>
   </si>
   <si>
-    <t>CM-minimum</t>
-  </si>
-  <si>
-    <t>CM-uitgebreid</t>
-  </si>
-  <si>
-    <t>CM-opleveren</t>
-  </si>
-  <si>
-    <t>CM-docrelease</t>
-  </si>
-  <si>
     <t>Config</t>
   </si>
   <si>
-    <t>LM-minimum</t>
-  </si>
-  <si>
-    <t>LM-uitgebreid</t>
-  </si>
-  <si>
-    <t>LM-opleveren</t>
-  </si>
-  <si>
-    <t>LM-docrelease</t>
-  </si>
-  <si>
     <t>en:en</t>
+  </si>
+  <si>
+    <t>CM: minimum</t>
+  </si>
+  <si>
+    <t>CM: uitgebreid</t>
+  </si>
+  <si>
+    <t>CM: opleveren</t>
+  </si>
+  <si>
+    <t>CM: docrelease</t>
+  </si>
+  <si>
+    <t>LM: minimum</t>
+  </si>
+  <si>
+    <t>LM: uitgebreid</t>
+  </si>
+  <si>
+    <t>LM: opleveren</t>
+  </si>
+  <si>
+    <t>LM: docrelease</t>
   </si>
 </sst>
 </file>
@@ -1172,9 +1172,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1190,6 +1187,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1483,11 +1483,11 @@
   </sheetPr>
   <dimension ref="A1:R123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M57" sqref="M57:P57"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1498,17 +1498,17 @@
     <col min="4" max="4" width="13.23046875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="17.3828125" customWidth="1"/>
-    <col min="7" max="7" width="3.921875" style="26" customWidth="1"/>
+    <col min="7" max="7" width="3.921875" style="25" customWidth="1"/>
     <col min="8" max="8" width="18.4609375" customWidth="1"/>
     <col min="9" max="9" width="17.61328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.3046875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.84375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.61328125" style="26" customWidth="1"/>
+    <col min="12" max="12" width="3.61328125" style="25" customWidth="1"/>
     <col min="13" max="13" width="18.4609375" customWidth="1"/>
     <col min="14" max="14" width="17.61328125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.3046875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.84375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.15234375" style="26" customWidth="1"/>
+    <col min="17" max="17" width="4.15234375" style="25" customWidth="1"/>
     <col min="18" max="18" width="27.3046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1531,66 +1531,66 @@
       <c r="F1" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="G1" s="22"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="L1" s="22"/>
+        <v>305</v>
+      </c>
+      <c r="L1" s="21"/>
       <c r="M1" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q1" s="22"/>
+        <v>305</v>
+      </c>
+      <c r="Q1" s="21"/>
       <c r="R1" s="3" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
-      <c r="G2" s="23"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="3" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="L2" s="23"/>
+        <v>310</v>
+      </c>
+      <c r="L2" s="22"/>
       <c r="M2" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q2" s="23"/>
+        <v>314</v>
+      </c>
+      <c r="Q2" s="22"/>
       <c r="R2" s="5"/>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
@@ -1609,13 +1609,13 @@
       <c r="E3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="L3" s="24"/>
+      <c r="G3" s="23"/>
+      <c r="L3" s="23"/>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
-      <c r="Q3" s="24"/>
+      <c r="Q3" s="23"/>
     </row>
     <row r="4" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
@@ -1636,13 +1636,13 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="G4" s="23"/>
+      <c r="L4" s="23"/>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="24"/>
+      <c r="Q4" s="23"/>
       <c r="R4" s="8" t="s">
         <v>223</v>
       </c>
@@ -1666,13 +1666,13 @@
       <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="L5" s="24"/>
+      <c r="G5" s="23"/>
+      <c r="L5" s="23"/>
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
-      <c r="Q5" s="24"/>
+      <c r="Q5" s="23"/>
       <c r="R5" s="8" t="s">
         <v>224</v>
       </c>
@@ -1693,49 +1693,49 @@
       <c r="E6" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="Q6" s="24"/>
+      <c r="G6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="20" t="b">
+      <c r="D7" s="27" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="L7" s="24"/>
+      <c r="G7" s="23"/>
+      <c r="L7" s="23"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
-      <c r="Q7" s="24"/>
+      <c r="Q7" s="23"/>
       <c r="R7" s="2" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="G8" s="24"/>
-      <c r="L8" s="24"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="G8" s="23"/>
+      <c r="L8" s="23"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
-      <c r="Q8" s="24"/>
+      <c r="Q8" s="23"/>
     </row>
     <row r="9" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
@@ -1756,9 +1756,9 @@
       <c r="F9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="Q9" s="24"/>
+      <c r="G9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="Q9" s="23"/>
     </row>
     <row r="10" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
@@ -1776,9 +1776,9 @@
       <c r="E10" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="Q10" s="24"/>
+      <c r="G10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="Q10" s="23"/>
     </row>
     <row r="11" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
@@ -1799,13 +1799,13 @@
       <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="L11" s="24"/>
+      <c r="G11" s="23"/>
+      <c r="L11" s="23"/>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
-      <c r="Q11" s="24"/>
+      <c r="Q11" s="23"/>
       <c r="R11" s="7"/>
     </row>
     <row r="12" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.4">
@@ -1824,8 +1824,8 @@
       <c r="E12" s="12" t="b">
         <v>1</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="L12" s="24"/>
+      <c r="G12" s="23"/>
+      <c r="L12" s="23"/>
       <c r="M12" s="12" t="s">
         <v>291</v>
       </c>
@@ -1838,7 +1838,7 @@
       <c r="P12" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="Q12" s="24"/>
+      <c r="Q12" s="23"/>
       <c r="R12" t="s">
         <v>292</v>
       </c>
@@ -1862,9 +1862,9 @@
       <c r="F13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="Q13" s="24"/>
+      <c r="G13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="Q13" s="23"/>
     </row>
     <row r="14" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
@@ -1882,7 +1882,7 @@
       <c r="E14" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G14" s="24"/>
+      <c r="G14" s="23"/>
       <c r="H14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1895,7 +1895,7 @@
       <c r="K14" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="L14" s="24"/>
+      <c r="L14" s="23"/>
       <c r="M14" s="17" t="s">
         <v>17</v>
       </c>
@@ -1908,7 +1908,7 @@
       <c r="P14" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="Q14" s="24"/>
+      <c r="Q14" s="23"/>
       <c r="R14" s="2" t="s">
         <v>250</v>
       </c>
@@ -1932,13 +1932,13 @@
       <c r="F15" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="G15" s="24"/>
-      <c r="L15" s="24"/>
+      <c r="G15" s="23"/>
+      <c r="L15" s="23"/>
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
-      <c r="Q15" s="24"/>
+      <c r="Q15" s="23"/>
     </row>
     <row r="16" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
@@ -1959,13 +1959,13 @@
       <c r="F16" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="G16" s="24"/>
-      <c r="L16" s="24"/>
+      <c r="G16" s="23"/>
+      <c r="L16" s="23"/>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
-      <c r="Q16" s="24"/>
+      <c r="Q16" s="23"/>
     </row>
     <row r="17" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
@@ -1982,16 +1982,16 @@
       <c r="F17" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="G17" s="24"/>
+      <c r="G17" s="23"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
-      <c r="L17" s="24"/>
+      <c r="L17" s="23"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
-      <c r="Q17" s="24"/>
+      <c r="Q17" s="23"/>
     </row>
     <row r="18" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
@@ -2009,13 +2009,13 @@
       <c r="E18" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G18" s="24"/>
-      <c r="L18" s="24"/>
+      <c r="G18" s="23"/>
+      <c r="L18" s="23"/>
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
-      <c r="Q18" s="24"/>
+      <c r="Q18" s="23"/>
     </row>
     <row r="19" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
@@ -2036,13 +2036,13 @@
       <c r="F19" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="G19" s="24"/>
-      <c r="L19" s="24"/>
+      <c r="G19" s="23"/>
+      <c r="L19" s="23"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="17"/>
       <c r="P19" s="17"/>
-      <c r="Q19" s="24"/>
+      <c r="Q19" s="23"/>
     </row>
     <row r="20" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
@@ -2063,13 +2063,13 @@
       <c r="F20" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="G20" s="24"/>
-      <c r="L20" s="24"/>
+      <c r="G20" s="23"/>
+      <c r="L20" s="23"/>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
       <c r="O20" s="17"/>
       <c r="P20" s="17"/>
-      <c r="Q20" s="24"/>
+      <c r="Q20" s="23"/>
     </row>
     <row r="21" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
@@ -2087,7 +2087,7 @@
       <c r="E21" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G21" s="24"/>
+      <c r="G21" s="23"/>
       <c r="H21" s="2" t="s">
         <v>14</v>
       </c>
@@ -2100,7 +2100,7 @@
       <c r="K21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L21" s="24"/>
+      <c r="L21" s="23"/>
       <c r="M21" s="17" t="s">
         <v>14</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="P21" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q21" s="24"/>
+      <c r="Q21" s="23"/>
     </row>
     <row r="22" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
@@ -2134,9 +2134,9 @@
       <c r="F22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="Q22" s="24"/>
+      <c r="G22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="Q22" s="23"/>
     </row>
     <row r="23" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
@@ -2154,9 +2154,9 @@
       <c r="E23" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="Q23" s="24"/>
+      <c r="G23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="Q23" s="23"/>
     </row>
     <row r="24" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
@@ -2174,7 +2174,7 @@
       <c r="E24" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G24" s="24"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="2" t="s">
         <v>14</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="K24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L24" s="24"/>
+      <c r="L24" s="23"/>
       <c r="M24" s="17" t="s">
         <v>14</v>
       </c>
@@ -2200,7 +2200,7 @@
       <c r="P24" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q24" s="24"/>
+      <c r="Q24" s="23"/>
     </row>
     <row r="25" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
@@ -2218,7 +2218,7 @@
       <c r="E25" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G25" s="24"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="2" t="s">
         <v>14</v>
       </c>
@@ -2231,7 +2231,7 @@
       <c r="K25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L25" s="24"/>
+      <c r="L25" s="23"/>
       <c r="M25" s="17" t="s">
         <v>14</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="P25" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q25" s="24"/>
+      <c r="Q25" s="23"/>
     </row>
     <row r="26" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
@@ -2265,13 +2265,13 @@
       <c r="F26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="24"/>
-      <c r="L26" s="24"/>
+      <c r="G26" s="23"/>
+      <c r="L26" s="23"/>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
-      <c r="Q26" s="24"/>
+      <c r="Q26" s="23"/>
       <c r="R26" s="8" t="s">
         <v>276</v>
       </c>
@@ -2292,7 +2292,7 @@
       <c r="E27" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G27" s="24"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="2" t="s">
         <v>14</v>
       </c>
@@ -2305,7 +2305,7 @@
       <c r="K27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L27" s="24"/>
+      <c r="L27" s="23"/>
       <c r="M27" s="17" t="s">
         <v>14</v>
       </c>
@@ -2318,7 +2318,7 @@
       <c r="P27" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q27" s="24"/>
+      <c r="Q27" s="23"/>
     </row>
     <row r="28" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
@@ -2339,13 +2339,13 @@
       <c r="F28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="24"/>
-      <c r="L28" s="24"/>
+      <c r="G28" s="23"/>
+      <c r="L28" s="23"/>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
       <c r="O28" s="17"/>
       <c r="P28" s="17"/>
-      <c r="Q28" s="24"/>
+      <c r="Q28" s="23"/>
       <c r="R28" s="2" t="s">
         <v>277</v>
       </c>
@@ -2366,9 +2366,9 @@
       <c r="E29" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="Q29" s="24"/>
+      <c r="G29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="Q29" s="23"/>
     </row>
     <row r="30" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="7" t="s">
@@ -2386,9 +2386,9 @@
       <c r="E30" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="Q30" s="24"/>
+      <c r="G30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="Q30" s="23"/>
     </row>
     <row r="31" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="7" t="s">
@@ -2409,9 +2409,9 @@
       <c r="F31" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="G31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="Q31" s="23"/>
     </row>
     <row r="32" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
@@ -2432,13 +2432,13 @@
       <c r="F32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G32" s="24"/>
-      <c r="L32" s="24"/>
+      <c r="G32" s="23"/>
+      <c r="L32" s="23"/>
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
       <c r="O32" s="17"/>
       <c r="P32" s="17"/>
-      <c r="Q32" s="24"/>
+      <c r="Q32" s="23"/>
     </row>
     <row r="33" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="7" t="s">
@@ -2459,9 +2459,9 @@
       <c r="F33" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="Q33" s="24"/>
+      <c r="G33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="Q33" s="23"/>
     </row>
     <row r="34" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
@@ -2479,7 +2479,7 @@
       <c r="E34" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G34" s="24"/>
+      <c r="G34" s="23"/>
       <c r="H34" s="17" t="s">
         <v>14</v>
       </c>
@@ -2492,7 +2492,7 @@
       <c r="K34" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="L34" s="24"/>
+      <c r="L34" s="23"/>
       <c r="M34" s="17" t="s">
         <v>14</v>
       </c>
@@ -2505,7 +2505,7 @@
       <c r="P34" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q34" s="24"/>
+      <c r="Q34" s="23"/>
     </row>
     <row r="35" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="7" t="s">
@@ -2526,9 +2526,9 @@
       <c r="F35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="Q35" s="24"/>
+      <c r="G35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="Q35" s="23"/>
     </row>
     <row r="36" spans="1:18" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A36" s="7" t="s">
@@ -2549,9 +2549,9 @@
       <c r="F36" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="24"/>
-      <c r="L36" s="24"/>
-      <c r="Q36" s="24"/>
+      <c r="G36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="Q36" s="23"/>
       <c r="R36" s="7" t="s">
         <v>205</v>
       </c>
@@ -2575,24 +2575,24 @@
       <c r="F37" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="G37" s="24"/>
-      <c r="L37" s="24"/>
-      <c r="Q37" s="24"/>
+      <c r="G37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="Q37" s="23"/>
       <c r="R37" s="7" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="38" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="20" t="b">
+      <c r="D38" s="27" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="2" t="b">
@@ -2601,26 +2601,26 @@
       <c r="F38" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G38" s="24"/>
-      <c r="L38" s="24"/>
+      <c r="G38" s="23"/>
+      <c r="L38" s="23"/>
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
       <c r="O38" s="17"/>
       <c r="P38" s="17"/>
-      <c r="Q38" s="24"/>
+      <c r="Q38" s="23"/>
     </row>
     <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="G39" s="24"/>
-      <c r="L39" s="24"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="G39" s="23"/>
+      <c r="L39" s="23"/>
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
       <c r="O39" s="17"/>
       <c r="P39" s="17"/>
-      <c r="Q39" s="24"/>
+      <c r="Q39" s="23"/>
     </row>
     <row r="40" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
@@ -2638,13 +2638,13 @@
       <c r="E40" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G40" s="24"/>
-      <c r="L40" s="24"/>
+      <c r="G40" s="23"/>
+      <c r="L40" s="23"/>
       <c r="M40" s="17"/>
       <c r="N40" s="17"/>
       <c r="O40" s="17"/>
       <c r="P40" s="17"/>
-      <c r="Q40" s="24"/>
+      <c r="Q40" s="23"/>
     </row>
     <row r="41" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
@@ -2662,13 +2662,13 @@
       <c r="E41" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G41" s="24"/>
-      <c r="L41" s="24"/>
+      <c r="G41" s="23"/>
+      <c r="L41" s="23"/>
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
       <c r="O41" s="17"/>
       <c r="P41" s="17"/>
-      <c r="Q41" s="24"/>
+      <c r="Q41" s="23"/>
     </row>
     <row r="42" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
@@ -2689,13 +2689,13 @@
       <c r="F42" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="G42" s="27"/>
-      <c r="L42" s="24"/>
+      <c r="G42" s="26"/>
+      <c r="L42" s="23"/>
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
       <c r="O42" s="17"/>
       <c r="P42" s="17"/>
-      <c r="Q42" s="24"/>
+      <c r="Q42" s="23"/>
       <c r="R42" s="2" t="s">
         <v>206</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="6"/>
-      <c r="G43" s="27"/>
+      <c r="G43" s="26"/>
       <c r="H43" s="17" t="s">
         <v>281</v>
       </c>
@@ -2726,7 +2726,7 @@
       <c r="K43" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L43" s="24"/>
+      <c r="L43" s="23"/>
       <c r="M43" s="17" t="s">
         <v>282</v>
       </c>
@@ -2739,7 +2739,7 @@
       <c r="P43" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q43" s="24"/>
+      <c r="Q43" s="23"/>
     </row>
     <row r="44" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
@@ -2760,9 +2760,9 @@
       <c r="F44" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="24"/>
-      <c r="L44" s="24"/>
-      <c r="Q44" s="24"/>
+      <c r="G44" s="23"/>
+      <c r="L44" s="23"/>
+      <c r="Q44" s="23"/>
       <c r="R44"/>
     </row>
     <row r="45" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2784,9 +2784,9 @@
       <c r="F45" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="G45" s="24"/>
-      <c r="L45" s="24"/>
-      <c r="Q45" s="24"/>
+      <c r="G45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="Q45" s="23"/>
     </row>
     <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
@@ -2807,13 +2807,13 @@
       <c r="F46" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G46" s="24"/>
-      <c r="L46" s="24"/>
+      <c r="G46" s="23"/>
+      <c r="L46" s="23"/>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
       <c r="O46" s="17"/>
       <c r="P46" s="17"/>
-      <c r="Q46" s="24"/>
+      <c r="Q46" s="23"/>
     </row>
     <row r="47" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A47" s="7" t="s">
@@ -2834,9 +2834,9 @@
       <c r="F47" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="24"/>
-      <c r="L47" s="24"/>
-      <c r="Q47" s="24"/>
+      <c r="G47" s="23"/>
+      <c r="L47" s="23"/>
+      <c r="Q47" s="23"/>
     </row>
     <row r="48" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A48" s="7" t="s">
@@ -2857,9 +2857,9 @@
       <c r="F48" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G48" s="24"/>
-      <c r="L48" s="24"/>
-      <c r="Q48" s="24"/>
+      <c r="G48" s="23"/>
+      <c r="L48" s="23"/>
+      <c r="Q48" s="23"/>
       <c r="R48" s="7" t="s">
         <v>208</v>
       </c>
@@ -2883,9 +2883,9 @@
       <c r="F49" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G49" s="24"/>
-      <c r="L49" s="24"/>
-      <c r="Q49" s="24"/>
+      <c r="G49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="Q49" s="23"/>
     </row>
     <row r="50" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A50" s="7" t="s">
@@ -2894,7 +2894,7 @@
       <c r="B50" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G50" s="24"/>
+      <c r="G50" s="23"/>
       <c r="H50" s="18" t="s">
         <v>300</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="K50" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="L50" s="24"/>
+      <c r="L50" s="23"/>
       <c r="M50" s="18" t="s">
         <v>300</v>
       </c>
@@ -2920,7 +2920,7 @@
       <c r="P50" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="Q50" s="24"/>
+      <c r="Q50" s="23"/>
     </row>
     <row r="51" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A51" s="7" t="s">
@@ -2935,7 +2935,7 @@
       <c r="D51" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G51" s="24"/>
+      <c r="G51" s="23"/>
       <c r="H51" s="7" t="s">
         <v>278</v>
       </c>
@@ -2948,7 +2948,7 @@
       <c r="K51" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="L51" s="24"/>
+      <c r="L51" s="23"/>
       <c r="M51" s="7" t="s">
         <v>278</v>
       </c>
@@ -2961,7 +2961,7 @@
       <c r="P51" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="Q51" s="24"/>
+      <c r="Q51" s="23"/>
     </row>
     <row r="52" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="7" t="s">
@@ -2982,9 +2982,9 @@
       <c r="F52" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="G52" s="24"/>
-      <c r="L52" s="24"/>
-      <c r="Q52" s="24"/>
+      <c r="G52" s="23"/>
+      <c r="L52" s="23"/>
+      <c r="Q52" s="23"/>
     </row>
     <row r="53" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A53" s="15" t="s">
@@ -3005,17 +3005,17 @@
       <c r="F53" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="G53" s="25"/>
+      <c r="G53" s="24"/>
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
-      <c r="L53" s="25"/>
+      <c r="L53" s="24"/>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
       <c r="O53" s="15"/>
       <c r="P53" s="15"/>
-      <c r="Q53" s="25"/>
+      <c r="Q53" s="24"/>
       <c r="R53" s="15" t="s">
         <v>264</v>
       </c>
@@ -3039,9 +3039,9 @@
       <c r="F54" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G54" s="24"/>
-      <c r="L54" s="24"/>
-      <c r="Q54" s="24"/>
+      <c r="G54" s="23"/>
+      <c r="L54" s="23"/>
+      <c r="Q54" s="23"/>
       <c r="R54" s="7" t="s">
         <v>209</v>
       </c>
@@ -3065,9 +3065,9 @@
       <c r="F55" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="G55" s="24"/>
-      <c r="L55" s="24"/>
-      <c r="Q55" s="24"/>
+      <c r="G55" s="23"/>
+      <c r="L55" s="23"/>
+      <c r="Q55" s="23"/>
       <c r="R55" s="7" t="s">
         <v>211</v>
       </c>
@@ -3091,9 +3091,9 @@
       <c r="F56" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="G56" s="24"/>
-      <c r="L56" s="24"/>
-      <c r="Q56" s="24"/>
+      <c r="G56" s="23"/>
+      <c r="L56" s="23"/>
+      <c r="Q56" s="23"/>
       <c r="R56" s="7" t="s">
         <v>248</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="E57" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G57" s="24"/>
+      <c r="G57" s="23"/>
       <c r="H57" s="2" t="s">
         <v>226</v>
       </c>
@@ -3127,20 +3127,20 @@
       <c r="K57" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="L57" s="24"/>
+      <c r="L57" s="23"/>
       <c r="M57" s="17" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="N57" s="17" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="O57" s="17" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="P57" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="Q57" s="24"/>
+        <v>306</v>
+      </c>
+      <c r="Q57" s="23"/>
       <c r="R57" s="2" t="s">
         <v>212</v>
       </c>
@@ -3164,13 +3164,13 @@
       <c r="F58" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="G58" s="24"/>
-      <c r="L58" s="24"/>
+      <c r="G58" s="23"/>
+      <c r="L58" s="23"/>
       <c r="M58" s="17"/>
       <c r="N58" s="17"/>
       <c r="O58" s="17"/>
       <c r="P58" s="17"/>
-      <c r="Q58" s="24"/>
+      <c r="Q58" s="23"/>
       <c r="R58" s="2" t="s">
         <v>213</v>
       </c>
@@ -3194,13 +3194,13 @@
       <c r="F59" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G59" s="24"/>
-      <c r="L59" s="24"/>
+      <c r="G59" s="23"/>
+      <c r="L59" s="23"/>
       <c r="M59" s="17"/>
       <c r="N59" s="17"/>
       <c r="O59" s="17"/>
       <c r="P59" s="17"/>
-      <c r="Q59" s="24"/>
+      <c r="Q59" s="23"/>
     </row>
     <row r="60" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
@@ -3218,7 +3218,7 @@
       <c r="E60" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G60" s="24"/>
+      <c r="G60" s="23"/>
       <c r="H60" s="17" t="s">
         <v>281</v>
       </c>
@@ -3231,7 +3231,7 @@
       <c r="K60" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L60" s="24"/>
+      <c r="L60" s="23"/>
       <c r="M60" s="17" t="s">
         <v>282</v>
       </c>
@@ -3244,7 +3244,7 @@
       <c r="P60" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q60" s="24"/>
+      <c r="Q60" s="23"/>
     </row>
     <row r="61" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
@@ -3265,13 +3265,13 @@
       <c r="F61" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G61" s="24"/>
-      <c r="L61" s="24"/>
+      <c r="G61" s="23"/>
+      <c r="L61" s="23"/>
       <c r="M61" s="17"/>
       <c r="N61" s="17"/>
       <c r="O61" s="17"/>
       <c r="P61" s="17"/>
-      <c r="Q61" s="24"/>
+      <c r="Q61" s="23"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
@@ -3313,13 +3313,13 @@
       <c r="F63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G63" s="24"/>
-      <c r="L63" s="24"/>
+      <c r="G63" s="23"/>
+      <c r="L63" s="23"/>
       <c r="M63" s="17"/>
       <c r="N63" s="17"/>
       <c r="O63" s="17"/>
       <c r="P63" s="17"/>
-      <c r="Q63" s="24"/>
+      <c r="Q63" s="23"/>
     </row>
     <row r="64" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
@@ -3340,13 +3340,13 @@
       <c r="F64" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G64" s="24"/>
-      <c r="L64" s="24"/>
+      <c r="G64" s="23"/>
+      <c r="L64" s="23"/>
       <c r="M64" s="17"/>
       <c r="N64" s="17"/>
       <c r="O64" s="17"/>
       <c r="P64" s="17"/>
-      <c r="Q64" s="24"/>
+      <c r="Q64" s="23"/>
     </row>
     <row r="65" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
@@ -3364,7 +3364,7 @@
       <c r="E65" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G65" s="24"/>
+      <c r="G65" s="23"/>
       <c r="H65" s="17" t="s">
         <v>281</v>
       </c>
@@ -3377,7 +3377,7 @@
       <c r="K65" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L65" s="24"/>
+      <c r="L65" s="23"/>
       <c r="M65" s="17" t="s">
         <v>282</v>
       </c>
@@ -3390,7 +3390,7 @@
       <c r="P65" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q65" s="24"/>
+      <c r="Q65" s="23"/>
     </row>
     <row r="66" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
@@ -3411,13 +3411,13 @@
       <c r="F66" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="G66" s="24"/>
-      <c r="L66" s="24"/>
+      <c r="G66" s="23"/>
+      <c r="L66" s="23"/>
       <c r="M66" s="17"/>
       <c r="N66" s="17"/>
       <c r="O66" s="17"/>
       <c r="P66" s="17"/>
-      <c r="Q66" s="24"/>
+      <c r="Q66" s="23"/>
     </row>
     <row r="67" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" s="7" t="s">
@@ -3438,9 +3438,9 @@
       <c r="F67" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="G67" s="24"/>
-      <c r="L67" s="24"/>
-      <c r="Q67" s="24"/>
+      <c r="G67" s="23"/>
+      <c r="L67" s="23"/>
+      <c r="Q67" s="23"/>
       <c r="R67" s="7" t="s">
         <v>249</v>
       </c>
@@ -3464,11 +3464,11 @@
       <c r="F68" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G68" s="24"/>
+      <c r="G68" s="23"/>
       <c r="H68" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L68" s="24"/>
+      <c r="L68" s="23"/>
       <c r="M68" s="17" t="s">
         <v>17</v>
       </c>
@@ -3481,7 +3481,7 @@
       <c r="P68" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q68" s="24"/>
+      <c r="Q68" s="23"/>
     </row>
     <row r="69" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A69" s="7" t="s">
@@ -3502,9 +3502,9 @@
       <c r="F69" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="G69" s="24"/>
-      <c r="L69" s="24"/>
-      <c r="Q69" s="24"/>
+      <c r="G69" s="23"/>
+      <c r="L69" s="23"/>
+      <c r="Q69" s="23"/>
       <c r="R69" s="8" t="s">
         <v>215</v>
       </c>
@@ -3525,7 +3525,7 @@
       <c r="E70" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G70" s="24"/>
+      <c r="G70" s="23"/>
       <c r="H70" s="17" t="s">
         <v>285</v>
       </c>
@@ -3538,7 +3538,7 @@
       <c r="K70" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="L70" s="24"/>
+      <c r="L70" s="23"/>
       <c r="M70" s="17" t="s">
         <v>286</v>
       </c>
@@ -3551,7 +3551,7 @@
       <c r="P70" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="Q70" s="24"/>
+      <c r="Q70" s="23"/>
     </row>
     <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
@@ -3572,13 +3572,13 @@
       <c r="F71" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G71" s="24"/>
-      <c r="L71" s="24"/>
+      <c r="G71" s="23"/>
+      <c r="L71" s="23"/>
       <c r="M71" s="17"/>
       <c r="N71" s="17"/>
       <c r="O71" s="17"/>
       <c r="P71" s="17"/>
-      <c r="Q71" s="24"/>
+      <c r="Q71" s="23"/>
     </row>
     <row r="72" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A72" s="7" t="s">
@@ -3599,9 +3599,9 @@
       <c r="F72" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G72" s="24"/>
-      <c r="L72" s="24"/>
-      <c r="Q72" s="24"/>
+      <c r="G72" s="23"/>
+      <c r="L72" s="23"/>
+      <c r="Q72" s="23"/>
       <c r="R72" s="8" t="s">
         <v>216</v>
       </c>
@@ -3625,9 +3625,9 @@
       <c r="F73" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G73" s="24"/>
-      <c r="L73" s="24"/>
-      <c r="Q73" s="24"/>
+      <c r="G73" s="23"/>
+      <c r="L73" s="23"/>
+      <c r="Q73" s="23"/>
       <c r="R73" s="7" t="s">
         <v>217</v>
       </c>
@@ -3651,13 +3651,13 @@
       <c r="F74" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G74" s="24"/>
-      <c r="L74" s="24"/>
+      <c r="G74" s="23"/>
+      <c r="L74" s="23"/>
       <c r="M74" s="17"/>
       <c r="N74" s="17"/>
       <c r="O74" s="17"/>
       <c r="P74" s="17"/>
-      <c r="Q74" s="24"/>
+      <c r="Q74" s="23"/>
     </row>
     <row r="75" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A75" s="17" t="s">
@@ -3666,7 +3666,7 @@
       <c r="B75" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C75" s="21" t="s">
+      <c r="C75" s="20" t="s">
         <v>295</v>
       </c>
       <c r="D75" s="17" t="b">
@@ -3678,9 +3678,9 @@
       <c r="F75" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G75" s="24"/>
-      <c r="L75" s="24"/>
-      <c r="Q75" s="24"/>
+      <c r="G75" s="23"/>
+      <c r="L75" s="23"/>
+      <c r="Q75" s="23"/>
     </row>
     <row r="76" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A76" s="7" t="s">
@@ -3694,7 +3694,7 @@
       <c r="E76" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G76" s="24"/>
+      <c r="G76" s="23"/>
       <c r="H76" s="7" t="s">
         <v>14</v>
       </c>
@@ -3707,7 +3707,7 @@
       <c r="K76" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L76" s="24"/>
+      <c r="L76" s="23"/>
       <c r="M76" s="7" t="s">
         <v>14</v>
       </c>
@@ -3720,16 +3720,16 @@
       <c r="P76" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Q76" s="24"/>
+      <c r="Q76" s="23"/>
     </row>
     <row r="77" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A77" s="21" t="s">
+      <c r="A77" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B77" s="21" t="s">
+      <c r="B77" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="21" t="s">
+      <c r="C77" s="20" t="s">
         <v>296</v>
       </c>
       <c r="D77" s="7" t="b">
@@ -3738,9 +3738,9 @@
       <c r="E77" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G77" s="24"/>
-      <c r="L77" s="24"/>
-      <c r="Q77" s="24"/>
+      <c r="G77" s="23"/>
+      <c r="L77" s="23"/>
+      <c r="Q77" s="23"/>
     </row>
     <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
@@ -3761,13 +3761,13 @@
       <c r="F78" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G78" s="24"/>
-      <c r="L78" s="24"/>
+      <c r="G78" s="23"/>
+      <c r="L78" s="23"/>
       <c r="M78" s="17"/>
       <c r="N78" s="17"/>
       <c r="O78" s="17"/>
       <c r="P78" s="17"/>
-      <c r="Q78" s="24"/>
+      <c r="Q78" s="23"/>
       <c r="R78" s="8" t="s">
         <v>218</v>
       </c>
@@ -3788,7 +3788,7 @@
       <c r="E79" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G79" s="24"/>
+      <c r="G79" s="23"/>
       <c r="H79" s="17" t="s">
         <v>273</v>
       </c>
@@ -3801,7 +3801,7 @@
       <c r="K79" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="L79" s="24"/>
+      <c r="L79" s="23"/>
       <c r="M79" s="17" t="s">
         <v>273</v>
       </c>
@@ -3814,7 +3814,7 @@
       <c r="P79" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="Q79" s="24"/>
+      <c r="Q79" s="23"/>
       <c r="R79" s="8" t="s">
         <v>293</v>
       </c>
@@ -3856,13 +3856,13 @@
       <c r="F81" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="G81" s="27"/>
-      <c r="L81" s="24"/>
+      <c r="G81" s="26"/>
+      <c r="L81" s="23"/>
       <c r="M81" s="17"/>
       <c r="N81" s="17"/>
       <c r="O81" s="17"/>
       <c r="P81" s="17"/>
-      <c r="Q81" s="24"/>
+      <c r="Q81" s="23"/>
     </row>
     <row r="82" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="7" t="s">
@@ -3879,9 +3879,9 @@
       <c r="F82" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="G82" s="24"/>
-      <c r="L82" s="24"/>
-      <c r="Q82" s="24"/>
+      <c r="G82" s="23"/>
+      <c r="L82" s="23"/>
+      <c r="Q82" s="23"/>
       <c r="R82" s="7" t="s">
         <v>289</v>
       </c>
@@ -3905,13 +3905,13 @@
       <c r="F83" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G83" s="24"/>
-      <c r="L83" s="24"/>
+      <c r="G83" s="23"/>
+      <c r="L83" s="23"/>
       <c r="M83" s="17"/>
       <c r="N83" s="17"/>
       <c r="O83" s="17"/>
       <c r="P83" s="17"/>
-      <c r="Q83" s="24"/>
+      <c r="Q83" s="23"/>
     </row>
     <row r="84" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
@@ -3932,13 +3932,13 @@
       <c r="F84" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="G84" s="27"/>
-      <c r="L84" s="24"/>
+      <c r="G84" s="26"/>
+      <c r="L84" s="23"/>
       <c r="M84" s="17"/>
       <c r="N84" s="17"/>
       <c r="O84" s="17"/>
       <c r="P84" s="17"/>
-      <c r="Q84" s="24"/>
+      <c r="Q84" s="23"/>
       <c r="R84" s="2" t="s">
         <v>219</v>
       </c>
@@ -3960,9 +3960,9 @@
         <v>1</v>
       </c>
       <c r="F85" s="6"/>
-      <c r="G85" s="27"/>
-      <c r="L85" s="24"/>
-      <c r="Q85" s="24"/>
+      <c r="G85" s="26"/>
+      <c r="L85" s="23"/>
+      <c r="Q85" s="23"/>
     </row>
     <row r="86" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
@@ -3983,13 +3983,13 @@
       <c r="F86" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G86" s="24"/>
-      <c r="L86" s="24"/>
+      <c r="G86" s="23"/>
+      <c r="L86" s="23"/>
       <c r="M86" s="17"/>
       <c r="N86" s="17"/>
       <c r="O86" s="17"/>
       <c r="P86" s="17"/>
-      <c r="Q86" s="24"/>
+      <c r="Q86" s="23"/>
     </row>
     <row r="87" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
@@ -4007,13 +4007,13 @@
       <c r="E87" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G87" s="24"/>
-      <c r="L87" s="24"/>
+      <c r="G87" s="23"/>
+      <c r="L87" s="23"/>
       <c r="M87" s="17"/>
       <c r="N87" s="17"/>
       <c r="O87" s="17"/>
       <c r="P87" s="17"/>
-      <c r="Q87" s="24"/>
+      <c r="Q87" s="23"/>
       <c r="R87" s="8" t="s">
         <v>220</v>
       </c>
@@ -4037,13 +4037,13 @@
       <c r="F88" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G88" s="24"/>
-      <c r="L88" s="24"/>
+      <c r="G88" s="23"/>
+      <c r="L88" s="23"/>
       <c r="M88" s="17"/>
       <c r="N88" s="17"/>
       <c r="O88" s="17"/>
       <c r="P88" s="17"/>
-      <c r="Q88" s="24"/>
+      <c r="Q88" s="23"/>
       <c r="R88" s="8" t="s">
         <v>241</v>
       </c>
@@ -4064,7 +4064,7 @@
       <c r="E89" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G89" s="24"/>
+      <c r="G89" s="23"/>
       <c r="H89" s="17" t="s">
         <v>281</v>
       </c>
@@ -4077,7 +4077,7 @@
       <c r="K89" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L89" s="24"/>
+      <c r="L89" s="23"/>
       <c r="M89" s="17" t="s">
         <v>282</v>
       </c>
@@ -4090,7 +4090,7 @@
       <c r="P89" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q89" s="24"/>
+      <c r="Q89" s="23"/>
       <c r="R89" s="2" t="s">
         <v>212</v>
       </c>
@@ -4114,9 +4114,9 @@
       <c r="F90" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="G90" s="24"/>
-      <c r="L90" s="24"/>
-      <c r="Q90" s="24"/>
+      <c r="G90" s="23"/>
+      <c r="L90" s="23"/>
+      <c r="Q90" s="23"/>
       <c r="R90" s="7" t="s">
         <v>217</v>
       </c>
@@ -4140,9 +4140,9 @@
       <c r="F91" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="G91" s="24"/>
-      <c r="L91" s="24"/>
-      <c r="Q91" s="24"/>
+      <c r="G91" s="23"/>
+      <c r="L91" s="23"/>
+      <c r="Q91" s="23"/>
       <c r="R91" s="7" t="s">
         <v>221</v>
       </c>
@@ -4166,9 +4166,9 @@
       <c r="F92" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G92" s="24"/>
-      <c r="L92" s="24"/>
-      <c r="Q92" s="24"/>
+      <c r="G92" s="23"/>
+      <c r="L92" s="23"/>
+      <c r="Q92" s="23"/>
       <c r="R92" s="7" t="s">
         <v>222</v>
       </c>
@@ -4189,7 +4189,7 @@
       <c r="E93" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G93" s="24"/>
+      <c r="G93" s="23"/>
       <c r="H93" s="2" t="s">
         <v>4</v>
       </c>
@@ -4202,7 +4202,7 @@
       <c r="K93" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L93" s="24"/>
+      <c r="L93" s="23"/>
       <c r="M93" s="17" t="s">
         <v>4</v>
       </c>
@@ -4215,7 +4215,7 @@
       <c r="P93" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q93" s="24"/>
+      <c r="Q93" s="23"/>
     </row>
     <row r="94" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
@@ -4233,7 +4233,7 @@
       <c r="E94" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G94" s="24"/>
+      <c r="G94" s="23"/>
       <c r="H94" s="2" t="s">
         <v>4</v>
       </c>
@@ -4246,7 +4246,7 @@
       <c r="K94" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L94" s="24"/>
+      <c r="L94" s="23"/>
       <c r="M94" s="17" t="s">
         <v>4</v>
       </c>
@@ -4259,7 +4259,7 @@
       <c r="P94" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q94" s="24"/>
+      <c r="Q94" s="23"/>
     </row>
     <row r="95" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
@@ -4277,7 +4277,7 @@
       <c r="E95" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G95" s="24"/>
+      <c r="G95" s="23"/>
       <c r="H95" s="2" t="s">
         <v>14</v>
       </c>
@@ -4290,7 +4290,7 @@
       <c r="K95" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L95" s="24"/>
+      <c r="L95" s="23"/>
       <c r="M95" s="17" t="s">
         <v>14</v>
       </c>
@@ -4303,7 +4303,7 @@
       <c r="P95" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q95" s="24"/>
+      <c r="Q95" s="23"/>
     </row>
     <row r="96" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="7" t="s">
@@ -4321,7 +4321,7 @@
       <c r="E96" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G96" s="24"/>
+      <c r="G96" s="23"/>
       <c r="H96" s="7" t="s">
         <v>14</v>
       </c>
@@ -4334,7 +4334,7 @@
       <c r="K96" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L96" s="24"/>
+      <c r="L96" s="23"/>
       <c r="M96" s="7" t="s">
         <v>14</v>
       </c>
@@ -4347,7 +4347,7 @@
       <c r="P96" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Q96" s="24"/>
+      <c r="Q96" s="23"/>
       <c r="R96" s="7" t="s">
         <v>289</v>
       </c>
@@ -4380,7 +4380,7 @@
       <c r="K97" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L97" s="24"/>
+      <c r="L97" s="23"/>
       <c r="M97" s="17" t="s">
         <v>290</v>
       </c>
@@ -4393,7 +4393,7 @@
       <c r="P97" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q97" s="24"/>
+      <c r="Q97" s="23"/>
       <c r="R97"/>
     </row>
     <row r="98" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -4412,7 +4412,7 @@
       <c r="E98" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G98" s="24"/>
+      <c r="G98" s="23"/>
       <c r="H98" s="2" t="s">
         <v>14</v>
       </c>
@@ -4425,7 +4425,7 @@
       <c r="K98" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L98" s="24"/>
+      <c r="L98" s="23"/>
       <c r="M98" s="17" t="s">
         <v>14</v>
       </c>
@@ -4438,7 +4438,7 @@
       <c r="P98" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q98" s="24"/>
+      <c r="Q98" s="23"/>
       <c r="R98" s="2" t="s">
         <v>203</v>
       </c>
@@ -4459,7 +4459,7 @@
       <c r="E99" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G99" s="24"/>
+      <c r="G99" s="23"/>
       <c r="H99" s="2" t="s">
         <v>14</v>
       </c>
@@ -4472,7 +4472,7 @@
       <c r="K99" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L99" s="24"/>
+      <c r="L99" s="23"/>
       <c r="M99" s="17" t="s">
         <v>14</v>
       </c>
@@ -4485,7 +4485,7 @@
       <c r="P99" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q99" s="24"/>
+      <c r="Q99" s="23"/>
     </row>
     <row r="100" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
@@ -4503,7 +4503,7 @@
       <c r="E100" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G100" s="24"/>
+      <c r="G100" s="23"/>
       <c r="H100" s="17" t="s">
         <v>273</v>
       </c>
@@ -4516,7 +4516,7 @@
       <c r="K100" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="L100" s="24"/>
+      <c r="L100" s="23"/>
       <c r="M100" s="17" t="s">
         <v>273</v>
       </c>
@@ -4529,7 +4529,7 @@
       <c r="P100" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="Q100" s="24"/>
+      <c r="Q100" s="23"/>
     </row>
     <row r="101" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
@@ -4550,13 +4550,13 @@
       <c r="F101" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G101" s="24"/>
-      <c r="L101" s="24"/>
+      <c r="G101" s="23"/>
+      <c r="L101" s="23"/>
       <c r="M101" s="17"/>
       <c r="N101" s="17"/>
       <c r="O101" s="17"/>
       <c r="P101" s="17"/>
-      <c r="Q101" s="24"/>
+      <c r="Q101" s="23"/>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R102"/>

</xml_diff>

<commit_message>
Fix: Missing Taggedvalue report in doc #45 Resolved https://github.com/Imvertor/Imvertor-Maven/issues/45
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="319">
   <si>
     <t>Name</t>
   </si>
@@ -970,6 +970,18 @@
   </si>
   <si>
     <t>LM: docrelease</t>
+  </si>
+  <si>
+    <t>messagecollapsekeys</t>
+  </si>
+  <si>
+    <t>Yes if similar messages should be collapsed. No if each message is to be represented in the report.</t>
+  </si>
+  <si>
+    <t>[system/message-collapse-keys]</t>
+  </si>
+  <si>
+    <t>since 1.47</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1133,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1187,6 +1199,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1481,13 +1496,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R123"/>
+  <dimension ref="A1:R124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="N57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="R61" sqref="R61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1497,7 +1512,7 @@
     <col min="3" max="3" width="50.69140625" customWidth="1"/>
     <col min="4" max="4" width="13.23046875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="17.3828125" customWidth="1"/>
+    <col min="6" max="6" width="30.53515625" customWidth="1"/>
     <col min="7" max="7" width="3.921875" style="25" customWidth="1"/>
     <col min="8" max="8" width="18.4609375" customWidth="1"/>
     <col min="9" max="9" width="17.61328125" bestFit="1" customWidth="1"/>
@@ -1698,16 +1713,16 @@
       <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="27" t="b">
+      <c r="D7" s="28" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1725,10 +1740,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
       <c r="G8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
@@ -2583,16 +2598,16 @@
       </c>
     </row>
     <row r="38" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="27" t="b">
+      <c r="D38" s="28" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="2" t="b">
@@ -2610,10 +2625,10 @@
       <c r="Q38" s="23"/>
     </row>
     <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
       <c r="G39" s="23"/>
       <c r="L39" s="23"/>
       <c r="M39" s="17"/>
@@ -3202,143 +3217,142 @@
       <c r="P59" s="17"/>
       <c r="Q59" s="23"/>
     </row>
-    <row r="60" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="2" t="s">
+    <row r="60" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A60" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="B60" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="D60" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="G60" s="23"/>
+      <c r="L60" s="23"/>
+      <c r="Q60" s="23"/>
+      <c r="R60" s="27" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E60" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G60" s="23"/>
-      <c r="H60" s="17" t="s">
+      <c r="D61" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E61" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" s="23"/>
+      <c r="H61" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I60" s="17" t="s">
+      <c r="I61" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J60" s="17" t="s">
+      <c r="J61" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K60" s="17" t="s">
+      <c r="K61" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L60" s="23"/>
-      <c r="M60" s="17" t="s">
+      <c r="L61" s="23"/>
+      <c r="M61" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N60" s="17" t="s">
+      <c r="N61" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O60" s="17" t="s">
+      <c r="O61" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P60" s="17" t="s">
+      <c r="P61" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q60" s="23"/>
-    </row>
-    <row r="61" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="2" t="s">
+      <c r="Q61" s="23"/>
+    </row>
+    <row r="62" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D61" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G61" s="23"/>
-      <c r="L61" s="23"/>
-      <c r="M61" s="17"/>
-      <c r="N61" s="17"/>
-      <c r="O61" s="17"/>
-      <c r="P61" s="17"/>
-      <c r="Q61" s="23"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
+      <c r="D62" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" s="23"/>
+      <c r="L62" s="23"/>
+      <c r="M62" s="17"/>
+      <c r="N62" s="17"/>
+      <c r="O62" s="17"/>
+      <c r="P62" s="17"/>
+      <c r="Q62" s="23"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
         <v>72</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>5</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>73</v>
       </c>
-      <c r="D62" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" t="s">
-        <v>4</v>
-      </c>
-      <c r="R62"/>
-    </row>
-    <row r="63" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D63" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G63" s="23"/>
-      <c r="L63" s="23"/>
-      <c r="M63" s="17"/>
-      <c r="N63" s="17"/>
-      <c r="O63" s="17"/>
-      <c r="P63" s="17"/>
-      <c r="Q63" s="23"/>
+      <c r="D63" t="b">
+        <v>1</v>
+      </c>
+      <c r="E63" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>4</v>
+      </c>
+      <c r="R63"/>
     </row>
     <row r="64" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
-        <v>74</v>
+        <v>233</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>75</v>
+        <v>247</v>
       </c>
       <c r="D64" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G64" s="23"/>
       <c r="L64" s="23"/>
@@ -3348,580 +3362,580 @@
       <c r="P64" s="17"/>
       <c r="Q64" s="23"/>
     </row>
-    <row r="65" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D65" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" s="23"/>
+      <c r="L65" s="23"/>
+      <c r="M65" s="17"/>
+      <c r="N65" s="17"/>
+      <c r="O65" s="17"/>
+      <c r="P65" s="17"/>
+      <c r="Q65" s="23"/>
+    </row>
+    <row r="66" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G65" s="23"/>
-      <c r="H65" s="17" t="s">
+      <c r="D66" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" s="23"/>
+      <c r="H66" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I65" s="17" t="s">
+      <c r="I66" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J65" s="17" t="s">
+      <c r="J66" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K65" s="17" t="s">
+      <c r="K66" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L65" s="23"/>
-      <c r="M65" s="17" t="s">
+      <c r="L66" s="23"/>
+      <c r="M66" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N65" s="17" t="s">
+      <c r="N66" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O65" s="17" t="s">
+      <c r="O66" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P65" s="17" t="s">
+      <c r="P66" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q65" s="23"/>
-    </row>
-    <row r="66" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" s="2" t="s">
+      <c r="Q66" s="23"/>
+    </row>
+    <row r="67" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="2" t="s">
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="G66" s="23"/>
-      <c r="L66" s="23"/>
-      <c r="M66" s="17"/>
-      <c r="N66" s="17"/>
-      <c r="O66" s="17"/>
-      <c r="P66" s="17"/>
-      <c r="Q66" s="23"/>
-    </row>
-    <row r="67" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D67" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>273</v>
       </c>
       <c r="G67" s="23"/>
       <c r="L67" s="23"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
       <c r="Q67" s="23"/>
-      <c r="R67" s="7" t="s">
+    </row>
+    <row r="68" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D68" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E68" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G68" s="23"/>
+      <c r="L68" s="23"/>
+      <c r="Q68" s="23"/>
+      <c r="R68" s="7" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="2" t="s">
+      <c r="D69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G68" s="23"/>
-      <c r="H68" s="2" t="s">
+      <c r="G69" s="23"/>
+      <c r="H69" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L68" s="23"/>
-      <c r="M68" s="17" t="s">
+      <c r="L69" s="23"/>
+      <c r="M69" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N68" s="17" t="s">
+      <c r="N69" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O68" s="17" t="s">
+      <c r="O69" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P68" s="17" t="s">
+      <c r="P69" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q68" s="23"/>
-    </row>
-    <row r="69" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A69" s="7" t="s">
+      <c r="Q69" s="23"/>
+    </row>
+    <row r="70" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A70" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B70" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C70" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D69" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="7" t="s">
+      <c r="D70" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="G69" s="23"/>
-      <c r="L69" s="23"/>
-      <c r="Q69" s="23"/>
-      <c r="R69" s="8" t="s">
+      <c r="G70" s="23"/>
+      <c r="L70" s="23"/>
+      <c r="Q70" s="23"/>
+      <c r="R70" s="8" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="70" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D70" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G70" s="23"/>
-      <c r="H70" s="17" t="s">
+      <c r="D71" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71" s="23"/>
+      <c r="H71" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="I70" s="17" t="s">
+      <c r="I71" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="J70" s="17" t="s">
+      <c r="J71" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="K70" s="17" t="s">
+      <c r="K71" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="L70" s="23"/>
-      <c r="M70" s="17" t="s">
+      <c r="L71" s="23"/>
+      <c r="M71" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="N70" s="17" t="s">
+      <c r="N71" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="O70" s="17" t="s">
+      <c r="O71" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="P70" s="17" t="s">
+      <c r="P71" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="Q70" s="23"/>
-    </row>
-    <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A71" s="2" t="s">
+      <c r="Q71" s="23"/>
+    </row>
+    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D71" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="2" t="s">
+      <c r="D72" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G71" s="23"/>
-      <c r="L71" s="23"/>
-      <c r="M71" s="17"/>
-      <c r="N71" s="17"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="17"/>
-      <c r="Q71" s="23"/>
-    </row>
-    <row r="72" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A72" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="G72" s="23"/>
       <c r="L72" s="23"/>
+      <c r="M72" s="17"/>
+      <c r="N72" s="17"/>
+      <c r="O72" s="17"/>
+      <c r="P72" s="17"/>
       <c r="Q72" s="23"/>
-      <c r="R72" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="73" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A73" s="7" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="D73" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E73" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="G73" s="23"/>
       <c r="L73" s="23"/>
       <c r="Q73" s="23"/>
-      <c r="R73" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" s="2" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A74" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D74" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E74" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>94</v>
+      <c r="R73" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A74" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D74" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G74" s="23"/>
       <c r="L74" s="23"/>
-      <c r="M74" s="17"/>
-      <c r="N74" s="17"/>
-      <c r="O74" s="17"/>
-      <c r="P74" s="17"/>
       <c r="Q74" s="23"/>
-    </row>
-    <row r="75" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A75" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="D75" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" s="17" t="s">
-        <v>4</v>
+      <c r="R74" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" s="2" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A75" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D75" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G75" s="23"/>
       <c r="L75" s="23"/>
+      <c r="M75" s="17"/>
+      <c r="N75" s="17"/>
+      <c r="O75" s="17"/>
+      <c r="P75" s="17"/>
       <c r="Q75" s="23"/>
     </row>
-    <row r="76" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="7" t="s">
+    <row r="76" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A76" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="D76" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" s="23"/>
+      <c r="L76" s="23"/>
+      <c r="Q76" s="23"/>
+    </row>
+    <row r="77" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="B76" s="19"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G76" s="23"/>
-      <c r="H76" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I76" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J76" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K76" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L76" s="23"/>
-      <c r="M76" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N76" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O76" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P76" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q76" s="23"/>
-    </row>
-    <row r="77" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A77" s="20" t="s">
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G77" s="23"/>
+      <c r="H77" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J77" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K77" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L77" s="23"/>
+      <c r="M77" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N77" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O77" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P77" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q77" s="23"/>
+    </row>
+    <row r="78" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A78" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B78" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="20" t="s">
+      <c r="C78" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="D77" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G77" s="23"/>
-      <c r="L77" s="23"/>
-      <c r="Q77" s="23"/>
-    </row>
-    <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>4</v>
+      <c r="D78" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G78" s="23"/>
       <c r="L78" s="23"/>
-      <c r="M78" s="17"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="17"/>
-      <c r="P78" s="17"/>
       <c r="Q78" s="23"/>
-      <c r="R78" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="79" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D79" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G79" s="23"/>
-      <c r="H79" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I79" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J79" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K79" s="17" t="s">
-        <v>273</v>
-      </c>
       <c r="L79" s="23"/>
-      <c r="M79" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="N79" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="O79" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="P79" s="17" t="s">
-        <v>273</v>
-      </c>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="17"/>
       <c r="Q79" s="23"/>
       <c r="R79" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D80" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G80" s="23"/>
+      <c r="H80" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="I80" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="J80" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="K80" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="L80" s="23"/>
+      <c r="M80" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N80" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O80" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="P80" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q80" s="23"/>
+      <c r="R80" s="8" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A80" t="s">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
         <v>198</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>199</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>200</v>
       </c>
-      <c r="D80" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" t="b">
-        <v>1</v>
-      </c>
-      <c r="R80"/>
-    </row>
-    <row r="81" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A81" s="13" t="s">
+      <c r="D81" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
+      <c r="R81"/>
+    </row>
+    <row r="82" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A82" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="B81" s="13" t="s">
+      <c r="B82" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="C81" s="13" t="s">
+      <c r="C82" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="D81" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E81" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="6" t="s">
+      <c r="D82" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="G81" s="26"/>
-      <c r="L81" s="23"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
-      <c r="Q81" s="23"/>
-    </row>
-    <row r="82" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="7" t="s">
+      <c r="G82" s="26"/>
+      <c r="L82" s="23"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="17"/>
+      <c r="Q82" s="23"/>
+    </row>
+    <row r="83" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="7" t="s">
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="G82" s="23"/>
-      <c r="L82" s="23"/>
-      <c r="Q82" s="23"/>
-      <c r="R82" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G83" s="23"/>
       <c r="L83" s="23"/>
-      <c r="M83" s="17"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
-      <c r="P83" s="17"/>
       <c r="Q83" s="23"/>
-    </row>
-    <row r="84" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="R83" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D84" s="2" t="b">
         <v>0</v>
@@ -3929,83 +3943,86 @@
       <c r="E84" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F84" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G84" s="26"/>
+      <c r="F84" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G84" s="23"/>
       <c r="L84" s="23"/>
       <c r="M84" s="17"/>
       <c r="N84" s="17"/>
       <c r="O84" s="17"/>
       <c r="P84" s="17"/>
       <c r="Q84" s="23"/>
-      <c r="R84" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A85" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="B85" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="D85" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E85" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="6"/>
+    </row>
+    <row r="85" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>287</v>
+      </c>
       <c r="G85" s="26"/>
       <c r="L85" s="23"/>
+      <c r="M85" s="17"/>
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="17"/>
       <c r="Q85" s="23"/>
-    </row>
-    <row r="86" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
+      <c r="R85" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A86" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="D86" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" s="6"/>
+      <c r="G86" s="26"/>
+      <c r="L86" s="23"/>
+      <c r="Q86" s="23"/>
+    </row>
+    <row r="87" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G86" s="23"/>
-      <c r="L86" s="23"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
-      <c r="Q86" s="23"/>
-    </row>
-    <row r="87" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="D87" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E87" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G87" s="23"/>
       <c r="L87" s="23"/>
@@ -4014,28 +4031,22 @@
       <c r="O87" s="17"/>
       <c r="P87" s="17"/>
       <c r="Q87" s="23"/>
-      <c r="R87" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="88" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
-        <v>104</v>
+        <v>201</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>107</v>
+        <v>202</v>
       </c>
       <c r="D88" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="G88" s="23"/>
       <c r="L88" s="23"/>
@@ -4045,91 +4056,95 @@
       <c r="P88" s="17"/>
       <c r="Q88" s="23"/>
       <c r="R88" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G89" s="23"/>
+      <c r="L89" s="23"/>
+      <c r="M89" s="17"/>
+      <c r="N89" s="17"/>
+      <c r="O89" s="17"/>
+      <c r="P89" s="17"/>
+      <c r="Q89" s="23"/>
+      <c r="R89" s="8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="89" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
+    <row r="90" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G89" s="23"/>
-      <c r="H89" s="17" t="s">
+      <c r="D90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" s="23"/>
+      <c r="H90" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I89" s="17" t="s">
+      <c r="I90" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J89" s="17" t="s">
+      <c r="J90" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K89" s="17" t="s">
+      <c r="K90" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L89" s="23"/>
-      <c r="M89" s="17" t="s">
+      <c r="L90" s="23"/>
+      <c r="M90" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N89" s="17" t="s">
+      <c r="N90" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O89" s="17" t="s">
+      <c r="O90" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P89" s="17" t="s">
+      <c r="P90" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q89" s="23"/>
-      <c r="R89" s="2" t="s">
+      <c r="Q90" s="23"/>
+      <c r="R90" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="90" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A90" s="7" t="s">
+    <row r="91" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A91" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B91" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C91" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="D90" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="G90" s="23"/>
-      <c r="L90" s="23"/>
-      <c r="Q90" s="23"/>
-      <c r="R90" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="D91" s="7" t="b">
         <v>1</v>
@@ -4144,91 +4159,73 @@
       <c r="L91" s="23"/>
       <c r="Q91" s="23"/>
       <c r="R91" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="92" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D92" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E92" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>14</v>
+        <v>234</v>
       </c>
       <c r="G92" s="23"/>
       <c r="L92" s="23"/>
       <c r="Q92" s="23"/>
       <c r="R92" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D93" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93" s="23"/>
+      <c r="L93" s="23"/>
+      <c r="Q93" s="23"/>
+      <c r="R93" s="7" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D93" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G93" s="23"/>
-      <c r="H93" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I93" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J93" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K93" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L93" s="23"/>
-      <c r="M93" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N93" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O93" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P93" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q93" s="23"/>
     </row>
     <row r="94" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>288</v>
+        <v>117</v>
       </c>
       <c r="D94" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94" s="2" t="b">
         <v>1</v>
@@ -4263,23 +4260,23 @@
     </row>
     <row r="95" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>120</v>
+        <v>288</v>
       </c>
       <c r="D95" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G95" s="23"/>
       <c r="H95" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>4</v>
@@ -4292,7 +4289,7 @@
       </c>
       <c r="L95" s="23"/>
       <c r="M95" s="17" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N95" s="17" t="s">
         <v>4</v>
@@ -4305,129 +4302,128 @@
       </c>
       <c r="Q95" s="23"/>
     </row>
-    <row r="96" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A96" s="7" t="s">
+    <row r="96" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D96" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G96" s="23"/>
+      <c r="H96" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L96" s="23"/>
+      <c r="M96" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N96" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O96" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P96" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q96" s="23"/>
+    </row>
+    <row r="97" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A97" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B96" s="7" t="s">
+      <c r="B97" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C96" s="7" t="s">
+      <c r="C97" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D96" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G96" s="23"/>
-      <c r="H96" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I96" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J96" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K96" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L96" s="23"/>
-      <c r="M96" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N96" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O96" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P96" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q96" s="23"/>
-      <c r="R96" s="7" t="s">
+      <c r="D97" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G97" s="23"/>
+      <c r="H97" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I97" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J97" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K97" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L97" s="23"/>
+      <c r="M97" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N97" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O97" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P97" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q97" s="23"/>
+      <c r="R97" s="7" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A97" t="s">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A98" t="s">
         <v>121</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B98" t="s">
         <v>122</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C98" t="s">
         <v>123</v>
       </c>
-      <c r="D97" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" t="b">
-        <v>0</v>
-      </c>
-      <c r="H97" s="16" t="s">
+      <c r="D98" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" t="b">
+        <v>0</v>
+      </c>
+      <c r="H98" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="I97" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J97" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K97" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L97" s="23"/>
-      <c r="M97" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="N97" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O97" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P97" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q97" s="23"/>
-      <c r="R97"/>
-    </row>
-    <row r="98" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D98" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G98" s="23"/>
-      <c r="H98" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K98" s="2" t="s">
+      <c r="I98" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J98" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K98" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L98" s="23"/>
       <c r="M98" s="17" t="s">
-        <v>14</v>
+        <v>290</v>
       </c>
       <c r="N98" s="17" t="s">
         <v>4</v>
@@ -4439,19 +4435,17 @@
         <v>4</v>
       </c>
       <c r="Q98" s="23"/>
-      <c r="R98" s="2" t="s">
-        <v>203</v>
-      </c>
+      <c r="R98"/>
     </row>
     <row r="99" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D99" s="2" t="b">
         <v>1</v>
@@ -4486,80 +4480,124 @@
         <v>4</v>
       </c>
       <c r="Q99" s="23"/>
+      <c r="R99" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="100" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>127</v>
+        <v>259</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D100" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E100" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100" s="23"/>
-      <c r="H100" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I100" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J100" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K100" s="17" t="s">
-        <v>273</v>
+      <c r="H100" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K100" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L100" s="23"/>
       <c r="M100" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N100" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O100" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P100" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q100" s="23"/>
+    </row>
+    <row r="101" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D101" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G101" s="23"/>
+      <c r="H101" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="N100" s="17" t="s">
+      <c r="I101" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="O100" s="17" t="s">
+      <c r="J101" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="P100" s="17" t="s">
+      <c r="K101" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="Q100" s="23"/>
-    </row>
-    <row r="101" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A101" s="2" t="s">
+      <c r="L101" s="23"/>
+      <c r="M101" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N101" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O101" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="P101" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q101" s="23"/>
+    </row>
+    <row r="102" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D101" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E101" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F101" s="2" t="s">
+      <c r="D102" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G101" s="23"/>
-      <c r="L101" s="23"/>
-      <c r="M101" s="17"/>
-      <c r="N101" s="17"/>
-      <c r="O101" s="17"/>
-      <c r="P101" s="17"/>
-      <c r="Q101" s="23"/>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R102"/>
+      <c r="G102" s="23"/>
+      <c r="L102" s="23"/>
+      <c r="M102" s="17"/>
+      <c r="N102" s="17"/>
+      <c r="O102" s="17"/>
+      <c r="P102" s="17"/>
+      <c r="Q102" s="23"/>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R103"/>
@@ -4623,6 +4661,9 @@
     </row>
     <row r="123" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R123"/>
+    </row>
+    <row r="124" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R124"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Choice elementen mogen wèl gelijk (data)type zijn https://github.com/Imvertor/Imvertor-Maven/issues/44
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="321">
   <si>
     <t>Name</t>
   </si>
@@ -982,6 +982,12 @@
   </si>
   <si>
     <t>since 1.47</t>
+  </si>
+  <si>
+    <t>allowscalarinunion</t>
+  </si>
+  <si>
+    <t>Yes if scalar values may occur in unions</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1139,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1202,6 +1208,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1496,13 +1512,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R124"/>
+  <dimension ref="A1:U125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="N57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R61" sqref="R61"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1527,7 +1543,7 @@
     <col min="18" max="18" width="27.3046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1577,7 +1593,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:21" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
       <c r="G2" s="22"/>
       <c r="H2" s="3" t="s">
@@ -1608,7 +1624,7 @@
       <c r="Q2" s="22"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:21" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>151</v>
       </c>
@@ -1632,7 +1648,7 @@
       <c r="P3" s="17"/>
       <c r="Q3" s="23"/>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1662,7 +1678,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1692,58 +1708,77 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="30" t="s">
+        <v>319</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>320</v>
+      </c>
+      <c r="D6" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="31"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+    </row>
+    <row r="7" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="Q6" s="23"/>
-    </row>
-    <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="b">
+      <c r="D7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="23"/>
       <c r="L7" s="23"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
       <c r="Q7" s="23"/>
-      <c r="R7" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
+    </row>
+    <row r="8" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="G8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
@@ -1751,228 +1786,217 @@
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="23"/>
-    </row>
-    <row r="9" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D9" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="R8" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
       <c r="G9" s="23"/>
       <c r="L9" s="23"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
       <c r="Q9" s="23"/>
     </row>
-    <row r="10" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D10" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E10" s="7" t="b">
         <v>1</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G10" s="23"/>
       <c r="L10" s="23"/>
       <c r="Q10" s="23"/>
     </row>
-    <row r="11" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="1:21" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A11" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>4</v>
+      <c r="C11" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G11" s="23"/>
       <c r="L11" s="23"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
       <c r="Q11" s="23"/>
-      <c r="R11" s="7"/>
-    </row>
-    <row r="12" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="D12" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12" t="b">
-        <v>1</v>
+    </row>
+    <row r="12" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G12" s="23"/>
       <c r="L12" s="23"/>
-      <c r="M12" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="O12" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="P12" s="17" t="s">
-        <v>291</v>
-      </c>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
       <c r="Q12" s="23"/>
-      <c r="R12" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>14</v>
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="D13" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="G13" s="23"/>
       <c r="L13" s="23"/>
+      <c r="M13" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="N13" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="P13" s="17" t="s">
+        <v>291</v>
+      </c>
       <c r="Q13" s="23"/>
-    </row>
-    <row r="14" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
+      <c r="R13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="Q14" s="23"/>
+    </row>
+    <row r="15" spans="1:21" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="2" t="s">
+      <c r="D15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="L14" s="23"/>
-      <c r="M14" s="17" t="s">
+      <c r="L15" s="23"/>
+      <c r="M15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N14" s="17" t="s">
+      <c r="N15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O14" s="17" t="s">
+      <c r="O15" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="P14" s="17" t="s">
+      <c r="P15" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="2" t="s">
+      <c r="Q15" s="23"/>
+      <c r="R15" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="D16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="G15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="23"/>
-    </row>
-    <row r="16" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="G16" s="23"/>
       <c r="L16" s="23"/>
@@ -1982,12 +2006,16 @@
       <c r="P16" s="17"/>
       <c r="Q16" s="23"/>
     </row>
-    <row r="17" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+        <v>237</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>245</v>
+      </c>
       <c r="D17" s="2" t="b">
         <v>1</v>
       </c>
@@ -1995,12 +2023,9 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="G17" s="23"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
       <c r="L17" s="23"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
@@ -2008,23 +2033,25 @@
       <c r="P17" s="17"/>
       <c r="Q17" s="23"/>
     </row>
-    <row r="18" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>162</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F18" s="2" t="s">
+        <v>273</v>
+      </c>
       <c r="G18" s="23"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
       <c r="L18" s="23"/>
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
@@ -2034,22 +2061,19 @@
     </row>
     <row r="19" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E19" s="2" t="b">
         <v>1</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>274</v>
       </c>
       <c r="G19" s="23"/>
       <c r="L19" s="23"/>
@@ -2059,15 +2083,15 @@
       <c r="P19" s="17"/>
       <c r="Q19" s="23"/>
     </row>
-    <row r="20" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
@@ -2076,7 +2100,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G20" s="23"/>
       <c r="L20" s="23"/>
@@ -2086,146 +2110,129 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="23"/>
     </row>
-    <row r="21" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="G21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="23"/>
+    </row>
+    <row r="22" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="2" t="s">
+      <c r="D22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="23"/>
+      <c r="H22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L21" s="23"/>
-      <c r="M21" s="17" t="s">
+      <c r="I22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="23"/>
+      <c r="M22" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="N21" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O21" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P21" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q21" s="23"/>
-    </row>
-    <row r="22" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A22" s="7" t="s">
+      <c r="N22" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P22" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="23"/>
+    </row>
+    <row r="23" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A23" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="Q22" s="23"/>
-    </row>
-    <row r="23" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>164</v>
+        <v>24</v>
       </c>
       <c r="D23" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="7" t="b">
         <v>1</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G23" s="23"/>
       <c r="L23" s="23"/>
       <c r="Q23" s="23"/>
     </row>
-    <row r="24" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="Q24" s="23"/>
+    </row>
+    <row r="25" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L24" s="23"/>
-      <c r="M24" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N24" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O24" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P24" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q24" s="23"/>
-    </row>
-    <row r="25" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D25" s="2" t="b">
         <v>0</v>
@@ -2238,7 +2245,7 @@
         <v>14</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>4</v>
@@ -2251,7 +2258,7 @@
         <v>14</v>
       </c>
       <c r="N25" s="17" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="O25" s="17" t="s">
         <v>4</v>
@@ -2261,139 +2268,163 @@
       </c>
       <c r="Q25" s="23"/>
     </row>
-    <row r="26" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D26" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="23"/>
+      <c r="H26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="23"/>
+      <c r="I26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L26" s="23"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
+      <c r="M26" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="Q26" s="23"/>
-      <c r="R26" s="8" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="27" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D27" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G27" s="23"/>
-      <c r="H27" s="2" t="s">
+      <c r="D28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" s="23"/>
+      <c r="H28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" s="23"/>
-      <c r="M27" s="17" t="s">
+      <c r="I28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" s="23"/>
+      <c r="M28" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="N27" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O27" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P27" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q27" s="23"/>
-    </row>
-    <row r="28" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
+      <c r="N28" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O28" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="23"/>
+    </row>
+    <row r="29" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2" t="s">
+      <c r="D29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="G28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D29" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="7" t="b">
-        <v>1</v>
       </c>
       <c r="G29" s="23"/>
       <c r="L29" s="23"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
       <c r="Q29" s="23"/>
-    </row>
-    <row r="30" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R29" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A30" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D30" s="7" t="b">
         <v>0</v>
@@ -2407,159 +2438,156 @@
     </row>
     <row r="31" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="7" t="s">
-        <v>35</v>
+        <v>168</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>5</v>
+        <v>169</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="D31" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E31" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="G31" s="23"/>
       <c r="L31" s="23"/>
       <c r="Q31" s="23"/>
     </row>
-    <row r="32" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="2" t="s">
+    <row r="32" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2" t="s">
+      <c r="C32" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G32" s="23"/>
       <c r="L32" s="23"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
       <c r="Q32" s="23"/>
     </row>
-    <row r="33" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A33" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="7" t="s">
+    <row r="33" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E33" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F33" s="7" t="s">
+      <c r="C33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G33" s="23"/>
       <c r="L33" s="23"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
       <c r="Q33" s="23"/>
     </row>
-    <row r="34" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A34" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="Q34" s="23"/>
+    </row>
+    <row r="35" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G34" s="23"/>
-      <c r="H34" s="17" t="s">
+      <c r="D35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" s="23"/>
+      <c r="H35" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="I34" s="17" t="s">
+      <c r="I35" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="J34" s="17" t="s">
+      <c r="J35" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K34" s="17" t="s">
+      <c r="K35" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="L34" s="23"/>
-      <c r="M34" s="17" t="s">
+      <c r="L35" s="23"/>
+      <c r="M35" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="N34" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O34" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P34" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q34" s="23"/>
-    </row>
-    <row r="35" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="7" t="s">
+      <c r="N35" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O35" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P35" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q35" s="23"/>
+    </row>
+    <row r="36" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D35" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="Q35" s="23"/>
-    </row>
-    <row r="36" spans="1:18" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A36" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>44</v>
+        <v>172</v>
       </c>
       <c r="D36" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>14</v>
@@ -2567,19 +2595,16 @@
       <c r="G36" s="23"/>
       <c r="L36" s="23"/>
       <c r="Q36" s="23"/>
-      <c r="R36" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="37" spans="1:18" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A37" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D37" s="7" t="b">
         <v>1</v>
@@ -2588,47 +2613,60 @@
         <v>0</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>234</v>
+        <v>14</v>
       </c>
       <c r="G37" s="23"/>
       <c r="L37" s="23"/>
       <c r="Q37" s="23"/>
       <c r="R37" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>14</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A38" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>234</v>
       </c>
       <c r="G38" s="23"/>
       <c r="L38" s="23"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
       <c r="Q38" s="23"/>
+      <c r="R38" s="7" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
+      <c r="A39" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G39" s="23"/>
       <c r="L39" s="23"/>
       <c r="M39" s="17"/>
@@ -2637,22 +2675,11 @@
       <c r="P39" s="17"/>
       <c r="Q39" s="23"/>
     </row>
-    <row r="40" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A40" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D40" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="40" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="32"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
       <c r="G40" s="23"/>
       <c r="L40" s="23"/>
       <c r="M40" s="17"/>
@@ -2661,21 +2688,21 @@
       <c r="P40" s="17"/>
       <c r="Q40" s="23"/>
     </row>
-    <row r="41" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
-        <v>50</v>
+        <v>173</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>51</v>
+        <v>175</v>
       </c>
       <c r="D41" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="23"/>
       <c r="L41" s="23"/>
@@ -2685,15 +2712,15 @@
       <c r="P41" s="17"/>
       <c r="Q41" s="23"/>
     </row>
-    <row r="42" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D42" s="2" t="b">
         <v>0</v>
@@ -2701,95 +2728,95 @@
       <c r="E42" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="G42" s="26"/>
+      <c r="G42" s="23"/>
       <c r="L42" s="23"/>
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
       <c r="O42" s="17"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="23"/>
-      <c r="R42" s="2" t="s">
+    </row>
+    <row r="43" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G43" s="26"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
+      <c r="Q43" s="23"/>
+      <c r="R43" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="2" t="s">
+    <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F43" s="6"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="17" t="s">
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I43" s="17" t="s">
+      <c r="I44" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J43" s="17" t="s">
+      <c r="J44" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K43" s="17" t="s">
+      <c r="K44" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L43" s="23"/>
-      <c r="M43" s="17" t="s">
+      <c r="L44" s="23"/>
+      <c r="M44" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N43" s="17" t="s">
+      <c r="N44" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O43" s="17" t="s">
+      <c r="O44" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P43" s="17" t="s">
+      <c r="P44" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q43" s="23"/>
-    </row>
-    <row r="44" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="7" t="s">
+      <c r="Q44" s="23"/>
+    </row>
+    <row r="45" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B45" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C45" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D44" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44"/>
-    </row>
-    <row r="45" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A45" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="D45" s="7" t="b">
         <v>0</v>
       </c>
@@ -2797,77 +2824,78 @@
         <v>1</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="G45" s="23"/>
       <c r="L45" s="23"/>
       <c r="Q45" s="23"/>
-    </row>
-    <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>14</v>
+      <c r="R45"/>
+    </row>
+    <row r="46" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A46" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D46" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="G46" s="23"/>
       <c r="L46" s="23"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="17"/>
-      <c r="O46" s="17"/>
-      <c r="P46" s="17"/>
       <c r="Q46" s="23"/>
     </row>
-    <row r="47" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="7" t="s">
+    <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D47" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" s="7" t="s">
+      <c r="C47" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G47" s="23"/>
       <c r="L47" s="23"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
       <c r="Q47" s="23"/>
     </row>
-    <row r="48" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D48" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>14</v>
@@ -2875,25 +2903,22 @@
       <c r="G48" s="23"/>
       <c r="L48" s="23"/>
       <c r="Q48" s="23"/>
-      <c r="R48" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="49" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A49" s="7" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>182</v>
+        <v>60</v>
       </c>
       <c r="D49" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E49" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>14</v>
@@ -2901,313 +2926,309 @@
       <c r="G49" s="23"/>
       <c r="L49" s="23"/>
       <c r="Q49" s="23"/>
-    </row>
-    <row r="50" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="R49" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D50" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="23"/>
+      <c r="L50" s="23"/>
+      <c r="Q50" s="23"/>
+    </row>
+    <row r="51" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A51" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B51" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G50" s="23"/>
-      <c r="H50" s="18" t="s">
+      <c r="G51" s="23"/>
+      <c r="H51" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="I50" s="18" t="s">
+      <c r="I51" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="J50" s="18" t="s">
+      <c r="J51" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="K50" s="18" t="s">
+      <c r="K51" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="L50" s="23"/>
-      <c r="M50" s="18" t="s">
+      <c r="L51" s="23"/>
+      <c r="M51" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="N50" s="18" t="s">
+      <c r="N51" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="O50" s="18" t="s">
+      <c r="O51" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="P50" s="18" t="s">
+      <c r="P51" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="Q50" s="23"/>
-    </row>
-    <row r="51" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A51" s="7" t="s">
+      <c r="Q51" s="23"/>
+    </row>
+    <row r="52" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A52" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B52" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C52" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D51" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G51" s="23"/>
-      <c r="H51" s="7" t="s">
+      <c r="D52" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" s="23"/>
+      <c r="H52" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="I51" s="7" t="s">
+      <c r="I52" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="J51" s="7" t="s">
+      <c r="J52" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="K51" s="7" t="s">
+      <c r="K52" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="L51" s="23"/>
-      <c r="M51" s="7" t="s">
+      <c r="L52" s="23"/>
+      <c r="M52" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="N51" s="7" t="s">
+      <c r="N52" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="O51" s="7" t="s">
+      <c r="O52" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="P51" s="7" t="s">
+      <c r="P52" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="Q51" s="23"/>
-    </row>
-    <row r="52" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="7" t="s">
+      <c r="Q52" s="23"/>
+    </row>
+    <row r="53" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B53" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C53" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="D52" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E52" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="7" t="s">
+      <c r="D53" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E53" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="G52" s="23"/>
-      <c r="L52" s="23"/>
-      <c r="Q52" s="23"/>
-    </row>
-    <row r="53" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A53" s="15" t="s">
+      <c r="G53" s="23"/>
+      <c r="L53" s="23"/>
+      <c r="Q53" s="23"/>
+    </row>
+    <row r="54" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A54" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B54" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C54" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="D53" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" s="15" t="s">
+      <c r="D54" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="G53" s="24"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="24"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="24"/>
-      <c r="R53" s="15" t="s">
+      <c r="G54" s="24"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="24"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="24"/>
+      <c r="R54" s="15" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="54" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A54" s="7" t="s">
+    <row r="55" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A55" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B55" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D54" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F54" s="7" t="s">
+      <c r="D55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="G54" s="23"/>
-      <c r="L54" s="23"/>
-      <c r="Q54" s="23"/>
-      <c r="R54" s="7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D55" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="G55" s="23"/>
       <c r="L55" s="23"/>
       <c r="Q55" s="23"/>
       <c r="R55" s="7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D56" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="G56" s="23"/>
       <c r="L56" s="23"/>
       <c r="Q56" s="23"/>
       <c r="R56" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A57" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E57" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G57" s="23"/>
+      <c r="L57" s="23"/>
+      <c r="Q57" s="23"/>
+      <c r="R57" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="57" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A58" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D57" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G57" s="23"/>
-      <c r="H57" s="2" t="s">
+      <c r="D58" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" s="23"/>
+      <c r="H58" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="I57" s="17" t="s">
+      <c r="I58" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="J57" s="17" t="s">
+      <c r="J58" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="K57" s="17" t="s">
+      <c r="K58" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="L57" s="23"/>
-      <c r="M57" s="17" t="s">
+      <c r="L58" s="23"/>
+      <c r="M58" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="N57" s="17" t="s">
+      <c r="N58" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="O57" s="17" t="s">
+      <c r="O58" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="P57" s="17" t="s">
+      <c r="P58" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="Q57" s="23"/>
-      <c r="R57" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A58" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D58" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G58" s="23"/>
-      <c r="L58" s="23"/>
-      <c r="M58" s="17"/>
-      <c r="N58" s="17"/>
-      <c r="O58" s="17"/>
-      <c r="P58" s="17"/>
       <c r="Q58" s="23"/>
       <c r="R58" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>189</v>
+        <v>10</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
       <c r="D59" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E59" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>214</v>
+        <v>280</v>
       </c>
       <c r="G59" s="23"/>
       <c r="L59" s="23"/>
@@ -3216,170 +3237,173 @@
       <c r="O59" s="17"/>
       <c r="P59" s="17"/>
       <c r="Q59" s="23"/>
-    </row>
-    <row r="60" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A60" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="B60" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="27" t="s">
-        <v>316</v>
-      </c>
-      <c r="D60" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="27" t="s">
-        <v>317</v>
+      <c r="R59" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A60" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D60" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="G60" s="23"/>
       <c r="L60" s="23"/>
+      <c r="M60" s="17"/>
+      <c r="N60" s="17"/>
+      <c r="O60" s="17"/>
+      <c r="P60" s="17"/>
       <c r="Q60" s="23"/>
-      <c r="R60" s="27" t="s">
+    </row>
+    <row r="61" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="B61" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="D61" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="G61" s="23"/>
+      <c r="L61" s="23"/>
+      <c r="Q61" s="23"/>
+      <c r="R61" s="27" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="61" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D61" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E61" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G61" s="23"/>
-      <c r="H61" s="17" t="s">
+      <c r="D62" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E62" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" s="23"/>
+      <c r="H62" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I61" s="17" t="s">
+      <c r="I62" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J61" s="17" t="s">
+      <c r="J62" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K61" s="17" t="s">
+      <c r="K62" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L61" s="23"/>
-      <c r="M61" s="17" t="s">
+      <c r="L62" s="23"/>
+      <c r="M62" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N61" s="17" t="s">
+      <c r="N62" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O61" s="17" t="s">
+      <c r="O62" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P61" s="17" t="s">
+      <c r="P62" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q61" s="23"/>
-    </row>
-    <row r="62" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="2" t="s">
+      <c r="Q62" s="23"/>
+    </row>
+    <row r="63" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" s="2" t="s">
+      <c r="D63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G62" s="23"/>
-      <c r="L62" s="23"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
-      <c r="P62" s="17"/>
-      <c r="Q62" s="23"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
+      <c r="G63" s="23"/>
+      <c r="L63" s="23"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
+      <c r="Q63" s="23"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
         <v>72</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>5</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>73</v>
       </c>
-      <c r="D63" t="b">
-        <v>1</v>
-      </c>
-      <c r="E63" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" t="s">
-        <v>4</v>
-      </c>
-      <c r="R63"/>
-    </row>
-    <row r="64" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A64" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D64" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G64" s="23"/>
-      <c r="L64" s="23"/>
-      <c r="M64" s="17"/>
-      <c r="N64" s="17"/>
-      <c r="O64" s="17"/>
-      <c r="P64" s="17"/>
-      <c r="Q64" s="23"/>
+      <c r="D64" t="b">
+        <v>1</v>
+      </c>
+      <c r="E64" t="b">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>4</v>
+      </c>
+      <c r="R64"/>
     </row>
     <row r="65" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
-        <v>74</v>
+        <v>233</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>75</v>
+        <v>247</v>
       </c>
       <c r="D65" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G65" s="23"/>
       <c r="L65" s="23"/>
@@ -3389,580 +3413,580 @@
       <c r="P65" s="17"/>
       <c r="Q65" s="23"/>
     </row>
-    <row r="66" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D66" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G66" s="23"/>
+      <c r="L66" s="23"/>
+      <c r="M66" s="17"/>
+      <c r="N66" s="17"/>
+      <c r="O66" s="17"/>
+      <c r="P66" s="17"/>
+      <c r="Q66" s="23"/>
+    </row>
+    <row r="67" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D66" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G66" s="23"/>
-      <c r="H66" s="17" t="s">
+      <c r="D67" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" s="23"/>
+      <c r="H67" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I66" s="17" t="s">
+      <c r="I67" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J66" s="17" t="s">
+      <c r="J67" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K66" s="17" t="s">
+      <c r="K67" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L66" s="23"/>
-      <c r="M66" s="17" t="s">
+      <c r="L67" s="23"/>
+      <c r="M67" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N66" s="17" t="s">
+      <c r="N67" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O66" s="17" t="s">
+      <c r="O67" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P66" s="17" t="s">
+      <c r="P67" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q66" s="23"/>
-    </row>
-    <row r="67" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" s="2" t="s">
+      <c r="Q67" s="23"/>
+    </row>
+    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="2" t="s">
+      <c r="D68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="G67" s="23"/>
-      <c r="L67" s="23"/>
-      <c r="M67" s="17"/>
-      <c r="N67" s="17"/>
-      <c r="O67" s="17"/>
-      <c r="P67" s="17"/>
-      <c r="Q67" s="23"/>
-    </row>
-    <row r="68" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D68" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>273</v>
       </c>
       <c r="G68" s="23"/>
       <c r="L68" s="23"/>
+      <c r="M68" s="17"/>
+      <c r="N68" s="17"/>
+      <c r="O68" s="17"/>
+      <c r="P68" s="17"/>
       <c r="Q68" s="23"/>
-      <c r="R68" s="7" t="s">
+    </row>
+    <row r="69" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D69" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E69" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G69" s="23"/>
+      <c r="L69" s="23"/>
+      <c r="Q69" s="23"/>
+      <c r="R69" s="7" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A69" s="2" t="s">
+    <row r="70" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A70" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F69" s="2" t="s">
+      <c r="D70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G69" s="23"/>
-      <c r="H69" s="2" t="s">
+      <c r="G70" s="23"/>
+      <c r="H70" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L69" s="23"/>
-      <c r="M69" s="17" t="s">
+      <c r="L70" s="23"/>
+      <c r="M70" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N69" s="17" t="s">
+      <c r="N70" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O69" s="17" t="s">
+      <c r="O70" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P69" s="17" t="s">
+      <c r="P70" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q69" s="23"/>
-    </row>
-    <row r="70" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A70" s="7" t="s">
+      <c r="Q70" s="23"/>
+    </row>
+    <row r="71" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A71" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C71" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D70" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="7" t="s">
+      <c r="D71" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="G70" s="23"/>
-      <c r="L70" s="23"/>
-      <c r="Q70" s="23"/>
-      <c r="R70" s="8" t="s">
+      <c r="G71" s="23"/>
+      <c r="L71" s="23"/>
+      <c r="Q71" s="23"/>
+      <c r="R71" s="8" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="71" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D71" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G71" s="23"/>
-      <c r="H71" s="17" t="s">
+      <c r="D72" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" s="23"/>
+      <c r="H72" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="I71" s="17" t="s">
+      <c r="I72" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="J71" s="17" t="s">
+      <c r="J72" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="K71" s="17" t="s">
+      <c r="K72" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="L71" s="23"/>
-      <c r="M71" s="17" t="s">
+      <c r="L72" s="23"/>
+      <c r="M72" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="N71" s="17" t="s">
+      <c r="N72" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="O71" s="17" t="s">
+      <c r="O72" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="P71" s="17" t="s">
+      <c r="P72" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="Q71" s="23"/>
-    </row>
-    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" s="2" t="s">
+      <c r="Q72" s="23"/>
+    </row>
+    <row r="73" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D72" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="2" t="s">
+      <c r="D73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G72" s="23"/>
-      <c r="L72" s="23"/>
-      <c r="M72" s="17"/>
-      <c r="N72" s="17"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="17"/>
-      <c r="Q72" s="23"/>
-    </row>
-    <row r="73" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A73" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D73" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="G73" s="23"/>
       <c r="L73" s="23"/>
+      <c r="M73" s="17"/>
+      <c r="N73" s="17"/>
+      <c r="O73" s="17"/>
+      <c r="P73" s="17"/>
       <c r="Q73" s="23"/>
-      <c r="R73" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="74" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A74" s="7" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="D74" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E74" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="G74" s="23"/>
       <c r="L74" s="23"/>
       <c r="Q74" s="23"/>
-      <c r="R74" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" s="2" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A75" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D75" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>94</v>
+      <c r="R74" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A75" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D75" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G75" s="23"/>
       <c r="L75" s="23"/>
-      <c r="M75" s="17"/>
-      <c r="N75" s="17"/>
-      <c r="O75" s="17"/>
-      <c r="P75" s="17"/>
       <c r="Q75" s="23"/>
-    </row>
-    <row r="76" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A76" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="D76" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" s="17" t="s">
-        <v>4</v>
+      <c r="R75" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D76" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G76" s="23"/>
       <c r="L76" s="23"/>
+      <c r="M76" s="17"/>
+      <c r="N76" s="17"/>
+      <c r="O76" s="17"/>
+      <c r="P76" s="17"/>
       <c r="Q76" s="23"/>
     </row>
-    <row r="77" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="7" t="s">
+    <row r="77" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A77" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="D77" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G77" s="23"/>
+      <c r="L77" s="23"/>
+      <c r="Q77" s="23"/>
+    </row>
+    <row r="78" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="B77" s="19"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G77" s="23"/>
-      <c r="H77" s="7" t="s">
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G78" s="23"/>
+      <c r="H78" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I77" s="7" t="s">
+      <c r="I78" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J77" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K77" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L77" s="23"/>
-      <c r="M77" s="7" t="s">
+      <c r="J78" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K78" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L78" s="23"/>
+      <c r="M78" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N77" s="7" t="s">
+      <c r="N78" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O77" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P77" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q77" s="23"/>
-    </row>
-    <row r="78" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A78" s="20" t="s">
+      <c r="O78" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P78" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q78" s="23"/>
+    </row>
+    <row r="79" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A79" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B78" s="20" t="s">
+      <c r="B79" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C78" s="20" t="s">
+      <c r="C79" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="D78" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G78" s="23"/>
-      <c r="L78" s="23"/>
-      <c r="Q78" s="23"/>
-    </row>
-    <row r="79" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A79" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>4</v>
+      <c r="D79" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G79" s="23"/>
       <c r="L79" s="23"/>
-      <c r="M79" s="17"/>
-      <c r="N79" s="17"/>
-      <c r="O79" s="17"/>
-      <c r="P79" s="17"/>
       <c r="Q79" s="23"/>
-      <c r="R79" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="80" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D80" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G80" s="23"/>
-      <c r="H80" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I80" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J80" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K80" s="17" t="s">
-        <v>273</v>
-      </c>
       <c r="L80" s="23"/>
-      <c r="M80" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="N80" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="O80" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="P80" s="17" t="s">
-        <v>273</v>
-      </c>
+      <c r="M80" s="17"/>
+      <c r="N80" s="17"/>
+      <c r="O80" s="17"/>
+      <c r="P80" s="17"/>
       <c r="Q80" s="23"/>
       <c r="R80" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A81" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81" s="23"/>
+      <c r="H81" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="I81" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="J81" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="K81" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="L81" s="23"/>
+      <c r="M81" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N81" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O81" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="P81" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q81" s="23"/>
+      <c r="R81" s="8" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A81" t="s">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
         <v>198</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>199</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>200</v>
       </c>
-      <c r="D81" t="b">
-        <v>0</v>
-      </c>
-      <c r="E81" t="b">
-        <v>1</v>
-      </c>
-      <c r="R81"/>
-    </row>
-    <row r="82" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A82" s="13" t="s">
+      <c r="D82" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" t="b">
+        <v>1</v>
+      </c>
+      <c r="R82"/>
+    </row>
+    <row r="83" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A83" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="B82" s="13" t="s">
+      <c r="B83" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="C83" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="D82" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="6" t="s">
+      <c r="D83" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="G82" s="26"/>
-      <c r="L82" s="23"/>
-      <c r="M82" s="17"/>
-      <c r="N82" s="17"/>
-      <c r="O82" s="17"/>
-      <c r="P82" s="17"/>
-      <c r="Q82" s="23"/>
-    </row>
-    <row r="83" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="7" t="s">
+      <c r="G83" s="26"/>
+      <c r="L83" s="23"/>
+      <c r="M83" s="17"/>
+      <c r="N83" s="17"/>
+      <c r="O83" s="17"/>
+      <c r="P83" s="17"/>
+      <c r="Q83" s="23"/>
+    </row>
+    <row r="84" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B83" s="19"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E83" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="7" t="s">
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="G83" s="23"/>
-      <c r="L83" s="23"/>
-      <c r="Q83" s="23"/>
-      <c r="R83" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G84" s="23"/>
       <c r="L84" s="23"/>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
-      <c r="P84" s="17"/>
       <c r="Q84" s="23"/>
-    </row>
-    <row r="85" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="R84" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D85" s="2" t="b">
         <v>0</v>
@@ -3970,83 +3994,86 @@
       <c r="E85" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F85" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G85" s="26"/>
+      <c r="F85" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G85" s="23"/>
       <c r="L85" s="23"/>
       <c r="M85" s="17"/>
       <c r="N85" s="17"/>
       <c r="O85" s="17"/>
       <c r="P85" s="17"/>
       <c r="Q85" s="23"/>
-      <c r="R85" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A86" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="B86" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="D86" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="6"/>
+    </row>
+    <row r="86" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A86" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D86" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>287</v>
+      </c>
       <c r="G86" s="26"/>
       <c r="L86" s="23"/>
+      <c r="M86" s="17"/>
+      <c r="N86" s="17"/>
+      <c r="O86" s="17"/>
+      <c r="P86" s="17"/>
       <c r="Q86" s="23"/>
-    </row>
-    <row r="87" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A87" s="2" t="s">
+      <c r="R86" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A87" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="B87" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="D87" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="6"/>
+      <c r="G87" s="26"/>
+      <c r="L87" s="23"/>
+      <c r="Q87" s="23"/>
+    </row>
+    <row r="88" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A88" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D87" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G87" s="23"/>
-      <c r="L87" s="23"/>
-      <c r="M87" s="17"/>
-      <c r="N87" s="17"/>
-      <c r="O87" s="17"/>
-      <c r="P87" s="17"/>
-      <c r="Q87" s="23"/>
-    </row>
-    <row r="88" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="D88" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E88" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G88" s="23"/>
       <c r="L88" s="23"/>
@@ -4055,28 +4082,22 @@
       <c r="O88" s="17"/>
       <c r="P88" s="17"/>
       <c r="Q88" s="23"/>
-      <c r="R88" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="89" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
-        <v>104</v>
+        <v>201</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>107</v>
+        <v>202</v>
       </c>
       <c r="D89" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="G89" s="23"/>
       <c r="L89" s="23"/>
@@ -4086,91 +4107,95 @@
       <c r="P89" s="17"/>
       <c r="Q89" s="23"/>
       <c r="R89" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G90" s="23"/>
+      <c r="L90" s="23"/>
+      <c r="M90" s="17"/>
+      <c r="N90" s="17"/>
+      <c r="O90" s="17"/>
+      <c r="P90" s="17"/>
+      <c r="Q90" s="23"/>
+      <c r="R90" s="8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="90" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G90" s="23"/>
-      <c r="H90" s="17" t="s">
+      <c r="D91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G91" s="23"/>
+      <c r="H91" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I90" s="17" t="s">
+      <c r="I91" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J90" s="17" t="s">
+      <c r="J91" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K90" s="17" t="s">
+      <c r="K91" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L90" s="23"/>
-      <c r="M90" s="17" t="s">
+      <c r="L91" s="23"/>
+      <c r="M91" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N90" s="17" t="s">
+      <c r="N91" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O90" s="17" t="s">
+      <c r="O91" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P90" s="17" t="s">
+      <c r="P91" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q90" s="23"/>
-      <c r="R90" s="2" t="s">
+      <c r="Q91" s="23"/>
+      <c r="R91" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="91" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A91" s="7" t="s">
+    <row r="92" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A92" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="B92" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C92" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="D91" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F91" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="G91" s="23"/>
-      <c r="L91" s="23"/>
-      <c r="Q91" s="23"/>
-      <c r="R91" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="D92" s="7" t="b">
         <v>1</v>
@@ -4185,91 +4210,73 @@
       <c r="L92" s="23"/>
       <c r="Q92" s="23"/>
       <c r="R92" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="93" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D93" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E93" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>14</v>
+        <v>234</v>
       </c>
       <c r="G93" s="23"/>
       <c r="L93" s="23"/>
       <c r="Q93" s="23"/>
       <c r="R93" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D94" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94" s="23"/>
+      <c r="L94" s="23"/>
+      <c r="Q94" s="23"/>
+      <c r="R94" s="7" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D94" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G94" s="23"/>
-      <c r="H94" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J94" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K94" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L94" s="23"/>
-      <c r="M94" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N94" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O94" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P94" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q94" s="23"/>
     </row>
     <row r="95" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>288</v>
+        <v>117</v>
       </c>
       <c r="D95" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" s="2" t="b">
         <v>1</v>
@@ -4304,23 +4311,23 @@
     </row>
     <row r="96" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>120</v>
+        <v>288</v>
       </c>
       <c r="D96" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E96" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G96" s="23"/>
       <c r="H96" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>4</v>
@@ -4333,142 +4340,141 @@
       </c>
       <c r="L96" s="23"/>
       <c r="M96" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N96" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O96" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P96" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q96" s="23"/>
+    </row>
+    <row r="97" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D97" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G97" s="23"/>
+      <c r="H97" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N96" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O96" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P96" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q96" s="23"/>
-    </row>
-    <row r="97" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A97" s="7" t="s">
+      <c r="I97" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K97" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L97" s="23"/>
+      <c r="M97" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N97" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O97" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P97" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q97" s="23"/>
+    </row>
+    <row r="98" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A98" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B97" s="7" t="s">
+      <c r="B98" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C97" s="7" t="s">
+      <c r="C98" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D97" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G97" s="23"/>
-      <c r="H97" s="7" t="s">
+      <c r="D98" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G98" s="23"/>
+      <c r="H98" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I97" s="7" t="s">
+      <c r="I98" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J97" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K97" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L97" s="23"/>
-      <c r="M97" s="7" t="s">
+      <c r="J98" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K98" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L98" s="23"/>
+      <c r="M98" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N97" s="7" t="s">
+      <c r="N98" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O97" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P97" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q97" s="23"/>
-      <c r="R97" s="7" t="s">
+      <c r="O98" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P98" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q98" s="23"/>
+      <c r="R98" s="7" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A98" t="s">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
         <v>121</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>122</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>123</v>
       </c>
-      <c r="D98" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" t="b">
-        <v>0</v>
-      </c>
-      <c r="H98" s="16" t="s">
+      <c r="D99" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H99" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="I98" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J98" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K98" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L98" s="23"/>
-      <c r="M98" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="N98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q98" s="23"/>
-      <c r="R98"/>
-    </row>
-    <row r="99" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D99" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E99" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G99" s="23"/>
-      <c r="H99" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I99" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J99" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K99" s="2" t="s">
+      <c r="I99" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J99" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K99" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L99" s="23"/>
       <c r="M99" s="17" t="s">
-        <v>14</v>
+        <v>290</v>
       </c>
       <c r="N99" s="17" t="s">
         <v>4</v>
@@ -4480,19 +4486,17 @@
         <v>4</v>
       </c>
       <c r="Q99" s="23"/>
-      <c r="R99" s="2" t="s">
-        <v>203</v>
-      </c>
+      <c r="R99"/>
     </row>
     <row r="100" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D100" s="2" t="b">
         <v>1</v>
@@ -4527,80 +4531,124 @@
         <v>4</v>
       </c>
       <c r="Q100" s="23"/>
+      <c r="R100" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="101" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>127</v>
+        <v>259</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D101" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E101" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G101" s="23"/>
-      <c r="H101" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I101" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J101" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K101" s="17" t="s">
-        <v>273</v>
+      <c r="H101" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L101" s="23"/>
       <c r="M101" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N101" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O101" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P101" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q101" s="23"/>
+    </row>
+    <row r="102" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D102" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G102" s="23"/>
+      <c r="H102" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="N101" s="17" t="s">
+      <c r="I102" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="O101" s="17" t="s">
+      <c r="J102" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="P101" s="17" t="s">
+      <c r="K102" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="Q101" s="23"/>
-    </row>
-    <row r="102" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A102" s="2" t="s">
+      <c r="L102" s="23"/>
+      <c r="M102" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N102" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O102" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="P102" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q102" s="23"/>
+    </row>
+    <row r="103" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D102" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" s="2" t="s">
+      <c r="D103" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F103" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G102" s="23"/>
-      <c r="L102" s="23"/>
-      <c r="M102" s="17"/>
-      <c r="N102" s="17"/>
-      <c r="O102" s="17"/>
-      <c r="P102" s="17"/>
-      <c r="Q102" s="23"/>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R103"/>
+      <c r="G103" s="23"/>
+      <c r="L103" s="23"/>
+      <c r="M103" s="17"/>
+      <c r="N103" s="17"/>
+      <c r="O103" s="17"/>
+      <c r="P103" s="17"/>
+      <c r="Q103" s="23"/>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R104"/>
@@ -4665,28 +4713,31 @@
     <row r="124" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R124"/>
     </row>
+    <row r="125" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R125"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F19" r:id="rId1"/>
-    <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="H50" r:id="rId3"/>
-    <hyperlink ref="I50" r:id="rId4"/>
-    <hyperlink ref="J50" r:id="rId5"/>
-    <hyperlink ref="M50" r:id="rId6"/>
-    <hyperlink ref="N50" r:id="rId7"/>
-    <hyperlink ref="O50" r:id="rId8"/>
-    <hyperlink ref="K50" r:id="rId9"/>
-    <hyperlink ref="P50" r:id="rId10"/>
+    <hyperlink ref="F20" r:id="rId1"/>
+    <hyperlink ref="F21" r:id="rId2"/>
+    <hyperlink ref="H51" r:id="rId3"/>
+    <hyperlink ref="I51" r:id="rId4"/>
+    <hyperlink ref="J51" r:id="rId5"/>
+    <hyperlink ref="M51" r:id="rId6"/>
+    <hyperlink ref="N51" r:id="rId7"/>
+    <hyperlink ref="O51" r:id="rId8"/>
+    <hyperlink ref="K51" r:id="rId9"/>
+    <hyperlink ref="P51" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId11"/>

</xml_diff>

<commit_message>
BRO bestandsnaam van een XSD aanpassen #49 https://github.com/Imvertor/Imvertor-Maven/issues/49
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="324">
   <si>
     <t>Name</t>
   </si>
@@ -988,6 +988,15 @@
   </si>
   <si>
     <t>Yes if scalar values may occur in unions</t>
+  </si>
+  <si>
+    <t>xsdfilename</t>
+  </si>
+  <si>
+    <t>The name of each XSD file generated by the ISO19136 module. Named parameters such as [application-name] may be used.</t>
+  </si>
+  <si>
+    <t>[work/xsd-domain].xsd</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1148,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1218,6 +1227,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1512,13 +1524,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U125"/>
+  <dimension ref="A1:U126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1764,16 +1776,16 @@
       <c r="Q7" s="23"/>
     </row>
     <row r="8" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="32" t="b">
+      <c r="D8" s="33" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
@@ -1791,10 +1803,10 @@
       </c>
     </row>
     <row r="9" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
       <c r="G9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="17"/>
@@ -2649,16 +2661,16 @@
       </c>
     </row>
     <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="32" t="b">
+      <c r="D39" s="33" t="b">
         <v>0</v>
       </c>
       <c r="E39" s="2" t="b">
@@ -2676,10 +2688,10 @@
       <c r="Q39" s="23"/>
     </row>
     <row r="40" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="32"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
       <c r="G40" s="23"/>
       <c r="L40" s="23"/>
       <c r="M40" s="17"/>
@@ -4623,35 +4635,55 @@
       </c>
       <c r="Q102" s="23"/>
     </row>
-    <row r="103" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A103" s="2" t="s">
+    <row r="103" spans="1:18" s="32" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A103" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B103" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C103" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="D103" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="G103" s="31"/>
+      <c r="L103" s="31"/>
+      <c r="Q103" s="31"/>
+    </row>
+    <row r="104" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A104" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B104" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D103" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F103" s="2" t="s">
+      <c r="D104" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F104" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G103" s="23"/>
-      <c r="L103" s="23"/>
-      <c r="M103" s="17"/>
-      <c r="N103" s="17"/>
-      <c r="O103" s="17"/>
-      <c r="P103" s="17"/>
-      <c r="Q103" s="23"/>
-    </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R104"/>
+      <c r="G104" s="23"/>
+      <c r="L104" s="23"/>
+      <c r="M104" s="17"/>
+      <c r="N104" s="17"/>
+      <c r="O104" s="17"/>
+      <c r="P104" s="17"/>
+      <c r="Q104" s="23"/>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R105"/>
@@ -4715,6 +4747,9 @@
     </row>
     <row r="125" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R125"/>
+    </row>
+    <row r="126" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R126"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
BRO Import aanpassingen https://github.com/Imvertor/Imvertor-Maven/issues/51
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="325">
   <si>
     <t>Name</t>
   </si>
@@ -997,6 +997,9 @@
   </si>
   <si>
     <t>[work/xsd-domain].xsd</t>
+  </si>
+  <si>
+    <t>GM_SENTINEL</t>
   </si>
 </sst>
 </file>
@@ -1527,10 +1530,10 @@
   <dimension ref="A1:U126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F104" sqref="F104"/>
+      <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3938,6 +3941,18 @@
       </c>
       <c r="E82" t="b">
         <v>1</v>
+      </c>
+      <c r="M82" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="N82" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="O82" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="P82" s="29" t="s">
+        <v>324</v>
       </c>
       <c r="R82"/>
     </row>

</xml_diff>

<commit_message>
Introduce listings of enums in catalog
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\gitprojects\Imvertor-Maven\src\main\resources\input\BRO\props\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\BRO\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="327">
   <si>
     <t>Name</t>
   </si>
@@ -1000,6 +1000,12 @@
   </si>
   <si>
     <t>GM_SENTINEL</t>
+  </si>
+  <si>
+    <t>includedoclist</t>
+  </si>
+  <si>
+    <t>Yes if codelists and reference lists that have a location must be read dynamically from that location and included in the model documentation.</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1157,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1230,6 +1236,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1527,13 +1536,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U126"/>
+  <dimension ref="A1:U127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B76" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
+      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1779,16 +1788,16 @@
       <c r="Q7" s="23"/>
     </row>
     <row r="8" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="33" t="b">
+      <c r="D8" s="34" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
@@ -1806,10 +1815,10 @@
       </c>
     </row>
     <row r="9" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
       <c r="G9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="17"/>
@@ -2125,7 +2134,7 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="23"/>
     </row>
-    <row r="21" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>137</v>
       </c>
@@ -2664,16 +2673,16 @@
       </c>
     </row>
     <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="33" t="s">
+      <c r="B39" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C39" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="33" t="b">
+      <c r="D39" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E39" s="2" t="b">
@@ -2691,10 +2700,10 @@
       <c r="Q39" s="23"/>
     </row>
     <row r="40" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="33"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
       <c r="G40" s="23"/>
       <c r="L40" s="23"/>
       <c r="M40" s="17"/>
@@ -3153,127 +3162,141 @@
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A57" s="7" t="s">
+    <row r="57" spans="1:18" s="33" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A57" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="B57" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="D57" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" s="31"/>
+      <c r="H57" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I57" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="J57" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="K57" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="L57" s="31"/>
+      <c r="M57" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="N57" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="O57" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="P57" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q57" s="31"/>
+    </row>
+    <row r="58" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A58" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B58" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C58" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F57" s="7" t="s">
+      <c r="D58" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="G57" s="23"/>
-      <c r="L57" s="23"/>
-      <c r="Q57" s="23"/>
-      <c r="R57" s="7" t="s">
+      <c r="G58" s="23"/>
+      <c r="L58" s="23"/>
+      <c r="Q58" s="23"/>
+      <c r="R58" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="58" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A59" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D58" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G58" s="23"/>
-      <c r="H58" s="2" t="s">
+      <c r="D59" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" s="23"/>
+      <c r="H59" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="I58" s="17" t="s">
+      <c r="I59" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="J58" s="17" t="s">
+      <c r="J59" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="K58" s="17" t="s">
+      <c r="K59" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="L58" s="23"/>
-      <c r="M58" s="17" t="s">
+      <c r="L59" s="23"/>
+      <c r="M59" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="N58" s="17" t="s">
+      <c r="N59" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="O58" s="17" t="s">
+      <c r="O59" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="P58" s="17" t="s">
+      <c r="P59" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="Q58" s="23"/>
-      <c r="R58" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A59" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D59" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G59" s="23"/>
-      <c r="L59" s="23"/>
-      <c r="M59" s="17"/>
-      <c r="N59" s="17"/>
-      <c r="O59" s="17"/>
-      <c r="P59" s="17"/>
       <c r="Q59" s="23"/>
       <c r="R59" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>189</v>
+        <v>10</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
       <c r="D60" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E60" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>214</v>
+        <v>280</v>
       </c>
       <c r="G60" s="23"/>
       <c r="L60" s="23"/>
@@ -3282,170 +3305,173 @@
       <c r="O60" s="17"/>
       <c r="P60" s="17"/>
       <c r="Q60" s="23"/>
-    </row>
-    <row r="61" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="B61" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="27" t="s">
-        <v>316</v>
-      </c>
-      <c r="D61" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="27" t="s">
-        <v>317</v>
+      <c r="R60" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D61" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="G61" s="23"/>
       <c r="L61" s="23"/>
+      <c r="M61" s="17"/>
+      <c r="N61" s="17"/>
+      <c r="O61" s="17"/>
+      <c r="P61" s="17"/>
       <c r="Q61" s="23"/>
-      <c r="R61" s="27" t="s">
+    </row>
+    <row r="62" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="B62" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="D62" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="G62" s="23"/>
+      <c r="L62" s="23"/>
+      <c r="Q62" s="23"/>
+      <c r="R62" s="27" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="62" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D62" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G62" s="23"/>
-      <c r="H62" s="17" t="s">
+      <c r="D63" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" s="23"/>
+      <c r="H63" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I62" s="17" t="s">
+      <c r="I63" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J62" s="17" t="s">
+      <c r="J63" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K62" s="17" t="s">
+      <c r="K63" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L62" s="23"/>
-      <c r="M62" s="17" t="s">
+      <c r="L63" s="23"/>
+      <c r="M63" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N62" s="17" t="s">
+      <c r="N63" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O62" s="17" t="s">
+      <c r="O63" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P62" s="17" t="s">
+      <c r="P63" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q62" s="23"/>
-    </row>
-    <row r="63" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" s="2" t="s">
+      <c r="Q63" s="23"/>
+    </row>
+    <row r="64" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G63" s="23"/>
-      <c r="L63" s="23"/>
-      <c r="M63" s="17"/>
-      <c r="N63" s="17"/>
-      <c r="O63" s="17"/>
-      <c r="P63" s="17"/>
-      <c r="Q63" s="23"/>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
+      <c r="D64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G64" s="23"/>
+      <c r="L64" s="23"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+      <c r="P64" s="17"/>
+      <c r="Q64" s="23"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A65" t="s">
         <v>72</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>5</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>73</v>
       </c>
-      <c r="D64" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" t="s">
-        <v>4</v>
-      </c>
-      <c r="R64"/>
-    </row>
-    <row r="65" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A65" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D65" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G65" s="23"/>
-      <c r="L65" s="23"/>
-      <c r="M65" s="17"/>
-      <c r="N65" s="17"/>
-      <c r="O65" s="17"/>
-      <c r="P65" s="17"/>
-      <c r="Q65" s="23"/>
+      <c r="D65" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>4</v>
+      </c>
+      <c r="R65"/>
     </row>
     <row r="66" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
-        <v>74</v>
+        <v>233</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>75</v>
+        <v>247</v>
       </c>
       <c r="D66" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G66" s="23"/>
       <c r="L66" s="23"/>
@@ -3455,592 +3481,592 @@
       <c r="P66" s="17"/>
       <c r="Q66" s="23"/>
     </row>
-    <row r="67" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="23"/>
+      <c r="L67" s="23"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
+      <c r="Q67" s="23"/>
+    </row>
+    <row r="68" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D67" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G67" s="23"/>
-      <c r="H67" s="17" t="s">
+      <c r="D68" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" s="23"/>
+      <c r="H68" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I67" s="17" t="s">
+      <c r="I68" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J67" s="17" t="s">
+      <c r="J68" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K67" s="17" t="s">
+      <c r="K68" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L67" s="23"/>
-      <c r="M67" s="17" t="s">
+      <c r="L68" s="23"/>
+      <c r="M68" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N67" s="17" t="s">
+      <c r="N68" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O67" s="17" t="s">
+      <c r="O68" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P67" s="17" t="s">
+      <c r="P68" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q67" s="23"/>
-    </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="2" t="s">
+      <c r="Q68" s="23"/>
+    </row>
+    <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="2" t="s">
+      <c r="D69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="G68" s="23"/>
-      <c r="L68" s="23"/>
-      <c r="M68" s="17"/>
-      <c r="N68" s="17"/>
-      <c r="O68" s="17"/>
-      <c r="P68" s="17"/>
-      <c r="Q68" s="23"/>
-    </row>
-    <row r="69" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D69" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E69" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>273</v>
       </c>
       <c r="G69" s="23"/>
       <c r="L69" s="23"/>
+      <c r="M69" s="17"/>
+      <c r="N69" s="17"/>
+      <c r="O69" s="17"/>
+      <c r="P69" s="17"/>
       <c r="Q69" s="23"/>
-      <c r="R69" s="7" t="s">
+    </row>
+    <row r="70" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D70" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G70" s="23"/>
+      <c r="L70" s="23"/>
+      <c r="Q70" s="23"/>
+      <c r="R70" s="7" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="70" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F70" s="2" t="s">
+      <c r="D71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G70" s="23"/>
-      <c r="H70" s="2" t="s">
+      <c r="G71" s="23"/>
+      <c r="H71" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L70" s="23"/>
-      <c r="M70" s="17" t="s">
+      <c r="L71" s="23"/>
+      <c r="M71" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N70" s="17" t="s">
+      <c r="N71" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O70" s="17" t="s">
+      <c r="O71" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P70" s="17" t="s">
+      <c r="P71" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q70" s="23"/>
-    </row>
-    <row r="71" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A71" s="7" t="s">
+      <c r="Q71" s="23"/>
+    </row>
+    <row r="72" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A72" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B72" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C72" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D71" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="7" t="s">
+      <c r="D72" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="G71" s="23"/>
-      <c r="L71" s="23"/>
-      <c r="Q71" s="23"/>
-      <c r="R71" s="8" t="s">
+      <c r="G72" s="23"/>
+      <c r="L72" s="23"/>
+      <c r="Q72" s="23"/>
+      <c r="R72" s="8" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D72" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G72" s="23"/>
-      <c r="H72" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="I72" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="J72" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="K72" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="L72" s="23"/>
-      <c r="M72" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="N72" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="O72" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="P72" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q72" s="23"/>
     </row>
     <row r="73" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" s="23"/>
+      <c r="H73" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="I73" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="J73" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="K73" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="L73" s="23"/>
+      <c r="M73" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="N73" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="O73" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="P73" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q73" s="23"/>
+    </row>
+    <row r="74" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="2" t="s">
+      <c r="D74" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G73" s="23"/>
-      <c r="L73" s="23"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
-      <c r="Q73" s="23"/>
-    </row>
-    <row r="74" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A74" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D74" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="G74" s="23"/>
       <c r="L74" s="23"/>
+      <c r="M74" s="17"/>
+      <c r="N74" s="17"/>
+      <c r="O74" s="17"/>
+      <c r="P74" s="17"/>
       <c r="Q74" s="23"/>
-      <c r="R74" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="75" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A75" s="7" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="D75" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E75" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="G75" s="23"/>
       <c r="L75" s="23"/>
       <c r="Q75" s="23"/>
-      <c r="R75" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A76" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D76" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>94</v>
+      <c r="R75" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A76" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D76" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G76" s="23"/>
       <c r="L76" s="23"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="17"/>
       <c r="Q76" s="23"/>
-    </row>
-    <row r="77" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A77" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="D77" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="17" t="s">
-        <v>4</v>
+      <c r="R76" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D77" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G77" s="23"/>
       <c r="L77" s="23"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
+      <c r="P77" s="17"/>
       <c r="Q77" s="23"/>
     </row>
-    <row r="78" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="7" t="s">
+    <row r="78" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A78" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="B78" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="D78" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G78" s="23"/>
+      <c r="L78" s="23"/>
+      <c r="Q78" s="23"/>
+    </row>
+    <row r="79" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="B78" s="19"/>
-      <c r="C78" s="19"/>
-      <c r="D78" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E78" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G78" s="23"/>
-      <c r="H78" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I78" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J78" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K78" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L78" s="23"/>
-      <c r="M78" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N78" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O78" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P78" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q78" s="23"/>
-    </row>
-    <row r="79" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A79" s="20" t="s">
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G79" s="23"/>
+      <c r="H79" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I79" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J79" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K79" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L79" s="23"/>
+      <c r="M79" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N79" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O79" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P79" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q79" s="23"/>
+    </row>
+    <row r="80" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A80" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B79" s="20" t="s">
+      <c r="B80" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="C80" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="D79" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G79" s="23"/>
-      <c r="L79" s="23"/>
-      <c r="Q79" s="23"/>
-    </row>
-    <row r="80" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A80" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>4</v>
+      <c r="D80" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G80" s="23"/>
       <c r="L80" s="23"/>
-      <c r="M80" s="17"/>
-      <c r="N80" s="17"/>
-      <c r="O80" s="17"/>
-      <c r="P80" s="17"/>
       <c r="Q80" s="23"/>
-      <c r="R80" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="81" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D81" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G81" s="23"/>
-      <c r="H81" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I81" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J81" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K81" s="17" t="s">
-        <v>273</v>
-      </c>
       <c r="L81" s="23"/>
-      <c r="M81" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="N81" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="O81" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="P81" s="17" t="s">
-        <v>273</v>
-      </c>
+      <c r="M81" s="17"/>
+      <c r="N81" s="17"/>
+      <c r="O81" s="17"/>
+      <c r="P81" s="17"/>
       <c r="Q81" s="23"/>
       <c r="R81" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G82" s="23"/>
+      <c r="H82" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="I82" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="J82" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="K82" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="L82" s="23"/>
+      <c r="M82" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N82" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O82" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="P82" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q82" s="23"/>
+      <c r="R82" s="8" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A82" t="s">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
         <v>198</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>199</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>200</v>
       </c>
-      <c r="D82" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" t="b">
-        <v>1</v>
-      </c>
-      <c r="M82" s="29" t="s">
+      <c r="D83" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" t="b">
+        <v>1</v>
+      </c>
+      <c r="M83" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="N82" s="29" t="s">
+      <c r="N83" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="O82" s="29" t="s">
+      <c r="O83" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="P82" s="29" t="s">
+      <c r="P83" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="R82"/>
-    </row>
-    <row r="83" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A83" s="13" t="s">
+      <c r="R83"/>
+    </row>
+    <row r="84" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A84" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="B83" s="13" t="s">
+      <c r="B84" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="C83" s="13" t="s">
+      <c r="C84" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="D83" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="6" t="s">
+      <c r="D84" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="G83" s="26"/>
-      <c r="L83" s="23"/>
-      <c r="M83" s="17"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
-      <c r="P83" s="17"/>
-      <c r="Q83" s="23"/>
-    </row>
-    <row r="84" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="7" t="s">
+      <c r="G84" s="26"/>
+      <c r="L84" s="23"/>
+      <c r="M84" s="17"/>
+      <c r="N84" s="17"/>
+      <c r="O84" s="17"/>
+      <c r="P84" s="17"/>
+      <c r="Q84" s="23"/>
+    </row>
+    <row r="85" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B84" s="19"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="7" t="s">
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="G84" s="23"/>
-      <c r="L84" s="23"/>
-      <c r="Q84" s="23"/>
-      <c r="R84" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D85" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G85" s="23"/>
       <c r="L85" s="23"/>
-      <c r="M85" s="17"/>
-      <c r="N85" s="17"/>
-      <c r="O85" s="17"/>
-      <c r="P85" s="17"/>
       <c r="Q85" s="23"/>
-    </row>
-    <row r="86" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="R85" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D86" s="2" t="b">
         <v>0</v>
@@ -4048,83 +4074,86 @@
       <c r="E86" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F86" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G86" s="26"/>
+      <c r="F86" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G86" s="23"/>
       <c r="L86" s="23"/>
       <c r="M86" s="17"/>
       <c r="N86" s="17"/>
       <c r="O86" s="17"/>
       <c r="P86" s="17"/>
       <c r="Q86" s="23"/>
-      <c r="R86" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A87" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="B87" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="D87" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="6"/>
+    </row>
+    <row r="87" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>287</v>
+      </c>
       <c r="G87" s="26"/>
       <c r="L87" s="23"/>
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
+      <c r="O87" s="17"/>
+      <c r="P87" s="17"/>
       <c r="Q87" s="23"/>
-    </row>
-    <row r="88" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
+      <c r="R87" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A88" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="B88" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="D88" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="6"/>
+      <c r="G88" s="26"/>
+      <c r="L88" s="23"/>
+      <c r="Q88" s="23"/>
+    </row>
+    <row r="89" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G88" s="23"/>
-      <c r="L88" s="23"/>
-      <c r="M88" s="17"/>
-      <c r="N88" s="17"/>
-      <c r="O88" s="17"/>
-      <c r="P88" s="17"/>
-      <c r="Q88" s="23"/>
-    </row>
-    <row r="89" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="D89" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E89" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G89" s="23"/>
       <c r="L89" s="23"/>
@@ -4133,28 +4162,22 @@
       <c r="O89" s="17"/>
       <c r="P89" s="17"/>
       <c r="Q89" s="23"/>
-      <c r="R89" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="90" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
-        <v>104</v>
+        <v>201</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>107</v>
+        <v>202</v>
       </c>
       <c r="D90" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="G90" s="23"/>
       <c r="L90" s="23"/>
@@ -4164,91 +4187,95 @@
       <c r="P90" s="17"/>
       <c r="Q90" s="23"/>
       <c r="R90" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G91" s="23"/>
+      <c r="L91" s="23"/>
+      <c r="M91" s="17"/>
+      <c r="N91" s="17"/>
+      <c r="O91" s="17"/>
+      <c r="P91" s="17"/>
+      <c r="Q91" s="23"/>
+      <c r="R91" s="8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="91" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
+    <row r="92" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G91" s="23"/>
-      <c r="H91" s="17" t="s">
+      <c r="D92" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E92" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G92" s="23"/>
+      <c r="H92" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I91" s="17" t="s">
+      <c r="I92" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J91" s="17" t="s">
+      <c r="J92" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K91" s="17" t="s">
+      <c r="K92" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L91" s="23"/>
-      <c r="M91" s="17" t="s">
+      <c r="L92" s="23"/>
+      <c r="M92" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N91" s="17" t="s">
+      <c r="N92" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O91" s="17" t="s">
+      <c r="O92" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P91" s="17" t="s">
+      <c r="P92" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q91" s="23"/>
-      <c r="R91" s="2" t="s">
+      <c r="Q92" s="23"/>
+      <c r="R92" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="92" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A92" s="7" t="s">
+    <row r="93" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A93" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B93" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="C93" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="D92" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E92" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="G92" s="23"/>
-      <c r="L92" s="23"/>
-      <c r="Q92" s="23"/>
-      <c r="R92" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="D93" s="7" t="b">
         <v>1</v>
@@ -4263,91 +4290,73 @@
       <c r="L93" s="23"/>
       <c r="Q93" s="23"/>
       <c r="R93" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="94" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D94" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E94" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>14</v>
+        <v>234</v>
       </c>
       <c r="G94" s="23"/>
       <c r="L94" s="23"/>
       <c r="Q94" s="23"/>
       <c r="R94" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D95" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G95" s="23"/>
+      <c r="L95" s="23"/>
+      <c r="Q95" s="23"/>
+      <c r="R95" s="7" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="95" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D95" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G95" s="23"/>
-      <c r="H95" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I95" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J95" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K95" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L95" s="23"/>
-      <c r="M95" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N95" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O95" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P95" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q95" s="23"/>
     </row>
     <row r="96" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>288</v>
+        <v>117</v>
       </c>
       <c r="D96" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
         <v>1</v>
@@ -4382,23 +4391,23 @@
     </row>
     <row r="97" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>120</v>
+        <v>288</v>
       </c>
       <c r="D97" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G97" s="23"/>
       <c r="H97" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>4</v>
@@ -4411,7 +4420,7 @@
       </c>
       <c r="L97" s="23"/>
       <c r="M97" s="17" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N97" s="17" t="s">
         <v>4</v>
@@ -4424,129 +4433,128 @@
       </c>
       <c r="Q97" s="23"/>
     </row>
-    <row r="98" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A98" s="7" t="s">
+    <row r="98" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D98" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G98" s="23"/>
+      <c r="H98" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K98" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L98" s="23"/>
+      <c r="M98" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N98" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O98" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P98" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q98" s="23"/>
+    </row>
+    <row r="99" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A99" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B99" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C99" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D98" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G98" s="23"/>
-      <c r="H98" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I98" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J98" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K98" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L98" s="23"/>
-      <c r="M98" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N98" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O98" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P98" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q98" s="23"/>
-      <c r="R98" s="7" t="s">
+      <c r="D99" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G99" s="23"/>
+      <c r="H99" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I99" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J99" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K99" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L99" s="23"/>
+      <c r="M99" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N99" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O99" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P99" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q99" s="23"/>
+      <c r="R99" s="7" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A99" t="s">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
         <v>121</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>122</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>123</v>
       </c>
-      <c r="D99" t="b">
-        <v>1</v>
-      </c>
-      <c r="E99" t="b">
-        <v>0</v>
-      </c>
-      <c r="H99" s="16" t="s">
+      <c r="D100" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="I99" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J99" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K99" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L99" s="23"/>
-      <c r="M99" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="N99" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O99" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P99" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q99" s="23"/>
-      <c r="R99"/>
-    </row>
-    <row r="100" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G100" s="23"/>
-      <c r="H100" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I100" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J100" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K100" s="2" t="s">
+      <c r="I100" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J100" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K100" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L100" s="23"/>
       <c r="M100" s="17" t="s">
-        <v>14</v>
+        <v>290</v>
       </c>
       <c r="N100" s="17" t="s">
         <v>4</v>
@@ -4558,19 +4566,17 @@
         <v>4</v>
       </c>
       <c r="Q100" s="23"/>
-      <c r="R100" s="2" t="s">
-        <v>203</v>
-      </c>
+      <c r="R100"/>
     </row>
     <row r="101" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D101" s="2" t="b">
         <v>1</v>
@@ -4605,103 +4611,147 @@
         <v>4</v>
       </c>
       <c r="Q101" s="23"/>
+      <c r="R101" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="102" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
-        <v>127</v>
+        <v>259</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D102" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E102" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G102" s="23"/>
-      <c r="H102" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I102" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J102" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K102" s="17" t="s">
-        <v>273</v>
+      <c r="H102" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K102" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L102" s="23"/>
       <c r="M102" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N102" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O102" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P102" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q102" s="23"/>
+    </row>
+    <row r="103" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D103" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G103" s="23"/>
+      <c r="H103" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="N102" s="17" t="s">
+      <c r="I103" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="O102" s="17" t="s">
+      <c r="J103" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="P102" s="17" t="s">
+      <c r="K103" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="Q102" s="23"/>
-    </row>
-    <row r="103" spans="1:18" s="32" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A103" s="32" t="s">
+      <c r="L103" s="23"/>
+      <c r="M103" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N103" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O103" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="P103" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q103" s="23"/>
+    </row>
+    <row r="104" spans="1:18" s="32" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A104" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="B103" s="32" t="s">
+      <c r="B104" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C103" s="32" t="s">
+      <c r="C104" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="D103" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F103" s="32" t="s">
+      <c r="D104" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" s="32" t="s">
         <v>323</v>
       </c>
-      <c r="G103" s="31"/>
-      <c r="L103" s="31"/>
-      <c r="Q103" s="31"/>
-    </row>
-    <row r="104" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A104" s="2" t="s">
+      <c r="G104" s="31"/>
+      <c r="L104" s="31"/>
+      <c r="Q104" s="31"/>
+    </row>
+    <row r="105" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A105" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D104" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E104" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F104" s="2" t="s">
+      <c r="D105" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G104" s="23"/>
-      <c r="L104" s="23"/>
-      <c r="M104" s="17"/>
-      <c r="N104" s="17"/>
-      <c r="O104" s="17"/>
-      <c r="P104" s="17"/>
-      <c r="Q104" s="23"/>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R105"/>
+      <c r="G105" s="23"/>
+      <c r="L105" s="23"/>
+      <c r="M105" s="17"/>
+      <c r="N105" s="17"/>
+      <c r="O105" s="17"/>
+      <c r="P105" s="17"/>
+      <c r="Q105" s="23"/>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R106"/>
@@ -4765,6 +4815,9 @@
     </row>
     <row r="126" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R126"/>
+    </row>
+    <row r="127" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R127"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
introductie van createxmlschemavariant en createjsonschemavariant
hernoemen van alle schemarules files naar XML-* en JSON-*
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="337">
   <si>
     <t>Name</t>
   </si>
@@ -906,9 +906,6 @@
     <t>only for logical</t>
   </si>
   <si>
-    <t>schema rules voor CM niet relevant; test moet worden verwijderd uit Imvertor.</t>
-  </si>
-  <si>
     <t>reportshortview</t>
   </si>
   <si>
@@ -1006,6 +1003,39 @@
   </si>
   <si>
     <t>Yes if codelists and reference lists that have a location must be read dynamically from that location and included in the model documentation.</t>
+  </si>
+  <si>
+    <t>createjsonschema</t>
+  </si>
+  <si>
+    <t>Yes if JSON schema must be generated</t>
+  </si>
+  <si>
+    <t>createjsonschemavariant</t>
+  </si>
+  <si>
+    <t>The name of the variant of the JSON schema generated.</t>
+  </si>
+  <si>
+    <t>no JSON for BRO</t>
+  </si>
+  <si>
+    <t>createxmlschemavariant</t>
+  </si>
+  <si>
+    <t>The name of the variant of the XML schema generated.</t>
+  </si>
+  <si>
+    <t>obsolete, replaced by createschemavariant name</t>
+  </si>
+  <si>
+    <t>OBSOLETE</t>
+  </si>
+  <si>
+    <t>ISO19136</t>
+  </si>
+  <si>
+    <t>NOT-USED</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1187,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1236,6 +1266,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1536,18 +1569,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U127"/>
+  <dimension ref="A1:U130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="27.84375" customWidth="1"/>
     <col min="2" max="2" width="19.3046875" customWidth="1"/>
     <col min="3" max="3" width="50.69140625" customWidth="1"/>
     <col min="4" max="4" width="13.23046875" customWidth="1"/>
@@ -1588,29 +1621,29 @@
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L1" s="21"/>
       <c r="M1" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Q1" s="21"/>
       <c r="R1" s="3" t="s">
@@ -1621,29 +1654,29 @@
       <c r="F2" s="3"/>
       <c r="G2" s="22"/>
       <c r="H2" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="L2" s="22"/>
       <c r="M2" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>314</v>
       </c>
       <c r="Q2" s="22"/>
       <c r="R2" s="5"/>
@@ -1734,13 +1767,13 @@
     </row>
     <row r="6" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D6" s="30" t="b">
         <v>0</v>
@@ -1788,16 +1821,16 @@
       <c r="Q7" s="23"/>
     </row>
     <row r="8" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="34" t="b">
+      <c r="D8" s="35" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
@@ -1815,10 +1848,10 @@
       </c>
     </row>
     <row r="9" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
       <c r="G9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="17"/>
@@ -2410,141 +2443,143 @@
       </c>
       <c r="Q28" s="23"/>
     </row>
-    <row r="29" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="34" t="s">
+        <v>326</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="D29" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="34" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="D30" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="G30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="34" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2" t="s">
+      <c r="D31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="G29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D30" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="Q30" s="23"/>
-    </row>
-    <row r="31" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D31" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="7" t="b">
-        <v>1</v>
       </c>
       <c r="G31" s="23"/>
       <c r="L31" s="23"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
       <c r="Q31" s="23"/>
-    </row>
-    <row r="32" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R31" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="7" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>5</v>
+        <v>166</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>36</v>
+        <v>167</v>
       </c>
       <c r="D32" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E32" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="G32" s="23"/>
       <c r="L32" s="23"/>
       <c r="Q32" s="23"/>
     </row>
-    <row r="33" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>14</v>
+    <row r="33" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G33" s="23"/>
       <c r="L33" s="23"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="17"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17"/>
       <c r="Q33" s="23"/>
     </row>
-    <row r="34" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D34" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E34" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>14</v>
@@ -2553,15 +2588,15 @@
       <c r="L34" s="23"/>
       <c r="Q34" s="23"/>
     </row>
-    <row r="35" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D35" s="2" t="b">
         <v>0</v>
@@ -2569,49 +2604,32 @@
       <c r="E35" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F35" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G35" s="23"/>
-      <c r="H35" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="K35" s="17" t="s">
-        <v>14</v>
-      </c>
       <c r="L35" s="23"/>
-      <c r="M35" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N35" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O35" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P35" s="17" t="s">
-        <v>4</v>
-      </c>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
       <c r="Q35" s="23"/>
     </row>
-    <row r="36" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A36" s="7" t="s">
-        <v>171</v>
+        <v>39</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="D36" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E36" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>14</v>
@@ -2620,137 +2638,166 @@
       <c r="L36" s="23"/>
       <c r="Q36" s="23"/>
     </row>
-    <row r="37" spans="1:18" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A37" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="7" t="s">
+    <row r="37" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>14</v>
+      <c r="C37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G37" s="23"/>
+      <c r="H37" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="L37" s="23"/>
+      <c r="M37" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P37" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="Q37" s="23"/>
-      <c r="R37" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A38" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="G38" s="23"/>
-      <c r="L38" s="23"/>
-      <c r="Q38" s="23"/>
-      <c r="R38" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="34" t="s">
+    </row>
+    <row r="38" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="34" t="s">
+        <v>331</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="D38" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="G38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="Q38" s="31"/>
+    </row>
+    <row r="39" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" s="2" t="s">
+      <c r="C39" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D39" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G39" s="23"/>
       <c r="L39" s="23"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17"/>
       <c r="Q39" s="23"/>
     </row>
-    <row r="40" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
+    <row r="40" spans="1:18" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A40" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="G40" s="23"/>
       <c r="L40" s="23"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="17"/>
-      <c r="P40" s="17"/>
       <c r="Q40" s="23"/>
-    </row>
-    <row r="41" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A41" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D41" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="2" t="b">
-        <v>0</v>
+      <c r="R40" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A41" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>234</v>
       </c>
       <c r="G41" s="23"/>
       <c r="L41" s="23"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
       <c r="Q41" s="23"/>
+      <c r="R41" s="7" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="42" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D42" s="2" t="b">
+      <c r="C42" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="35" t="b">
         <v>0</v>
       </c>
       <c r="E42" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G42" s="23"/>
       <c r="L42" s="23"/>
@@ -2760,160 +2807,147 @@
       <c r="P42" s="17"/>
       <c r="Q42" s="23"/>
     </row>
-    <row r="43" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A43" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="G43" s="26"/>
+    <row r="43" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="G43" s="23"/>
       <c r="L43" s="23"/>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
       <c r="O43" s="17"/>
       <c r="P43" s="17"/>
       <c r="Q43" s="23"/>
-      <c r="R43" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="44" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
+        <v>173</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="D44" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F44" s="6"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="J44" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="K44" s="17" t="s">
-        <v>281</v>
-      </c>
+      <c r="G44" s="23"/>
       <c r="L44" s="23"/>
-      <c r="M44" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="N44" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="O44" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="P44" s="17" t="s">
-        <v>282</v>
-      </c>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
       <c r="Q44" s="23"/>
     </row>
-    <row r="45" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B45" s="7" t="s">
+    <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D45" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>4</v>
+      <c r="C45" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G45" s="23"/>
       <c r="L45" s="23"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17"/>
       <c r="Q45" s="23"/>
-      <c r="R45"/>
-    </row>
-    <row r="46" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A46" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D46" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="G46" s="23"/>
+    </row>
+    <row r="46" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G46" s="26"/>
       <c r="L46" s="23"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
       <c r="Q46" s="23"/>
+      <c r="R46" s="2" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
       <c r="D47" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G47" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="6"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="I47" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="J47" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="K47" s="17" t="s">
+        <v>281</v>
+      </c>
       <c r="L47" s="23"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="17"/>
-      <c r="O47" s="17"/>
-      <c r="P47" s="17"/>
+      <c r="M47" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="N47" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="O47" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="P47" s="17" t="s">
+        <v>282</v>
+      </c>
       <c r="Q47" s="23"/>
     </row>
     <row r="48" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="7" t="s">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="D48" s="7" t="b">
         <v>0</v>
@@ -2922,508 +2956,485 @@
         <v>1</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G48" s="23"/>
       <c r="L48" s="23"/>
       <c r="Q48" s="23"/>
-    </row>
-    <row r="49" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="R48"/>
+    </row>
+    <row r="49" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="7" t="s">
-        <v>59</v>
+        <v>178</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="D49" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E49" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="G49" s="23"/>
       <c r="L49" s="23"/>
       <c r="Q49" s="23"/>
-      <c r="R49" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B50" s="7" t="s">
+    </row>
+    <row r="50" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D50" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="7" t="s">
+      <c r="C50" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G50" s="23"/>
       <c r="L50" s="23"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
       <c r="Q50" s="23"/>
     </row>
-    <row r="51" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A51" s="7" t="s">
-        <v>299</v>
+        <v>57</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D51" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G51" s="23"/>
-      <c r="H51" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="I51" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="J51" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="K51" s="18" t="s">
-        <v>300</v>
-      </c>
       <c r="L51" s="23"/>
-      <c r="M51" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="N51" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="O51" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="P51" s="18" t="s">
-        <v>300</v>
-      </c>
       <c r="Q51" s="23"/>
     </row>
     <row r="52" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A52" s="7" t="s">
-        <v>183</v>
+        <v>59</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>155</v>
+        <v>5</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="D52" s="7" t="b">
         <v>0</v>
       </c>
+      <c r="E52" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="G52" s="23"/>
-      <c r="H52" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="I52" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="J52" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="K52" s="7" t="s">
-        <v>278</v>
-      </c>
       <c r="L52" s="23"/>
-      <c r="M52" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="N52" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="O52" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="P52" s="7" t="s">
-        <v>278</v>
-      </c>
       <c r="Q52" s="23"/>
+      <c r="R52" s="7" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="53" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="7" t="s">
-        <v>301</v>
+        <v>181</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>302</v>
+        <v>5</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>303</v>
+        <v>182</v>
       </c>
       <c r="D53" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>304</v>
+        <v>14</v>
       </c>
       <c r="G53" s="23"/>
       <c r="L53" s="23"/>
       <c r="Q53" s="23"/>
     </row>
-    <row r="54" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A54" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="D54" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="G54" s="24"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="24"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="24"/>
-      <c r="R54" s="15" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A54" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G54" s="23"/>
+      <c r="H54" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="I54" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="J54" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="K54" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="L54" s="23"/>
+      <c r="M54" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="N54" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="O54" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="P54" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q54" s="23"/>
+    </row>
+    <row r="55" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A55" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D55" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="E55" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="G55" s="23"/>
+      <c r="H55" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>278</v>
+      </c>
       <c r="L55" s="23"/>
+      <c r="M55" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="N55" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="O55" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="P55" s="7" t="s">
+        <v>278</v>
+      </c>
       <c r="Q55" s="23"/>
-      <c r="R55" s="7" t="s">
-        <v>209</v>
-      </c>
     </row>
     <row r="56" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="7" t="s">
-        <v>61</v>
+        <v>300</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>12</v>
+        <v>301</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>62</v>
+        <v>302</v>
       </c>
       <c r="D56" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>210</v>
+        <v>303</v>
       </c>
       <c r="G56" s="23"/>
       <c r="L56" s="23"/>
       <c r="Q56" s="23"/>
-      <c r="R56" s="7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" s="33" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A57" s="33" t="s">
-        <v>325</v>
-      </c>
-      <c r="B57" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" s="33" t="s">
-        <v>326</v>
-      </c>
-      <c r="D57" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="G57" s="31"/>
-      <c r="H57" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I57" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="J57" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="K57" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="L57" s="31"/>
-      <c r="M57" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="N57" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="O57" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="P57" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q57" s="31"/>
+    </row>
+    <row r="57" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A57" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="D57" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="G57" s="24"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="24"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
+      <c r="Q57" s="24"/>
+      <c r="R57" s="15" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="58" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="7" t="s">
-        <v>63</v>
+        <v>185</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>64</v>
+        <v>186</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>65</v>
+        <v>187</v>
       </c>
       <c r="D58" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>234</v>
+        <v>17</v>
       </c>
       <c r="G58" s="23"/>
       <c r="L58" s="23"/>
       <c r="Q58" s="23"/>
       <c r="R58" s="7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A59" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D59" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="2" t="b">
-        <v>0</v>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="G59" s="23"/>
-      <c r="H59" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="I59" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="J59" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="K59" s="17" t="s">
-        <v>226</v>
-      </c>
       <c r="L59" s="23"/>
-      <c r="M59" s="17" t="s">
-        <v>306</v>
-      </c>
-      <c r="N59" s="17" t="s">
-        <v>306</v>
-      </c>
-      <c r="O59" s="17" t="s">
-        <v>306</v>
-      </c>
-      <c r="P59" s="17" t="s">
-        <v>306</v>
-      </c>
       <c r="Q59" s="23"/>
-      <c r="R59" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A60" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D60" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G60" s="23"/>
-      <c r="L60" s="23"/>
-      <c r="M60" s="17"/>
-      <c r="N60" s="17"/>
-      <c r="O60" s="17"/>
-      <c r="P60" s="17"/>
-      <c r="Q60" s="23"/>
-      <c r="R60" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D61" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>214</v>
+      <c r="R59" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" s="33" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A60" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="B60" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="D60" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G60" s="31"/>
+      <c r="H60" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I60" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="J60" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="K60" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="L60" s="31"/>
+      <c r="M60" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="N60" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="O60" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="P60" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q60" s="31"/>
+    </row>
+    <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D61" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E61" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>234</v>
       </c>
       <c r="G61" s="23"/>
       <c r="L61" s="23"/>
-      <c r="M61" s="17"/>
-      <c r="N61" s="17"/>
-      <c r="O61" s="17"/>
-      <c r="P61" s="17"/>
       <c r="Q61" s="23"/>
-    </row>
-    <row r="62" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="B62" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="27" t="s">
-        <v>316</v>
-      </c>
-      <c r="D62" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="27" t="s">
-        <v>317</v>
+      <c r="R61" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D62" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G62" s="23"/>
+      <c r="H62" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I62" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="J62" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="K62" s="17" t="s">
+        <v>226</v>
+      </c>
       <c r="L62" s="23"/>
+      <c r="M62" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="N62" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="O62" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="P62" s="17" t="s">
+        <v>305</v>
+      </c>
       <c r="Q62" s="23"/>
-      <c r="R62" s="27" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R62" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D63" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F63" s="2" t="s">
+        <v>280</v>
+      </c>
       <c r="G63" s="23"/>
-      <c r="H63" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="I63" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="J63" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="K63" s="17" t="s">
-        <v>281</v>
-      </c>
       <c r="L63" s="23"/>
-      <c r="M63" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="N63" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="O63" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="P63" s="17" t="s">
-        <v>282</v>
-      </c>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
       <c r="Q63" s="23"/>
+      <c r="R63" s="2" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="64" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>5</v>
+        <v>189</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D64" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E64" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="G64" s="23"/>
       <c r="L64" s="23"/>
@@ -3433,36 +3444,41 @@
       <c r="P64" s="17"/>
       <c r="Q64" s="23"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
-        <v>72</v>
-      </c>
-      <c r="B65" t="s">
+    <row r="65" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A65" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="B65" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C65" t="s">
-        <v>73</v>
-      </c>
-      <c r="D65" t="b">
-        <v>1</v>
-      </c>
-      <c r="E65" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" t="s">
-        <v>4</v>
-      </c>
-      <c r="R65"/>
-    </row>
-    <row r="66" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="C65" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="D65" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="G65" s="23"/>
+      <c r="L65" s="23"/>
+      <c r="Q65" s="23"/>
+      <c r="R65" s="27" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
-        <v>233</v>
+        <v>70</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>247</v>
+        <v>71</v>
       </c>
       <c r="D66" s="2" t="b">
         <v>1</v>
@@ -3470,26 +3486,43 @@
       <c r="E66" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F66" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G66" s="23"/>
+      <c r="H66" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="I66" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="J66" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="K66" s="17" t="s">
+        <v>281</v>
+      </c>
       <c r="L66" s="23"/>
-      <c r="M66" s="17"/>
-      <c r="N66" s="17"/>
-      <c r="O66" s="17"/>
-      <c r="P66" s="17"/>
+      <c r="M66" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="N66" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="O66" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="P66" s="17" t="s">
+        <v>282</v>
+      </c>
       <c r="Q66" s="23"/>
     </row>
     <row r="67" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
-        <v>74</v>
+        <v>191</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>75</v>
+        <v>192</v>
       </c>
       <c r="D67" s="2" t="b">
         <v>0</v>
@@ -3498,7 +3531,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G67" s="23"/>
       <c r="L67" s="23"/>
@@ -3508,68 +3541,45 @@
       <c r="P67" s="17"/>
       <c r="Q67" s="23"/>
     </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D68" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G68" s="23"/>
-      <c r="H68" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="I68" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="J68" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="K68" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="L68" s="23"/>
-      <c r="M68" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="N68" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="O68" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="P68" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q68" s="23"/>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>73</v>
+      </c>
+      <c r="D68" t="b">
+        <v>1</v>
+      </c>
+      <c r="E68" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>4</v>
+      </c>
+      <c r="R68"/>
     </row>
     <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>78</v>
+        <v>233</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>80</v>
+        <v>247</v>
       </c>
       <c r="D69" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>283</v>
+        <v>14</v>
       </c>
       <c r="G69" s="23"/>
       <c r="L69" s="23"/>
@@ -3579,176 +3589,177 @@
       <c r="P69" s="17"/>
       <c r="Q69" s="23"/>
     </row>
-    <row r="70" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D70" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>273</v>
+    <row r="70" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A70" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G70" s="23"/>
       <c r="L70" s="23"/>
+      <c r="M70" s="17"/>
+      <c r="N70" s="17"/>
+      <c r="O70" s="17"/>
+      <c r="P70" s="17"/>
       <c r="Q70" s="23"/>
-      <c r="R70" s="7" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="71" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
-        <v>193</v>
+        <v>76</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>194</v>
+        <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>195</v>
+        <v>77</v>
       </c>
       <c r="D71" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F71" s="2" t="s">
-        <v>284</v>
-      </c>
       <c r="G71" s="23"/>
-      <c r="H71" s="2" t="s">
-        <v>17</v>
+      <c r="H71" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="I71" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="J71" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="K71" s="17" t="s">
+        <v>281</v>
       </c>
       <c r="L71" s="23"/>
       <c r="M71" s="17" t="s">
-        <v>17</v>
+        <v>282</v>
       </c>
       <c r="N71" s="17" t="s">
-        <v>17</v>
+        <v>282</v>
       </c>
       <c r="O71" s="17" t="s">
-        <v>17</v>
+        <v>282</v>
       </c>
       <c r="P71" s="17" t="s">
-        <v>17</v>
+        <v>282</v>
       </c>
       <c r="Q71" s="23"/>
     </row>
-    <row r="72" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A72" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D72" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>227</v>
+    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="G72" s="23"/>
       <c r="L72" s="23"/>
+      <c r="M72" s="17"/>
+      <c r="N72" s="17"/>
+      <c r="O72" s="17"/>
+      <c r="P72" s="17"/>
       <c r="Q72" s="23"/>
-      <c r="R72" s="8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B73" s="2" t="s">
+    </row>
+    <row r="73" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>0</v>
+      <c r="C73" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>273</v>
       </c>
       <c r="G73" s="23"/>
-      <c r="H73" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="I73" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="J73" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="K73" s="17" t="s">
-        <v>285</v>
-      </c>
       <c r="L73" s="23"/>
-      <c r="M73" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="N73" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="O73" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="P73" s="17" t="s">
-        <v>286</v>
-      </c>
       <c r="Q73" s="23"/>
-    </row>
-    <row r="74" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R73" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>85</v>
+        <v>193</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>87</v>
+        <v>194</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>88</v>
+        <v>195</v>
       </c>
       <c r="D74" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>86</v>
+        <v>284</v>
       </c>
       <c r="G74" s="23"/>
+      <c r="H74" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="L74" s="23"/>
-      <c r="M74" s="17"/>
-      <c r="N74" s="17"/>
-      <c r="O74" s="17"/>
-      <c r="P74" s="17"/>
+      <c r="M74" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N74" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="O74" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="P74" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="Q74" s="23"/>
     </row>
-    <row r="75" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A75" s="7" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>91</v>
+        <v>174</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>92</v>
+        <v>197</v>
       </c>
       <c r="D75" s="7" t="b">
         <v>0</v>
@@ -3757,59 +3768,77 @@
         <v>1</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>90</v>
+        <v>227</v>
       </c>
       <c r="G75" s="23"/>
       <c r="L75" s="23"/>
       <c r="Q75" s="23"/>
       <c r="R75" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A76" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D76" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>14</v>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D76" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G76" s="23"/>
+      <c r="H76" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="I76" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="J76" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="K76" s="17" t="s">
+        <v>285</v>
+      </c>
       <c r="L76" s="23"/>
+      <c r="M76" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="N76" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="O76" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="P76" s="17" t="s">
+        <v>286</v>
+      </c>
       <c r="Q76" s="23"/>
-      <c r="R76" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="77" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D77" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G77" s="23"/>
       <c r="L77" s="23"/>
@@ -3819,290 +3848,280 @@
       <c r="P77" s="17"/>
       <c r="Q77" s="23"/>
     </row>
-    <row r="78" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A78" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="D78" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" s="17" t="s">
-        <v>4</v>
+    <row r="78" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A78" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D78" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="G78" s="23"/>
       <c r="L78" s="23"/>
       <c r="Q78" s="23"/>
-    </row>
-    <row r="79" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R78" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A79" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="B79" s="19"/>
-      <c r="C79" s="19"/>
+        <v>145</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="D79" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G79" s="23"/>
-      <c r="H79" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I79" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J79" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K79" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="L79" s="23"/>
-      <c r="M79" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N79" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O79" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P79" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="Q79" s="23"/>
-    </row>
-    <row r="80" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A80" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="B80" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="D80" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="7" t="b">
-        <v>1</v>
+      <c r="R79" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D80" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G80" s="23"/>
       <c r="L80" s="23"/>
+      <c r="M80" s="17"/>
+      <c r="N80" s="17"/>
+      <c r="O80" s="17"/>
+      <c r="P80" s="17"/>
       <c r="Q80" s="23"/>
     </row>
-    <row r="81" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B81" s="2" t="s">
+    <row r="81" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A81" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B81" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="2" t="s">
+      <c r="C81" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="D81" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G81" s="23"/>
       <c r="L81" s="23"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
       <c r="Q81" s="23"/>
-      <c r="R81" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A82" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D82" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2" t="b">
-        <v>0</v>
+    </row>
+    <row r="82" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G82" s="23"/>
-      <c r="H82" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I82" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J82" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K82" s="17" t="s">
-        <v>273</v>
+      <c r="H82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J82" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K82" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="L82" s="23"/>
-      <c r="M82" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="N82" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="O82" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="P82" s="17" t="s">
-        <v>273</v>
+      <c r="M82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O82" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P82" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="Q82" s="23"/>
-      <c r="R82" s="8" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A83" t="s">
-        <v>198</v>
-      </c>
-      <c r="B83" t="s">
-        <v>199</v>
-      </c>
-      <c r="C83" t="s">
-        <v>200</v>
-      </c>
-      <c r="D83" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" t="b">
-        <v>1</v>
-      </c>
-      <c r="M83" s="29" t="s">
-        <v>324</v>
-      </c>
-      <c r="N83" s="29" t="s">
-        <v>324</v>
-      </c>
-      <c r="O83" s="29" t="s">
-        <v>324</v>
-      </c>
-      <c r="P83" s="29" t="s">
-        <v>324</v>
-      </c>
-      <c r="R83"/>
-    </row>
-    <row r="84" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A84" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="B84" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D84" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="G84" s="26"/>
+    </row>
+    <row r="83" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A83" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B83" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="D83" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G83" s="23"/>
+      <c r="L83" s="23"/>
+      <c r="Q83" s="23"/>
+    </row>
+    <row r="84" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G84" s="23"/>
       <c r="L84" s="23"/>
       <c r="M84" s="17"/>
       <c r="N84" s="17"/>
       <c r="O84" s="17"/>
       <c r="P84" s="17"/>
       <c r="Q84" s="23"/>
-    </row>
-    <row r="85" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="B85" s="19"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>273</v>
+      <c r="R84" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>334</v>
       </c>
       <c r="G85" s="23"/>
+      <c r="H85" s="17"/>
+      <c r="I85" s="17"/>
+      <c r="J85" s="17"/>
+      <c r="K85" s="17"/>
       <c r="L85" s="23"/>
+      <c r="M85" s="17"/>
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="17"/>
       <c r="Q85" s="23"/>
-      <c r="R85" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G86" s="23"/>
-      <c r="L86" s="23"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
-      <c r="Q86" s="23"/>
-    </row>
-    <row r="87" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A87" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D87" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="2" t="b">
+      <c r="R85" s="8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>198</v>
+      </c>
+      <c r="B86" t="s">
+        <v>199</v>
+      </c>
+      <c r="C86" t="s">
+        <v>200</v>
+      </c>
+      <c r="D86" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" t="b">
+        <v>1</v>
+      </c>
+      <c r="M86" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="N86" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="O86" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="P86" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="R86"/>
+    </row>
+    <row r="87" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A87" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D87" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="13" t="b">
         <v>1</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="G87" s="26"/>
       <c r="L87" s="23"/>
@@ -4111,40 +4130,38 @@
       <c r="O87" s="17"/>
       <c r="P87" s="17"/>
       <c r="Q87" s="23"/>
-      <c r="R87" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A88" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="B88" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="D88" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" s="6"/>
-      <c r="G88" s="26"/>
+    </row>
+    <row r="88" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G88" s="23"/>
       <c r="L88" s="23"/>
       <c r="Q88" s="23"/>
-    </row>
-    <row r="89" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="R88" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D89" s="2" t="b">
         <v>0</v>
@@ -4163,15 +4180,15 @@
       <c r="P89" s="17"/>
       <c r="Q89" s="23"/>
     </row>
-    <row r="90" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
-        <v>201</v>
+        <v>100</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>202</v>
+        <v>101</v>
       </c>
       <c r="D90" s="2" t="b">
         <v>0</v>
@@ -4179,382 +4196,326 @@
       <c r="E90" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G90" s="23"/>
+      <c r="F90" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G90" s="26"/>
       <c r="L90" s="23"/>
       <c r="M90" s="17"/>
       <c r="N90" s="17"/>
       <c r="O90" s="17"/>
       <c r="P90" s="17"/>
       <c r="Q90" s="23"/>
-      <c r="R90" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G91" s="23"/>
+      <c r="R90" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="D91" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="6"/>
+      <c r="G91" s="26"/>
       <c r="L91" s="23"/>
-      <c r="M91" s="17"/>
-      <c r="N91" s="17"/>
-      <c r="O91" s="17"/>
-      <c r="P91" s="17"/>
       <c r="Q91" s="23"/>
-      <c r="R91" s="8" t="s">
-        <v>241</v>
-      </c>
     </row>
     <row r="92" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D92" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G92" s="23"/>
-      <c r="H92" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="I92" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="J92" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="K92" s="17" t="s">
-        <v>281</v>
-      </c>
       <c r="L92" s="23"/>
-      <c r="M92" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="N92" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="O92" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="P92" s="17" t="s">
-        <v>282</v>
-      </c>
+      <c r="M92" s="17"/>
+      <c r="N92" s="17"/>
+      <c r="O92" s="17"/>
+      <c r="P92" s="17"/>
       <c r="Q92" s="23"/>
-      <c r="R92" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A93" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D93" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F93" s="7" t="s">
-        <v>234</v>
+    </row>
+    <row r="93" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D93" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G93" s="23"/>
       <c r="L93" s="23"/>
+      <c r="M93" s="17"/>
+      <c r="N93" s="17"/>
+      <c r="O93" s="17"/>
+      <c r="P93" s="17"/>
       <c r="Q93" s="23"/>
-      <c r="R93" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D94" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F94" s="7" t="s">
-        <v>234</v>
+      <c r="R93" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="G94" s="23"/>
       <c r="L94" s="23"/>
+      <c r="M94" s="17"/>
+      <c r="N94" s="17"/>
+      <c r="O94" s="17"/>
+      <c r="P94" s="17"/>
       <c r="Q94" s="23"/>
-      <c r="R94" s="7" t="s">
+      <c r="R94" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D95" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G95" s="23"/>
+      <c r="H95" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="I95" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="J95" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="K95" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="L95" s="23"/>
+      <c r="M95" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="N95" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="O95" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="P95" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q95" s="23"/>
+      <c r="R95" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A96" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D96" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G96" s="23"/>
+      <c r="L96" s="23"/>
+      <c r="Q96" s="23"/>
+      <c r="R96" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D97" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G97" s="23"/>
+      <c r="L97" s="23"/>
+      <c r="Q97" s="23"/>
+      <c r="R97" s="7" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="95" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="7" t="s">
+    <row r="98" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B95" s="7" t="s">
+      <c r="B98" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C98" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D95" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G95" s="23"/>
-      <c r="L95" s="23"/>
-      <c r="Q95" s="23"/>
-      <c r="R95" s="7" t="s">
+      <c r="D98" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G98" s="23"/>
+      <c r="L98" s="23"/>
+      <c r="Q98" s="23"/>
+      <c r="R98" s="7" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="96" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="2" t="s">
+    <row r="99" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G96" s="23"/>
-      <c r="H96" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I96" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J96" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K96" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L96" s="23"/>
-      <c r="M96" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N96" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O96" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P96" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q96" s="23"/>
-    </row>
-    <row r="97" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="2" t="s">
+      <c r="D99" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G99" s="23"/>
+      <c r="H99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L99" s="23"/>
+      <c r="M99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q99" s="23"/>
+    </row>
+    <row r="100" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="D97" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G97" s="23"/>
-      <c r="H97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L97" s="23"/>
-      <c r="M97" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N97" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O97" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P97" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q97" s="23"/>
-    </row>
-    <row r="98" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D98" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G98" s="23"/>
-      <c r="H98" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L98" s="23"/>
-      <c r="M98" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q98" s="23"/>
-    </row>
-    <row r="99" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A99" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D99" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G99" s="23"/>
-      <c r="H99" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I99" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J99" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K99" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L99" s="23"/>
-      <c r="M99" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N99" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O99" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P99" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q99" s="23"/>
-      <c r="R99" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A100" t="s">
-        <v>121</v>
-      </c>
-      <c r="B100" t="s">
-        <v>122</v>
-      </c>
-      <c r="C100" t="s">
-        <v>123</v>
-      </c>
-      <c r="D100" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" t="b">
-        <v>0</v>
-      </c>
-      <c r="H100" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="I100" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J100" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K100" s="16" t="s">
+      <c r="D100" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G100" s="23"/>
+      <c r="H100" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K100" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L100" s="23"/>
       <c r="M100" s="17" t="s">
-        <v>290</v>
+        <v>4</v>
       </c>
       <c r="N100" s="17" t="s">
         <v>4</v>
@@ -4566,20 +4527,19 @@
         <v>4</v>
       </c>
       <c r="Q100" s="23"/>
-      <c r="R100"/>
     </row>
     <row r="101" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D101" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101" s="2" t="b">
         <v>1</v>
@@ -4611,156 +4571,282 @@
         <v>4</v>
       </c>
       <c r="Q101" s="23"/>
-      <c r="R101" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B102" s="2" t="s">
+    </row>
+    <row r="102" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A102" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B102" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D102" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="b">
+      <c r="C102" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D102" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G102" s="23"/>
-      <c r="H102" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K102" s="2" t="s">
+      <c r="H102" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I102" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J102" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K102" s="7" t="s">
         <v>4</v>
       </c>
       <c r="L102" s="23"/>
-      <c r="M102" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N102" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O102" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P102" s="17" t="s">
+      <c r="M102" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N102" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O102" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P102" s="7" t="s">
         <v>4</v>
       </c>
       <c r="Q102" s="23"/>
-    </row>
-    <row r="103" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D103" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G103" s="23"/>
-      <c r="H103" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I103" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J103" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K103" s="17" t="s">
-        <v>273</v>
+      <c r="R102" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A103" t="s">
+        <v>121</v>
+      </c>
+      <c r="B103" t="s">
+        <v>122</v>
+      </c>
+      <c r="C103" t="s">
+        <v>123</v>
+      </c>
+      <c r="D103" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" t="b">
+        <v>0</v>
+      </c>
+      <c r="H103" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="I103" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J103" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K103" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="L103" s="23"/>
       <c r="M103" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="N103" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O103" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P103" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q103" s="23"/>
+      <c r="R103"/>
+    </row>
+    <row r="104" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D104" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G104" s="23"/>
+      <c r="H104" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L104" s="23"/>
+      <c r="M104" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N104" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O104" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P104" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q104" s="23"/>
+      <c r="R104" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D105" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G105" s="23"/>
+      <c r="H105" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L105" s="23"/>
+      <c r="M105" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N105" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O105" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P105" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q105" s="23"/>
+    </row>
+    <row r="106" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D106" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G106" s="23"/>
+      <c r="H106" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="N103" s="17" t="s">
+      <c r="I106" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="O103" s="17" t="s">
+      <c r="J106" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="P103" s="17" t="s">
+      <c r="K106" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="Q103" s="23"/>
-    </row>
-    <row r="104" spans="1:18" s="32" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A104" s="32" t="s">
+      <c r="L106" s="23"/>
+      <c r="M106" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N106" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O106" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="P106" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q106" s="23"/>
+    </row>
+    <row r="107" spans="1:18" s="32" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A107" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="B107" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C107" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="B104" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="C104" s="32" t="s">
+      <c r="D107" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F107" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="D104" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E104" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F104" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="G104" s="31"/>
-      <c r="L104" s="31"/>
-      <c r="Q104" s="31"/>
-    </row>
-    <row r="105" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A105" s="2" t="s">
+      <c r="G107" s="31"/>
+      <c r="L107" s="31"/>
+      <c r="Q107" s="31"/>
+    </row>
+    <row r="108" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A108" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D105" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E105" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F105" s="2" t="s">
+      <c r="D108" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F108" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G105" s="23"/>
-      <c r="L105" s="23"/>
-      <c r="M105" s="17"/>
-      <c r="N105" s="17"/>
-      <c r="O105" s="17"/>
-      <c r="P105" s="17"/>
-      <c r="Q105" s="23"/>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R106"/>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R107"/>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R108"/>
+      <c r="G108" s="23"/>
+      <c r="L108" s="23"/>
+      <c r="M108" s="17"/>
+      <c r="N108" s="17"/>
+      <c r="O108" s="17"/>
+      <c r="P108" s="17"/>
+      <c r="Q108" s="23"/>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R109"/>
@@ -4818,6 +4904,15 @@
     </row>
     <row r="127" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R127"/>
+    </row>
+    <row r="128" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R128"/>
+    </row>
+    <row r="129" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R129"/>
+    </row>
+    <row r="130" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R130"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4825,22 +4920,22 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1"/>
     <hyperlink ref="F21" r:id="rId2"/>
-    <hyperlink ref="H51" r:id="rId3"/>
-    <hyperlink ref="I51" r:id="rId4"/>
-    <hyperlink ref="J51" r:id="rId5"/>
-    <hyperlink ref="M51" r:id="rId6"/>
-    <hyperlink ref="N51" r:id="rId7"/>
-    <hyperlink ref="O51" r:id="rId8"/>
-    <hyperlink ref="K51" r:id="rId9"/>
-    <hyperlink ref="P51" r:id="rId10"/>
+    <hyperlink ref="H54" r:id="rId3"/>
+    <hyperlink ref="I54" r:id="rId4"/>
+    <hyperlink ref="J54" r:id="rId5"/>
+    <hyperlink ref="M54" r:id="rId6"/>
+    <hyperlink ref="N54" r:id="rId7"/>
+    <hyperlink ref="O54" r:id="rId8"/>
+    <hyperlink ref="K54" r:id="rId9"/>
+    <hyperlink ref="P54" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId11"/>

</xml_diff>

<commit_message>
BRO introduction of second "office" format (msword & respec)
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="339">
   <si>
     <t>Name</t>
   </si>
@@ -1030,13 +1030,25 @@
   </si>
   <si>
     <t>NOT-USED</t>
+  </si>
+  <si>
+    <t>createofficevariant</t>
+  </si>
+  <si>
+    <t>respec/msword</t>
+  </si>
+  <si>
+    <t>Specify the type of office file. Multiple formats are allowed, separate list by whitespace.</t>
+  </si>
+  <si>
+    <t>respec msword</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1113,6 +1125,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1181,7 +1207,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1263,6 +1289,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1557,13 +1601,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R129"/>
+  <dimension ref="A1:R130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomRight" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1774,16 +1818,16 @@
       <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="33" t="b">
+      <c r="D7" s="39" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1801,10 +1845,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
       <c r="G8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
@@ -2478,293 +2522,298 @@
         <v>277</v>
       </c>
     </row>
-    <row r="31" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A31" s="7" t="s">
+    <row r="31" spans="1:18" s="33" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A31" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>336</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="D31" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="G31" s="29"/>
+      <c r="L31" s="29"/>
+    </row>
+    <row r="32" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A32" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C32" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="D31" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="Q31" s="23"/>
-    </row>
-    <row r="32" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="7" t="s">
+      <c r="D32" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="Q32" s="35"/>
+    </row>
+    <row r="33" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B33" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C33" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D32" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="Q32" s="23"/>
-    </row>
-    <row r="33" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="7" t="s">
+      <c r="D33" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="Q33" s="35"/>
+    </row>
+    <row r="34" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B34" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E33" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="Q33" s="23"/>
-    </row>
-    <row r="34" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A34" s="2" t="s">
+      <c r="D34" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="Q34" s="35"/>
+    </row>
+    <row r="35" spans="1:18" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A35" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="23"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17"/>
-      <c r="Q34" s="23"/>
-    </row>
-    <row r="35" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A35" s="7" t="s">
+      <c r="D35" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="Q35" s="35"/>
+    </row>
+    <row r="36" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A36" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C36" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="Q35" s="23"/>
-    </row>
-    <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="2" t="s">
+      <c r="D36" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="Q36" s="35"/>
+    </row>
+    <row r="37" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" s="23"/>
-      <c r="H36" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="L36" s="23"/>
-      <c r="M36" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N36" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O36" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P36" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q36" s="23"/>
-    </row>
-    <row r="37" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="32" t="s">
+      <c r="D37" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" s="35"/>
+      <c r="H37" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="K37" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L37" s="35"/>
+      <c r="M37" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="N37" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="O37" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="P37" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="35"/>
+    </row>
+    <row r="38" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="36" t="s">
         <v>329</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B38" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="32" t="s">
+      <c r="C38" s="36" t="s">
         <v>330</v>
       </c>
-      <c r="D37" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="32" t="s">
+      <c r="D38" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="36" t="s">
         <v>333</v>
       </c>
-      <c r="G37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="Q37" s="29"/>
-    </row>
-    <row r="38" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="7" t="s">
+      <c r="G38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="Q38" s="35"/>
+    </row>
+    <row r="39" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B39" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C39" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="D38" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="23"/>
-      <c r="L38" s="23"/>
-      <c r="Q38" s="23"/>
-    </row>
-    <row r="39" spans="1:18" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A39" s="7" t="s">
+      <c r="D39" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="Q39" s="35"/>
+    </row>
+    <row r="40" spans="1:18" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A40" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B40" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C40" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="23"/>
-      <c r="L39" s="23"/>
-      <c r="Q39" s="23"/>
-      <c r="R39" s="7" t="s">
+      <c r="D40" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="38"/>
+      <c r="L40" s="38"/>
+      <c r="Q40" s="38"/>
+      <c r="R40" s="37" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A40" s="7" t="s">
+    <row r="41" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A41" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B41" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C41" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F40" s="7" t="s">
+      <c r="D41" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="G40" s="23"/>
-      <c r="L40" s="23"/>
-      <c r="Q40" s="23"/>
-      <c r="R40" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G41" s="23"/>
       <c r="L41" s="23"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
       <c r="Q41" s="23"/>
+      <c r="R41" s="7" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="42" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="33"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
+      <c r="A42" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G42" s="23"/>
       <c r="L42" s="23"/>
       <c r="M42" s="17"/>
@@ -2773,22 +2822,11 @@
       <c r="P42" s="17"/>
       <c r="Q42" s="23"/>
     </row>
-    <row r="43" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A43" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D43" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="43" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="39"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
       <c r="G43" s="23"/>
       <c r="L43" s="23"/>
       <c r="M43" s="17"/>
@@ -2797,21 +2835,21 @@
       <c r="P43" s="17"/>
       <c r="Q43" s="23"/>
     </row>
-    <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
-        <v>50</v>
+        <v>173</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>51</v>
+        <v>175</v>
       </c>
       <c r="D44" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="23"/>
       <c r="L44" s="23"/>
@@ -2821,15 +2859,15 @@
       <c r="P44" s="17"/>
       <c r="Q44" s="23"/>
     </row>
-    <row r="45" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D45" s="2" t="b">
         <v>0</v>
@@ -2837,95 +2875,95 @@
       <c r="E45" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F45" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="G45" s="26"/>
+      <c r="G45" s="23"/>
       <c r="L45" s="23"/>
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
       <c r="O45" s="17"/>
       <c r="P45" s="17"/>
       <c r="Q45" s="23"/>
-      <c r="R45" s="2" t="s">
+    </row>
+    <row r="46" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G46" s="26"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="23"/>
+      <c r="R46" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E46" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F46" s="6"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="17" t="s">
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" s="6"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I46" s="17" t="s">
+      <c r="I47" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J46" s="17" t="s">
+      <c r="J47" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K46" s="17" t="s">
+      <c r="K47" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L46" s="23"/>
-      <c r="M46" s="17" t="s">
+      <c r="L47" s="23"/>
+      <c r="M47" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N46" s="17" t="s">
+      <c r="N47" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O46" s="17" t="s">
+      <c r="O47" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P46" s="17" t="s">
+      <c r="P47" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q46" s="23"/>
-    </row>
-    <row r="47" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="7" t="s">
+      <c r="Q47" s="23"/>
+    </row>
+    <row r="48" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B48" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C48" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D47" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G47" s="23"/>
-      <c r="L47" s="23"/>
-      <c r="Q47" s="23"/>
-      <c r="R47"/>
-    </row>
-    <row r="48" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A48" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="D48" s="7" t="b">
         <v>0</v>
       </c>
@@ -2933,77 +2971,78 @@
         <v>1</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="G48" s="23"/>
       <c r="L48" s="23"/>
       <c r="Q48" s="23"/>
-    </row>
-    <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D49" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>14</v>
+      <c r="R48"/>
+    </row>
+    <row r="49" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A49" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="G49" s="23"/>
       <c r="L49" s="23"/>
-      <c r="M49" s="17"/>
-      <c r="N49" s="17"/>
-      <c r="O49" s="17"/>
-      <c r="P49" s="17"/>
       <c r="Q49" s="23"/>
     </row>
-    <row r="50" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B50" s="7" t="s">
+    <row r="50" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D50" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="7" t="s">
+      <c r="C50" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G50" s="23"/>
       <c r="L50" s="23"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
       <c r="Q50" s="23"/>
     </row>
-    <row r="51" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A51" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D51" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E51" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>14</v>
@@ -3011,25 +3050,22 @@
       <c r="G51" s="23"/>
       <c r="L51" s="23"/>
       <c r="Q51" s="23"/>
-      <c r="R51" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="52" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A52" s="7" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>182</v>
+        <v>60</v>
       </c>
       <c r="D52" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E52" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>14</v>
@@ -3037,357 +3073,353 @@
       <c r="G52" s="23"/>
       <c r="L52" s="23"/>
       <c r="Q52" s="23"/>
-    </row>
-    <row r="53" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="R52" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D53" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" s="23"/>
+      <c r="L53" s="23"/>
+      <c r="Q53" s="23"/>
+    </row>
+    <row r="54" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A54" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B54" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G53" s="23"/>
-      <c r="H53" s="18" t="s">
+      <c r="G54" s="23"/>
+      <c r="H54" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="I53" s="18" t="s">
+      <c r="I54" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="J53" s="18" t="s">
+      <c r="J54" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="K53" s="18" t="s">
+      <c r="K54" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="L53" s="23"/>
-      <c r="M53" s="18" t="s">
+      <c r="L54" s="23"/>
+      <c r="M54" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="N53" s="18" t="s">
+      <c r="N54" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="O53" s="18" t="s">
+      <c r="O54" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="P53" s="18" t="s">
+      <c r="P54" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="Q53" s="23"/>
-    </row>
-    <row r="54" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A54" s="7" t="s">
+      <c r="Q54" s="23"/>
+    </row>
+    <row r="55" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A55" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B55" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D54" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G54" s="23"/>
-      <c r="H54" s="7" t="s">
+      <c r="D55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" s="23"/>
+      <c r="H55" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="I54" s="7" t="s">
+      <c r="I55" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="J54" s="7" t="s">
+      <c r="J55" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="K54" s="7" t="s">
+      <c r="K55" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="L54" s="23"/>
-      <c r="M54" s="7" t="s">
+      <c r="L55" s="23"/>
+      <c r="M55" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="N54" s="7" t="s">
+      <c r="N55" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="O54" s="7" t="s">
+      <c r="O55" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="P54" s="7" t="s">
+      <c r="P55" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="Q54" s="23"/>
-    </row>
-    <row r="55" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="7" t="s">
+      <c r="Q55" s="23"/>
+    </row>
+    <row r="56" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B56" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="D55" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E55" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="7" t="s">
+      <c r="D56" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E56" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="G55" s="23"/>
-      <c r="L55" s="23"/>
-      <c r="Q55" s="23"/>
-    </row>
-    <row r="56" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A56" s="15" t="s">
+      <c r="G56" s="23"/>
+      <c r="L56" s="23"/>
+      <c r="Q56" s="23"/>
+    </row>
+    <row r="57" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A57" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B57" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C57" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="D56" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="15" t="s">
+      <c r="D57" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="G56" s="24"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="15"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="24"/>
-      <c r="M56" s="15"/>
-      <c r="N56" s="15"/>
-      <c r="O56" s="15"/>
-      <c r="P56" s="15"/>
-      <c r="Q56" s="24"/>
-      <c r="R56" s="15" t="s">
+      <c r="G57" s="24"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="24"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
+      <c r="Q57" s="24"/>
+      <c r="R57" s="15" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="57" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A57" s="7" t="s">
+    <row r="58" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A58" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B58" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C58" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F57" s="7" t="s">
+      <c r="D58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="G57" s="23"/>
-      <c r="L57" s="23"/>
-      <c r="Q57" s="23"/>
-      <c r="R57" s="7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="G58" s="23"/>
       <c r="L58" s="23"/>
       <c r="Q58" s="23"/>
       <c r="R58" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G59" s="23"/>
+      <c r="L59" s="23"/>
+      <c r="Q59" s="23"/>
+      <c r="R59" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="59" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A59" s="31" t="s">
+    <row r="60" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A60" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="B59" s="31" t="s">
+      <c r="B60" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="31" t="s">
+      <c r="C60" s="31" t="s">
         <v>323</v>
       </c>
-      <c r="D59" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G59" s="29"/>
-      <c r="H59" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="I59" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="J59" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="K59" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="L59" s="29"/>
-      <c r="M59" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="N59" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="O59" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="P59" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q59" s="29"/>
-    </row>
-    <row r="60" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A60" s="7" t="s">
+      <c r="D60" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G60" s="29"/>
+      <c r="H60" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I60" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="J60" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K60" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L60" s="29"/>
+      <c r="M60" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="N60" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="O60" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P60" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q60" s="29"/>
+    </row>
+    <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B61" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C61" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F60" s="7" t="s">
+      <c r="D61" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E61" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F61" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="G60" s="23"/>
-      <c r="L60" s="23"/>
-      <c r="Q60" s="23"/>
-      <c r="R60" s="7" t="s">
+      <c r="G61" s="23"/>
+      <c r="L61" s="23"/>
+      <c r="Q61" s="23"/>
+      <c r="R61" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="61" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D61" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G61" s="23"/>
-      <c r="H61" s="2" t="s">
+      <c r="D62" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" s="23"/>
+      <c r="H62" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="I61" s="17" t="s">
+      <c r="I62" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="J61" s="17" t="s">
+      <c r="J62" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="K61" s="17" t="s">
+      <c r="K62" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="L61" s="23"/>
-      <c r="M61" s="17" t="s">
+      <c r="L62" s="23"/>
+      <c r="M62" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="N61" s="17" t="s">
+      <c r="N62" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="O61" s="17" t="s">
+      <c r="O62" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="P61" s="17" t="s">
+      <c r="P62" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="Q61" s="23"/>
-      <c r="R61" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A62" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G62" s="23"/>
-      <c r="L62" s="23"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
-      <c r="P62" s="17"/>
       <c r="Q62" s="23"/>
       <c r="R62" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>189</v>
+        <v>10</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
       <c r="D63" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E63" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>214</v>
+        <v>280</v>
       </c>
       <c r="G63" s="23"/>
       <c r="L63" s="23"/>
@@ -3396,170 +3428,173 @@
       <c r="O63" s="17"/>
       <c r="P63" s="17"/>
       <c r="Q63" s="23"/>
-    </row>
-    <row r="64" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A64" s="27" t="s">
-        <v>314</v>
-      </c>
-      <c r="B64" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="D64" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="27" t="s">
-        <v>316</v>
+      <c r="R63" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="G64" s="23"/>
       <c r="L64" s="23"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+      <c r="P64" s="17"/>
       <c r="Q64" s="23"/>
-      <c r="R64" s="27" t="s">
+    </row>
+    <row r="65" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A65" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="B65" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="D65" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="G65" s="23"/>
+      <c r="L65" s="23"/>
+      <c r="Q65" s="23"/>
+      <c r="R65" s="27" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="65" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D65" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G65" s="23"/>
-      <c r="H65" s="17" t="s">
+      <c r="D66" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" s="23"/>
+      <c r="H66" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I65" s="17" t="s">
+      <c r="I66" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J65" s="17" t="s">
+      <c r="J66" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K65" s="17" t="s">
+      <c r="K66" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L65" s="23"/>
-      <c r="M65" s="17" t="s">
+      <c r="L66" s="23"/>
+      <c r="M66" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N65" s="17" t="s">
+      <c r="N66" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O65" s="17" t="s">
+      <c r="O66" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P65" s="17" t="s">
+      <c r="P66" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q65" s="23"/>
-    </row>
-    <row r="66" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" s="2" t="s">
+      <c r="Q66" s="23"/>
+    </row>
+    <row r="67" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G66" s="23"/>
-      <c r="L66" s="23"/>
-      <c r="M66" s="17"/>
-      <c r="N66" s="17"/>
-      <c r="O66" s="17"/>
-      <c r="P66" s="17"/>
-      <c r="Q66" s="23"/>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A67" t="s">
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G67" s="23"/>
+      <c r="L67" s="23"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
+      <c r="Q67" s="23"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
         <v>72</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>5</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>73</v>
       </c>
-      <c r="D67" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" t="s">
-        <v>4</v>
-      </c>
-      <c r="R67"/>
-    </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D68" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G68" s="23"/>
-      <c r="L68" s="23"/>
-      <c r="M68" s="17"/>
-      <c r="N68" s="17"/>
-      <c r="O68" s="17"/>
-      <c r="P68" s="17"/>
-      <c r="Q68" s="23"/>
+      <c r="D68" t="b">
+        <v>1</v>
+      </c>
+      <c r="E68" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>4</v>
+      </c>
+      <c r="R68"/>
     </row>
     <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>74</v>
+        <v>233</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>75</v>
+        <v>247</v>
       </c>
       <c r="D69" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G69" s="23"/>
       <c r="L69" s="23"/>
@@ -3569,454 +3604,447 @@
       <c r="P69" s="17"/>
       <c r="Q69" s="23"/>
     </row>
-    <row r="70" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" s="23"/>
+      <c r="L70" s="23"/>
+      <c r="M70" s="17"/>
+      <c r="N70" s="17"/>
+      <c r="O70" s="17"/>
+      <c r="P70" s="17"/>
+      <c r="Q70" s="23"/>
+    </row>
+    <row r="71" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D70" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G70" s="23"/>
-      <c r="H70" s="17" t="s">
+      <c r="D71" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71" s="23"/>
+      <c r="H71" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I70" s="17" t="s">
+      <c r="I71" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J70" s="17" t="s">
+      <c r="J71" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K70" s="17" t="s">
+      <c r="K71" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L70" s="23"/>
-      <c r="M70" s="17" t="s">
+      <c r="L71" s="23"/>
+      <c r="M71" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N70" s="17" t="s">
+      <c r="N71" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O70" s="17" t="s">
+      <c r="O71" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P70" s="17" t="s">
+      <c r="P71" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q70" s="23"/>
-    </row>
-    <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A71" s="2" t="s">
+      <c r="Q71" s="23"/>
+    </row>
+    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" s="2" t="s">
+      <c r="D72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="G71" s="23"/>
-      <c r="L71" s="23"/>
-      <c r="M71" s="17"/>
-      <c r="N71" s="17"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="17"/>
-      <c r="Q71" s="23"/>
-    </row>
-    <row r="72" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D72" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>273</v>
       </c>
       <c r="G72" s="23"/>
       <c r="L72" s="23"/>
+      <c r="M72" s="17"/>
+      <c r="N72" s="17"/>
+      <c r="O72" s="17"/>
+      <c r="P72" s="17"/>
       <c r="Q72" s="23"/>
-      <c r="R72" s="7" t="s">
+    </row>
+    <row r="73" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G73" s="23"/>
+      <c r="L73" s="23"/>
+      <c r="Q73" s="23"/>
+      <c r="R73" s="7" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
+    <row r="74" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A74" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="2" t="s">
+      <c r="D74" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G73" s="23"/>
-      <c r="H73" s="2" t="s">
+      <c r="G74" s="23"/>
+      <c r="H74" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L73" s="23"/>
-      <c r="M73" s="17" t="s">
+      <c r="L74" s="23"/>
+      <c r="M74" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N73" s="17" t="s">
+      <c r="N74" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O73" s="17" t="s">
+      <c r="O74" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P73" s="17" t="s">
+      <c r="P74" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q73" s="23"/>
-    </row>
-    <row r="74" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A74" s="7" t="s">
+      <c r="Q74" s="23"/>
+    </row>
+    <row r="75" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A75" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B75" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C75" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D74" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="7" t="s">
+      <c r="D75" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="G74" s="23"/>
-      <c r="L74" s="23"/>
-      <c r="Q74" s="23"/>
-      <c r="R74" s="8" t="s">
+      <c r="G75" s="23"/>
+      <c r="L75" s="23"/>
+      <c r="Q75" s="23"/>
+      <c r="R75" s="8" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D75" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G75" s="23"/>
-      <c r="H75" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="I75" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="J75" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="K75" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="L75" s="23"/>
-      <c r="M75" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="N75" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="O75" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="P75" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q75" s="23"/>
     </row>
     <row r="76" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D76" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" s="23"/>
+      <c r="H76" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="I76" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="J76" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="K76" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="L76" s="23"/>
+      <c r="M76" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="N76" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="O76" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="P76" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q76" s="23"/>
+    </row>
+    <row r="77" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D76" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" s="2" t="s">
+      <c r="D77" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G76" s="23"/>
-      <c r="L76" s="23"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="17"/>
-      <c r="Q76" s="23"/>
-    </row>
-    <row r="77" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A77" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D77" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="G77" s="23"/>
       <c r="L77" s="23"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
+      <c r="P77" s="17"/>
       <c r="Q77" s="23"/>
-      <c r="R77" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="78" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A78" s="7" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="D78" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E78" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="G78" s="23"/>
       <c r="L78" s="23"/>
       <c r="Q78" s="23"/>
-      <c r="R78" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A79" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D79" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>94</v>
+      <c r="R78" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A79" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D79" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G79" s="23"/>
       <c r="L79" s="23"/>
-      <c r="M79" s="17"/>
-      <c r="N79" s="17"/>
-      <c r="O79" s="17"/>
-      <c r="P79" s="17"/>
       <c r="Q79" s="23"/>
-    </row>
-    <row r="80" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A80" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="D80" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="17" t="s">
-        <v>4</v>
+      <c r="R79" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D80" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G80" s="23"/>
       <c r="L80" s="23"/>
+      <c r="M80" s="17"/>
+      <c r="N80" s="17"/>
+      <c r="O80" s="17"/>
+      <c r="P80" s="17"/>
       <c r="Q80" s="23"/>
     </row>
-    <row r="81" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="7" t="s">
+    <row r="81" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A81" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B81" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="D81" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G81" s="23"/>
+      <c r="L81" s="23"/>
+      <c r="Q81" s="23"/>
+    </row>
+    <row r="82" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="B81" s="19"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G81" s="23"/>
-      <c r="H81" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I81" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J81" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K81" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L81" s="23"/>
-      <c r="M81" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N81" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O81" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P81" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q81" s="23"/>
-    </row>
-    <row r="82" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A82" s="20" t="s">
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G82" s="23"/>
+      <c r="H82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J82" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K82" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L82" s="23"/>
+      <c r="M82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O82" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P82" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q82" s="23"/>
+    </row>
+    <row r="83" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A83" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B82" s="20" t="s">
+      <c r="B83" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C82" s="20" t="s">
+      <c r="C83" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="D82" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G82" s="23"/>
-      <c r="L82" s="23"/>
-      <c r="Q82" s="23"/>
-    </row>
-    <row r="83" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A83" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>4</v>
+      <c r="D83" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G83" s="23"/>
       <c r="L83" s="23"/>
-      <c r="M83" s="17"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
-      <c r="P83" s="17"/>
       <c r="Q83" s="23"/>
-      <c r="R83" s="8" t="s">
-        <v>218</v>
-      </c>
     </row>
     <row r="84" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D84" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E84" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>332</v>
+        <v>4</v>
       </c>
       <c r="G84" s="23"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="17"/>
-      <c r="J84" s="17"/>
-      <c r="K84" s="17"/>
       <c r="L84" s="23"/>
       <c r="M84" s="17"/>
       <c r="N84" s="17"/>
@@ -4024,124 +4052,131 @@
       <c r="P84" s="17"/>
       <c r="Q84" s="23"/>
       <c r="R84" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="G85" s="23"/>
+      <c r="H85" s="17"/>
+      <c r="I85" s="17"/>
+      <c r="J85" s="17"/>
+      <c r="K85" s="17"/>
+      <c r="L85" s="23"/>
+      <c r="M85" s="17"/>
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="17"/>
+      <c r="Q85" s="23"/>
+      <c r="R85" s="8" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A85" t="s">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
         <v>198</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>199</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>200</v>
       </c>
-      <c r="D85" t="b">
-        <v>0</v>
-      </c>
-      <c r="E85" t="b">
-        <v>1</v>
-      </c>
-      <c r="M85" s="28" t="s">
+      <c r="D86" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" t="b">
+        <v>1</v>
+      </c>
+      <c r="M86" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="N85" s="28" t="s">
+      <c r="N86" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="O85" s="28" t="s">
+      <c r="O86" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="P85" s="28" t="s">
+      <c r="P86" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="R85"/>
-    </row>
-    <row r="86" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A86" s="13" t="s">
+      <c r="R86"/>
+    </row>
+    <row r="87" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A87" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="B86" s="13" t="s">
+      <c r="B87" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="C86" s="13" t="s">
+      <c r="C87" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="D86" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="6" t="s">
+      <c r="D87" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="G86" s="26"/>
-      <c r="L86" s="23"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
-      <c r="Q86" s="23"/>
-    </row>
-    <row r="87" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="7" t="s">
+      <c r="G87" s="26"/>
+      <c r="L87" s="23"/>
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
+      <c r="O87" s="17"/>
+      <c r="P87" s="17"/>
+      <c r="Q87" s="23"/>
+    </row>
+    <row r="88" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B87" s="19"/>
-      <c r="C87" s="19"/>
-      <c r="D87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="7" t="s">
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="G87" s="23"/>
-      <c r="L87" s="23"/>
-      <c r="Q87" s="23"/>
-      <c r="R87" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G88" s="23"/>
       <c r="L88" s="23"/>
-      <c r="M88" s="17"/>
-      <c r="N88" s="17"/>
-      <c r="O88" s="17"/>
-      <c r="P88" s="17"/>
       <c r="Q88" s="23"/>
-    </row>
-    <row r="89" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="R88" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D89" s="2" t="b">
         <v>0</v>
@@ -4149,83 +4184,86 @@
       <c r="E89" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F89" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G89" s="26"/>
+      <c r="F89" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G89" s="23"/>
       <c r="L89" s="23"/>
       <c r="M89" s="17"/>
       <c r="N89" s="17"/>
       <c r="O89" s="17"/>
       <c r="P89" s="17"/>
       <c r="Q89" s="23"/>
-      <c r="R89" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A90" s="17" t="s">
-        <v>296</v>
-      </c>
-      <c r="B90" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="D90" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="6"/>
+    </row>
+    <row r="90" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D90" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>287</v>
+      </c>
       <c r="G90" s="26"/>
       <c r="L90" s="23"/>
+      <c r="M90" s="17"/>
+      <c r="N90" s="17"/>
+      <c r="O90" s="17"/>
+      <c r="P90" s="17"/>
       <c r="Q90" s="23"/>
-    </row>
-    <row r="91" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
+      <c r="R90" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="D91" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="6"/>
+      <c r="G91" s="26"/>
+      <c r="L91" s="23"/>
+      <c r="Q91" s="23"/>
+    </row>
+    <row r="92" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D91" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G91" s="23"/>
-      <c r="L91" s="23"/>
-      <c r="M91" s="17"/>
-      <c r="N91" s="17"/>
-      <c r="O91" s="17"/>
-      <c r="P91" s="17"/>
-      <c r="Q91" s="23"/>
-    </row>
-    <row r="92" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="D92" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E92" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G92" s="23"/>
       <c r="L92" s="23"/>
@@ -4234,28 +4272,22 @@
       <c r="O92" s="17"/>
       <c r="P92" s="17"/>
       <c r="Q92" s="23"/>
-      <c r="R92" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="93" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>104</v>
+        <v>201</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>107</v>
+        <v>202</v>
       </c>
       <c r="D93" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="G93" s="23"/>
       <c r="L93" s="23"/>
@@ -4265,91 +4297,95 @@
       <c r="P93" s="17"/>
       <c r="Q93" s="23"/>
       <c r="R93" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G94" s="23"/>
+      <c r="L94" s="23"/>
+      <c r="M94" s="17"/>
+      <c r="N94" s="17"/>
+      <c r="O94" s="17"/>
+      <c r="P94" s="17"/>
+      <c r="Q94" s="23"/>
+      <c r="R94" s="8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="94" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A94" s="2" t="s">
+    <row r="95" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D94" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G94" s="23"/>
-      <c r="H94" s="17" t="s">
+      <c r="D95" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G95" s="23"/>
+      <c r="H95" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I94" s="17" t="s">
+      <c r="I95" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J94" s="17" t="s">
+      <c r="J95" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K94" s="17" t="s">
+      <c r="K95" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L94" s="23"/>
-      <c r="M94" s="17" t="s">
+      <c r="L95" s="23"/>
+      <c r="M95" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N94" s="17" t="s">
+      <c r="N95" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O94" s="17" t="s">
+      <c r="O95" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P94" s="17" t="s">
+      <c r="P95" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q94" s="23"/>
-      <c r="R94" s="2" t="s">
+      <c r="Q95" s="23"/>
+      <c r="R95" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="95" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A95" s="7" t="s">
+    <row r="96" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A96" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B95" s="7" t="s">
+      <c r="B96" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C96" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="D95" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="G95" s="23"/>
-      <c r="L95" s="23"/>
-      <c r="Q95" s="23"/>
-      <c r="R95" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B96" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="D96" s="7" t="b">
         <v>1</v>
@@ -4364,91 +4400,73 @@
       <c r="L96" s="23"/>
       <c r="Q96" s="23"/>
       <c r="R96" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="97" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D97" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E97" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>14</v>
+        <v>234</v>
       </c>
       <c r="G97" s="23"/>
       <c r="L97" s="23"/>
       <c r="Q97" s="23"/>
       <c r="R97" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D98" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G98" s="23"/>
+      <c r="L98" s="23"/>
+      <c r="Q98" s="23"/>
+      <c r="R98" s="7" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="98" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D98" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G98" s="23"/>
-      <c r="H98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L98" s="23"/>
-      <c r="M98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q98" s="23"/>
     </row>
     <row r="99" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>288</v>
+        <v>117</v>
       </c>
       <c r="D99" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99" s="2" t="b">
         <v>1</v>
@@ -4483,23 +4501,23 @@
     </row>
     <row r="100" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>120</v>
+        <v>288</v>
       </c>
       <c r="D100" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G100" s="23"/>
       <c r="H100" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I100" s="2" t="s">
         <v>4</v>
@@ -4512,7 +4530,7 @@
       </c>
       <c r="L100" s="23"/>
       <c r="M100" s="17" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N100" s="17" t="s">
         <v>4</v>
@@ -4525,129 +4543,128 @@
       </c>
       <c r="Q100" s="23"/>
     </row>
-    <row r="101" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A101" s="7" t="s">
+    <row r="101" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D101" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G101" s="23"/>
+      <c r="H101" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L101" s="23"/>
+      <c r="M101" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N101" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O101" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P101" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q101" s="23"/>
+    </row>
+    <row r="102" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A102" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B102" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="7" t="s">
+      <c r="C102" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D101" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G101" s="23"/>
-      <c r="H101" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I101" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J101" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K101" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L101" s="23"/>
-      <c r="M101" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N101" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O101" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P101" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q101" s="23"/>
-      <c r="R101" s="7" t="s">
+      <c r="D102" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G102" s="23"/>
+      <c r="H102" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I102" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J102" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K102" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L102" s="23"/>
+      <c r="M102" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N102" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O102" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P102" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q102" s="23"/>
+      <c r="R102" s="7" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A102" t="s">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A103" t="s">
         <v>121</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>122</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>123</v>
       </c>
-      <c r="D102" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" t="b">
-        <v>0</v>
-      </c>
-      <c r="H102" s="16" t="s">
+      <c r="D103" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" t="b">
+        <v>0</v>
+      </c>
+      <c r="H103" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="I102" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J102" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K102" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L102" s="23"/>
-      <c r="M102" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="N102" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O102" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P102" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q102" s="23"/>
-      <c r="R102"/>
-    </row>
-    <row r="103" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D103" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G103" s="23"/>
-      <c r="H103" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J103" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K103" s="2" t="s">
+      <c r="I103" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J103" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K103" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L103" s="23"/>
       <c r="M103" s="17" t="s">
-        <v>14</v>
+        <v>290</v>
       </c>
       <c r="N103" s="17" t="s">
         <v>4</v>
@@ -4659,19 +4676,17 @@
         <v>4</v>
       </c>
       <c r="Q103" s="23"/>
-      <c r="R103" s="2" t="s">
-        <v>203</v>
-      </c>
+      <c r="R103"/>
     </row>
     <row r="104" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D104" s="2" t="b">
         <v>1</v>
@@ -4706,103 +4721,147 @@
         <v>4</v>
       </c>
       <c r="Q104" s="23"/>
+      <c r="R104" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="105" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
-        <v>127</v>
+        <v>259</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D105" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E105" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G105" s="23"/>
-      <c r="H105" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I105" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J105" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K105" s="17" t="s">
-        <v>273</v>
+      <c r="H105" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L105" s="23"/>
       <c r="M105" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N105" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O105" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P105" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q105" s="23"/>
+    </row>
+    <row r="106" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D106" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G106" s="23"/>
+      <c r="H106" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="N105" s="17" t="s">
+      <c r="I106" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="O105" s="17" t="s">
+      <c r="J106" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="P105" s="17" t="s">
+      <c r="K106" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="Q105" s="23"/>
-    </row>
-    <row r="106" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A106" s="30" t="s">
+      <c r="L106" s="23"/>
+      <c r="M106" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N106" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O106" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="P106" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q106" s="23"/>
+    </row>
+    <row r="107" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A107" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="B106" s="30" t="s">
+      <c r="B107" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C106" s="30" t="s">
+      <c r="C107" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="D106" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F106" s="30" t="s">
+      <c r="D107" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F107" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="G106" s="29"/>
-      <c r="L106" s="29"/>
-      <c r="Q106" s="29"/>
-    </row>
-    <row r="107" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
+      <c r="G107" s="29"/>
+      <c r="L107" s="29"/>
+      <c r="Q107" s="29"/>
+    </row>
+    <row r="108" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A108" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F107" s="2" t="s">
+      <c r="D108" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F108" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G107" s="23"/>
-      <c r="L107" s="23"/>
-      <c r="M107" s="17"/>
-      <c r="N107" s="17"/>
-      <c r="O107" s="17"/>
-      <c r="P107" s="17"/>
-      <c r="Q107" s="23"/>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R108"/>
+      <c r="G108" s="23"/>
+      <c r="L108" s="23"/>
+      <c r="M108" s="17"/>
+      <c r="N108" s="17"/>
+      <c r="O108" s="17"/>
+      <c r="P108" s="17"/>
+      <c r="Q108" s="23"/>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R109"/>
@@ -4866,6 +4925,9 @@
     </row>
     <row r="129" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R129"/>
+    </row>
+    <row r="130" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R130"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4873,22 +4935,22 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1"/>
     <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="H53" r:id="rId3"/>
-    <hyperlink ref="I53" r:id="rId4"/>
-    <hyperlink ref="J53" r:id="rId5"/>
-    <hyperlink ref="M53" r:id="rId6"/>
-    <hyperlink ref="N53" r:id="rId7"/>
-    <hyperlink ref="O53" r:id="rId8"/>
-    <hyperlink ref="K53" r:id="rId9"/>
-    <hyperlink ref="P53" r:id="rId10"/>
+    <hyperlink ref="H54" r:id="rId3"/>
+    <hyperlink ref="I54" r:id="rId4"/>
+    <hyperlink ref="J54" r:id="rId5"/>
+    <hyperlink ref="M54" r:id="rId6"/>
+    <hyperlink ref="N54" r:id="rId7"/>
+    <hyperlink ref="O54" r:id="rId8"/>
+    <hyperlink ref="K54" r:id="rId9"/>
+    <hyperlink ref="P54" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId11"/>

</xml_diff>

<commit_message>
BRO registratieobject Code TV, en datum opname optioneel
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="339">
   <si>
     <t>Name</t>
   </si>
@@ -1042,9 +1042,6 @@
   </si>
   <si>
     <t>respec msword</t>
-  </si>
-  <si>
-    <t>respec</t>
   </si>
 </sst>
 </file>
@@ -1210,7 +1207,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1310,6 +1307,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1610,10 +1610,10 @@
   <dimension ref="A1:R130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O31" sqref="O31"/>
+      <selection pane="bottomRight" activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1824,16 +1824,16 @@
       <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="40" t="b">
+      <c r="D7" s="41" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1851,10 +1851,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="G8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
@@ -2514,20 +2514,32 @@
       <c r="E30" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="G30" s="23"/>
       <c r="H30" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="I30" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="K30" s="40" t="s">
+        <v>32</v>
+      </c>
       <c r="L30" s="23"/>
       <c r="M30" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
+      <c r="N30" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="O30" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="P30" s="40" t="s">
+        <v>17</v>
+      </c>
       <c r="Q30" s="23"/>
       <c r="R30" s="2" t="s">
         <v>277</v>
@@ -2560,15 +2572,6 @@
         <v>338</v>
       </c>
       <c r="L31" s="29"/>
-      <c r="N31" s="33" t="s">
-        <v>339</v>
-      </c>
-      <c r="O31" s="33" t="s">
-        <v>339</v>
-      </c>
-      <c r="P31" s="33" t="s">
-        <v>339</v>
-      </c>
       <c r="Q31" s="29"/>
     </row>
     <row r="32" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2823,16 +2826,16 @@
       </c>
     </row>
     <row r="42" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D42" s="40" t="b">
+      <c r="D42" s="41" t="b">
         <v>0</v>
       </c>
       <c r="E42" s="2" t="b">
@@ -2850,10 +2853,10 @@
       <c r="Q42" s="23"/>
     </row>
     <row r="43" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
       <c r="G43" s="23"/>
       <c r="L43" s="23"/>
       <c r="M43" s="17"/>

</xml_diff>

<commit_message>
BRO SKOS implementatie (met side-effect op alle xlsx properties alle owners)
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="347">
   <si>
     <t>Name</t>
   </si>
@@ -1042,6 +1042,30 @@
   </si>
   <si>
     <t>respec msword</t>
+  </si>
+  <si>
+    <t>createskos</t>
+  </si>
+  <si>
+    <t>Yes if SKOS RDF must be generated</t>
+  </si>
+  <si>
+    <t>skosrules</t>
+  </si>
+  <si>
+    <t>Only when skos generated</t>
+  </si>
+  <si>
+    <t>The name of the SKOS rules file</t>
+  </si>
+  <si>
+    <t>The name of the SHACL rules file</t>
+  </si>
+  <si>
+    <t>validateskos</t>
+  </si>
+  <si>
+    <t>Yes if SKOS RDF must be validated after it has been generated</t>
   </si>
 </sst>
 </file>
@@ -1607,13 +1631,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R130"/>
+  <dimension ref="A1:R133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P31" sqref="P31"/>
+      <selection pane="bottomRight" activeCell="A105" sqref="A105:XFD105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2637,226 +2661,248 @@
       <c r="L34" s="35"/>
       <c r="Q34" s="35"/>
     </row>
-    <row r="35" spans="1:18" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A35" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="36" t="s">
+    <row r="35" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="34" t="s">
+        <v>339</v>
+      </c>
+      <c r="B35" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="36" t="s">
+      <c r="C35" s="34" t="s">
+        <v>340</v>
+      </c>
+      <c r="D35" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="35"/>
+      <c r="H35" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="K35" s="34" t="s">
+        <v>4</v>
+      </c>
       <c r="L35" s="35"/>
       <c r="Q35" s="35"/>
     </row>
-    <row r="36" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A36" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="34" t="s">
+    <row r="36" spans="1:18" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A36" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="F36" s="34" t="s">
+      <c r="C36" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="36" t="s">
         <v>14</v>
       </c>
       <c r="G36" s="35"/>
       <c r="L36" s="35"/>
       <c r="Q36" s="35"/>
     </row>
-    <row r="37" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="36" t="s">
+    <row r="37" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A37" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="36" t="b">
-        <v>1</v>
+      <c r="C37" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" s="34" t="s">
+        <v>14</v>
       </c>
       <c r="G37" s="35"/>
-      <c r="H37" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="I37" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J37" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="K37" s="36" t="s">
-        <v>14</v>
-      </c>
       <c r="L37" s="35"/>
-      <c r="M37" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="N37" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="O37" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="P37" s="36" t="s">
-        <v>4</v>
-      </c>
       <c r="Q37" s="35"/>
     </row>
     <row r="38" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="35"/>
+      <c r="H38" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L38" s="35"/>
+      <c r="M38" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="N38" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="O38" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="P38" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q38" s="35"/>
+    </row>
+    <row r="39" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="36" t="s">
         <v>329</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B39" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C39" s="36" t="s">
         <v>330</v>
       </c>
-      <c r="D38" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="36" t="s">
+      <c r="D39" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="36" t="s">
         <v>333</v>
-      </c>
-      <c r="G38" s="35"/>
-      <c r="L38" s="35"/>
-      <c r="Q38" s="35"/>
-    </row>
-    <row r="39" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="B39" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="D39" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" s="34" t="s">
-        <v>14</v>
       </c>
       <c r="G39" s="35"/>
       <c r="L39" s="35"/>
       <c r="Q39" s="35"/>
     </row>
-    <row r="40" spans="1:18" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A40" s="37" t="s">
+    <row r="40" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D40" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="Q40" s="35"/>
+    </row>
+    <row r="41" spans="1:18" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A41" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="37" t="s">
+      <c r="B41" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="37" t="s">
+      <c r="C41" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="F40" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" s="38"/>
-      <c r="L40" s="38"/>
-      <c r="Q40" s="38"/>
-      <c r="R40" s="37" t="s">
+      <c r="D41" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="38"/>
+      <c r="L41" s="38"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="37" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="41" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A41" s="7" t="s">
+    <row r="42" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A42" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B42" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C42" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F41" s="7" t="s">
+      <c r="D42" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="G41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="Q41" s="23"/>
-      <c r="R41" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="41" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G42" s="23"/>
       <c r="L42" s="23"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="17"/>
-      <c r="O42" s="17"/>
-      <c r="P42" s="17"/>
       <c r="Q42" s="23"/>
+      <c r="R42" s="7" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="43" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
+      <c r="A43" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G43" s="23"/>
       <c r="L43" s="23"/>
       <c r="M43" s="17"/>
@@ -2865,22 +2911,11 @@
       <c r="P43" s="17"/>
       <c r="Q43" s="23"/>
     </row>
-    <row r="44" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A44" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D44" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
       <c r="G44" s="23"/>
       <c r="L44" s="23"/>
       <c r="M44" s="17"/>
@@ -2889,21 +2924,21 @@
       <c r="P44" s="17"/>
       <c r="Q44" s="23"/>
     </row>
-    <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
-        <v>50</v>
+        <v>173</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>51</v>
+        <v>175</v>
       </c>
       <c r="D45" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" s="23"/>
       <c r="L45" s="23"/>
@@ -2913,15 +2948,15 @@
       <c r="P45" s="17"/>
       <c r="Q45" s="23"/>
     </row>
-    <row r="46" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D46" s="2" t="b">
         <v>0</v>
@@ -2929,95 +2964,95 @@
       <c r="E46" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="G46" s="26"/>
+      <c r="G46" s="23"/>
       <c r="L46" s="23"/>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
       <c r="O46" s="17"/>
       <c r="P46" s="17"/>
       <c r="Q46" s="23"/>
-      <c r="R46" s="2" t="s">
+    </row>
+    <row r="47" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G47" s="26"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="23"/>
+      <c r="R47" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E47" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="17" t="s">
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I47" s="17" t="s">
+      <c r="I48" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J47" s="17" t="s">
+      <c r="J48" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K47" s="17" t="s">
+      <c r="K48" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L47" s="23"/>
-      <c r="M47" s="17" t="s">
+      <c r="L48" s="23"/>
+      <c r="M48" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N47" s="17" t="s">
+      <c r="N48" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O47" s="17" t="s">
+      <c r="O48" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P47" s="17" t="s">
+      <c r="P48" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q47" s="23"/>
-    </row>
-    <row r="48" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="7" t="s">
+      <c r="Q48" s="23"/>
+    </row>
+    <row r="49" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B49" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C49" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D48" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G48" s="23"/>
-      <c r="L48" s="23"/>
-      <c r="Q48" s="23"/>
-      <c r="R48"/>
-    </row>
-    <row r="49" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A49" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="D49" s="7" t="b">
         <v>0</v>
       </c>
@@ -3025,77 +3060,78 @@
         <v>1</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="G49" s="23"/>
       <c r="L49" s="23"/>
       <c r="Q49" s="23"/>
-    </row>
-    <row r="50" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D50" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>14</v>
+      <c r="R49"/>
+    </row>
+    <row r="50" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A50" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="G50" s="23"/>
       <c r="L50" s="23"/>
-      <c r="M50" s="17"/>
-      <c r="N50" s="17"/>
-      <c r="O50" s="17"/>
-      <c r="P50" s="17"/>
       <c r="Q50" s="23"/>
     </row>
-    <row r="51" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B51" s="7" t="s">
+    <row r="51" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D51" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" s="7" t="s">
+      <c r="C51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G51" s="23"/>
       <c r="L51" s="23"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
       <c r="Q51" s="23"/>
     </row>
-    <row r="52" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D52" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E52" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>14</v>
@@ -3103,25 +3139,22 @@
       <c r="G52" s="23"/>
       <c r="L52" s="23"/>
       <c r="Q52" s="23"/>
-      <c r="R52" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="53" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A53" s="7" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>182</v>
+        <v>60</v>
       </c>
       <c r="D53" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E53" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>14</v>
@@ -3129,357 +3162,353 @@
       <c r="G53" s="23"/>
       <c r="L53" s="23"/>
       <c r="Q53" s="23"/>
-    </row>
-    <row r="54" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="R53" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D54" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" s="23"/>
+      <c r="L54" s="23"/>
+      <c r="Q54" s="23"/>
+    </row>
+    <row r="55" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A55" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B55" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G54" s="23"/>
-      <c r="H54" s="18" t="s">
+      <c r="G55" s="23"/>
+      <c r="H55" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="I54" s="18" t="s">
+      <c r="I55" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="J54" s="18" t="s">
+      <c r="J55" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="K54" s="18" t="s">
+      <c r="K55" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="L54" s="23"/>
-      <c r="M54" s="18" t="s">
+      <c r="L55" s="23"/>
+      <c r="M55" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="N54" s="18" t="s">
+      <c r="N55" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="O54" s="18" t="s">
+      <c r="O55" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="P54" s="18" t="s">
+      <c r="P55" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="Q54" s="23"/>
-    </row>
-    <row r="55" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A55" s="7" t="s">
+      <c r="Q55" s="23"/>
+    </row>
+    <row r="56" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A56" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B56" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D55" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G55" s="23"/>
-      <c r="H55" s="7" t="s">
+      <c r="D56" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" s="23"/>
+      <c r="H56" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="I55" s="7" t="s">
+      <c r="I56" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="J55" s="7" t="s">
+      <c r="J56" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="K55" s="7" t="s">
+      <c r="K56" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="L55" s="23"/>
-      <c r="M55" s="7" t="s">
+      <c r="L56" s="23"/>
+      <c r="M56" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="N55" s="7" t="s">
+      <c r="N56" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="O55" s="7" t="s">
+      <c r="O56" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="P55" s="7" t="s">
+      <c r="P56" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="Q55" s="23"/>
-    </row>
-    <row r="56" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="7" t="s">
+      <c r="Q56" s="23"/>
+    </row>
+    <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B57" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C57" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="D56" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E56" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="7" t="s">
+      <c r="D57" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E57" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="G56" s="23"/>
-      <c r="L56" s="23"/>
-      <c r="Q56" s="23"/>
-    </row>
-    <row r="57" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A57" s="15" t="s">
+      <c r="G57" s="23"/>
+      <c r="L57" s="23"/>
+      <c r="Q57" s="23"/>
+    </row>
+    <row r="58" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A58" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B58" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C58" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="D57" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="15" t="s">
+      <c r="D58" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="G57" s="24"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="24"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
-      <c r="P57" s="15"/>
-      <c r="Q57" s="24"/>
-      <c r="R57" s="15" t="s">
+      <c r="G58" s="24"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15"/>
+      <c r="O58" s="15"/>
+      <c r="P58" s="15"/>
+      <c r="Q58" s="24"/>
+      <c r="R58" s="15" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="58" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A58" s="7" t="s">
+    <row r="59" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A59" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F58" s="7" t="s">
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F59" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="G58" s="23"/>
-      <c r="L58" s="23"/>
-      <c r="Q58" s="23"/>
-      <c r="R58" s="7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="G59" s="23"/>
       <c r="L59" s="23"/>
       <c r="Q59" s="23"/>
       <c r="R59" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G60" s="23"/>
+      <c r="L60" s="23"/>
+      <c r="Q60" s="23"/>
+      <c r="R60" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="60" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A60" s="31" t="s">
+    <row r="61" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A61" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="B60" s="31" t="s">
+      <c r="B61" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C60" s="31" t="s">
+      <c r="C61" s="31" t="s">
         <v>323</v>
       </c>
-      <c r="D60" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G60" s="29"/>
-      <c r="H60" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="I60" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="J60" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="K60" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="L60" s="29"/>
-      <c r="M60" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="N60" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="O60" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="P60" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q60" s="29"/>
-    </row>
-    <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="7" t="s">
+      <c r="D61" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G61" s="29"/>
+      <c r="H61" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I61" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="J61" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K61" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L61" s="29"/>
+      <c r="M61" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="N61" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="O61" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P61" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q61" s="29"/>
+    </row>
+    <row r="62" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C62" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D61" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F61" s="7" t="s">
+      <c r="D62" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="G61" s="23"/>
-      <c r="L61" s="23"/>
-      <c r="Q61" s="23"/>
-      <c r="R61" s="7" t="s">
+      <c r="G62" s="23"/>
+      <c r="L62" s="23"/>
+      <c r="Q62" s="23"/>
+      <c r="R62" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="62" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G62" s="23"/>
-      <c r="H62" s="2" t="s">
+      <c r="D63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" s="23"/>
+      <c r="H63" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="I62" s="17" t="s">
+      <c r="I63" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="J62" s="17" t="s">
+      <c r="J63" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="K62" s="17" t="s">
+      <c r="K63" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="L62" s="23"/>
-      <c r="M62" s="17" t="s">
+      <c r="L63" s="23"/>
+      <c r="M63" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="N62" s="17" t="s">
+      <c r="N63" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="O62" s="17" t="s">
+      <c r="O63" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="P62" s="17" t="s">
+      <c r="P63" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="Q62" s="23"/>
-      <c r="R62" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A63" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G63" s="23"/>
-      <c r="L63" s="23"/>
-      <c r="M63" s="17"/>
-      <c r="N63" s="17"/>
-      <c r="O63" s="17"/>
-      <c r="P63" s="17"/>
       <c r="Q63" s="23"/>
       <c r="R63" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>189</v>
+        <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
       <c r="D64" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E64" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>214</v>
+        <v>280</v>
       </c>
       <c r="G64" s="23"/>
       <c r="L64" s="23"/>
@@ -3488,170 +3517,173 @@
       <c r="O64" s="17"/>
       <c r="P64" s="17"/>
       <c r="Q64" s="23"/>
-    </row>
-    <row r="65" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A65" s="27" t="s">
-        <v>314</v>
-      </c>
-      <c r="B65" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C65" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="D65" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" s="27" t="s">
-        <v>316</v>
+      <c r="R64" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A65" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D65" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="G65" s="23"/>
       <c r="L65" s="23"/>
+      <c r="M65" s="17"/>
+      <c r="N65" s="17"/>
+      <c r="O65" s="17"/>
+      <c r="P65" s="17"/>
       <c r="Q65" s="23"/>
-      <c r="R65" s="27" t="s">
+    </row>
+    <row r="66" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A66" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="B66" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="D66" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="G66" s="23"/>
+      <c r="L66" s="23"/>
+      <c r="Q66" s="23"/>
+      <c r="R66" s="27" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="66" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D66" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G66" s="23"/>
-      <c r="H66" s="17" t="s">
+      <c r="D67" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" s="23"/>
+      <c r="H67" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I66" s="17" t="s">
+      <c r="I67" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J66" s="17" t="s">
+      <c r="J67" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K66" s="17" t="s">
+      <c r="K67" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L66" s="23"/>
-      <c r="M66" s="17" t="s">
+      <c r="L67" s="23"/>
+      <c r="M67" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N66" s="17" t="s">
+      <c r="N67" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O66" s="17" t="s">
+      <c r="O67" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P66" s="17" t="s">
+      <c r="P67" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q66" s="23"/>
-    </row>
-    <row r="67" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" s="2" t="s">
+      <c r="Q67" s="23"/>
+    </row>
+    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G67" s="23"/>
-      <c r="L67" s="23"/>
-      <c r="M67" s="17"/>
-      <c r="N67" s="17"/>
-      <c r="O67" s="17"/>
-      <c r="P67" s="17"/>
-      <c r="Q67" s="23"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A68" t="s">
+      <c r="D68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G68" s="23"/>
+      <c r="L68" s="23"/>
+      <c r="M68" s="17"/>
+      <c r="N68" s="17"/>
+      <c r="O68" s="17"/>
+      <c r="P68" s="17"/>
+      <c r="Q68" s="23"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
         <v>72</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>5</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>73</v>
       </c>
-      <c r="D68" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" t="s">
-        <v>4</v>
-      </c>
-      <c r="R68"/>
-    </row>
-    <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A69" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D69" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G69" s="23"/>
-      <c r="L69" s="23"/>
-      <c r="M69" s="17"/>
-      <c r="N69" s="17"/>
-      <c r="O69" s="17"/>
-      <c r="P69" s="17"/>
-      <c r="Q69" s="23"/>
+      <c r="D69" t="b">
+        <v>1</v>
+      </c>
+      <c r="E69" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>4</v>
+      </c>
+      <c r="R69"/>
     </row>
     <row r="70" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
-        <v>74</v>
+        <v>233</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>75</v>
+        <v>247</v>
       </c>
       <c r="D70" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G70" s="23"/>
       <c r="L70" s="23"/>
@@ -3661,454 +3693,447 @@
       <c r="P70" s="17"/>
       <c r="Q70" s="23"/>
     </row>
-    <row r="71" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G71" s="23"/>
+      <c r="L71" s="23"/>
+      <c r="M71" s="17"/>
+      <c r="N71" s="17"/>
+      <c r="O71" s="17"/>
+      <c r="P71" s="17"/>
+      <c r="Q71" s="23"/>
+    </row>
+    <row r="72" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D71" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G71" s="23"/>
-      <c r="H71" s="17" t="s">
+      <c r="D72" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" s="23"/>
+      <c r="H72" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I71" s="17" t="s">
+      <c r="I72" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J71" s="17" t="s">
+      <c r="J72" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K71" s="17" t="s">
+      <c r="K72" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L71" s="23"/>
-      <c r="M71" s="17" t="s">
+      <c r="L72" s="23"/>
+      <c r="M72" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N71" s="17" t="s">
+      <c r="N72" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="O71" s="17" t="s">
+      <c r="O72" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="P71" s="17" t="s">
+      <c r="P72" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="Q71" s="23"/>
-    </row>
-    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" s="2" t="s">
+      <c r="Q72" s="23"/>
+    </row>
+    <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D72" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F72" s="2" t="s">
+      <c r="D73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="G72" s="23"/>
-      <c r="L72" s="23"/>
-      <c r="M72" s="17"/>
-      <c r="N72" s="17"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="17"/>
-      <c r="Q72" s="23"/>
-    </row>
-    <row r="73" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D73" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>273</v>
       </c>
       <c r="G73" s="23"/>
       <c r="L73" s="23"/>
+      <c r="M73" s="17"/>
+      <c r="N73" s="17"/>
+      <c r="O73" s="17"/>
+      <c r="P73" s="17"/>
       <c r="Q73" s="23"/>
-      <c r="R73" s="7" t="s">
+    </row>
+    <row r="74" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D74" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G74" s="23"/>
+      <c r="L74" s="23"/>
+      <c r="Q74" s="23"/>
+      <c r="R74" s="7" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="74" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A75" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D74" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F74" s="2" t="s">
+      <c r="D75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G74" s="23"/>
-      <c r="H74" s="2" t="s">
+      <c r="G75" s="23"/>
+      <c r="H75" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L74" s="23"/>
-      <c r="M74" s="17" t="s">
+      <c r="L75" s="23"/>
+      <c r="M75" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N74" s="17" t="s">
+      <c r="N75" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O74" s="17" t="s">
+      <c r="O75" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P74" s="17" t="s">
+      <c r="P75" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q74" s="23"/>
-    </row>
-    <row r="75" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A75" s="7" t="s">
+      <c r="Q75" s="23"/>
+    </row>
+    <row r="76" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A76" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B76" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="C76" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D75" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" s="7" t="s">
+      <c r="D76" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="G75" s="23"/>
-      <c r="L75" s="23"/>
-      <c r="Q75" s="23"/>
-      <c r="R75" s="8" t="s">
+      <c r="G76" s="23"/>
+      <c r="L76" s="23"/>
+      <c r="Q76" s="23"/>
+      <c r="R76" s="8" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D76" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G76" s="23"/>
-      <c r="H76" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="I76" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="J76" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="K76" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="L76" s="23"/>
-      <c r="M76" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="N76" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="O76" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="P76" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q76" s="23"/>
     </row>
     <row r="77" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D77" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" s="23"/>
+      <c r="H77" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="I77" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="J77" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="K77" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="L77" s="23"/>
+      <c r="M77" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="N77" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="O77" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="P77" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q77" s="23"/>
+    </row>
+    <row r="78" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D77" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="2" t="s">
+      <c r="D78" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G77" s="23"/>
-      <c r="L77" s="23"/>
-      <c r="M77" s="17"/>
-      <c r="N77" s="17"/>
-      <c r="O77" s="17"/>
-      <c r="P77" s="17"/>
-      <c r="Q77" s="23"/>
-    </row>
-    <row r="78" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A78" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D78" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="G78" s="23"/>
       <c r="L78" s="23"/>
+      <c r="M78" s="17"/>
+      <c r="N78" s="17"/>
+      <c r="O78" s="17"/>
+      <c r="P78" s="17"/>
       <c r="Q78" s="23"/>
-      <c r="R78" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="79" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A79" s="7" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="D79" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E79" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="G79" s="23"/>
       <c r="L79" s="23"/>
       <c r="Q79" s="23"/>
-      <c r="R79" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A80" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>94</v>
+      <c r="R79" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A80" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D80" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G80" s="23"/>
       <c r="L80" s="23"/>
-      <c r="M80" s="17"/>
-      <c r="N80" s="17"/>
-      <c r="O80" s="17"/>
-      <c r="P80" s="17"/>
       <c r="Q80" s="23"/>
-    </row>
-    <row r="81" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A81" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="B81" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="D81" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E81" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="17" t="s">
-        <v>4</v>
+      <c r="R80" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A81" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G81" s="23"/>
       <c r="L81" s="23"/>
+      <c r="M81" s="17"/>
+      <c r="N81" s="17"/>
+      <c r="O81" s="17"/>
+      <c r="P81" s="17"/>
       <c r="Q81" s="23"/>
     </row>
-    <row r="82" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="7" t="s">
+    <row r="82" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A82" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="D82" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G82" s="23"/>
+      <c r="L82" s="23"/>
+      <c r="Q82" s="23"/>
+    </row>
+    <row r="83" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G82" s="23"/>
-      <c r="H82" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I82" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J82" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K82" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L82" s="23"/>
-      <c r="M82" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N82" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O82" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P82" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q82" s="23"/>
-    </row>
-    <row r="83" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A83" s="20" t="s">
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G83" s="23"/>
+      <c r="H83" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I83" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J83" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K83" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L83" s="23"/>
+      <c r="M83" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N83" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O83" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P83" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q83" s="23"/>
+    </row>
+    <row r="84" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A84" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B83" s="20" t="s">
+      <c r="B84" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C83" s="20" t="s">
+      <c r="C84" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="D83" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G83" s="23"/>
-      <c r="L83" s="23"/>
-      <c r="Q83" s="23"/>
-    </row>
-    <row r="84" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>4</v>
+      <c r="D84" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G84" s="23"/>
       <c r="L84" s="23"/>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
-      <c r="P84" s="17"/>
       <c r="Q84" s="23"/>
-      <c r="R84" s="8" t="s">
-        <v>218</v>
-      </c>
     </row>
     <row r="85" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D85" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>332</v>
+        <v>4</v>
       </c>
       <c r="G85" s="23"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="17"/>
-      <c r="J85" s="17"/>
-      <c r="K85" s="17"/>
       <c r="L85" s="23"/>
       <c r="M85" s="17"/>
       <c r="N85" s="17"/>
@@ -4116,124 +4141,135 @@
       <c r="P85" s="17"/>
       <c r="Q85" s="23"/>
       <c r="R85" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A86" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D86" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="G86" s="23"/>
+      <c r="H86" s="17"/>
+      <c r="I86" s="17"/>
+      <c r="J86" s="17"/>
+      <c r="K86" s="17"/>
+      <c r="L86" s="23"/>
+      <c r="M86" s="17"/>
+      <c r="N86" s="17"/>
+      <c r="O86" s="17"/>
+      <c r="P86" s="17"/>
+      <c r="Q86" s="23"/>
+      <c r="R86" s="8" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A86" t="s">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A87" t="s">
         <v>198</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>199</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>200</v>
       </c>
-      <c r="D86" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" t="b">
-        <v>1</v>
-      </c>
-      <c r="M86" s="28" t="s">
+      <c r="D87" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" t="b">
+        <v>1</v>
+      </c>
+      <c r="M87" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="N86" s="28" t="s">
+      <c r="N87" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="O86" s="28" t="s">
+      <c r="O87" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="P86" s="28" t="s">
+      <c r="P87" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="R86"/>
-    </row>
-    <row r="87" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A87" s="13" t="s">
+      <c r="R87"/>
+    </row>
+    <row r="88" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A88" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="B87" s="13" t="s">
+      <c r="B88" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="C87" s="13" t="s">
+      <c r="C88" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="D87" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="6" t="s">
+      <c r="D88" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="G87" s="26"/>
-      <c r="L87" s="23"/>
-      <c r="M87" s="17"/>
-      <c r="N87" s="17"/>
-      <c r="O87" s="17"/>
-      <c r="P87" s="17"/>
-      <c r="Q87" s="23"/>
-    </row>
-    <row r="88" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="7" t="s">
+      <c r="G88" s="26"/>
+      <c r="L88" s="23"/>
+      <c r="M88" s="17"/>
+      <c r="N88" s="17"/>
+      <c r="O88" s="17"/>
+      <c r="P88" s="17"/>
+      <c r="Q88" s="23"/>
+    </row>
+    <row r="89" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" s="7" t="s">
+      <c r="B89" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" s="28" t="s">
+        <v>344</v>
+      </c>
+      <c r="D89" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="28" t="s">
         <v>273</v>
-      </c>
-      <c r="G88" s="23"/>
-      <c r="L88" s="23"/>
-      <c r="Q88" s="23"/>
-      <c r="R88" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D89" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G89" s="23"/>
       <c r="L89" s="23"/>
-      <c r="M89" s="17"/>
-      <c r="N89" s="17"/>
-      <c r="O89" s="17"/>
-      <c r="P89" s="17"/>
       <c r="Q89" s="23"/>
-    </row>
-    <row r="90" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="R89" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D90" s="2" t="b">
         <v>0</v>
@@ -4241,50 +4277,52 @@
       <c r="E90" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F90" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G90" s="26"/>
+      <c r="F90" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G90" s="23"/>
       <c r="L90" s="23"/>
       <c r="M90" s="17"/>
       <c r="N90" s="17"/>
       <c r="O90" s="17"/>
       <c r="P90" s="17"/>
       <c r="Q90" s="23"/>
-      <c r="R90" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="17" t="s">
-        <v>296</v>
-      </c>
-      <c r="B91" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="D91" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="6"/>
-      <c r="G91" s="26"/>
-      <c r="L91" s="23"/>
-      <c r="Q91" s="23"/>
-    </row>
-    <row r="92" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="91" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="B91" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" s="28" t="s">
+        <v>343</v>
+      </c>
+      <c r="D91" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="28" t="s">
+        <v>273</v>
+      </c>
+      <c r="G91" s="29"/>
+      <c r="L91" s="29"/>
+      <c r="Q91" s="29"/>
+      <c r="R91" s="7" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D92" s="2" t="b">
         <v>0</v>
@@ -4292,62 +4330,59 @@
       <c r="E92" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F92" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G92" s="23"/>
+      <c r="F92" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G92" s="26"/>
       <c r="L92" s="23"/>
       <c r="M92" s="17"/>
       <c r="N92" s="17"/>
       <c r="O92" s="17"/>
       <c r="P92" s="17"/>
       <c r="Q92" s="23"/>
-    </row>
-    <row r="93" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B93" s="2" t="s">
+      <c r="R92" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="B93" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D93" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G93" s="23"/>
+      <c r="C93" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="D93" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="6"/>
+      <c r="G93" s="26"/>
       <c r="L93" s="23"/>
-      <c r="M93" s="17"/>
-      <c r="N93" s="17"/>
-      <c r="O93" s="17"/>
-      <c r="P93" s="17"/>
       <c r="Q93" s="23"/>
-      <c r="R93" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="94" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D94" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="G94" s="23"/>
       <c r="L94" s="23"/>
@@ -4356,232 +4391,198 @@
       <c r="O94" s="17"/>
       <c r="P94" s="17"/>
       <c r="Q94" s="23"/>
-      <c r="R94" s="8" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="95" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>108</v>
+        <v>201</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>109</v>
+        <v>202</v>
       </c>
       <c r="D95" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G95" s="23"/>
-      <c r="H95" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="I95" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="J95" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="K95" s="17" t="s">
-        <v>281</v>
-      </c>
       <c r="L95" s="23"/>
-      <c r="M95" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="N95" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="O95" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="P95" s="17" t="s">
-        <v>282</v>
-      </c>
+      <c r="M95" s="17"/>
+      <c r="N95" s="17"/>
+      <c r="O95" s="17"/>
+      <c r="P95" s="17"/>
       <c r="Q95" s="23"/>
-      <c r="R95" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A96" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B96" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D96" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E96" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>234</v>
+      <c r="R95" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A96" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="G96" s="23"/>
       <c r="L96" s="23"/>
+      <c r="M96" s="17"/>
+      <c r="N96" s="17"/>
+      <c r="O96" s="17"/>
+      <c r="P96" s="17"/>
       <c r="Q96" s="23"/>
-      <c r="R96" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D97" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F97" s="7" t="s">
+      <c r="R96" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A97" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D97" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G97" s="23"/>
+      <c r="H97" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="I97" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="J97" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="K97" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="L97" s="23"/>
+      <c r="M97" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="N97" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="O97" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="P97" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q97" s="23"/>
+      <c r="R97" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A98" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D98" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F98" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="G97" s="23"/>
-      <c r="L97" s="23"/>
-      <c r="Q97" s="23"/>
-      <c r="R97" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D98" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="G98" s="23"/>
       <c r="L98" s="23"/>
       <c r="Q98" s="23"/>
       <c r="R98" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D99" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G99" s="23"/>
+      <c r="L99" s="23"/>
+      <c r="Q99" s="23"/>
+      <c r="R99" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D100" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G100" s="23"/>
+      <c r="L100" s="23"/>
+      <c r="Q100" s="23"/>
+      <c r="R100" s="7" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="99" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D99" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G99" s="23"/>
-      <c r="H99" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I99" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J99" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K99" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L99" s="23"/>
-      <c r="M99" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N99" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O99" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P99" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q99" s="23"/>
-    </row>
-    <row r="100" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="D100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G100" s="23"/>
-      <c r="H100" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I100" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J100" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K100" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L100" s="23"/>
-      <c r="M100" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N100" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O100" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P100" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q100" s="23"/>
     </row>
     <row r="101" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D101" s="2" t="b">
         <v>0</v>
@@ -4591,7 +4592,7 @@
       </c>
       <c r="G101" s="23"/>
       <c r="H101" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I101" s="2" t="s">
         <v>4</v>
@@ -4604,7 +4605,7 @@
       </c>
       <c r="L101" s="23"/>
       <c r="M101" s="17" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N101" s="17" t="s">
         <v>4</v>
@@ -4617,290 +4618,418 @@
       </c>
       <c r="Q101" s="23"/>
     </row>
-    <row r="102" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A102" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B102" s="7" t="s">
+    <row r="102" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C102" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D102" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" s="7" t="b">
+      <c r="C102" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D102" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G102" s="23"/>
-      <c r="H102" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I102" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J102" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K102" s="7" t="s">
+      <c r="H102" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K102" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L102" s="23"/>
-      <c r="M102" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N102" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O102" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P102" s="7" t="s">
+      <c r="M102" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N102" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O102" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P102" s="17" t="s">
         <v>4</v>
       </c>
       <c r="Q102" s="23"/>
-      <c r="R102" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A103" t="s">
-        <v>121</v>
-      </c>
-      <c r="B103" t="s">
-        <v>122</v>
-      </c>
-      <c r="C103" t="s">
-        <v>123</v>
-      </c>
-      <c r="D103" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" t="b">
-        <v>0</v>
-      </c>
-      <c r="H103" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="I103" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J103" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K103" s="16" t="s">
+    </row>
+    <row r="103" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D103" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G103" s="23"/>
+      <c r="H103" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J103" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K103" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L103" s="23"/>
       <c r="M103" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N103" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O103" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P103" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q103" s="23"/>
+    </row>
+    <row r="104" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="B104" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D104" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" s="28"/>
+      <c r="G104" s="23"/>
+      <c r="H104" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I104" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J104" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K104" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L104" s="23"/>
+      <c r="M104" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N104" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O104" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P104" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q104" s="23"/>
+      <c r="R104" s="28" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="28" t="s">
+        <v>345</v>
+      </c>
+      <c r="B105" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="28" t="s">
+        <v>346</v>
+      </c>
+      <c r="D105" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" s="28"/>
+      <c r="G105" s="29"/>
+      <c r="H105" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I105" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J105" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K105" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L105" s="29"/>
+      <c r="M105" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N105" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O105" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P105" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q105" s="29"/>
+      <c r="R105" s="28" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
+        <v>121</v>
+      </c>
+      <c r="B106" t="s">
+        <v>122</v>
+      </c>
+      <c r="C106" t="s">
+        <v>123</v>
+      </c>
+      <c r="D106" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" t="b">
+        <v>0</v>
+      </c>
+      <c r="H106" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="N103" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O103" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P103" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q103" s="23"/>
-      <c r="R103"/>
-    </row>
-    <row r="104" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D104" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E104" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G104" s="23"/>
-      <c r="H104" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L104" s="23"/>
-      <c r="M104" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N104" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O104" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P104" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q104" s="23"/>
-      <c r="R104" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D105" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E105" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G105" s="23"/>
-      <c r="H105" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I105" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J105" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K105" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L105" s="23"/>
-      <c r="M105" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N105" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O105" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P105" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q105" s="23"/>
-    </row>
-    <row r="106" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D106" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G106" s="23"/>
-      <c r="H106" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I106" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J106" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K106" s="17" t="s">
-        <v>273</v>
+      <c r="I106" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J106" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K106" s="16" t="s">
+        <v>4</v>
       </c>
       <c r="L106" s="23"/>
       <c r="M106" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="N106" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O106" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P106" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q106" s="23"/>
+      <c r="R106"/>
+    </row>
+    <row r="107" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D107" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G107" s="23"/>
+      <c r="H107" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L107" s="23"/>
+      <c r="M107" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N107" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O107" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P107" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q107" s="23"/>
+      <c r="R107" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D108" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G108" s="23"/>
+      <c r="H108" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L108" s="23"/>
+      <c r="M108" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N108" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O108" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P108" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q108" s="23"/>
+    </row>
+    <row r="109" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G109" s="23"/>
+      <c r="H109" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="N106" s="17" t="s">
+      <c r="I109" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="O106" s="17" t="s">
+      <c r="J109" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="P106" s="17" t="s">
+      <c r="K109" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="Q106" s="23"/>
-    </row>
-    <row r="107" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A107" s="30" t="s">
+      <c r="L109" s="23"/>
+      <c r="M109" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N109" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O109" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="P109" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q109" s="23"/>
+    </row>
+    <row r="110" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A110" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="B107" s="30" t="s">
+      <c r="B110" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C107" s="30" t="s">
+      <c r="C110" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="D107" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F107" s="30" t="s">
+      <c r="D110" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="G107" s="29"/>
-      <c r="L107" s="29"/>
-      <c r="Q107" s="29"/>
-    </row>
-    <row r="108" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A108" s="2" t="s">
+      <c r="G110" s="29"/>
+      <c r="L110" s="29"/>
+      <c r="Q110" s="29"/>
+    </row>
+    <row r="111" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A111" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D108" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E108" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F108" s="2" t="s">
+      <c r="D111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F111" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G108" s="23"/>
-      <c r="L108" s="23"/>
-      <c r="M108" s="17"/>
-      <c r="N108" s="17"/>
-      <c r="O108" s="17"/>
-      <c r="P108" s="17"/>
-      <c r="Q108" s="23"/>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R109"/>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R110"/>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R111"/>
+      <c r="G111" s="23"/>
+      <c r="L111" s="23"/>
+      <c r="M111" s="17"/>
+      <c r="N111" s="17"/>
+      <c r="O111" s="17"/>
+      <c r="P111" s="17"/>
+      <c r="Q111" s="23"/>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R112"/>
@@ -4958,6 +5087,15 @@
     </row>
     <row r="130" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R130"/>
+    </row>
+    <row r="131" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R131"/>
+    </row>
+    <row r="132" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R132"/>
+    </row>
+    <row r="133" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R133"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4965,22 +5103,22 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1"/>
     <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="H54" r:id="rId3"/>
-    <hyperlink ref="I54" r:id="rId4"/>
-    <hyperlink ref="J54" r:id="rId5"/>
-    <hyperlink ref="M54" r:id="rId6"/>
-    <hyperlink ref="N54" r:id="rId7"/>
-    <hyperlink ref="O54" r:id="rId8"/>
-    <hyperlink ref="K54" r:id="rId9"/>
-    <hyperlink ref="P54" r:id="rId10"/>
+    <hyperlink ref="H55" r:id="rId3"/>
+    <hyperlink ref="I55" r:id="rId4"/>
+    <hyperlink ref="J55" r:id="rId5"/>
+    <hyperlink ref="M55" r:id="rId6"/>
+    <hyperlink ref="N55" r:id="rId7"/>
+    <hyperlink ref="O55" r:id="rId8"/>
+    <hyperlink ref="K55" r:id="rId9"/>
+    <hyperlink ref="P55" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId11"/>

</xml_diff>

<commit_message>
BRO introductie van meerdere GIThub repositories, en nieuwe tagged value "afkorting" op het model
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="351">
   <si>
     <t>Name</t>
   </si>
@@ -861,9 +861,6 @@
     <t>Gaat naar GIThub</t>
   </si>
   <si>
-    <t>/BROprogramma/[registration-object-abbreviation]</t>
-  </si>
-  <si>
     <t>Not relevant for this owner, or defined by the system.</t>
   </si>
   <si>
@@ -876,9 +873,6 @@
     <t>BRO-LOGICAL</t>
   </si>
   <si>
-    <t>[registration-object-abbreviation]-cat</t>
-  </si>
-  <si>
     <t>git</t>
   </si>
   <si>
@@ -924,9 +918,6 @@
     <t>giturl</t>
   </si>
   <si>
-    <t>https://broprogramma.github.io/[registration-object-abbreviation]/</t>
-  </si>
-  <si>
     <t>gitcomment</t>
   </si>
   <si>
@@ -1066,6 +1057,27 @@
   </si>
   <si>
     <t>Yes if SKOS RDF must be validated after it has been generated</t>
+  </si>
+  <si>
+    <t>gitcfg</t>
+  </si>
+  <si>
+    <t>Name of the GIT configuration used by Imvertor to gain access to the GIT repository. The name must have been configured in the server.</t>
+  </si>
+  <si>
+    <t>bro</t>
+  </si>
+  <si>
+    <t>URL of the Github IO (pages) location</t>
+  </si>
+  <si>
+    <t>https://broprogramma.github.io/[model-abbreviation]/</t>
+  </si>
+  <si>
+    <t>/BROprogramma/[model-abbreviation]</t>
+  </si>
+  <si>
+    <t>[model-abbreviation]-cat</t>
   </si>
 </sst>
 </file>
@@ -1631,13 +1643,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R133"/>
+  <dimension ref="A1:R134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A105" sqref="A105:XFD105"/>
+      <selection pane="bottomRight" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1683,29 +1695,29 @@
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="L1" s="21"/>
       <c r="M1" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="Q1" s="21"/>
       <c r="R1" s="3" t="s">
@@ -1716,29 +1728,29 @@
       <c r="F2" s="3"/>
       <c r="G2" s="22"/>
       <c r="H2" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>309</v>
       </c>
       <c r="L2" s="22"/>
       <c r="M2" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>310</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>313</v>
       </c>
       <c r="Q2" s="22"/>
       <c r="R2" s="5"/>
@@ -1977,20 +1989,20 @@
       <c r="G12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="Q12" s="23"/>
       <c r="R12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -2472,13 +2484,13 @@
     </row>
     <row r="28" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="32" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B28" s="32" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D28" s="32" t="b">
         <v>0</v>
@@ -2493,18 +2505,18 @@
       <c r="L28" s="29"/>
       <c r="Q28" s="29"/>
       <c r="R28" s="32" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="32" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B29" s="32" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D29" s="32" t="b">
         <v>0</v>
@@ -2513,13 +2525,13 @@
         <v>1</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G29" s="29"/>
       <c r="L29" s="29"/>
       <c r="Q29" s="29"/>
       <c r="R29" s="32" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="30" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2571,13 +2583,13 @@
     </row>
     <row r="31" spans="1:18" s="33" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A31" s="33" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D31" s="33" t="b">
         <v>0</v>
@@ -2587,13 +2599,13 @@
       </c>
       <c r="G31" s="29"/>
       <c r="I31" s="33" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="J31" s="39" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="K31" s="39" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="L31" s="29"/>
       <c r="Q31" s="29"/>
@@ -2663,13 +2675,13 @@
     </row>
     <row r="35" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="34" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B35" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D35" s="34" t="b">
         <v>0</v>
@@ -2788,22 +2800,22 @@
     </row>
     <row r="39" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="36" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C39" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="D39" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="36" t="s">
         <v>330</v>
-      </c>
-      <c r="D39" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" s="36" t="s">
-        <v>333</v>
       </c>
       <c r="G39" s="35"/>
       <c r="L39" s="35"/>
@@ -3017,29 +3029,29 @@
       <c r="F48" s="6"/>
       <c r="G48" s="26"/>
       <c r="H48" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I48" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J48" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K48" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L48" s="23"/>
       <c r="M48" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N48" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O48" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P48" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q48" s="23"/>
     </row>
@@ -3189,356 +3201,336 @@
       <c r="L54" s="23"/>
       <c r="Q54" s="23"/>
     </row>
-    <row r="55" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A55" s="7" t="s">
+    <row r="55" spans="1:18" s="28" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A55" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="D55" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="G55" s="24"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="24"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="24"/>
+      <c r="R55" s="15"/>
+    </row>
+    <row r="56" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B56" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="C56" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="D56" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="G56" s="23"/>
+      <c r="L56" s="23"/>
+      <c r="Q56" s="23"/>
+    </row>
+    <row r="57" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A57" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G55" s="23"/>
-      <c r="H55" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="I55" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="J55" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="K55" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="L55" s="23"/>
-      <c r="M55" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="N55" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="O55" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="P55" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q55" s="23"/>
-    </row>
-    <row r="56" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A56" s="7" t="s">
+      <c r="C57" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D57" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="G57" s="23"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="23"/>
+      <c r="M57" s="18"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
+      <c r="P57" s="18"/>
+      <c r="Q57" s="23"/>
+    </row>
+    <row r="58" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A58" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B58" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C58" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D56" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G56" s="23"/>
-      <c r="H56" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="I56" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="J56" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="K56" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="L56" s="23"/>
-      <c r="M56" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="N56" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="O56" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="P56" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="Q56" s="23"/>
-    </row>
-    <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="D57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G57" s="23"/>
-      <c r="L57" s="23"/>
-      <c r="Q57" s="23"/>
-    </row>
-    <row r="58" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A58" s="15" t="s">
+      <c r="D58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="G58" s="23"/>
+      <c r="L58" s="23"/>
+      <c r="Q58" s="23"/>
+    </row>
+    <row r="59" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A59" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B59" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C59" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="D58" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="15" t="s">
+      <c r="D59" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="G58" s="24"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="24"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
-      <c r="O58" s="15"/>
-      <c r="P58" s="15"/>
-      <c r="Q58" s="24"/>
-      <c r="R58" s="15" t="s">
+      <c r="G59" s="24"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="24"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15"/>
+      <c r="O59" s="15"/>
+      <c r="P59" s="15"/>
+      <c r="Q59" s="24"/>
+      <c r="R59" s="15" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="59" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A59" s="7" t="s">
+    <row r="60" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A60" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F59" s="7" t="s">
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="G59" s="23"/>
-      <c r="L59" s="23"/>
-      <c r="Q59" s="23"/>
-      <c r="R59" s="7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="G60" s="23"/>
       <c r="L60" s="23"/>
       <c r="Q60" s="23"/>
       <c r="R60" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G61" s="23"/>
+      <c r="L61" s="23"/>
+      <c r="Q61" s="23"/>
+      <c r="R61" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="61" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A61" s="31" t="s">
-        <v>322</v>
-      </c>
-      <c r="B61" s="31" t="s">
+    <row r="62" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A62" s="31" t="s">
+        <v>319</v>
+      </c>
+      <c r="B62" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="31" t="s">
-        <v>323</v>
-      </c>
-      <c r="D61" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G61" s="29"/>
-      <c r="H61" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="I61" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="J61" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="K61" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="L61" s="29"/>
-      <c r="M61" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="N61" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="O61" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="P61" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q61" s="29"/>
-    </row>
-    <row r="62" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="7" t="s">
+      <c r="C62" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="D62" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G62" s="29"/>
+      <c r="H62" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I62" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="J62" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K62" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L62" s="29"/>
+      <c r="M62" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="N62" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="O62" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P62" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q62" s="29"/>
+    </row>
+    <row r="63" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B63" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C63" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D62" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" s="7" t="s">
+      <c r="D63" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E63" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="G62" s="23"/>
-      <c r="L62" s="23"/>
-      <c r="Q62" s="23"/>
-      <c r="R62" s="7" t="s">
+      <c r="G63" s="23"/>
+      <c r="L63" s="23"/>
+      <c r="Q63" s="23"/>
+      <c r="R63" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="63" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G63" s="23"/>
-      <c r="H63" s="2" t="s">
+      <c r="D64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" s="23"/>
+      <c r="H64" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="I63" s="17" t="s">
+      <c r="I64" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="J63" s="17" t="s">
+      <c r="J64" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="K63" s="17" t="s">
+      <c r="K64" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="L63" s="23"/>
-      <c r="M63" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="N63" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="O63" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="P63" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q63" s="23"/>
-      <c r="R63" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A64" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D64" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G64" s="23"/>
       <c r="L64" s="23"/>
-      <c r="M64" s="17"/>
-      <c r="N64" s="17"/>
-      <c r="O64" s="17"/>
-      <c r="P64" s="17"/>
+      <c r="M64" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="N64" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="O64" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="P64" s="17" t="s">
+        <v>302</v>
+      </c>
       <c r="Q64" s="23"/>
       <c r="R64" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>189</v>
+        <v>10</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
       <c r="D65" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E65" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>214</v>
+        <v>279</v>
       </c>
       <c r="G65" s="23"/>
       <c r="L65" s="23"/>
@@ -3547,170 +3539,173 @@
       <c r="O65" s="17"/>
       <c r="P65" s="17"/>
       <c r="Q65" s="23"/>
-    </row>
-    <row r="66" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" s="27" t="s">
-        <v>314</v>
-      </c>
-      <c r="B66" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="D66" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="27" t="s">
-        <v>316</v>
+      <c r="R65" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A66" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D66" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="G66" s="23"/>
       <c r="L66" s="23"/>
+      <c r="M66" s="17"/>
+      <c r="N66" s="17"/>
+      <c r="O66" s="17"/>
+      <c r="P66" s="17"/>
       <c r="Q66" s="23"/>
-      <c r="R66" s="27" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="2" t="s">
+    </row>
+    <row r="67" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="B67" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="D67" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="27" t="s">
+        <v>313</v>
+      </c>
+      <c r="G67" s="23"/>
+      <c r="L67" s="23"/>
+      <c r="Q67" s="23"/>
+      <c r="R67" s="27" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D67" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G67" s="23"/>
-      <c r="H67" s="17" t="s">
+      <c r="D68" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" s="23"/>
+      <c r="H68" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="I68" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="J68" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="K68" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="L68" s="23"/>
+      <c r="M68" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I67" s="17" t="s">
+      <c r="N68" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J67" s="17" t="s">
+      <c r="O68" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K67" s="17" t="s">
+      <c r="P68" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L67" s="23"/>
-      <c r="M67" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="N67" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="O67" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="P67" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q67" s="23"/>
-    </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="2" t="s">
+      <c r="Q68" s="23"/>
+    </row>
+    <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G68" s="23"/>
-      <c r="L68" s="23"/>
-      <c r="M68" s="17"/>
-      <c r="N68" s="17"/>
-      <c r="O68" s="17"/>
-      <c r="P68" s="17"/>
-      <c r="Q68" s="23"/>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A69" t="s">
+      <c r="D69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G69" s="23"/>
+      <c r="L69" s="23"/>
+      <c r="M69" s="17"/>
+      <c r="N69" s="17"/>
+      <c r="O69" s="17"/>
+      <c r="P69" s="17"/>
+      <c r="Q69" s="23"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A70" t="s">
         <v>72</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>5</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>73</v>
       </c>
-      <c r="D69" t="b">
-        <v>1</v>
-      </c>
-      <c r="E69" t="b">
-        <v>0</v>
-      </c>
-      <c r="F69" t="s">
-        <v>4</v>
-      </c>
-      <c r="R69"/>
-    </row>
-    <row r="70" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D70" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G70" s="23"/>
-      <c r="L70" s="23"/>
-      <c r="M70" s="17"/>
-      <c r="N70" s="17"/>
-      <c r="O70" s="17"/>
-      <c r="P70" s="17"/>
-      <c r="Q70" s="23"/>
+      <c r="D70" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>4</v>
+      </c>
+      <c r="R70"/>
     </row>
     <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
-        <v>74</v>
+        <v>233</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>75</v>
+        <v>247</v>
       </c>
       <c r="D71" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G71" s="23"/>
       <c r="L71" s="23"/>
@@ -3720,454 +3715,447 @@
       <c r="P71" s="17"/>
       <c r="Q71" s="23"/>
     </row>
-    <row r="72" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" s="23"/>
+      <c r="L72" s="23"/>
+      <c r="M72" s="17"/>
+      <c r="N72" s="17"/>
+      <c r="O72" s="17"/>
+      <c r="P72" s="17"/>
+      <c r="Q72" s="23"/>
+    </row>
+    <row r="73" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D72" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G72" s="23"/>
-      <c r="H72" s="17" t="s">
+      <c r="D73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" s="23"/>
+      <c r="H73" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="I73" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="J73" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="K73" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="L73" s="23"/>
+      <c r="M73" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I72" s="17" t="s">
+      <c r="N73" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J72" s="17" t="s">
+      <c r="O73" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K72" s="17" t="s">
+      <c r="P73" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L72" s="23"/>
-      <c r="M72" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="N72" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="O72" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="P72" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q72" s="23"/>
-    </row>
-    <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
+      <c r="Q73" s="23"/>
+    </row>
+    <row r="74" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A74" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="G73" s="23"/>
-      <c r="L73" s="23"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
-      <c r="Q73" s="23"/>
-    </row>
-    <row r="74" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D74" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E74" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>273</v>
+      <c r="D74" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>350</v>
       </c>
       <c r="G74" s="23"/>
       <c r="L74" s="23"/>
+      <c r="M74" s="17"/>
+      <c r="N74" s="17"/>
+      <c r="O74" s="17"/>
+      <c r="P74" s="17"/>
       <c r="Q74" s="23"/>
-      <c r="R74" s="7" t="s">
+    </row>
+    <row r="75" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D75" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E75" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G75" s="23"/>
+      <c r="L75" s="23"/>
+      <c r="Q75" s="23"/>
+      <c r="R75" s="7" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="75" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A75" s="2" t="s">
+    <row r="76" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D75" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="G75" s="23"/>
-      <c r="H75" s="2" t="s">
+      <c r="D76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G76" s="23"/>
+      <c r="H76" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L75" s="23"/>
-      <c r="M75" s="17" t="s">
+      <c r="L76" s="23"/>
+      <c r="M76" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N75" s="17" t="s">
+      <c r="N76" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O75" s="17" t="s">
+      <c r="O76" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P75" s="17" t="s">
+      <c r="P76" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q75" s="23"/>
-    </row>
-    <row r="76" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A76" s="7" t="s">
+      <c r="Q76" s="23"/>
+    </row>
+    <row r="77" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A77" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B77" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C77" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D76" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" s="7" t="s">
+      <c r="D77" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="G76" s="23"/>
-      <c r="L76" s="23"/>
-      <c r="Q76" s="23"/>
-      <c r="R76" s="8" t="s">
+      <c r="G77" s="23"/>
+      <c r="L77" s="23"/>
+      <c r="Q77" s="23"/>
+      <c r="R77" s="8" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D77" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G77" s="23"/>
-      <c r="H77" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="I77" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="J77" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="K77" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="L77" s="23"/>
-      <c r="M77" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="N77" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="O77" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="P77" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q77" s="23"/>
     </row>
     <row r="78" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D78" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G78" s="23"/>
+      <c r="H78" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="I78" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="J78" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="K78" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="L78" s="23"/>
+      <c r="M78" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="N78" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="O78" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="P78" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q78" s="23"/>
+    </row>
+    <row r="79" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D78" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" s="2" t="s">
+      <c r="D79" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F79" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G78" s="23"/>
-      <c r="L78" s="23"/>
-      <c r="M78" s="17"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="17"/>
-      <c r="P78" s="17"/>
-      <c r="Q78" s="23"/>
-    </row>
-    <row r="79" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A79" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D79" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="G79" s="23"/>
       <c r="L79" s="23"/>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="17"/>
       <c r="Q79" s="23"/>
-      <c r="R79" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="80" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A80" s="7" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="D80" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E80" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="G80" s="23"/>
       <c r="L80" s="23"/>
       <c r="Q80" s="23"/>
-      <c r="R80" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>94</v>
+      <c r="R80" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A81" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D81" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G81" s="23"/>
       <c r="L81" s="23"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
       <c r="Q81" s="23"/>
-    </row>
-    <row r="82" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A82" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="D82" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="17" t="s">
-        <v>4</v>
+      <c r="R81" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G82" s="23"/>
       <c r="L82" s="23"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="17"/>
       <c r="Q82" s="23"/>
     </row>
-    <row r="83" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="7" t="s">
+    <row r="83" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A83" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="B83" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="D83" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G83" s="23"/>
+      <c r="L83" s="23"/>
+      <c r="Q83" s="23"/>
+    </row>
+    <row r="84" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="B83" s="19"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E83" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G83" s="23"/>
-      <c r="H83" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I83" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J83" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K83" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L83" s="23"/>
-      <c r="M83" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N83" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O83" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P83" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q83" s="23"/>
-    </row>
-    <row r="84" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A84" s="20" t="s">
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G84" s="23"/>
+      <c r="H84" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J84" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K84" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L84" s="23"/>
+      <c r="M84" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N84" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O84" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P84" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q84" s="23"/>
+    </row>
+    <row r="85" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A85" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B84" s="20" t="s">
+      <c r="B85" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C84" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="D84" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G84" s="23"/>
-      <c r="L84" s="23"/>
-      <c r="Q84" s="23"/>
-    </row>
-    <row r="85" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A85" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D85" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>4</v>
+      <c r="C85" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="D85" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G85" s="23"/>
       <c r="L85" s="23"/>
-      <c r="M85" s="17"/>
-      <c r="N85" s="17"/>
-      <c r="O85" s="17"/>
-      <c r="P85" s="17"/>
       <c r="Q85" s="23"/>
-      <c r="R85" s="8" t="s">
-        <v>218</v>
-      </c>
     </row>
     <row r="86" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D86" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>332</v>
+        <v>4</v>
       </c>
       <c r="G86" s="23"/>
-      <c r="H86" s="17"/>
-      <c r="I86" s="17"/>
-      <c r="J86" s="17"/>
-      <c r="K86" s="17"/>
       <c r="L86" s="23"/>
       <c r="M86" s="17"/>
       <c r="N86" s="17"/>
@@ -4175,238 +4163,248 @@
       <c r="P86" s="17"/>
       <c r="Q86" s="23"/>
       <c r="R86" s="8" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A87" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="G87" s="23"/>
+      <c r="H87" s="17"/>
+      <c r="I87" s="17"/>
+      <c r="J87" s="17"/>
+      <c r="K87" s="17"/>
+      <c r="L87" s="23"/>
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
+      <c r="O87" s="17"/>
+      <c r="P87" s="17"/>
+      <c r="Q87" s="23"/>
+      <c r="R87" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
         <v>198</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>199</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>200</v>
       </c>
-      <c r="D87" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" t="b">
-        <v>1</v>
-      </c>
-      <c r="M87" s="28" t="s">
-        <v>321</v>
-      </c>
-      <c r="N87" s="28" t="s">
-        <v>321</v>
-      </c>
-      <c r="O87" s="28" t="s">
-        <v>321</v>
-      </c>
-      <c r="P87" s="28" t="s">
-        <v>321</v>
-      </c>
-      <c r="R87"/>
-    </row>
-    <row r="88" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A88" s="13" t="s">
+      <c r="D88" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+      <c r="M88" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="N88" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="O88" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="P88" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="R88"/>
+    </row>
+    <row r="89" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A89" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="B88" s="13" t="s">
+      <c r="B89" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C89" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="D88" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" s="6" t="s">
+      <c r="D89" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="G88" s="26"/>
-      <c r="L88" s="23"/>
-      <c r="M88" s="17"/>
-      <c r="N88" s="17"/>
-      <c r="O88" s="17"/>
-      <c r="P88" s="17"/>
-      <c r="Q88" s="23"/>
-    </row>
-    <row r="89" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="28" t="s">
+      <c r="G89" s="26"/>
+      <c r="L89" s="23"/>
+      <c r="M89" s="17"/>
+      <c r="N89" s="17"/>
+      <c r="O89" s="17"/>
+      <c r="P89" s="17"/>
+      <c r="Q89" s="23"/>
+    </row>
+    <row r="90" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="B89" s="28" t="s">
+      <c r="B90" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="28" t="s">
-        <v>344</v>
-      </c>
-      <c r="D89" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="28" t="s">
+      <c r="C90" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="D90" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="28" t="s">
         <v>273</v>
-      </c>
-      <c r="G89" s="23"/>
-      <c r="L89" s="23"/>
-      <c r="Q89" s="23"/>
-      <c r="R89" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D90" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G90" s="23"/>
       <c r="L90" s="23"/>
-      <c r="M90" s="17"/>
-      <c r="N90" s="17"/>
-      <c r="O90" s="17"/>
-      <c r="P90" s="17"/>
       <c r="Q90" s="23"/>
-    </row>
-    <row r="91" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="28" t="s">
-        <v>341</v>
-      </c>
-      <c r="B91" s="28" t="s">
+      <c r="R90" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D91" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G91" s="23"/>
+      <c r="L91" s="23"/>
+      <c r="M91" s="17"/>
+      <c r="N91" s="17"/>
+      <c r="O91" s="17"/>
+      <c r="P91" s="17"/>
+      <c r="Q91" s="23"/>
+    </row>
+    <row r="92" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="28" t="s">
+        <v>338</v>
+      </c>
+      <c r="B92" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="28" t="s">
-        <v>343</v>
-      </c>
-      <c r="D91" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="28" t="s">
+      <c r="C92" s="28" t="s">
+        <v>340</v>
+      </c>
+      <c r="D92" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E92" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="G91" s="29"/>
-      <c r="L91" s="29"/>
-      <c r="Q91" s="29"/>
-      <c r="R91" s="7" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A92" s="2" t="s">
+      <c r="G92" s="29"/>
+      <c r="L92" s="29"/>
+      <c r="Q92" s="29"/>
+      <c r="R92" s="7" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A93" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D92" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G92" s="26"/>
-      <c r="L92" s="23"/>
-      <c r="M92" s="17"/>
-      <c r="N92" s="17"/>
-      <c r="O92" s="17"/>
-      <c r="P92" s="17"/>
-      <c r="Q92" s="23"/>
-      <c r="R92" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A93" s="17" t="s">
-        <v>296</v>
-      </c>
-      <c r="B93" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="D93" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="6"/>
+      <c r="D93" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="G93" s="26"/>
       <c r="L93" s="23"/>
+      <c r="M93" s="17"/>
+      <c r="N93" s="17"/>
+      <c r="O93" s="17"/>
+      <c r="P93" s="17"/>
       <c r="Q93" s="23"/>
-    </row>
-    <row r="94" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A94" s="2" t="s">
+      <c r="R93" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A94" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="B94" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="D94" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="6"/>
+      <c r="G94" s="26"/>
+      <c r="L94" s="23"/>
+      <c r="Q94" s="23"/>
+    </row>
+    <row r="95" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D94" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G94" s="23"/>
-      <c r="L94" s="23"/>
-      <c r="M94" s="17"/>
-      <c r="N94" s="17"/>
-      <c r="O94" s="17"/>
-      <c r="P94" s="17"/>
-      <c r="Q94" s="23"/>
-    </row>
-    <row r="95" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="D95" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E95" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G95" s="23"/>
       <c r="L95" s="23"/>
@@ -4415,28 +4413,22 @@
       <c r="O95" s="17"/>
       <c r="P95" s="17"/>
       <c r="Q95" s="23"/>
-      <c r="R95" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="96" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>104</v>
+        <v>201</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>107</v>
+        <v>202</v>
       </c>
       <c r="D96" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="G96" s="23"/>
       <c r="L96" s="23"/>
@@ -4446,91 +4438,95 @@
       <c r="P96" s="17"/>
       <c r="Q96" s="23"/>
       <c r="R96" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A97" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D97" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G97" s="23"/>
+      <c r="L97" s="23"/>
+      <c r="M97" s="17"/>
+      <c r="N97" s="17"/>
+      <c r="O97" s="17"/>
+      <c r="P97" s="17"/>
+      <c r="Q97" s="23"/>
+      <c r="R97" s="8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="97" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A97" s="2" t="s">
+    <row r="98" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D97" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G97" s="23"/>
-      <c r="H97" s="17" t="s">
+      <c r="D98" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G98" s="23"/>
+      <c r="H98" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="I98" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="J98" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="K98" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="L98" s="23"/>
+      <c r="M98" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="I97" s="17" t="s">
+      <c r="N98" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="J97" s="17" t="s">
+      <c r="O98" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K97" s="17" t="s">
+      <c r="P98" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L97" s="23"/>
-      <c r="M97" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="N97" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="O97" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="P97" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q97" s="23"/>
-      <c r="R97" s="2" t="s">
+      <c r="Q98" s="23"/>
+      <c r="R98" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A98" s="7" t="s">
+    <row r="99" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A99" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B99" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C99" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="D98" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F98" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="G98" s="23"/>
-      <c r="L98" s="23"/>
-      <c r="Q98" s="23"/>
-      <c r="R98" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="D99" s="7" t="b">
         <v>1</v>
@@ -4545,91 +4541,73 @@
       <c r="L99" s="23"/>
       <c r="Q99" s="23"/>
       <c r="R99" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="100" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D100" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E100" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>14</v>
+        <v>234</v>
       </c>
       <c r="G100" s="23"/>
       <c r="L100" s="23"/>
       <c r="Q100" s="23"/>
       <c r="R100" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D101" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G101" s="23"/>
+      <c r="L101" s="23"/>
+      <c r="Q101" s="23"/>
+      <c r="R101" s="7" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="101" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D101" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G101" s="23"/>
-      <c r="H101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L101" s="23"/>
-      <c r="M101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q101" s="23"/>
     </row>
     <row r="102" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>288</v>
+        <v>117</v>
       </c>
       <c r="D102" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" s="2" t="b">
         <v>1</v>
@@ -4664,23 +4642,23 @@
     </row>
     <row r="103" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>120</v>
+        <v>286</v>
       </c>
       <c r="D103" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G103" s="23"/>
       <c r="H103" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>4</v>
@@ -4693,7 +4671,7 @@
       </c>
       <c r="L103" s="23"/>
       <c r="M103" s="17" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N103" s="17" t="s">
         <v>4</v>
@@ -4706,63 +4684,59 @@
       </c>
       <c r="Q103" s="23"/>
     </row>
-    <row r="104" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="B104" s="28" t="s">
+    <row r="104" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C104" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="D104" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E104" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F104" s="28"/>
+      <c r="C104" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D104" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="G104" s="23"/>
-      <c r="H104" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I104" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J104" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K104" s="28" t="s">
+      <c r="H104" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K104" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L104" s="23"/>
-      <c r="M104" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N104" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O104" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P104" s="28" t="s">
+      <c r="M104" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N104" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O104" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P104" s="17" t="s">
         <v>4</v>
       </c>
       <c r="Q104" s="23"/>
-      <c r="R104" s="28" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="105" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="28" t="s">
-        <v>345</v>
+        <v>149</v>
       </c>
       <c r="B105" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C105" s="28" t="s">
-        <v>346</v>
+        <v>150</v>
       </c>
       <c r="D105" s="28" t="b">
         <v>0</v>
@@ -4771,7 +4745,7 @@
         <v>1</v>
       </c>
       <c r="F105" s="28"/>
-      <c r="G105" s="29"/>
+      <c r="G105" s="23"/>
       <c r="H105" s="28" t="s">
         <v>14</v>
       </c>
@@ -4784,7 +4758,7 @@
       <c r="K105" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="L105" s="29"/>
+      <c r="L105" s="23"/>
       <c r="M105" s="28" t="s">
         <v>14</v>
       </c>
@@ -4797,87 +4771,90 @@
       <c r="P105" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="Q105" s="29"/>
+      <c r="Q105" s="23"/>
       <c r="R105" s="28" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="28" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A106" t="s">
+      <c r="B106" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="28" t="s">
+        <v>343</v>
+      </c>
+      <c r="D106" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" s="28"/>
+      <c r="G106" s="29"/>
+      <c r="H106" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I106" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J106" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K106" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L106" s="29"/>
+      <c r="M106" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N106" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O106" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P106" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q106" s="29"/>
+      <c r="R106" s="28" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A107" t="s">
         <v>121</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B107" t="s">
         <v>122</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C107" t="s">
         <v>123</v>
       </c>
-      <c r="D106" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" t="b">
-        <v>0</v>
-      </c>
-      <c r="H106" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="I106" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J106" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K106" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L106" s="23"/>
-      <c r="M106" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="N106" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O106" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P106" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q106" s="23"/>
-      <c r="R106"/>
-    </row>
-    <row r="107" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G107" s="23"/>
-      <c r="H107" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K107" s="2" t="s">
+      <c r="D107" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" t="b">
+        <v>0</v>
+      </c>
+      <c r="H107" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="I107" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J107" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K107" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L107" s="23"/>
       <c r="M107" s="17" t="s">
-        <v>14</v>
+        <v>288</v>
       </c>
       <c r="N107" s="17" t="s">
         <v>4</v>
@@ -4889,19 +4866,17 @@
         <v>4</v>
       </c>
       <c r="Q107" s="23"/>
-      <c r="R107" s="2" t="s">
-        <v>203</v>
-      </c>
+      <c r="R107"/>
     </row>
     <row r="108" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D108" s="2" t="b">
         <v>1</v>
@@ -4936,103 +4911,147 @@
         <v>4</v>
       </c>
       <c r="Q108" s="23"/>
+      <c r="R108" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="109" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
-        <v>127</v>
+        <v>259</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D109" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E109" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G109" s="23"/>
-      <c r="H109" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I109" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J109" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K109" s="17" t="s">
-        <v>273</v>
+      <c r="H109" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K109" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L109" s="23"/>
       <c r="M109" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q109" s="23"/>
+    </row>
+    <row r="110" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G110" s="23"/>
+      <c r="H110" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="N109" s="17" t="s">
+      <c r="I110" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="O109" s="17" t="s">
+      <c r="J110" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="P109" s="17" t="s">
+      <c r="K110" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="Q109" s="23"/>
-    </row>
-    <row r="110" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A110" s="30" t="s">
-        <v>318</v>
-      </c>
-      <c r="B110" s="30" t="s">
+      <c r="L110" s="23"/>
+      <c r="M110" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N110" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O110" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="P110" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q110" s="23"/>
+    </row>
+    <row r="111" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A111" s="30" t="s">
+        <v>315</v>
+      </c>
+      <c r="B111" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C110" s="30" t="s">
-        <v>319</v>
-      </c>
-      <c r="D110" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" s="30" t="s">
-        <v>320</v>
-      </c>
-      <c r="G110" s="29"/>
-      <c r="L110" s="29"/>
-      <c r="Q110" s="29"/>
-    </row>
-    <row r="111" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A111" s="2" t="s">
+      <c r="C111" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="D111" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="30" t="s">
+        <v>317</v>
+      </c>
+      <c r="G111" s="29"/>
+      <c r="L111" s="29"/>
+      <c r="Q111" s="29"/>
+    </row>
+    <row r="112" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A112" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D111" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F111" s="2" t="s">
+      <c r="D112" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F112" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G111" s="23"/>
-      <c r="L111" s="23"/>
-      <c r="M111" s="17"/>
-      <c r="N111" s="17"/>
-      <c r="O111" s="17"/>
-      <c r="P111" s="17"/>
-      <c r="Q111" s="23"/>
-    </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R112"/>
+      <c r="G112" s="23"/>
+      <c r="L112" s="23"/>
+      <c r="M112" s="17"/>
+      <c r="N112" s="17"/>
+      <c r="O112" s="17"/>
+      <c r="P112" s="17"/>
+      <c r="Q112" s="23"/>
     </row>
     <row r="113" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R113"/>
@@ -5096,6 +5115,9 @@
     </row>
     <row r="133" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R133"/>
+    </row>
+    <row r="134" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R134"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5111,17 +5133,10 @@
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1"/>
     <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="H55" r:id="rId3"/>
-    <hyperlink ref="I55" r:id="rId4"/>
-    <hyperlink ref="J55" r:id="rId5"/>
-    <hyperlink ref="M55" r:id="rId6"/>
-    <hyperlink ref="N55" r:id="rId7"/>
-    <hyperlink ref="O55" r:id="rId8"/>
-    <hyperlink ref="K55" r:id="rId9"/>
-    <hyperlink ref="P55" r:id="rId10"/>
+    <hyperlink ref="F57" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId11"/>
+  <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -5149,7 +5164,7 @@
         <v>256</v>
       </c>
       <c r="B3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
BRO: aanpassingen Concept register JSON
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="356">
   <si>
     <t>Name</t>
   </si>
@@ -1078,6 +1078,21 @@
   </si>
   <si>
     <t>[model-abbreviation]-cat</t>
+  </si>
+  <si>
+    <t>createjsonconcepts</t>
+  </si>
+  <si>
+    <t>Yes if JSON concepts must be generated</t>
+  </si>
+  <si>
+    <t>jsonconceptsname</t>
+  </si>
+  <si>
+    <t>The name of the JSON concepts file generated</t>
+  </si>
+  <si>
+    <t>[model-abbreviation]-concepts</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1258,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1343,6 +1358,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1643,13 +1664,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R134"/>
+  <dimension ref="A1:R136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F72" sqref="F72"/>
+      <selection pane="bottomRight" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1860,16 +1881,16 @@
       <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="41" t="b">
+      <c r="D7" s="43" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1887,10 +1908,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
       <c r="G8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
@@ -2482,41 +2503,59 @@
       </c>
       <c r="Q27" s="23"/>
     </row>
-    <row r="28" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="32" t="s">
-        <v>321</v>
-      </c>
-      <c r="B28" s="32" t="s">
+    <row r="28" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="41" t="s">
+        <v>351</v>
+      </c>
+      <c r="B28" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="32" t="s">
-        <v>322</v>
-      </c>
-      <c r="D28" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>14</v>
+      <c r="C28" s="41" t="s">
+        <v>352</v>
+      </c>
+      <c r="D28" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="41" t="b">
+        <v>1</v>
       </c>
       <c r="G28" s="29"/>
+      <c r="H28" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="41" t="s">
+        <v>4</v>
+      </c>
       <c r="L28" s="29"/>
+      <c r="M28" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="O28" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="P28" s="41" t="s">
+        <v>14</v>
+      </c>
       <c r="Q28" s="29"/>
-      <c r="R28" s="32" t="s">
-        <v>325</v>
-      </c>
     </row>
     <row r="29" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="32" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D29" s="32" t="b">
         <v>0</v>
@@ -2525,7 +2564,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>331</v>
+        <v>14</v>
       </c>
       <c r="G29" s="29"/>
       <c r="L29" s="29"/>
@@ -2534,111 +2573,117 @@
         <v>325</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>324</v>
+      </c>
+      <c r="D30" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="G30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="32" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" s="23"/>
-      <c r="H30" s="2" t="s">
+      <c r="D31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="23"/>
+      <c r="H31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="40" t="s">
+      <c r="I31" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="40" t="s">
+      <c r="J31" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="K30" s="40" t="s">
+      <c r="K31" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="L30" s="23"/>
-      <c r="M30" s="17" t="s">
+      <c r="L31" s="23"/>
+      <c r="M31" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N30" s="40" t="s">
+      <c r="N31" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="O30" s="40" t="s">
+      <c r="O31" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="P30" s="40" t="s">
+      <c r="P31" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="23"/>
-      <c r="R30" s="2" t="s">
+      <c r="Q31" s="23"/>
+      <c r="R31" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="31" spans="1:18" s="33" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A31" s="33" t="s">
+    <row r="32" spans="1:18" s="33" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A32" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B32" s="33" t="s">
         <v>333</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C32" s="33" t="s">
         <v>334</v>
       </c>
-      <c r="D31" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" s="29"/>
-      <c r="I31" s="33" t="s">
+      <c r="D32" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="29"/>
+      <c r="I32" s="33" t="s">
         <v>335</v>
       </c>
-      <c r="J31" s="39" t="s">
+      <c r="J32" s="39" t="s">
         <v>335</v>
       </c>
-      <c r="K31" s="39" t="s">
+      <c r="K32" s="39" t="s">
         <v>335</v>
       </c>
-      <c r="L31" s="29"/>
-      <c r="Q31" s="29"/>
-    </row>
-    <row r="32" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A32" s="34" t="s">
+      <c r="L32" s="29"/>
+      <c r="Q32" s="29"/>
+    </row>
+    <row r="33" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A33" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B33" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C33" s="34" t="s">
         <v>167</v>
-      </c>
-      <c r="D32" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="Q32" s="35"/>
-    </row>
-    <row r="33" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="B33" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="C33" s="34" t="s">
-        <v>170</v>
       </c>
       <c r="D33" s="34" t="b">
         <v>0</v>
@@ -2652,22 +2697,19 @@
     </row>
     <row r="34" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="34" t="s">
-        <v>35</v>
+        <v>168</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>5</v>
+        <v>169</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="D34" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E34" s="34" t="b">
         <v>1</v>
-      </c>
-      <c r="F34" s="34" t="s">
-        <v>14</v>
       </c>
       <c r="G34" s="35"/>
       <c r="L34" s="35"/>
@@ -2675,13 +2717,13 @@
     </row>
     <row r="35" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="34" t="s">
-        <v>336</v>
+        <v>35</v>
       </c>
       <c r="B35" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>337</v>
+        <v>36</v>
       </c>
       <c r="D35" s="34" t="b">
         <v>0</v>
@@ -2693,241 +2735,251 @@
         <v>14</v>
       </c>
       <c r="G35" s="35"/>
-      <c r="H35" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="J35" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="K35" s="34" t="s">
-        <v>4</v>
-      </c>
       <c r="L35" s="35"/>
       <c r="Q35" s="35"/>
     </row>
-    <row r="36" spans="1:18" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A36" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="36" t="s">
+    <row r="36" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="B36" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="36" t="s">
+      <c r="C36" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="D36" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G36" s="35"/>
+      <c r="H36" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="K36" s="34" t="s">
+        <v>4</v>
+      </c>
       <c r="L36" s="35"/>
       <c r="Q36" s="35"/>
     </row>
-    <row r="37" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A37" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="34" t="s">
+    <row r="37" spans="1:18" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A37" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="F37" s="34" t="s">
+      <c r="C37" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="36" t="s">
         <v>14</v>
       </c>
       <c r="G37" s="35"/>
       <c r="L37" s="35"/>
       <c r="Q37" s="35"/>
     </row>
-    <row r="38" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="36" t="s">
+    <row r="38" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A38" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="36" t="b">
-        <v>1</v>
+      <c r="C38" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" s="34" t="s">
+        <v>14</v>
       </c>
       <c r="G38" s="35"/>
-      <c r="H38" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="K38" s="36" t="s">
-        <v>14</v>
-      </c>
       <c r="L38" s="35"/>
-      <c r="M38" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="N38" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="O38" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="P38" s="36" t="s">
-        <v>4</v>
-      </c>
       <c r="Q38" s="35"/>
     </row>
     <row r="39" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="35"/>
+      <c r="H39" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L39" s="35"/>
+      <c r="M39" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="N39" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="O39" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="P39" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q39" s="35"/>
+    </row>
+    <row r="40" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="36" t="s">
         <v>326</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B40" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C40" s="36" t="s">
         <v>327</v>
       </c>
-      <c r="D39" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" s="36" t="s">
+      <c r="D40" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" s="36" t="s">
         <v>330</v>
-      </c>
-      <c r="G39" s="35"/>
-      <c r="L39" s="35"/>
-      <c r="Q39" s="35"/>
-    </row>
-    <row r="40" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="B40" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="D40" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="34" t="s">
-        <v>14</v>
       </c>
       <c r="G40" s="35"/>
       <c r="L40" s="35"/>
       <c r="Q40" s="35"/>
     </row>
-    <row r="41" spans="1:18" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A41" s="37" t="s">
+    <row r="41" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D41" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="35"/>
+      <c r="L41" s="35"/>
+      <c r="Q41" s="35"/>
+    </row>
+    <row r="42" spans="1:18" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A42" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B42" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="C42" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="F41" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="38"/>
-      <c r="L41" s="38"/>
-      <c r="Q41" s="38"/>
-      <c r="R41" s="37" t="s">
+      <c r="D42" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="38"/>
+      <c r="L42" s="38"/>
+      <c r="Q42" s="38"/>
+      <c r="R42" s="37" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="42" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A42" s="7" t="s">
+    <row r="43" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A43" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B43" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C43" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D42" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42" s="7" t="s">
+      <c r="D43" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E43" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="G42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="Q42" s="23"/>
-      <c r="R42" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="41" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G43" s="23"/>
       <c r="L43" s="23"/>
-      <c r="M43" s="17"/>
-      <c r="N43" s="17"/>
-      <c r="O43" s="17"/>
-      <c r="P43" s="17"/>
       <c r="Q43" s="23"/>
+      <c r="R43" s="7" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
+      <c r="A44" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G44" s="23"/>
       <c r="L44" s="23"/>
       <c r="M44" s="17"/>
@@ -2936,22 +2988,11 @@
       <c r="P44" s="17"/>
       <c r="Q44" s="23"/>
     </row>
-    <row r="45" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A45" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D45" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
       <c r="G45" s="23"/>
       <c r="L45" s="23"/>
       <c r="M45" s="17"/>
@@ -2960,21 +3001,21 @@
       <c r="P45" s="17"/>
       <c r="Q45" s="23"/>
     </row>
-    <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
-        <v>50</v>
+        <v>173</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>51</v>
+        <v>175</v>
       </c>
       <c r="D46" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="23"/>
       <c r="L46" s="23"/>
@@ -2984,15 +3025,15 @@
       <c r="P46" s="17"/>
       <c r="Q46" s="23"/>
     </row>
-    <row r="47" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D47" s="2" t="b">
         <v>0</v>
@@ -3000,95 +3041,95 @@
       <c r="E47" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F47" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="G47" s="26"/>
+      <c r="G47" s="23"/>
       <c r="L47" s="23"/>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
       <c r="O47" s="17"/>
       <c r="P47" s="17"/>
       <c r="Q47" s="23"/>
-      <c r="R47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A48" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G48" s="26"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="23"/>
+      <c r="R48" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F48" s="6"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="17" t="s">
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="I48" s="17" t="s">
+      <c r="I49" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="J48" s="17" t="s">
+      <c r="J49" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="K48" s="17" t="s">
+      <c r="K49" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="L48" s="23"/>
-      <c r="M48" s="17" t="s">
+      <c r="L49" s="23"/>
+      <c r="M49" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="N48" s="17" t="s">
+      <c r="N49" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="O48" s="17" t="s">
+      <c r="O49" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="P48" s="17" t="s">
+      <c r="P49" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="Q48" s="23"/>
-    </row>
-    <row r="49" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="7" t="s">
+      <c r="Q49" s="23"/>
+    </row>
+    <row r="50" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B50" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C50" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D49" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G49" s="23"/>
-      <c r="L49" s="23"/>
-      <c r="Q49" s="23"/>
-      <c r="R49"/>
-    </row>
-    <row r="50" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A50" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="D50" s="7" t="b">
         <v>0</v>
       </c>
@@ -3096,77 +3137,78 @@
         <v>1</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>225</v>
+        <v>4</v>
       </c>
       <c r="G50" s="23"/>
       <c r="L50" s="23"/>
       <c r="Q50" s="23"/>
-    </row>
-    <row r="51" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D51" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>14</v>
+      <c r="R50"/>
+    </row>
+    <row r="51" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A51" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D51" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="G51" s="23"/>
       <c r="L51" s="23"/>
-      <c r="M51" s="17"/>
-      <c r="N51" s="17"/>
-      <c r="O51" s="17"/>
-      <c r="P51" s="17"/>
       <c r="Q51" s="23"/>
     </row>
-    <row r="52" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B52" s="7" t="s">
+    <row r="52" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D52" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="7" t="s">
+      <c r="C52" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G52" s="23"/>
       <c r="L52" s="23"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="17"/>
       <c r="Q52" s="23"/>
     </row>
-    <row r="53" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D53" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E53" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>14</v>
@@ -3174,25 +3216,22 @@
       <c r="G53" s="23"/>
       <c r="L53" s="23"/>
       <c r="Q53" s="23"/>
-      <c r="R53" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="54" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A54" s="7" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>182</v>
+        <v>60</v>
       </c>
       <c r="D54" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E54" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>14</v>
@@ -3200,506 +3239,507 @@
       <c r="G54" s="23"/>
       <c r="L54" s="23"/>
       <c r="Q54" s="23"/>
-    </row>
-    <row r="55" spans="1:18" s="28" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A55" s="15" t="s">
+      <c r="R54" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G55" s="23"/>
+      <c r="L55" s="23"/>
+      <c r="Q55" s="23"/>
+    </row>
+    <row r="56" spans="1:18" s="28" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A56" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B56" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C56" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="D55" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="15" t="s">
+      <c r="D56" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="G55" s="24"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="24"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
-      <c r="Q55" s="24"/>
-      <c r="R55" s="15"/>
-    </row>
-    <row r="56" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="7" t="s">
+      <c r="G56" s="24"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="24"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="15"/>
+      <c r="O56" s="15"/>
+      <c r="P56" s="15"/>
+      <c r="Q56" s="24"/>
+      <c r="R56" s="15"/>
+    </row>
+    <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B57" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C57" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="D56" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="7" t="s">
+      <c r="D57" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="G56" s="23"/>
-      <c r="L56" s="23"/>
-      <c r="Q56" s="23"/>
-    </row>
-    <row r="57" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A57" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="18" t="s">
-        <v>348</v>
-      </c>
       <c r="G57" s="23"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
       <c r="L57" s="23"/>
-      <c r="M57" s="18"/>
-      <c r="N57" s="18"/>
-      <c r="O57" s="18"/>
-      <c r="P57" s="18"/>
       <c r="Q57" s="23"/>
     </row>
     <row r="58" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="G58" s="23"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="23"/>
+      <c r="M58" s="18"/>
+      <c r="N58" s="18"/>
+      <c r="O58" s="18"/>
+      <c r="P58" s="18"/>
+      <c r="Q58" s="23"/>
+    </row>
+    <row r="59" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A59" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="7" t="s">
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="G58" s="23"/>
-      <c r="L58" s="23"/>
-      <c r="Q58" s="23"/>
-    </row>
-    <row r="59" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A59" s="15" t="s">
+      <c r="G59" s="23"/>
+      <c r="L59" s="23"/>
+      <c r="Q59" s="23"/>
+    </row>
+    <row r="60" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A60" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B60" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C60" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="D59" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="15" t="s">
+      <c r="D60" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="G59" s="24"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="15"/>
-      <c r="L59" s="24"/>
-      <c r="M59" s="15"/>
-      <c r="N59" s="15"/>
-      <c r="O59" s="15"/>
-      <c r="P59" s="15"/>
-      <c r="Q59" s="24"/>
-      <c r="R59" s="15" t="s">
+      <c r="G60" s="24"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="24"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="15"/>
+      <c r="Q60" s="24"/>
+      <c r="R60" s="15" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A60" s="7" t="s">
+    <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B61" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C61" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F60" s="7" t="s">
+      <c r="D61" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F61" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="G60" s="23"/>
-      <c r="L60" s="23"/>
-      <c r="Q60" s="23"/>
-      <c r="R60" s="7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="G61" s="23"/>
       <c r="L61" s="23"/>
       <c r="Q61" s="23"/>
       <c r="R61" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G62" s="23"/>
+      <c r="L62" s="23"/>
+      <c r="Q62" s="23"/>
+      <c r="R62" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="62" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A62" s="31" t="s">
+    <row r="63" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A63" s="31" t="s">
         <v>319</v>
       </c>
-      <c r="B62" s="31" t="s">
+      <c r="B63" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="31" t="s">
+      <c r="C63" s="31" t="s">
         <v>320</v>
       </c>
-      <c r="D62" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G62" s="29"/>
-      <c r="H62" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="I62" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="J62" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="K62" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="L62" s="29"/>
-      <c r="M62" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="N62" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="O62" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="P62" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q62" s="29"/>
-    </row>
-    <row r="63" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" s="7" t="s">
+      <c r="D63" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G63" s="29"/>
+      <c r="H63" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I63" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="J63" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K63" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L63" s="29"/>
+      <c r="M63" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="N63" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="O63" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P63" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q63" s="29"/>
+    </row>
+    <row r="64" spans="1:18" s="42" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="42" t="s">
+        <v>353</v>
+      </c>
+      <c r="B64" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="42" t="s">
+        <v>354</v>
+      </c>
+      <c r="D64" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="42" t="s">
+        <v>355</v>
+      </c>
+      <c r="G64" s="29"/>
+      <c r="L64" s="29"/>
+      <c r="Q64" s="29"/>
+    </row>
+    <row r="65" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A65" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B65" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C65" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D63" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E63" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" s="7" t="s">
+      <c r="D65" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="G63" s="23"/>
-      <c r="L63" s="23"/>
-      <c r="Q63" s="23"/>
-      <c r="R63" s="7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A64" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D64" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G64" s="23"/>
-      <c r="H64" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="I64" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="J64" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="K64" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="L64" s="23"/>
-      <c r="M64" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="N64" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="O64" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="P64" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q64" s="23"/>
-      <c r="R64" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A65" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>279</v>
       </c>
       <c r="G65" s="23"/>
       <c r="L65" s="23"/>
-      <c r="M65" s="17"/>
-      <c r="N65" s="17"/>
-      <c r="O65" s="17"/>
-      <c r="P65" s="17"/>
       <c r="Q65" s="23"/>
-      <c r="R65" s="2" t="s">
-        <v>213</v>
+      <c r="R65" s="7" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="66" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
-        <v>188</v>
+        <v>66</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>189</v>
+        <v>67</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>190</v>
+        <v>144</v>
       </c>
       <c r="D66" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E66" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>214</v>
+        <v>0</v>
       </c>
       <c r="G66" s="23"/>
+      <c r="H66" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I66" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="J66" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="K66" s="17" t="s">
+        <v>226</v>
+      </c>
       <c r="L66" s="23"/>
-      <c r="M66" s="17"/>
-      <c r="N66" s="17"/>
-      <c r="O66" s="17"/>
-      <c r="P66" s="17"/>
+      <c r="M66" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="N66" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="O66" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="P66" s="17" t="s">
+        <v>302</v>
+      </c>
       <c r="Q66" s="23"/>
-    </row>
-    <row r="67" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" s="27" t="s">
-        <v>311</v>
-      </c>
-      <c r="B67" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="27" t="s">
-        <v>312</v>
-      </c>
-      <c r="D67" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="27" t="s">
-        <v>313</v>
+      <c r="R66" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>279</v>
       </c>
       <c r="G67" s="23"/>
       <c r="L67" s="23"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
       <c r="Q67" s="23"/>
-      <c r="R67" s="27" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R67" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
-        <v>70</v>
+        <v>188</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>10</v>
+        <v>189</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>71</v>
+        <v>190</v>
       </c>
       <c r="D68" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="G68" s="23"/>
-      <c r="H68" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="I68" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="J68" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="K68" s="17" t="s">
-        <v>280</v>
-      </c>
       <c r="L68" s="23"/>
-      <c r="M68" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="N68" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="O68" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="P68" s="17" t="s">
-        <v>281</v>
-      </c>
+      <c r="M68" s="17"/>
+      <c r="N68" s="17"/>
+      <c r="O68" s="17"/>
+      <c r="P68" s="17"/>
       <c r="Q68" s="23"/>
     </row>
-    <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A69" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B69" s="2" t="s">
+    <row r="69" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="B69" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>14</v>
+      <c r="C69" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="D69" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="27" t="s">
+        <v>313</v>
       </c>
       <c r="G69" s="23"/>
       <c r="L69" s="23"/>
-      <c r="M69" s="17"/>
-      <c r="N69" s="17"/>
-      <c r="O69" s="17"/>
-      <c r="P69" s="17"/>
       <c r="Q69" s="23"/>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A70" t="s">
-        <v>72</v>
-      </c>
-      <c r="B70" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" t="s">
-        <v>73</v>
-      </c>
-      <c r="D70" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" t="b">
-        <v>0</v>
-      </c>
-      <c r="F70" t="s">
-        <v>4</v>
-      </c>
-      <c r="R70"/>
+      <c r="R69" s="27" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D70" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G70" s="23"/>
+      <c r="H70" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="I70" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="J70" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="K70" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="L70" s="23"/>
+      <c r="M70" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="N70" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="O70" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="P70" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q70" s="23"/>
     </row>
     <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
-        <v>233</v>
+        <v>191</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>247</v>
+        <v>192</v>
       </c>
       <c r="D71" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71" s="2" t="b">
         <v>0</v>
@@ -3715,42 +3755,36 @@
       <c r="P71" s="17"/>
       <c r="Q71" s="23"/>
     </row>
-    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B72" s="2" t="s">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D72" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G72" s="23"/>
-      <c r="L72" s="23"/>
-      <c r="M72" s="17"/>
-      <c r="N72" s="17"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="17"/>
-      <c r="Q72" s="23"/>
-    </row>
-    <row r="73" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="C72" t="s">
+        <v>73</v>
+      </c>
+      <c r="D72" t="b">
+        <v>1</v>
+      </c>
+      <c r="E72" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" t="s">
+        <v>4</v>
+      </c>
+      <c r="R72"/>
+    </row>
+    <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
-        <v>76</v>
+        <v>233</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>77</v>
+        <v>247</v>
       </c>
       <c r="D73" s="2" t="b">
         <v>1</v>
@@ -3758,43 +3792,26 @@
       <c r="E73" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F73" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G73" s="23"/>
-      <c r="H73" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="I73" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="J73" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="K73" s="17" t="s">
-        <v>280</v>
-      </c>
       <c r="L73" s="23"/>
-      <c r="M73" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="N73" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="O73" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="P73" s="17" t="s">
-        <v>281</v>
-      </c>
+      <c r="M73" s="17"/>
+      <c r="N73" s="17"/>
+      <c r="O73" s="17"/>
+      <c r="P73" s="17"/>
       <c r="Q73" s="23"/>
     </row>
     <row r="74" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D74" s="2" t="b">
         <v>0</v>
@@ -3803,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>350</v>
+        <v>4</v>
       </c>
       <c r="G74" s="23"/>
       <c r="L74" s="23"/>
@@ -3813,41 +3830,59 @@
       <c r="P74" s="17"/>
       <c r="Q74" s="23"/>
     </row>
-    <row r="75" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B75" s="7" t="s">
+    <row r="75" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D75" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>273</v>
+      <c r="C75" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D75" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G75" s="23"/>
+      <c r="H75" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="I75" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="J75" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="K75" s="17" t="s">
+        <v>280</v>
+      </c>
       <c r="L75" s="23"/>
+      <c r="M75" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="N75" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="O75" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="P75" s="17" t="s">
+        <v>281</v>
+      </c>
       <c r="Q75" s="23"/>
-      <c r="R75" s="7" t="s">
-        <v>249</v>
-      </c>
     </row>
     <row r="76" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>193</v>
+        <v>78</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>194</v>
+        <v>79</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>195</v>
+        <v>80</v>
       </c>
       <c r="D76" s="2" t="b">
         <v>0</v>
@@ -3856,453 +3891,453 @@
         <v>0</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>282</v>
+        <v>350</v>
       </c>
       <c r="G76" s="23"/>
-      <c r="H76" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="L76" s="23"/>
-      <c r="M76" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="N76" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="O76" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="P76" s="17" t="s">
-        <v>17</v>
-      </c>
+      <c r="M76" s="17"/>
+      <c r="N76" s="17"/>
+      <c r="O76" s="17"/>
+      <c r="P76" s="17"/>
       <c r="Q76" s="23"/>
     </row>
-    <row r="77" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A77" s="7" t="s">
-        <v>196</v>
+        <v>81</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>174</v>
+        <v>10</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>197</v>
+        <v>82</v>
       </c>
       <c r="D77" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="G77" s="23"/>
       <c r="L77" s="23"/>
       <c r="Q77" s="23"/>
-      <c r="R77" s="8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R77" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
-        <v>83</v>
+        <v>193</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>10</v>
+        <v>194</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>84</v>
+        <v>195</v>
       </c>
       <c r="D78" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F78" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="G78" s="23"/>
-      <c r="H78" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="I78" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="J78" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="K78" s="17" t="s">
-        <v>283</v>
+      <c r="H78" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="L78" s="23"/>
       <c r="M78" s="17" t="s">
-        <v>284</v>
+        <v>17</v>
       </c>
       <c r="N78" s="17" t="s">
-        <v>284</v>
+        <v>17</v>
       </c>
       <c r="O78" s="17" t="s">
-        <v>284</v>
+        <v>17</v>
       </c>
       <c r="P78" s="17" t="s">
-        <v>284</v>
+        <v>17</v>
       </c>
       <c r="Q78" s="23"/>
     </row>
-    <row r="79" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D79" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>86</v>
+    <row r="79" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A79" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D79" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>227</v>
       </c>
       <c r="G79" s="23"/>
       <c r="L79" s="23"/>
-      <c r="M79" s="17"/>
-      <c r="N79" s="17"/>
-      <c r="O79" s="17"/>
-      <c r="P79" s="17"/>
       <c r="Q79" s="23"/>
-    </row>
-    <row r="80" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A80" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D80" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>90</v>
+      <c r="R79" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D80" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G80" s="23"/>
+      <c r="H80" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="I80" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="J80" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="K80" s="17" t="s">
+        <v>283</v>
+      </c>
       <c r="L80" s="23"/>
+      <c r="M80" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="N80" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="O80" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="P80" s="17" t="s">
+        <v>284</v>
+      </c>
       <c r="Q80" s="23"/>
-      <c r="R80" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A81" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D81" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E81" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>14</v>
+    </row>
+    <row r="81" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="G81" s="23"/>
       <c r="L81" s="23"/>
+      <c r="M81" s="17"/>
+      <c r="N81" s="17"/>
+      <c r="O81" s="17"/>
+      <c r="P81" s="17"/>
       <c r="Q81" s="23"/>
-      <c r="R81" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A82" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D82" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>94</v>
+    </row>
+    <row r="82" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A82" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D82" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="G82" s="23"/>
       <c r="L82" s="23"/>
-      <c r="M82" s="17"/>
-      <c r="N82" s="17"/>
-      <c r="O82" s="17"/>
-      <c r="P82" s="17"/>
       <c r="Q82" s="23"/>
-    </row>
-    <row r="83" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A83" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="B83" s="17" t="s">
+      <c r="R82" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A83" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B83" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C83" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="D83" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="17" t="s">
-        <v>4</v>
+      <c r="C83" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D83" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G83" s="23"/>
       <c r="L83" s="23"/>
       <c r="Q83" s="23"/>
-    </row>
-    <row r="84" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="B84" s="19"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="7" t="b">
-        <v>1</v>
+      <c r="R83" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G84" s="23"/>
-      <c r="H84" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I84" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J84" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K84" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="L84" s="23"/>
-      <c r="M84" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N84" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O84" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P84" s="7" t="s">
-        <v>4</v>
-      </c>
+      <c r="M84" s="17"/>
+      <c r="N84" s="17"/>
+      <c r="O84" s="17"/>
+      <c r="P84" s="17"/>
       <c r="Q84" s="23"/>
     </row>
-    <row r="85" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A85" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="B85" s="20" t="s">
+    <row r="85" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A85" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="B85" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="D85" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E85" s="7" t="b">
-        <v>1</v>
+        <v>292</v>
+      </c>
+      <c r="D85" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" s="17" t="s">
+        <v>4</v>
       </c>
       <c r="G85" s="23"/>
       <c r="L85" s="23"/>
       <c r="Q85" s="23"/>
     </row>
-    <row r="86" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
+    <row r="86" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B86" s="19"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G86" s="23"/>
+      <c r="H86" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I86" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J86" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K86" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L86" s="23"/>
+      <c r="M86" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N86" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O86" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P86" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q86" s="23"/>
+    </row>
+    <row r="87" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A87" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B87" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="D87" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G87" s="23"/>
+      <c r="L87" s="23"/>
+      <c r="Q87" s="23"/>
+    </row>
+    <row r="88" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A88" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G86" s="23"/>
-      <c r="L86" s="23"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
-      <c r="Q86" s="23"/>
-      <c r="R86" s="8" t="s">
+      <c r="D88" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G88" s="23"/>
+      <c r="L88" s="23"/>
+      <c r="M88" s="17"/>
+      <c r="N88" s="17"/>
+      <c r="O88" s="17"/>
+      <c r="P88" s="17"/>
+      <c r="Q88" s="23"/>
+      <c r="R88" s="8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="87" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A87" s="2" t="s">
+    <row r="89" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D87" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F87" s="2" t="s">
+      <c r="D89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="G87" s="23"/>
-      <c r="H87" s="17"/>
-      <c r="I87" s="17"/>
-      <c r="J87" s="17"/>
-      <c r="K87" s="17"/>
-      <c r="L87" s="23"/>
-      <c r="M87" s="17"/>
-      <c r="N87" s="17"/>
-      <c r="O87" s="17"/>
-      <c r="P87" s="17"/>
-      <c r="Q87" s="23"/>
-      <c r="R87" s="8" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A88" t="s">
-        <v>198</v>
-      </c>
-      <c r="B88" t="s">
-        <v>199</v>
-      </c>
-      <c r="C88" t="s">
-        <v>200</v>
-      </c>
-      <c r="D88" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" t="b">
-        <v>1</v>
-      </c>
-      <c r="M88" s="28" t="s">
-        <v>318</v>
-      </c>
-      <c r="N88" s="28" t="s">
-        <v>318</v>
-      </c>
-      <c r="O88" s="28" t="s">
-        <v>318</v>
-      </c>
-      <c r="P88" s="28" t="s">
-        <v>318</v>
-      </c>
-      <c r="R88"/>
-    </row>
-    <row r="89" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="B89" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="C89" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D89" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="G89" s="26"/>
+      <c r="G89" s="23"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="17"/>
+      <c r="J89" s="17"/>
+      <c r="K89" s="17"/>
       <c r="L89" s="23"/>
       <c r="M89" s="17"/>
       <c r="N89" s="17"/>
       <c r="O89" s="17"/>
       <c r="P89" s="17"/>
       <c r="Q89" s="23"/>
-    </row>
-    <row r="90" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="B90" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C90" s="28" t="s">
-        <v>341</v>
-      </c>
-      <c r="D90" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="28" t="s">
-        <v>273</v>
-      </c>
-      <c r="G90" s="23"/>
-      <c r="L90" s="23"/>
-      <c r="Q90" s="23"/>
-      <c r="R90" s="7" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D91" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G91" s="23"/>
+      <c r="R89" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
+        <v>198</v>
+      </c>
+      <c r="B90" t="s">
+        <v>199</v>
+      </c>
+      <c r="C90" t="s">
+        <v>200</v>
+      </c>
+      <c r="D90" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+      <c r="M90" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="N90" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="O90" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="P90" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="R90"/>
+    </row>
+    <row r="91" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D91" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G91" s="26"/>
       <c r="L91" s="23"/>
       <c r="M91" s="17"/>
       <c r="N91" s="17"/>
@@ -4312,13 +4347,13 @@
     </row>
     <row r="92" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="28" t="s">
-        <v>338</v>
+        <v>236</v>
       </c>
       <c r="B92" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D92" s="28" t="b">
         <v>1</v>
@@ -4329,22 +4364,22 @@
       <c r="F92" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="G92" s="29"/>
-      <c r="L92" s="29"/>
-      <c r="Q92" s="29"/>
+      <c r="G92" s="23"/>
+      <c r="L92" s="23"/>
+      <c r="Q92" s="23"/>
       <c r="R92" s="7" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D93" s="2" t="b">
         <v>0</v>
@@ -4352,50 +4387,52 @@
       <c r="E93" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F93" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="G93" s="26"/>
+      <c r="F93" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93" s="23"/>
       <c r="L93" s="23"/>
       <c r="M93" s="17"/>
       <c r="N93" s="17"/>
       <c r="O93" s="17"/>
       <c r="P93" s="17"/>
       <c r="Q93" s="23"/>
-      <c r="R93" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A94" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="B94" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="17" t="s">
-        <v>295</v>
-      </c>
-      <c r="D94" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="6"/>
-      <c r="G94" s="26"/>
-      <c r="L94" s="23"/>
-      <c r="Q94" s="23"/>
-    </row>
-    <row r="95" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="94" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="28" t="s">
+        <v>338</v>
+      </c>
+      <c r="B94" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" s="28" t="s">
+        <v>340</v>
+      </c>
+      <c r="D94" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="28" t="s">
+        <v>273</v>
+      </c>
+      <c r="G94" s="29"/>
+      <c r="L94" s="29"/>
+      <c r="Q94" s="29"/>
+      <c r="R94" s="7" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D95" s="2" t="b">
         <v>0</v>
@@ -4403,62 +4440,59 @@
       <c r="E95" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F95" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G95" s="23"/>
+      <c r="F95" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="G95" s="26"/>
       <c r="L95" s="23"/>
       <c r="M95" s="17"/>
       <c r="N95" s="17"/>
       <c r="O95" s="17"/>
       <c r="P95" s="17"/>
       <c r="Q95" s="23"/>
-    </row>
-    <row r="96" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B96" s="2" t="s">
+      <c r="R95" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A96" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="B96" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G96" s="23"/>
+      <c r="C96" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="D96" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" s="6"/>
+      <c r="G96" s="26"/>
       <c r="L96" s="23"/>
-      <c r="M96" s="17"/>
-      <c r="N96" s="17"/>
-      <c r="O96" s="17"/>
-      <c r="P96" s="17"/>
       <c r="Q96" s="23"/>
-      <c r="R96" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="97" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D97" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="G97" s="23"/>
       <c r="L97" s="23"/>
@@ -4467,232 +4501,198 @@
       <c r="O97" s="17"/>
       <c r="P97" s="17"/>
       <c r="Q97" s="23"/>
-      <c r="R97" s="8" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="98" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
-        <v>108</v>
+        <v>201</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>109</v>
+        <v>202</v>
       </c>
       <c r="D98" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98" s="23"/>
-      <c r="H98" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="I98" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="J98" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="K98" s="17" t="s">
-        <v>280</v>
-      </c>
       <c r="L98" s="23"/>
-      <c r="M98" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="N98" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="O98" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="P98" s="17" t="s">
-        <v>281</v>
-      </c>
+      <c r="M98" s="17"/>
+      <c r="N98" s="17"/>
+      <c r="O98" s="17"/>
+      <c r="P98" s="17"/>
       <c r="Q98" s="23"/>
-      <c r="R98" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A99" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D99" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E99" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F99" s="7" t="s">
-        <v>234</v>
+      <c r="R98" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A99" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="G99" s="23"/>
       <c r="L99" s="23"/>
+      <c r="M99" s="17"/>
+      <c r="N99" s="17"/>
+      <c r="O99" s="17"/>
+      <c r="P99" s="17"/>
       <c r="Q99" s="23"/>
-      <c r="R99" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D100" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F100" s="7" t="s">
+      <c r="R99" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A100" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D100" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G100" s="23"/>
+      <c r="H100" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="I100" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="J100" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="K100" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="L100" s="23"/>
+      <c r="M100" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="N100" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="O100" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="P100" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q100" s="23"/>
+      <c r="R100" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A101" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D101" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F101" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="G100" s="23"/>
-      <c r="L100" s="23"/>
-      <c r="Q100" s="23"/>
-      <c r="R100" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B101" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D101" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E101" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F101" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="G101" s="23"/>
       <c r="L101" s="23"/>
       <c r="Q101" s="23"/>
       <c r="R101" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D102" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G102" s="23"/>
+      <c r="L102" s="23"/>
+      <c r="Q102" s="23"/>
+      <c r="R102" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D103" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G103" s="23"/>
+      <c r="L103" s="23"/>
+      <c r="Q103" s="23"/>
+      <c r="R103" s="7" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="102" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G102" s="23"/>
-      <c r="H102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L102" s="23"/>
-      <c r="M102" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N102" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O102" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P102" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q102" s="23"/>
-    </row>
-    <row r="103" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D103" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G103" s="23"/>
-      <c r="H103" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J103" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L103" s="23"/>
-      <c r="M103" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N103" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O103" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P103" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q103" s="23"/>
     </row>
     <row r="104" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D104" s="2" t="b">
         <v>0</v>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="G104" s="23"/>
       <c r="H104" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>4</v>
@@ -4715,7 +4715,7 @@
       </c>
       <c r="L104" s="23"/>
       <c r="M104" s="17" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N104" s="17" t="s">
         <v>4</v>
@@ -4728,225 +4728,221 @@
       </c>
       <c r="Q104" s="23"/>
     </row>
-    <row r="105" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="28" t="s">
+    <row r="105" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D105" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G105" s="23"/>
+      <c r="H105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L105" s="23"/>
+      <c r="M105" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N105" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O105" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P105" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q105" s="23"/>
+    </row>
+    <row r="106" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D106" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G106" s="23"/>
+      <c r="H106" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J106" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L106" s="23"/>
+      <c r="M106" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N106" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O106" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P106" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q106" s="23"/>
+    </row>
+    <row r="107" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="B105" s="28" t="s">
+      <c r="B107" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C105" s="28" t="s">
+      <c r="C107" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="D105" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E105" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F105" s="28"/>
-      <c r="G105" s="23"/>
-      <c r="H105" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I105" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J105" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K105" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L105" s="23"/>
-      <c r="M105" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N105" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O105" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P105" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q105" s="23"/>
-      <c r="R105" s="28" t="s">
+      <c r="D107" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F107" s="28"/>
+      <c r="G107" s="23"/>
+      <c r="H107" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I107" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J107" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K107" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L107" s="23"/>
+      <c r="M107" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N107" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O107" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P107" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q107" s="23"/>
+      <c r="R107" s="28" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="106" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="28" t="s">
+    <row r="108" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="28" t="s">
         <v>342</v>
       </c>
-      <c r="B106" s="28" t="s">
+      <c r="B108" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C106" s="28" t="s">
+      <c r="C108" s="28" t="s">
         <v>343</v>
       </c>
-      <c r="D106" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E106" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F106" s="28"/>
-      <c r="G106" s="29"/>
-      <c r="H106" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I106" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J106" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K106" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L106" s="29"/>
-      <c r="M106" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N106" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O106" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P106" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q106" s="29"/>
-      <c r="R106" s="28" t="s">
+      <c r="D108" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F108" s="28"/>
+      <c r="G108" s="29"/>
+      <c r="H108" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I108" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J108" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K108" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L108" s="29"/>
+      <c r="M108" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N108" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O108" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P108" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q108" s="29"/>
+      <c r="R108" s="28" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A107" t="s">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A109" t="s">
         <v>121</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B109" t="s">
         <v>122</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C109" t="s">
         <v>123</v>
       </c>
-      <c r="D107" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" t="b">
-        <v>0</v>
-      </c>
-      <c r="H107" s="16" t="s">
+      <c r="D109" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" t="b">
+        <v>0</v>
+      </c>
+      <c r="H109" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="I107" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J107" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K107" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L107" s="23"/>
-      <c r="M107" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="N107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q107" s="23"/>
-      <c r="R107"/>
-    </row>
-    <row r="108" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D108" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E108" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G108" s="23"/>
-      <c r="H108" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L108" s="23"/>
-      <c r="M108" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N108" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O108" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P108" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q108" s="23"/>
-      <c r="R108" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G109" s="23"/>
-      <c r="H109" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K109" s="2" t="s">
+      <c r="I109" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J109" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K109" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L109" s="23"/>
       <c r="M109" s="17" t="s">
-        <v>14</v>
+        <v>288</v>
       </c>
       <c r="N109" s="17" t="s">
         <v>4</v>
@@ -4958,147 +4954,233 @@
         <v>4</v>
       </c>
       <c r="Q109" s="23"/>
+      <c r="R109"/>
     </row>
     <row r="110" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D110" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E110" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G110" s="23"/>
-      <c r="H110" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="I110" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="J110" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="K110" s="17" t="s">
-        <v>273</v>
+      <c r="H110" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K110" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L110" s="23"/>
       <c r="M110" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N110" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O110" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P110" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q110" s="23"/>
+      <c r="R110" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G111" s="23"/>
+      <c r="H111" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L111" s="23"/>
+      <c r="M111" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N111" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O111" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P111" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q111" s="23"/>
+    </row>
+    <row r="112" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D112" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G112" s="23"/>
+      <c r="H112" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="N110" s="17" t="s">
+      <c r="I112" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="O110" s="17" t="s">
+      <c r="J112" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="P110" s="17" t="s">
+      <c r="K112" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="Q110" s="23"/>
-    </row>
-    <row r="111" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A111" s="30" t="s">
+      <c r="L112" s="23"/>
+      <c r="M112" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N112" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O112" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="P112" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q112" s="23"/>
+    </row>
+    <row r="113" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A113" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="B111" s="30" t="s">
+      <c r="B113" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C111" s="30" t="s">
+      <c r="C113" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="D111" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" s="30" t="s">
+      <c r="D113" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F113" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="G111" s="29"/>
-      <c r="L111" s="29"/>
-      <c r="Q111" s="29"/>
-    </row>
-    <row r="112" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A112" s="2" t="s">
+      <c r="G113" s="29"/>
+      <c r="L113" s="29"/>
+      <c r="Q113" s="29"/>
+    </row>
+    <row r="114" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A114" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D112" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F112" s="2" t="s">
+      <c r="D114" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F114" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G112" s="23"/>
-      <c r="L112" s="23"/>
-      <c r="M112" s="17"/>
-      <c r="N112" s="17"/>
-      <c r="O112" s="17"/>
-      <c r="P112" s="17"/>
-      <c r="Q112" s="23"/>
-    </row>
-    <row r="113" spans="18:18" x14ac:dyDescent="0.4">
-      <c r="R113"/>
-    </row>
-    <row r="114" spans="18:18" x14ac:dyDescent="0.4">
-      <c r="R114"/>
-    </row>
-    <row r="115" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="G114" s="23"/>
+      <c r="L114" s="23"/>
+      <c r="M114" s="17"/>
+      <c r="N114" s="17"/>
+      <c r="O114" s="17"/>
+      <c r="P114" s="17"/>
+      <c r="Q114" s="23"/>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R115"/>
     </row>
-    <row r="116" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R116"/>
     </row>
-    <row r="117" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R117"/>
     </row>
-    <row r="118" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R118"/>
     </row>
-    <row r="119" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R119"/>
     </row>
-    <row r="120" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R120"/>
     </row>
-    <row r="121" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R121"/>
     </row>
-    <row r="122" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R122"/>
     </row>
-    <row r="123" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R123"/>
     </row>
-    <row r="124" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R124"/>
     </row>
-    <row r="125" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R125"/>
     </row>
-    <row r="126" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R126"/>
     </row>
-    <row r="127" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R127"/>
     </row>
-    <row r="128" spans="18:18" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R128"/>
     </row>
     <row r="129" spans="18:18" x14ac:dyDescent="0.4">
@@ -5118,6 +5200,12 @@
     </row>
     <row r="134" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R134"/>
+    </row>
+    <row r="135" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R135"/>
+    </row>
+    <row r="136" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R136"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5125,15 +5213,15 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1"/>
     <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="F57" r:id="rId3"/>
+    <hyperlink ref="F58" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
Nieuwe interpretatie van cli/migrate, nu name.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="356">
   <si>
     <t>Name</t>
   </si>
@@ -603,9 +603,6 @@
     <t>migrate</t>
   </si>
   <si>
-    <t>Yes if the source XMI file must be migrated to the new metamodel.</t>
-  </si>
-  <si>
     <t>passoffice</t>
   </si>
   <si>
@@ -1093,6 +1090,9 @@
   </si>
   <si>
     <t>[model-abbreviation]-concepts</t>
+  </si>
+  <si>
+    <t>Specify a name if the source XMI file must be migrated to a (new) metamodel.</t>
   </si>
 </sst>
 </file>
@@ -1670,7 +1670,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A64" sqref="A64"/>
+      <selection pane="bottomRight" activeCell="A71" sqref="A71:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1706,72 +1706,72 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>229</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>230</v>
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L1" s="21"/>
       <c r="M1" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q1" s="21"/>
       <c r="R1" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
       <c r="G2" s="22"/>
       <c r="H2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>306</v>
       </c>
       <c r="L2" s="22"/>
       <c r="M2" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="Q2" s="22"/>
       <c r="R2" s="5"/>
@@ -1827,7 +1827,7 @@
       <c r="P4" s="17"/>
       <c r="Q4" s="23"/>
       <c r="R4" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -1857,7 +1857,7 @@
       <c r="P5" s="17"/>
       <c r="Q5" s="23"/>
       <c r="R5" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -1904,7 +1904,7 @@
       <c r="P7" s="17"/>
       <c r="Q7" s="23"/>
       <c r="R7" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -1993,13 +1993,13 @@
     </row>
     <row r="12" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>266</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>267</v>
       </c>
       <c r="D12" s="12" t="b">
         <v>0</v>
@@ -2010,20 +2010,20 @@
       <c r="G12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Q12" s="23"/>
       <c r="R12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -2073,10 +2073,10 @@
         <v>17</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L14" s="23"/>
       <c r="M14" s="17" t="s">
@@ -2086,14 +2086,14 @@
         <v>17</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P14" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q14" s="23"/>
       <c r="R14" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2113,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G15" s="23"/>
       <c r="L15" s="23"/>
@@ -2125,22 +2125,22 @@
     </row>
     <row r="16" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="G16" s="23"/>
       <c r="L16" s="23"/>
@@ -2152,7 +2152,7 @@
     </row>
     <row r="17" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -2163,7 +2163,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G17" s="23"/>
       <c r="I17" s="17"/>
@@ -2217,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G19" s="23"/>
       <c r="L19" s="23"/>
@@ -2244,7 +2244,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G20" s="23"/>
       <c r="L20" s="23"/>
@@ -2456,7 +2456,7 @@
       <c r="P26" s="17"/>
       <c r="Q26" s="23"/>
       <c r="R26" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2505,13 +2505,13 @@
     </row>
     <row r="28" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="41" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D28" s="41" t="b">
         <v>0</v>
@@ -2549,13 +2549,13 @@
     </row>
     <row r="29" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B29" s="32" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D29" s="32" t="b">
         <v>0</v>
@@ -2570,18 +2570,18 @@
       <c r="L29" s="29"/>
       <c r="Q29" s="29"/>
       <c r="R29" s="32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="30" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="32" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B30" s="32" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D30" s="32" t="b">
         <v>0</v>
@@ -2590,13 +2590,13 @@
         <v>1</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G30" s="29"/>
       <c r="L30" s="29"/>
       <c r="Q30" s="29"/>
       <c r="R30" s="32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2643,18 +2643,18 @@
       </c>
       <c r="Q31" s="23"/>
       <c r="R31" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="33" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="B32" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="C32" s="33" t="s">
         <v>333</v>
-      </c>
-      <c r="C32" s="33" t="s">
-        <v>334</v>
       </c>
       <c r="D32" s="33" t="b">
         <v>0</v>
@@ -2664,13 +2664,13 @@
       </c>
       <c r="G32" s="29"/>
       <c r="I32" s="33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J32" s="39" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K32" s="39" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L32" s="29"/>
       <c r="Q32" s="29"/>
@@ -2740,13 +2740,13 @@
     </row>
     <row r="36" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B36" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D36" s="34" t="b">
         <v>0</v>
@@ -2865,13 +2865,13 @@
     </row>
     <row r="40" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="36" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B40" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D40" s="36" t="b">
         <v>0</v>
@@ -2880,7 +2880,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="36" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G40" s="35"/>
       <c r="L40" s="35"/>
@@ -2932,7 +2932,7 @@
       <c r="L42" s="38"/>
       <c r="Q42" s="38"/>
       <c r="R42" s="37" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="43" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2952,13 +2952,13 @@
         <v>0</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G43" s="23"/>
       <c r="L43" s="23"/>
       <c r="Q43" s="23"/>
       <c r="R43" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -3066,7 +3066,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G48" s="26"/>
       <c r="L48" s="23"/>
@@ -3076,12 +3076,12 @@
       <c r="P48" s="17"/>
       <c r="Q48" s="23"/>
       <c r="R48" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -3094,29 +3094,29 @@
       <c r="F49" s="6"/>
       <c r="G49" s="26"/>
       <c r="H49" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J49" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K49" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L49" s="23"/>
       <c r="M49" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N49" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O49" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P49" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q49" s="23"/>
     </row>
@@ -3161,7 +3161,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G51" s="23"/>
       <c r="L51" s="23"/>
@@ -3240,7 +3240,7 @@
       <c r="L54" s="23"/>
       <c r="Q54" s="23"/>
       <c r="R54" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -3268,22 +3268,22 @@
     </row>
     <row r="56" spans="1:18" s="28" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A56" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B56" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C56" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="D56" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="15" t="s">
         <v>345</v>
-      </c>
-      <c r="D56" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="15" t="s">
-        <v>346</v>
       </c>
       <c r="G56" s="24"/>
       <c r="H56" s="15"/>
@@ -3300,22 +3300,22 @@
     </row>
     <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A57" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="C57" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="D57" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>299</v>
-      </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>300</v>
       </c>
       <c r="G57" s="23"/>
       <c r="L57" s="23"/>
@@ -3323,22 +3323,22 @@
     </row>
     <row r="58" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>87</v>
       </c>
       <c r="C58" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="18" t="s">
         <v>347</v>
-      </c>
-      <c r="D58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="18" t="s">
-        <v>348</v>
       </c>
       <c r="G58" s="23"/>
       <c r="H58" s="18"/>
@@ -3369,7 +3369,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G59" s="23"/>
       <c r="L59" s="23"/>
@@ -3377,22 +3377,22 @@
     </row>
     <row r="60" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A60" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="B60" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="C60" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="D60" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="15" t="s">
         <v>262</v>
-      </c>
-      <c r="D60" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="15" t="s">
-        <v>263</v>
       </c>
       <c r="G60" s="24"/>
       <c r="H60" s="15"/>
@@ -3406,7 +3406,7 @@
       <c r="P60" s="15"/>
       <c r="Q60" s="24"/>
       <c r="R60" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3432,7 +3432,7 @@
       <c r="L61" s="23"/>
       <c r="Q61" s="23"/>
       <c r="R61" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -3452,24 +3452,24 @@
         <v>1</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G62" s="23"/>
       <c r="L62" s="23"/>
       <c r="Q62" s="23"/>
       <c r="R62" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="63" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A63" s="31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B63" s="31" t="s">
         <v>5</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D63" s="31" t="b">
         <v>0</v>
@@ -3507,22 +3507,22 @@
     </row>
     <row r="64" spans="1:18" s="42" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A64" s="42" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B64" s="42" t="s">
         <v>10</v>
       </c>
       <c r="C64" s="42" t="s">
+        <v>353</v>
+      </c>
+      <c r="D64" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="42" t="s">
         <v>354</v>
-      </c>
-      <c r="D64" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="42" t="s">
-        <v>355</v>
       </c>
       <c r="G64" s="29"/>
       <c r="L64" s="29"/>
@@ -3545,13 +3545,13 @@
         <v>0</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G65" s="23"/>
       <c r="L65" s="23"/>
       <c r="Q65" s="23"/>
       <c r="R65" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="66" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3572,33 +3572,33 @@
       </c>
       <c r="G66" s="23"/>
       <c r="H66" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I66" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J66" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K66" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L66" s="23"/>
       <c r="M66" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N66" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="O66" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P66" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q66" s="23"/>
       <c r="R66" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -3618,7 +3618,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G67" s="23"/>
       <c r="L67" s="23"/>
@@ -3628,7 +3628,7 @@
       <c r="P67" s="17"/>
       <c r="Q67" s="23"/>
       <c r="R67" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3648,7 +3648,7 @@
         <v>1</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G68" s="23"/>
       <c r="L68" s="23"/>
@@ -3660,28 +3660,28 @@
     </row>
     <row r="69" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="27" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B69" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="D69" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="27" t="s">
         <v>312</v>
-      </c>
-      <c r="D69" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="27" t="s">
-        <v>313</v>
       </c>
       <c r="G69" s="23"/>
       <c r="L69" s="23"/>
       <c r="Q69" s="23"/>
       <c r="R69" s="27" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="70" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -3702,29 +3702,29 @@
       </c>
       <c r="G70" s="23"/>
       <c r="H70" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I70" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J70" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K70" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L70" s="23"/>
       <c r="M70" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N70" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O70" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P70" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q70" s="23"/>
     </row>
@@ -3733,19 +3733,16 @@
         <v>191</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>192</v>
+        <v>355</v>
       </c>
       <c r="D71" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G71" s="23"/>
       <c r="L71" s="23"/>
@@ -3778,13 +3775,13 @@
     </row>
     <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D73" s="2" t="b">
         <v>1</v>
@@ -3848,29 +3845,29 @@
       </c>
       <c r="G75" s="23"/>
       <c r="H75" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I75" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J75" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K75" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L75" s="23"/>
       <c r="M75" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N75" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O75" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P75" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q75" s="23"/>
     </row>
@@ -3891,7 +3888,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G76" s="23"/>
       <c r="L76" s="23"/>
@@ -3918,25 +3915,25 @@
         <v>0</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G77" s="23"/>
       <c r="L77" s="23"/>
       <c r="Q77" s="23"/>
       <c r="R77" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="D78" s="2" t="b">
         <v>0</v>
       </c>
@@ -3944,7 +3941,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G78" s="23"/>
       <c r="H78" s="2" t="s">
@@ -3967,13 +3964,13 @@
     </row>
     <row r="79" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A79" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>174</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D79" s="7" t="b">
         <v>0</v>
@@ -3982,13 +3979,13 @@
         <v>1</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G79" s="23"/>
       <c r="L79" s="23"/>
       <c r="Q79" s="23"/>
       <c r="R79" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -4009,29 +4006,29 @@
       </c>
       <c r="G80" s="23"/>
       <c r="H80" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I80" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J80" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K80" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L80" s="23"/>
       <c r="M80" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N80" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O80" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P80" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q80" s="23"/>
     </row>
@@ -4085,7 +4082,7 @@
       <c r="L82" s="23"/>
       <c r="Q82" s="23"/>
       <c r="R82" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="83" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -4111,7 +4108,7 @@
       <c r="L83" s="23"/>
       <c r="Q83" s="23"/>
       <c r="R83" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="84" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
@@ -4143,13 +4140,13 @@
     </row>
     <row r="85" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A85" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B85" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D85" s="17" t="b">
         <v>0</v>
@@ -4166,7 +4163,7 @@
     </row>
     <row r="86" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
@@ -4206,13 +4203,13 @@
     </row>
     <row r="87" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A87" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B87" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C87" s="20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D87" s="7" t="b">
         <v>0</v>
@@ -4251,7 +4248,7 @@
       <c r="P88" s="17"/>
       <c r="Q88" s="23"/>
       <c r="R88" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="89" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4271,7 +4268,7 @@
         <v>0</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G89" s="23"/>
       <c r="H89" s="17"/>
@@ -4285,19 +4282,19 @@
       <c r="P89" s="17"/>
       <c r="Q89" s="23"/>
       <c r="R89" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
+        <v>197</v>
+      </c>
+      <c r="B90" t="s">
         <v>198</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>199</v>
       </c>
-      <c r="C90" t="s">
-        <v>200</v>
-      </c>
       <c r="D90" t="b">
         <v>0</v>
       </c>
@@ -4305,37 +4302,37 @@
         <v>1</v>
       </c>
       <c r="M90" s="28" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N90" s="28" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O90" s="28" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P90" s="28" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R90"/>
     </row>
     <row r="91" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A91" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="B91" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="B91" s="13" t="s">
+      <c r="C91" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="D91" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="D91" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="6" t="s">
-        <v>271</v>
       </c>
       <c r="G91" s="26"/>
       <c r="L91" s="23"/>
@@ -4347,13 +4344,13 @@
     </row>
     <row r="92" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B92" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D92" s="28" t="b">
         <v>1</v>
@@ -4362,13 +4359,13 @@
         <v>1</v>
       </c>
       <c r="F92" s="28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G92" s="23"/>
       <c r="L92" s="23"/>
       <c r="Q92" s="23"/>
       <c r="R92" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="93" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4400,13 +4397,13 @@
     </row>
     <row r="94" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B94" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C94" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D94" s="28" t="b">
         <v>1</v>
@@ -4415,13 +4412,13 @@
         <v>1</v>
       </c>
       <c r="F94" s="28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G94" s="29"/>
       <c r="L94" s="29"/>
       <c r="Q94" s="29"/>
       <c r="R94" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="95" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
@@ -4441,7 +4438,7 @@
         <v>1</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G95" s="26"/>
       <c r="L95" s="23"/>
@@ -4451,18 +4448,18 @@
       <c r="P95" s="17"/>
       <c r="Q95" s="23"/>
       <c r="R95" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="96" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B96" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D96" s="17" t="b">
         <v>0</v>
@@ -4504,13 +4501,13 @@
     </row>
     <row r="98" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D98" s="2" t="b">
         <v>0</v>
@@ -4526,7 +4523,7 @@
       <c r="P98" s="17"/>
       <c r="Q98" s="23"/>
       <c r="R98" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="99" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
@@ -4556,7 +4553,7 @@
       <c r="P99" s="17"/>
       <c r="Q99" s="23"/>
       <c r="R99" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="100" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4577,33 +4574,33 @@
       </c>
       <c r="G100" s="23"/>
       <c r="H100" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I100" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J100" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K100" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L100" s="23"/>
       <c r="M100" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N100" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O100" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P100" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q100" s="23"/>
       <c r="R100" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="101" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -4623,13 +4620,13 @@
         <v>0</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G101" s="23"/>
       <c r="L101" s="23"/>
       <c r="Q101" s="23"/>
       <c r="R101" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="102" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -4649,13 +4646,13 @@
         <v>0</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G102" s="23"/>
       <c r="L102" s="23"/>
       <c r="Q102" s="23"/>
       <c r="R102" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="103" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -4681,7 +4678,7 @@
       <c r="L103" s="23"/>
       <c r="Q103" s="23"/>
       <c r="R103" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="104" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -4736,7 +4733,7 @@
         <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D105" s="2" t="b">
         <v>1</v>
@@ -4861,18 +4858,18 @@
       </c>
       <c r="Q107" s="23"/>
       <c r="R107" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="108" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B108" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D108" s="28" t="b">
         <v>0</v>
@@ -4909,7 +4906,7 @@
       </c>
       <c r="Q108" s="29"/>
       <c r="R108" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.4">
@@ -4929,7 +4926,7 @@
         <v>0</v>
       </c>
       <c r="H109" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I109" s="16" t="s">
         <v>4</v>
@@ -4942,7 +4939,7 @@
       </c>
       <c r="L109" s="23"/>
       <c r="M109" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N109" s="17" t="s">
         <v>4</v>
@@ -5000,12 +4997,12 @@
       </c>
       <c r="Q110" s="23"/>
       <c r="R110" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="111" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>5</v>
@@ -5065,50 +5062,50 @@
       </c>
       <c r="G112" s="23"/>
       <c r="H112" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I112" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J112" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K112" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L112" s="23"/>
       <c r="M112" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N112" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O112" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P112" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q112" s="23"/>
     </row>
     <row r="113" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A113" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B113" s="30" t="s">
         <v>79</v>
       </c>
       <c r="C113" s="30" t="s">
+        <v>315</v>
+      </c>
+      <c r="D113" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F113" s="30" t="s">
         <v>316</v>
-      </c>
-      <c r="D113" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F113" s="30" t="s">
-        <v>317</v>
       </c>
       <c r="G113" s="29"/>
       <c r="L113" s="29"/>
@@ -5131,7 +5128,7 @@
         <v>0</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G114" s="23"/>
       <c r="L114" s="23"/>
@@ -5244,48 +5241,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
[bro] [kadaster] cli/createeaprofile expliciet gezet
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="360">
   <si>
     <t>Name</t>
   </si>
@@ -1099,6 +1099,12 @@
   </si>
   <si>
     <t>Name of the visuals file</t>
+  </si>
+  <si>
+    <t>createeatoolbox</t>
+  </si>
+  <si>
+    <t>Should an EA toolbox be generated?</t>
   </si>
 </sst>
 </file>
@@ -1264,7 +1270,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1364,6 +1370,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1673,13 +1682,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R137"/>
+  <dimension ref="A1:R138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D94" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M113" sqref="M113:P113"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1890,16 +1899,16 @@
       <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="44" t="b">
+      <c r="D7" s="45" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1917,10 +1926,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
       <c r="G8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
@@ -2438,159 +2447,177 @@
       </c>
       <c r="Q25" s="23"/>
     </row>
-    <row r="26" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="44" t="s">
+        <v>358</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>359</v>
+      </c>
+      <c r="D26" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" s="29"/>
+      <c r="M26" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="N26" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="O26" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="29"/>
+    </row>
+    <row r="27" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="8" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D27" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G27" s="23"/>
-      <c r="H27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" s="23"/>
-      <c r="M27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N27" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O27" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P27" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q27" s="23"/>
-    </row>
-    <row r="28" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="41" t="s">
+      <c r="D28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" s="23"/>
+      <c r="H28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" s="23"/>
+      <c r="M28" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O28" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="23"/>
+    </row>
+    <row r="29" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="41" t="s">
         <v>350</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B29" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="41" t="s">
+      <c r="C29" s="41" t="s">
         <v>351</v>
       </c>
-      <c r="D28" s="41" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28" s="41" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" s="29"/>
-      <c r="H28" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="J28" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="K28" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="L28" s="29"/>
-      <c r="M28" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="N28" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="O28" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="P28" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q28" s="29"/>
-    </row>
-    <row r="29" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="32" t="s">
-        <v>320</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="32" t="s">
-        <v>321</v>
-      </c>
-      <c r="D29" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>14</v>
+      <c r="D29" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="41" t="b">
+        <v>1</v>
       </c>
       <c r="G29" s="29"/>
+      <c r="H29" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="41" t="s">
+        <v>4</v>
+      </c>
       <c r="L29" s="29"/>
+      <c r="M29" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="O29" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="P29" s="41" t="s">
+        <v>14</v>
+      </c>
       <c r="Q29" s="29"/>
-      <c r="R29" s="32" t="s">
-        <v>324</v>
-      </c>
     </row>
     <row r="30" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="32" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D30" s="32" t="b">
         <v>0</v>
@@ -2599,7 +2626,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>330</v>
+        <v>14</v>
       </c>
       <c r="G30" s="29"/>
       <c r="L30" s="29"/>
@@ -2608,111 +2635,117 @@
         <v>324</v>
       </c>
     </row>
-    <row r="31" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="D31" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>330</v>
+      </c>
+      <c r="G31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="32" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" s="23"/>
-      <c r="H31" s="2" t="s">
+      <c r="D32" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="23"/>
+      <c r="H32" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I31" s="40" t="s">
+      <c r="I32" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="J31" s="40" t="s">
+      <c r="J32" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="K31" s="40" t="s">
+      <c r="K32" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="L31" s="23"/>
-      <c r="M31" s="17" t="s">
+      <c r="L32" s="23"/>
+      <c r="M32" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N31" s="40" t="s">
+      <c r="N32" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="O31" s="40" t="s">
+      <c r="O32" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="P31" s="40" t="s">
+      <c r="P32" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="23"/>
-      <c r="R31" s="2" t="s">
+      <c r="Q32" s="23"/>
+      <c r="R32" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="32" spans="1:18" s="33" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A32" s="33" t="s">
+    <row r="33" spans="1:18" s="33" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A33" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B33" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C33" s="33" t="s">
         <v>333</v>
       </c>
-      <c r="D32" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" s="29"/>
-      <c r="I32" s="33" t="s">
+      <c r="D33" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="29"/>
+      <c r="I33" s="33" t="s">
         <v>334</v>
       </c>
-      <c r="J32" s="39" t="s">
+      <c r="J33" s="39" t="s">
         <v>334</v>
       </c>
-      <c r="K32" s="39" t="s">
+      <c r="K33" s="39" t="s">
         <v>334</v>
       </c>
-      <c r="L32" s="29"/>
-      <c r="Q32" s="29"/>
-    </row>
-    <row r="33" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A33" s="34" t="s">
+      <c r="L33" s="29"/>
+      <c r="Q33" s="29"/>
+    </row>
+    <row r="34" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A34" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B34" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C34" s="34" t="s">
         <v>167</v>
-      </c>
-      <c r="D33" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E33" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="G33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="Q33" s="35"/>
-    </row>
-    <row r="34" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>170</v>
       </c>
       <c r="D34" s="34" t="b">
         <v>0</v>
@@ -2726,22 +2759,19 @@
     </row>
     <row r="35" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="34" t="s">
-        <v>35</v>
+        <v>168</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>5</v>
+        <v>169</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="D35" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E35" s="34" t="b">
         <v>1</v>
-      </c>
-      <c r="F35" s="34" t="s">
-        <v>14</v>
       </c>
       <c r="G35" s="35"/>
       <c r="L35" s="35"/>
@@ -2749,13 +2779,13 @@
     </row>
     <row r="36" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="34" t="s">
-        <v>335</v>
+        <v>35</v>
       </c>
       <c r="B36" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>336</v>
+        <v>36</v>
       </c>
       <c r="D36" s="34" t="b">
         <v>0</v>
@@ -2767,241 +2797,251 @@
         <v>14</v>
       </c>
       <c r="G36" s="35"/>
-      <c r="H36" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="J36" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="K36" s="34" t="s">
-        <v>4</v>
-      </c>
       <c r="L36" s="35"/>
       <c r="Q36" s="35"/>
     </row>
-    <row r="37" spans="1:18" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A37" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="36" t="s">
+    <row r="37" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="B37" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="36" t="s">
+      <c r="C37" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="D37" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G37" s="35"/>
+      <c r="H37" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="34" t="s">
+        <v>4</v>
+      </c>
       <c r="L37" s="35"/>
       <c r="Q37" s="35"/>
     </row>
-    <row r="38" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A38" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="34" t="s">
+    <row r="38" spans="1:18" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A38" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="F38" s="34" t="s">
+      <c r="C38" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="36" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="35"/>
       <c r="L38" s="35"/>
       <c r="Q38" s="35"/>
     </row>
-    <row r="39" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="36" t="s">
+    <row r="39" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A39" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="36" t="b">
-        <v>1</v>
+      <c r="C39" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39" s="34" t="s">
+        <v>14</v>
       </c>
       <c r="G39" s="35"/>
-      <c r="H39" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="I39" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J39" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="K39" s="36" t="s">
-        <v>14</v>
-      </c>
       <c r="L39" s="35"/>
-      <c r="M39" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="N39" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="O39" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="P39" s="36" t="s">
-        <v>4</v>
-      </c>
       <c r="Q39" s="35"/>
     </row>
     <row r="40" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="35"/>
+      <c r="H40" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="K40" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L40" s="35"/>
+      <c r="M40" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="N40" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="O40" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="P40" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q40" s="35"/>
+    </row>
+    <row r="41" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="36" t="s">
         <v>325</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B41" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="C41" s="36" t="s">
         <v>326</v>
       </c>
-      <c r="D40" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="36" t="s">
+      <c r="D41" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="36" t="s">
         <v>329</v>
-      </c>
-      <c r="G40" s="35"/>
-      <c r="L40" s="35"/>
-      <c r="Q40" s="35"/>
-    </row>
-    <row r="41" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="B41" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="D41" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="34" t="s">
-        <v>14</v>
       </c>
       <c r="G41" s="35"/>
       <c r="L41" s="35"/>
       <c r="Q41" s="35"/>
     </row>
-    <row r="42" spans="1:18" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A42" s="37" t="s">
+    <row r="42" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D42" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="35"/>
+      <c r="L42" s="35"/>
+      <c r="Q42" s="35"/>
+    </row>
+    <row r="43" spans="1:18" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A43" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B43" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C43" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="38"/>
-      <c r="L42" s="38"/>
-      <c r="Q42" s="38"/>
-      <c r="R42" s="37" t="s">
+      <c r="D43" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E43" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="37" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A43" s="7" t="s">
+    <row r="44" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A44" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B44" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C44" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F43" s="7" t="s">
+      <c r="D44" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="G43" s="23"/>
-      <c r="L43" s="23"/>
-      <c r="Q43" s="23"/>
-      <c r="R43" s="7" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="44" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G44" s="23"/>
       <c r="L44" s="23"/>
-      <c r="M44" s="17"/>
-      <c r="N44" s="17"/>
-      <c r="O44" s="17"/>
-      <c r="P44" s="17"/>
       <c r="Q44" s="23"/>
+      <c r="R44" s="7" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="44"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
+      <c r="A45" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G45" s="23"/>
       <c r="L45" s="23"/>
       <c r="M45" s="17"/>
@@ -3010,22 +3050,11 @@
       <c r="P45" s="17"/>
       <c r="Q45" s="23"/>
     </row>
-    <row r="46" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A46" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D46" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="45"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
       <c r="G46" s="23"/>
       <c r="L46" s="23"/>
       <c r="M46" s="17"/>
@@ -3034,21 +3063,21 @@
       <c r="P46" s="17"/>
       <c r="Q46" s="23"/>
     </row>
-    <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>50</v>
+        <v>173</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>51</v>
+        <v>175</v>
       </c>
       <c r="D47" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" s="23"/>
       <c r="L47" s="23"/>
@@ -3058,15 +3087,15 @@
       <c r="P47" s="17"/>
       <c r="Q47" s="23"/>
     </row>
-    <row r="48" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D48" s="2" t="b">
         <v>0</v>
@@ -3074,95 +3103,95 @@
       <c r="E48" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F48" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="G48" s="26"/>
+      <c r="G48" s="23"/>
       <c r="L48" s="23"/>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
       <c r="O48" s="17"/>
       <c r="P48" s="17"/>
       <c r="Q48" s="23"/>
-      <c r="R48" s="2" t="s">
+    </row>
+    <row r="49" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A49" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G49" s="26"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="23"/>
+      <c r="R49" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F49" s="6"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="17" t="s">
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="I49" s="17" t="s">
+      <c r="I50" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="J49" s="17" t="s">
+      <c r="J50" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="K49" s="17" t="s">
+      <c r="K50" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="L49" s="23"/>
-      <c r="M49" s="17" t="s">
+      <c r="L50" s="23"/>
+      <c r="M50" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="N49" s="17" t="s">
+      <c r="N50" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="O49" s="17" t="s">
+      <c r="O50" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="P49" s="17" t="s">
+      <c r="P50" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="Q49" s="23"/>
-    </row>
-    <row r="50" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="7" t="s">
+      <c r="Q50" s="23"/>
+    </row>
+    <row r="51" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B51" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D50" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G50" s="23"/>
-      <c r="L50" s="23"/>
-      <c r="Q50" s="23"/>
-      <c r="R50"/>
-    </row>
-    <row r="51" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A51" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="D51" s="7" t="b">
         <v>0</v>
       </c>
@@ -3170,77 +3199,78 @@
         <v>1</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>224</v>
+        <v>4</v>
       </c>
       <c r="G51" s="23"/>
       <c r="L51" s="23"/>
       <c r="Q51" s="23"/>
-    </row>
-    <row r="52" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D52" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>14</v>
+      <c r="R51"/>
+    </row>
+    <row r="52" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A52" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D52" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="G52" s="23"/>
       <c r="L52" s="23"/>
-      <c r="M52" s="17"/>
-      <c r="N52" s="17"/>
-      <c r="O52" s="17"/>
-      <c r="P52" s="17"/>
       <c r="Q52" s="23"/>
     </row>
-    <row r="53" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="7" t="s">
+    <row r="53" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D53" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" s="7" t="s">
+      <c r="C53" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G53" s="23"/>
       <c r="L53" s="23"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
       <c r="Q53" s="23"/>
     </row>
-    <row r="54" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D54" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E54" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>14</v>
@@ -3248,25 +3278,22 @@
       <c r="G54" s="23"/>
       <c r="L54" s="23"/>
       <c r="Q54" s="23"/>
-      <c r="R54" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="55" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A55" s="7" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>182</v>
+        <v>60</v>
       </c>
       <c r="D55" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E55" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>14</v>
@@ -3274,390 +3301,386 @@
       <c r="G55" s="23"/>
       <c r="L55" s="23"/>
       <c r="Q55" s="23"/>
-    </row>
-    <row r="56" spans="1:18" s="28" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A56" s="15" t="s">
+      <c r="R55" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D56" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" s="23"/>
+      <c r="L56" s="23"/>
+      <c r="Q56" s="23"/>
+    </row>
+    <row r="57" spans="1:18" s="28" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A57" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B57" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C57" s="14" t="s">
         <v>344</v>
       </c>
-      <c r="D56" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="15" t="s">
+      <c r="D57" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="G56" s="24"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="15"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="24"/>
-      <c r="M56" s="15"/>
-      <c r="N56" s="15"/>
-      <c r="O56" s="15"/>
-      <c r="P56" s="15"/>
-      <c r="Q56" s="24"/>
-      <c r="R56" s="15"/>
-    </row>
-    <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="7" t="s">
+      <c r="G57" s="24"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="24"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
+      <c r="Q57" s="24"/>
+      <c r="R57" s="15"/>
+    </row>
+    <row r="58" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B58" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C58" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="7" t="s">
+      <c r="D58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="G57" s="23"/>
-      <c r="L57" s="23"/>
-      <c r="Q57" s="23"/>
-    </row>
-    <row r="58" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A58" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="D58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="18" t="s">
-        <v>347</v>
-      </c>
       <c r="G58" s="23"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="18"/>
-      <c r="K58" s="18"/>
       <c r="L58" s="23"/>
-      <c r="M58" s="18"/>
-      <c r="N58" s="18"/>
-      <c r="O58" s="18"/>
-      <c r="P58" s="18"/>
       <c r="Q58" s="23"/>
     </row>
     <row r="59" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A59" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="G59" s="23"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="23"/>
+      <c r="M59" s="18"/>
+      <c r="N59" s="18"/>
+      <c r="O59" s="18"/>
+      <c r="P59" s="18"/>
+      <c r="Q59" s="23"/>
+    </row>
+    <row r="60" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A60" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="7" t="s">
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="G59" s="23"/>
-      <c r="L59" s="23"/>
-      <c r="Q59" s="23"/>
-    </row>
-    <row r="60" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A60" s="15" t="s">
+      <c r="G60" s="23"/>
+      <c r="L60" s="23"/>
+      <c r="Q60" s="23"/>
+    </row>
+    <row r="61" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B61" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C61" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="D60" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="15" t="s">
+      <c r="D61" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="G60" s="24"/>
-      <c r="H60" s="15"/>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="24"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
-      <c r="O60" s="15"/>
-      <c r="P60" s="15"/>
-      <c r="Q60" s="24"/>
-      <c r="R60" s="15" t="s">
+      <c r="G61" s="24"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="24"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
+      <c r="Q61" s="24"/>
+      <c r="R61" s="15" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="7" t="s">
+    <row r="62" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C62" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F61" s="7" t="s">
+      <c r="D62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="G61" s="23"/>
-      <c r="L61" s="23"/>
-      <c r="Q61" s="23"/>
-      <c r="R61" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D62" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="G62" s="23"/>
       <c r="L62" s="23"/>
       <c r="Q62" s="23"/>
       <c r="R62" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D63" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G63" s="23"/>
+      <c r="L63" s="23"/>
+      <c r="Q63" s="23"/>
+      <c r="R63" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="63" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A63" s="31" t="s">
+    <row r="64" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A64" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="B63" s="31" t="s">
+      <c r="B64" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="31" t="s">
+      <c r="C64" s="31" t="s">
         <v>319</v>
       </c>
-      <c r="D63" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G63" s="29"/>
-      <c r="H63" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="I63" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="J63" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="K63" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="L63" s="29"/>
-      <c r="M63" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="N63" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="O63" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="P63" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q63" s="29"/>
-    </row>
-    <row r="64" spans="1:18" s="42" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="42" t="s">
+      <c r="D64" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G64" s="29"/>
+      <c r="H64" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I64" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="J64" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K64" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L64" s="29"/>
+      <c r="M64" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="N64" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="O64" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P64" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q64" s="29"/>
+    </row>
+    <row r="65" spans="1:18" s="42" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="B64" s="42" t="s">
+      <c r="B65" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C64" s="42" t="s">
+      <c r="C65" s="42" t="s">
         <v>353</v>
       </c>
-      <c r="D64" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="42" t="s">
+      <c r="D65" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="G64" s="29"/>
-      <c r="L64" s="29"/>
-      <c r="Q64" s="29"/>
-    </row>
-    <row r="65" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A65" s="7" t="s">
+      <c r="G65" s="29"/>
+      <c r="L65" s="29"/>
+      <c r="Q65" s="29"/>
+    </row>
+    <row r="66" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A66" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B66" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C66" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D65" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E65" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" s="7" t="s">
+      <c r="D66" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G65" s="23"/>
-      <c r="L65" s="23"/>
-      <c r="Q65" s="23"/>
-      <c r="R65" s="7" t="s">
+      <c r="G66" s="23"/>
+      <c r="L66" s="23"/>
+      <c r="Q66" s="23"/>
+      <c r="R66" s="7" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="66" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G66" s="23"/>
-      <c r="H66" s="2" t="s">
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" s="23"/>
+      <c r="H67" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="I66" s="17" t="s">
+      <c r="I67" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="J66" s="17" t="s">
+      <c r="J67" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="K66" s="17" t="s">
+      <c r="K67" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="L66" s="23"/>
-      <c r="M66" s="17" t="s">
+      <c r="L67" s="23"/>
+      <c r="M67" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="N66" s="17" t="s">
+      <c r="N67" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="O66" s="17" t="s">
+      <c r="O67" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="P66" s="17" t="s">
+      <c r="P67" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="Q66" s="23"/>
-      <c r="R66" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A67" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="G67" s="23"/>
-      <c r="L67" s="23"/>
-      <c r="M67" s="17"/>
-      <c r="N67" s="17"/>
-      <c r="O67" s="17"/>
-      <c r="P67" s="17"/>
       <c r="Q67" s="23"/>
       <c r="R67" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>189</v>
+        <v>10</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
       <c r="D68" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E68" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>213</v>
+        <v>278</v>
       </c>
       <c r="G68" s="23"/>
       <c r="L68" s="23"/>
@@ -3666,167 +3689,170 @@
       <c r="O68" s="17"/>
       <c r="P68" s="17"/>
       <c r="Q68" s="23"/>
-    </row>
-    <row r="69" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A69" s="27" t="s">
-        <v>310</v>
-      </c>
-      <c r="B69" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="27" t="s">
-        <v>311</v>
-      </c>
-      <c r="D69" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="27" t="s">
-        <v>312</v>
+      <c r="R68" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="G69" s="23"/>
       <c r="L69" s="23"/>
+      <c r="M69" s="17"/>
+      <c r="N69" s="17"/>
+      <c r="O69" s="17"/>
+      <c r="P69" s="17"/>
       <c r="Q69" s="23"/>
-      <c r="R69" s="27" t="s">
+    </row>
+    <row r="70" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A70" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B70" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="D70" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="G70" s="23"/>
+      <c r="L70" s="23"/>
+      <c r="Q70" s="23"/>
+      <c r="R70" s="27" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="70" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D70" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G70" s="23"/>
-      <c r="H70" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="I70" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="J70" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="K70" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="L70" s="23"/>
-      <c r="M70" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="N70" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="O70" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="P70" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q70" s="23"/>
-    </row>
-    <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A71" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D71" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71" s="23"/>
+      <c r="H71" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="I71" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="J71" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="K71" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="L71" s="23"/>
+      <c r="M71" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="N71" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="O71" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="P71" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q71" s="23"/>
+    </row>
+    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="D71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G71" s="23"/>
-      <c r="L71" s="23"/>
-      <c r="M71" s="17"/>
-      <c r="N71" s="17"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="17"/>
-      <c r="Q71" s="23"/>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
+      <c r="D72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G72" s="23"/>
+      <c r="L72" s="23"/>
+      <c r="M72" s="17"/>
+      <c r="N72" s="17"/>
+      <c r="O72" s="17"/>
+      <c r="P72" s="17"/>
+      <c r="Q72" s="23"/>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
         <v>72</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>5</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>73</v>
       </c>
-      <c r="D72" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" t="b">
-        <v>0</v>
-      </c>
-      <c r="F72" t="s">
-        <v>4</v>
-      </c>
-      <c r="R72"/>
-    </row>
-    <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G73" s="23"/>
-      <c r="L73" s="23"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
-      <c r="Q73" s="23"/>
+      <c r="D73" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R73"/>
     </row>
     <row r="74" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>74</v>
+        <v>232</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>75</v>
+        <v>246</v>
       </c>
       <c r="D74" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G74" s="23"/>
       <c r="L74" s="23"/>
@@ -3836,454 +3862,447 @@
       <c r="P74" s="17"/>
       <c r="Q74" s="23"/>
     </row>
-    <row r="75" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G75" s="23"/>
+      <c r="L75" s="23"/>
+      <c r="M75" s="17"/>
+      <c r="N75" s="17"/>
+      <c r="O75" s="17"/>
+      <c r="P75" s="17"/>
+      <c r="Q75" s="23"/>
+    </row>
+    <row r="76" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D75" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G75" s="23"/>
-      <c r="H75" s="17" t="s">
+      <c r="D76" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" s="23"/>
+      <c r="H76" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="I75" s="17" t="s">
+      <c r="I76" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="J75" s="17" t="s">
+      <c r="J76" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="K75" s="17" t="s">
+      <c r="K76" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="L75" s="23"/>
-      <c r="M75" s="17" t="s">
+      <c r="L76" s="23"/>
+      <c r="M76" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="N75" s="17" t="s">
+      <c r="N76" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="O75" s="17" t="s">
+      <c r="O76" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="P75" s="17" t="s">
+      <c r="P76" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="Q75" s="23"/>
-    </row>
-    <row r="76" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A76" s="2" t="s">
+      <c r="Q76" s="23"/>
+    </row>
+    <row r="77" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="2" t="s">
+      <c r="D77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="G76" s="23"/>
-      <c r="L76" s="23"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="17"/>
-      <c r="Q76" s="23"/>
-    </row>
-    <row r="77" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D77" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>272</v>
       </c>
       <c r="G77" s="23"/>
       <c r="L77" s="23"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
+      <c r="P77" s="17"/>
       <c r="Q77" s="23"/>
-      <c r="R77" s="7" t="s">
+    </row>
+    <row r="78" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D78" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="G78" s="23"/>
+      <c r="L78" s="23"/>
+      <c r="Q78" s="23"/>
+      <c r="R78" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
+    <row r="79" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" s="2" t="s">
+      <c r="D79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="G78" s="23"/>
-      <c r="H78" s="2" t="s">
+      <c r="G79" s="23"/>
+      <c r="H79" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L78" s="23"/>
-      <c r="M78" s="17" t="s">
+      <c r="L79" s="23"/>
+      <c r="M79" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N78" s="17" t="s">
+      <c r="N79" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O78" s="17" t="s">
+      <c r="O79" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P78" s="17" t="s">
+      <c r="P79" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q78" s="23"/>
-    </row>
-    <row r="79" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A79" s="7" t="s">
+      <c r="Q79" s="23"/>
+    </row>
+    <row r="80" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A80" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B80" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C80" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D79" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" s="7" t="s">
+      <c r="D80" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="G79" s="23"/>
-      <c r="L79" s="23"/>
-      <c r="Q79" s="23"/>
-      <c r="R79" s="8" t="s">
+      <c r="G80" s="23"/>
+      <c r="L80" s="23"/>
+      <c r="Q80" s="23"/>
+      <c r="R80" s="8" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G80" s="23"/>
-      <c r="H80" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="I80" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="J80" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="K80" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="L80" s="23"/>
-      <c r="M80" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="N80" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="O80" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="P80" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q80" s="23"/>
     </row>
     <row r="81" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81" s="23"/>
+      <c r="H81" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="I81" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="J81" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="K81" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="L81" s="23"/>
+      <c r="M81" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="N81" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="O81" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="P81" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q81" s="23"/>
+    </row>
+    <row r="82" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="2" t="s">
+      <c r="D82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G81" s="23"/>
-      <c r="L81" s="23"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
-      <c r="Q81" s="23"/>
-    </row>
-    <row r="82" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A82" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D82" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="G82" s="23"/>
       <c r="L82" s="23"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="17"/>
       <c r="Q82" s="23"/>
-      <c r="R82" s="8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="83" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A83" s="7" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="D83" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E83" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="G83" s="23"/>
       <c r="L83" s="23"/>
       <c r="Q83" s="23"/>
-      <c r="R83" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>94</v>
+      <c r="R83" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A84" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D84" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G84" s="23"/>
       <c r="L84" s="23"/>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
-      <c r="P84" s="17"/>
       <c r="Q84" s="23"/>
-    </row>
-    <row r="85" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A85" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="B85" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="D85" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E85" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="17" t="s">
-        <v>4</v>
+      <c r="R84" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G85" s="23"/>
       <c r="L85" s="23"/>
+      <c r="M85" s="17"/>
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="17"/>
       <c r="Q85" s="23"/>
     </row>
-    <row r="86" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="7" t="s">
+    <row r="86" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A86" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="D86" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G86" s="23"/>
+      <c r="L86" s="23"/>
+      <c r="Q86" s="23"/>
+    </row>
+    <row r="87" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="B86" s="19"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E86" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G86" s="23"/>
-      <c r="H86" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I86" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J86" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K86" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L86" s="23"/>
-      <c r="M86" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N86" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O86" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P86" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q86" s="23"/>
-    </row>
-    <row r="87" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A87" s="20" t="s">
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G87" s="23"/>
+      <c r="H87" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I87" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J87" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K87" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L87" s="23"/>
+      <c r="M87" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N87" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O87" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P87" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q87" s="23"/>
+    </row>
+    <row r="88" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A88" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="B87" s="20" t="s">
+      <c r="B88" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C87" s="20" t="s">
+      <c r="C88" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="D87" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G87" s="23"/>
-      <c r="L87" s="23"/>
-      <c r="Q87" s="23"/>
-    </row>
-    <row r="88" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>4</v>
+      <c r="D88" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G88" s="23"/>
       <c r="L88" s="23"/>
-      <c r="M88" s="17"/>
-      <c r="N88" s="17"/>
-      <c r="O88" s="17"/>
-      <c r="P88" s="17"/>
       <c r="Q88" s="23"/>
-      <c r="R88" s="8" t="s">
-        <v>217</v>
-      </c>
     </row>
     <row r="89" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D89" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>328</v>
+        <v>4</v>
       </c>
       <c r="G89" s="23"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="17"/>
-      <c r="J89" s="17"/>
-      <c r="K89" s="17"/>
       <c r="L89" s="23"/>
       <c r="M89" s="17"/>
       <c r="N89" s="17"/>
@@ -4291,238 +4310,248 @@
       <c r="P89" s="17"/>
       <c r="Q89" s="23"/>
       <c r="R89" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G90" s="23"/>
+      <c r="H90" s="17"/>
+      <c r="I90" s="17"/>
+      <c r="J90" s="17"/>
+      <c r="K90" s="17"/>
+      <c r="L90" s="23"/>
+      <c r="M90" s="17"/>
+      <c r="N90" s="17"/>
+      <c r="O90" s="17"/>
+      <c r="P90" s="17"/>
+      <c r="Q90" s="23"/>
+      <c r="R90" s="8" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A90" t="s">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
         <v>197</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>198</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>199</v>
       </c>
-      <c r="D90" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" t="b">
-        <v>1</v>
-      </c>
-      <c r="M90" s="28" t="s">
+      <c r="D91" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" t="b">
+        <v>1</v>
+      </c>
+      <c r="M91" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="N90" s="28" t="s">
+      <c r="N91" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="O90" s="28" t="s">
+      <c r="O91" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="P90" s="28" t="s">
+      <c r="P91" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="R90"/>
-    </row>
-    <row r="91" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="13" t="s">
+      <c r="R91"/>
+    </row>
+    <row r="92" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="B91" s="13" t="s">
+      <c r="B92" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C92" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="D91" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="6" t="s">
+      <c r="D92" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="G91" s="26"/>
-      <c r="L91" s="23"/>
-      <c r="M91" s="17"/>
-      <c r="N91" s="17"/>
-      <c r="O91" s="17"/>
-      <c r="P91" s="17"/>
-      <c r="Q91" s="23"/>
-    </row>
-    <row r="92" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="28" t="s">
+      <c r="G92" s="26"/>
+      <c r="L92" s="23"/>
+      <c r="M92" s="17"/>
+      <c r="N92" s="17"/>
+      <c r="O92" s="17"/>
+      <c r="P92" s="17"/>
+      <c r="Q92" s="23"/>
+    </row>
+    <row r="93" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="B92" s="28" t="s">
+      <c r="B93" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C92" s="28" t="s">
+      <c r="C93" s="28" t="s">
         <v>340</v>
       </c>
-      <c r="D92" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E92" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="28" t="s">
+      <c r="D93" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="28" t="s">
         <v>272</v>
-      </c>
-      <c r="G92" s="23"/>
-      <c r="L92" s="23"/>
-      <c r="Q92" s="23"/>
-      <c r="R92" s="7" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D93" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G93" s="23"/>
       <c r="L93" s="23"/>
-      <c r="M93" s="17"/>
-      <c r="N93" s="17"/>
-      <c r="O93" s="17"/>
-      <c r="P93" s="17"/>
       <c r="Q93" s="23"/>
-    </row>
-    <row r="94" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="28" t="s">
+      <c r="R93" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D94" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94" s="23"/>
+      <c r="L94" s="23"/>
+      <c r="M94" s="17"/>
+      <c r="N94" s="17"/>
+      <c r="O94" s="17"/>
+      <c r="P94" s="17"/>
+      <c r="Q94" s="23"/>
+    </row>
+    <row r="95" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="28" t="s">
         <v>337</v>
       </c>
-      <c r="B94" s="28" t="s">
+      <c r="B95" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C94" s="28" t="s">
+      <c r="C95" s="28" t="s">
         <v>339</v>
       </c>
-      <c r="D94" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="28" t="s">
+      <c r="D95" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="G94" s="29"/>
-      <c r="L94" s="29"/>
-      <c r="Q94" s="29"/>
-      <c r="R94" s="7" t="s">
+      <c r="G95" s="29"/>
+      <c r="L95" s="29"/>
+      <c r="Q95" s="29"/>
+      <c r="R95" s="7" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="95" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A95" s="2" t="s">
+    <row r="96" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A96" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D95" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="6" t="s">
+      <c r="D96" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="G95" s="26"/>
-      <c r="L95" s="23"/>
-      <c r="M95" s="17"/>
-      <c r="N95" s="17"/>
-      <c r="O95" s="17"/>
-      <c r="P95" s="17"/>
-      <c r="Q95" s="23"/>
-      <c r="R95" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A96" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="B96" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="D96" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" s="6"/>
       <c r="G96" s="26"/>
       <c r="L96" s="23"/>
+      <c r="M96" s="17"/>
+      <c r="N96" s="17"/>
+      <c r="O96" s="17"/>
+      <c r="P96" s="17"/>
       <c r="Q96" s="23"/>
-    </row>
-    <row r="97" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A97" s="2" t="s">
+      <c r="R96" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A97" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B97" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="D97" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="6"/>
+      <c r="G97" s="26"/>
+      <c r="L97" s="23"/>
+      <c r="Q97" s="23"/>
+    </row>
+    <row r="98" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D97" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G97" s="23"/>
-      <c r="L97" s="23"/>
-      <c r="M97" s="17"/>
-      <c r="N97" s="17"/>
-      <c r="O97" s="17"/>
-      <c r="P97" s="17"/>
-      <c r="Q97" s="23"/>
-    </row>
-    <row r="98" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>201</v>
+        <v>103</v>
       </c>
       <c r="D98" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E98" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G98" s="23"/>
       <c r="L98" s="23"/>
@@ -4531,28 +4560,22 @@
       <c r="O98" s="17"/>
       <c r="P98" s="17"/>
       <c r="Q98" s="23"/>
-      <c r="R98" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="99" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="D99" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="G99" s="23"/>
       <c r="L99" s="23"/>
@@ -4562,91 +4585,95 @@
       <c r="P99" s="17"/>
       <c r="Q99" s="23"/>
       <c r="R99" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A100" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D100" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G100" s="23"/>
+      <c r="L100" s="23"/>
+      <c r="M100" s="17"/>
+      <c r="N100" s="17"/>
+      <c r="O100" s="17"/>
+      <c r="P100" s="17"/>
+      <c r="Q100" s="23"/>
+      <c r="R100" s="8" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="100" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A100" s="2" t="s">
+    <row r="101" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A101" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G100" s="23"/>
-      <c r="H100" s="17" t="s">
+      <c r="D101" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G101" s="23"/>
+      <c r="H101" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="I100" s="17" t="s">
+      <c r="I101" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="J100" s="17" t="s">
+      <c r="J101" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="K100" s="17" t="s">
+      <c r="K101" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="L100" s="23"/>
-      <c r="M100" s="17" t="s">
+      <c r="L101" s="23"/>
+      <c r="M101" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="N100" s="17" t="s">
+      <c r="N101" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="O100" s="17" t="s">
+      <c r="O101" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="P100" s="17" t="s">
+      <c r="P101" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="Q100" s="23"/>
-      <c r="R100" s="2" t="s">
+      <c r="Q101" s="23"/>
+      <c r="R101" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="101" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A101" s="7" t="s">
+    <row r="102" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A102" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B102" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C101" s="7" t="s">
+      <c r="C102" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="D101" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E101" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F101" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="G101" s="23"/>
-      <c r="L101" s="23"/>
-      <c r="Q101" s="23"/>
-      <c r="R101" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="D102" s="7" t="b">
         <v>1</v>
@@ -4661,91 +4688,73 @@
       <c r="L102" s="23"/>
       <c r="Q102" s="23"/>
       <c r="R102" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="103" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D103" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E103" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="G103" s="23"/>
       <c r="L103" s="23"/>
       <c r="Q103" s="23"/>
       <c r="R103" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D104" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G104" s="23"/>
+      <c r="L104" s="23"/>
+      <c r="Q104" s="23"/>
+      <c r="R104" s="7" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="104" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D104" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E104" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G104" s="23"/>
-      <c r="H104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L104" s="23"/>
-      <c r="M104" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N104" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O104" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P104" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q104" s="23"/>
     </row>
     <row r="105" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>285</v>
+        <v>117</v>
       </c>
       <c r="D105" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105" s="2" t="b">
         <v>1</v>
@@ -4780,23 +4789,23 @@
     </row>
     <row r="106" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>120</v>
+        <v>285</v>
       </c>
       <c r="D106" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G106" s="23"/>
       <c r="H106" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>4</v>
@@ -4809,7 +4818,7 @@
       </c>
       <c r="L106" s="23"/>
       <c r="M106" s="17" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N106" s="17" t="s">
         <v>4</v>
@@ -4822,178 +4831,177 @@
       </c>
       <c r="Q106" s="23"/>
     </row>
-    <row r="107" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="B107" s="28" t="s">
+    <row r="107" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C107" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="D107" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E107" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F107" s="28"/>
+      <c r="C107" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D107" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="G107" s="23"/>
-      <c r="H107" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I107" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J107" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K107" s="28" t="s">
+      <c r="H107" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K107" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L107" s="23"/>
-      <c r="M107" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N107" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O107" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P107" s="28" t="s">
+      <c r="M107" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N107" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O107" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P107" s="17" t="s">
         <v>4</v>
       </c>
       <c r="Q107" s="23"/>
-      <c r="R107" s="28" t="s">
-        <v>286</v>
-      </c>
     </row>
     <row r="108" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="28" t="s">
-        <v>341</v>
+        <v>149</v>
       </c>
       <c r="B108" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D108" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F108" s="28"/>
+      <c r="G108" s="23"/>
+      <c r="H108" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I108" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J108" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K108" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L108" s="23"/>
+      <c r="M108" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N108" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O108" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P108" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q108" s="23"/>
+      <c r="R108" s="28" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="B109" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="28" t="s">
         <v>342</v>
       </c>
-      <c r="D108" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E108" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F108" s="28"/>
-      <c r="G108" s="29"/>
-      <c r="H108" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I108" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J108" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K108" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L108" s="29"/>
-      <c r="M108" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N108" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O108" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P108" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q108" s="29"/>
-      <c r="R108" s="28" t="s">
+      <c r="D109" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E109" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" s="28"/>
+      <c r="G109" s="29"/>
+      <c r="H109" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I109" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J109" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K109" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L109" s="29"/>
+      <c r="M109" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N109" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O109" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P109" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q109" s="29"/>
+      <c r="R109" s="28" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A109" t="s">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A110" t="s">
         <v>121</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>122</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C110" t="s">
         <v>123</v>
       </c>
-      <c r="D109" t="b">
-        <v>1</v>
-      </c>
-      <c r="E109" t="b">
-        <v>0</v>
-      </c>
-      <c r="H109" s="16" t="s">
+      <c r="D110" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" t="b">
+        <v>0</v>
+      </c>
+      <c r="H110" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="I109" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J109" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K109" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L109" s="23"/>
-      <c r="M109" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="N109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q109" s="23"/>
-      <c r="R109"/>
-    </row>
-    <row r="110" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D110" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G110" s="23"/>
-      <c r="H110" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K110" s="2" t="s">
+      <c r="I110" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J110" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K110" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L110" s="23"/>
       <c r="M110" s="17" t="s">
-        <v>14</v>
+        <v>287</v>
       </c>
       <c r="N110" s="17" t="s">
         <v>4</v>
@@ -5005,19 +5013,17 @@
         <v>4</v>
       </c>
       <c r="Q110" s="23"/>
-      <c r="R110" s="2" t="s">
-        <v>202</v>
-      </c>
+      <c r="R110"/>
     </row>
     <row r="111" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
-        <v>258</v>
+        <v>124</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D111" s="2" t="b">
         <v>1</v>
@@ -5052,147 +5058,191 @@
         <v>4</v>
       </c>
       <c r="Q111" s="23"/>
+      <c r="R111" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="112" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
-        <v>127</v>
+        <v>258</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D112" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E112" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G112" s="23"/>
-      <c r="H112" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="I112" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="J112" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="K112" s="17" t="s">
-        <v>272</v>
+      <c r="H112" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K112" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L112" s="23"/>
       <c r="M112" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q112" s="23"/>
+    </row>
+    <row r="113" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D113" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G113" s="23"/>
+      <c r="H113" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="N112" s="17" t="s">
+      <c r="I113" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="O112" s="17" t="s">
+      <c r="J113" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="P112" s="17" t="s">
+      <c r="K113" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="Q112" s="23"/>
-    </row>
-    <row r="113" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="43" t="s">
+      <c r="L113" s="23"/>
+      <c r="M113" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="N113" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="O113" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="P113" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q113" s="23"/>
+    </row>
+    <row r="114" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="43" t="s">
         <v>356</v>
       </c>
-      <c r="B113" s="43" t="s">
+      <c r="B114" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C113" s="43" t="s">
+      <c r="C114" s="43" t="s">
         <v>357</v>
       </c>
-      <c r="D113" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="G113" s="29"/>
-      <c r="H113" s="43" t="s">
+      <c r="D114" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G114" s="29"/>
+      <c r="H114" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="I113" s="43" t="s">
+      <c r="I114" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="J113" s="43" t="s">
+      <c r="J114" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="K113" s="43" t="s">
+      <c r="K114" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="L113" s="29"/>
-      <c r="M113" s="43" t="s">
+      <c r="L114" s="29"/>
+      <c r="M114" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="N113" s="43" t="s">
+      <c r="N114" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="O113" s="43" t="s">
+      <c r="O114" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="P113" s="43" t="s">
+      <c r="P114" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="Q113" s="29"/>
-    </row>
-    <row r="114" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A114" s="30" t="s">
+      <c r="Q114" s="29"/>
+    </row>
+    <row r="115" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A115" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="B114" s="30" t="s">
+      <c r="B115" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C114" s="30" t="s">
+      <c r="C115" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="D114" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E114" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F114" s="30" t="s">
+      <c r="D115" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F115" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G114" s="29"/>
-      <c r="L114" s="29"/>
-      <c r="Q114" s="29"/>
-    </row>
-    <row r="115" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A115" s="2" t="s">
+      <c r="G115" s="29"/>
+      <c r="L115" s="29"/>
+      <c r="Q115" s="29"/>
+    </row>
+    <row r="116" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A116" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D115" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F115" s="2" t="s">
+      <c r="D116" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F116" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G115" s="23"/>
-      <c r="L115" s="23"/>
-      <c r="M115" s="17"/>
-      <c r="N115" s="17"/>
-      <c r="O115" s="17"/>
-      <c r="P115" s="17"/>
-      <c r="Q115" s="23"/>
-    </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R116"/>
+      <c r="G116" s="23"/>
+      <c r="L116" s="23"/>
+      <c r="M116" s="17"/>
+      <c r="N116" s="17"/>
+      <c r="O116" s="17"/>
+      <c r="P116" s="17"/>
+      <c r="Q116" s="23"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R117"/>
@@ -5256,6 +5306,9 @@
     </row>
     <row r="137" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R137"/>
+    </row>
+    <row r="138" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R138"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5263,15 +5316,15 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1"/>
     <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="F58" r:id="rId3"/>
+    <hyperlink ref="F59" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
Nativescalars property toegevoegd aan alle props
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="362">
   <si>
     <t>Name</t>
   </si>
@@ -1105,6 +1105,12 @@
   </si>
   <si>
     <t>Should an EA toolbox be generated?</t>
+  </si>
+  <si>
+    <t>nativescalars</t>
+  </si>
+  <si>
+    <t>Yes if scalar types may be entered without reference to a UML datatype</t>
   </si>
 </sst>
 </file>
@@ -1270,7 +1276,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1370,6 +1376,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1682,13 +1691,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R138"/>
+  <dimension ref="A1:R139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD26"/>
+      <selection pane="bottomRight" activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1899,16 +1908,16 @@
       <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="45" t="b">
+      <c r="D7" s="46" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1926,10 +1935,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
       <c r="G8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
@@ -3024,16 +3033,16 @@
       </c>
     </row>
     <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="45" t="s">
+      <c r="B45" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="45" t="s">
+      <c r="C45" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="45" t="b">
+      <c r="D45" s="46" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="2" t="b">
@@ -3051,10 +3060,10 @@
       <c r="Q45" s="23"/>
     </row>
     <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="45"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
       <c r="G46" s="23"/>
       <c r="L46" s="23"/>
       <c r="M46" s="17"/>
@@ -3835,51 +3844,47 @@
       </c>
       <c r="R73"/>
     </row>
-    <row r="74" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A74" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B74" s="2" t="s">
+    <row r="74" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A74" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="B74" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D74" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E74" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G74" s="23"/>
-      <c r="L74" s="23"/>
-      <c r="M74" s="17"/>
-      <c r="N74" s="17"/>
-      <c r="O74" s="17"/>
-      <c r="P74" s="17"/>
-      <c r="Q74" s="23"/>
+      <c r="C74" s="34" t="s">
+        <v>361</v>
+      </c>
+      <c r="D74" s="45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G74" s="29"/>
+      <c r="L74" s="29"/>
+      <c r="Q74" s="29"/>
     </row>
     <row r="75" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>74</v>
+        <v>232</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>75</v>
+        <v>246</v>
       </c>
       <c r="D75" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E75" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G75" s="23"/>
       <c r="L75" s="23"/>
@@ -3889,454 +3894,447 @@
       <c r="P75" s="17"/>
       <c r="Q75" s="23"/>
     </row>
-    <row r="76" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" s="23"/>
+      <c r="L76" s="23"/>
+      <c r="M76" s="17"/>
+      <c r="N76" s="17"/>
+      <c r="O76" s="17"/>
+      <c r="P76" s="17"/>
+      <c r="Q76" s="23"/>
+    </row>
+    <row r="77" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D76" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G76" s="23"/>
-      <c r="H76" s="17" t="s">
+      <c r="D77" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" s="23"/>
+      <c r="H77" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="I76" s="17" t="s">
+      <c r="I77" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="J76" s="17" t="s">
+      <c r="J77" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="K76" s="17" t="s">
+      <c r="K77" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="L76" s="23"/>
-      <c r="M76" s="17" t="s">
+      <c r="L77" s="23"/>
+      <c r="M77" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="N76" s="17" t="s">
+      <c r="N77" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="O76" s="17" t="s">
+      <c r="O77" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="P76" s="17" t="s">
+      <c r="P77" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="Q76" s="23"/>
-    </row>
-    <row r="77" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A77" s="2" t="s">
+      <c r="Q77" s="23"/>
+    </row>
+    <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D77" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F77" s="2" t="s">
+      <c r="D78" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="G77" s="23"/>
-      <c r="L77" s="23"/>
-      <c r="M77" s="17"/>
-      <c r="N77" s="17"/>
-      <c r="O77" s="17"/>
-      <c r="P77" s="17"/>
-      <c r="Q77" s="23"/>
-    </row>
-    <row r="78" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D78" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E78" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>272</v>
       </c>
       <c r="G78" s="23"/>
       <c r="L78" s="23"/>
+      <c r="M78" s="17"/>
+      <c r="N78" s="17"/>
+      <c r="O78" s="17"/>
+      <c r="P78" s="17"/>
       <c r="Q78" s="23"/>
-      <c r="R78" s="7" t="s">
+    </row>
+    <row r="79" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D79" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="G79" s="23"/>
+      <c r="L79" s="23"/>
+      <c r="Q79" s="23"/>
+      <c r="R79" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="79" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A79" s="2" t="s">
+    <row r="80" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="2" t="s">
+      <c r="D80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="G79" s="23"/>
-      <c r="H79" s="2" t="s">
+      <c r="G80" s="23"/>
+      <c r="H80" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L79" s="23"/>
-      <c r="M79" s="17" t="s">
+      <c r="L80" s="23"/>
+      <c r="M80" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N79" s="17" t="s">
+      <c r="N80" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O79" s="17" t="s">
+      <c r="O80" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P79" s="17" t="s">
+      <c r="P80" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q79" s="23"/>
-    </row>
-    <row r="80" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A80" s="7" t="s">
+      <c r="Q80" s="23"/>
+    </row>
+    <row r="81" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A81" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B81" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C81" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D80" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="7" t="s">
+      <c r="D81" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="G80" s="23"/>
-      <c r="L80" s="23"/>
-      <c r="Q80" s="23"/>
-      <c r="R80" s="8" t="s">
+      <c r="G81" s="23"/>
+      <c r="L81" s="23"/>
+      <c r="Q81" s="23"/>
+      <c r="R81" s="8" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G81" s="23"/>
-      <c r="H81" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="I81" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="J81" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="K81" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="L81" s="23"/>
-      <c r="M81" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="N81" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="O81" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="P81" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q81" s="23"/>
     </row>
     <row r="82" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G82" s="23"/>
+      <c r="H82" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="I82" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="J82" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="K82" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="L82" s="23"/>
+      <c r="M82" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="N82" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="O82" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="P82" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q82" s="23"/>
+    </row>
+    <row r="83" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D82" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="2" t="s">
+      <c r="D83" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G82" s="23"/>
-      <c r="L82" s="23"/>
-      <c r="M82" s="17"/>
-      <c r="N82" s="17"/>
-      <c r="O82" s="17"/>
-      <c r="P82" s="17"/>
-      <c r="Q82" s="23"/>
-    </row>
-    <row r="83" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A83" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D83" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="G83" s="23"/>
       <c r="L83" s="23"/>
+      <c r="M83" s="17"/>
+      <c r="N83" s="17"/>
+      <c r="O83" s="17"/>
+      <c r="P83" s="17"/>
       <c r="Q83" s="23"/>
-      <c r="R83" s="8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="84" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A84" s="7" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="D84" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E84" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="G84" s="23"/>
       <c r="L84" s="23"/>
       <c r="Q84" s="23"/>
-      <c r="R84" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A85" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>94</v>
+      <c r="R84" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A85" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D85" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G85" s="23"/>
       <c r="L85" s="23"/>
-      <c r="M85" s="17"/>
-      <c r="N85" s="17"/>
-      <c r="O85" s="17"/>
-      <c r="P85" s="17"/>
       <c r="Q85" s="23"/>
-    </row>
-    <row r="86" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A86" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="B86" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="D86" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="17" t="s">
-        <v>4</v>
+      <c r="R85" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A86" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D86" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G86" s="23"/>
       <c r="L86" s="23"/>
+      <c r="M86" s="17"/>
+      <c r="N86" s="17"/>
+      <c r="O86" s="17"/>
+      <c r="P86" s="17"/>
       <c r="Q86" s="23"/>
     </row>
-    <row r="87" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="7" t="s">
+    <row r="87" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A87" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="B87" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="D87" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G87" s="23"/>
+      <c r="L87" s="23"/>
+      <c r="Q87" s="23"/>
+    </row>
+    <row r="88" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="B87" s="19"/>
-      <c r="C87" s="19"/>
-      <c r="D87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G87" s="23"/>
-      <c r="H87" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I87" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J87" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K87" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L87" s="23"/>
-      <c r="M87" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N87" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O87" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P87" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q87" s="23"/>
-    </row>
-    <row r="88" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A88" s="20" t="s">
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G88" s="23"/>
+      <c r="H88" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I88" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J88" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K88" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L88" s="23"/>
+      <c r="M88" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N88" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O88" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P88" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q88" s="23"/>
+    </row>
+    <row r="89" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A89" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="B88" s="20" t="s">
+      <c r="B89" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C88" s="20" t="s">
+      <c r="C89" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="D88" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G88" s="23"/>
-      <c r="L88" s="23"/>
-      <c r="Q88" s="23"/>
-    </row>
-    <row r="89" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D89" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>4</v>
+      <c r="D89" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G89" s="23"/>
       <c r="L89" s="23"/>
-      <c r="M89" s="17"/>
-      <c r="N89" s="17"/>
-      <c r="O89" s="17"/>
-      <c r="P89" s="17"/>
       <c r="Q89" s="23"/>
-      <c r="R89" s="8" t="s">
-        <v>217</v>
-      </c>
     </row>
     <row r="90" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D90" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>328</v>
+        <v>4</v>
       </c>
       <c r="G90" s="23"/>
-      <c r="H90" s="17"/>
-      <c r="I90" s="17"/>
-      <c r="J90" s="17"/>
-      <c r="K90" s="17"/>
       <c r="L90" s="23"/>
       <c r="M90" s="17"/>
       <c r="N90" s="17"/>
@@ -4344,238 +4342,248 @@
       <c r="P90" s="17"/>
       <c r="Q90" s="23"/>
       <c r="R90" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G91" s="23"/>
+      <c r="H91" s="17"/>
+      <c r="I91" s="17"/>
+      <c r="J91" s="17"/>
+      <c r="K91" s="17"/>
+      <c r="L91" s="23"/>
+      <c r="M91" s="17"/>
+      <c r="N91" s="17"/>
+      <c r="O91" s="17"/>
+      <c r="P91" s="17"/>
+      <c r="Q91" s="23"/>
+      <c r="R91" s="8" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A91" t="s">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
         <v>197</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>198</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
         <v>199</v>
       </c>
-      <c r="D91" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" t="b">
-        <v>1</v>
-      </c>
-      <c r="M91" s="28" t="s">
+      <c r="D92" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+      <c r="M92" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="N91" s="28" t="s">
+      <c r="N92" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="O91" s="28" t="s">
+      <c r="O92" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="P91" s="28" t="s">
+      <c r="P92" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="R91"/>
-    </row>
-    <row r="92" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A92" s="13" t="s">
+      <c r="R92"/>
+    </row>
+    <row r="93" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="B92" s="13" t="s">
+      <c r="B93" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C93" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="D92" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="6" t="s">
+      <c r="D93" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="G92" s="26"/>
-      <c r="L92" s="23"/>
-      <c r="M92" s="17"/>
-      <c r="N92" s="17"/>
-      <c r="O92" s="17"/>
-      <c r="P92" s="17"/>
-      <c r="Q92" s="23"/>
-    </row>
-    <row r="93" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="28" t="s">
+      <c r="G93" s="26"/>
+      <c r="L93" s="23"/>
+      <c r="M93" s="17"/>
+      <c r="N93" s="17"/>
+      <c r="O93" s="17"/>
+      <c r="P93" s="17"/>
+      <c r="Q93" s="23"/>
+    </row>
+    <row r="94" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="B93" s="28" t="s">
+      <c r="B94" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C93" s="28" t="s">
+      <c r="C94" s="28" t="s">
         <v>340</v>
       </c>
-      <c r="D93" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="28" t="s">
+      <c r="D94" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="28" t="s">
         <v>272</v>
-      </c>
-      <c r="G93" s="23"/>
-      <c r="L93" s="23"/>
-      <c r="Q93" s="23"/>
-      <c r="R93" s="7" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D94" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G94" s="23"/>
       <c r="L94" s="23"/>
-      <c r="M94" s="17"/>
-      <c r="N94" s="17"/>
-      <c r="O94" s="17"/>
-      <c r="P94" s="17"/>
       <c r="Q94" s="23"/>
-    </row>
-    <row r="95" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="28" t="s">
+      <c r="R94" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D95" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G95" s="23"/>
+      <c r="L95" s="23"/>
+      <c r="M95" s="17"/>
+      <c r="N95" s="17"/>
+      <c r="O95" s="17"/>
+      <c r="P95" s="17"/>
+      <c r="Q95" s="23"/>
+    </row>
+    <row r="96" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="28" t="s">
         <v>337</v>
       </c>
-      <c r="B95" s="28" t="s">
+      <c r="B96" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C95" s="28" t="s">
+      <c r="C96" s="28" t="s">
         <v>339</v>
       </c>
-      <c r="D95" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="28" t="s">
+      <c r="D96" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="G95" s="29"/>
-      <c r="L95" s="29"/>
-      <c r="Q95" s="29"/>
-      <c r="R95" s="7" t="s">
+      <c r="G96" s="29"/>
+      <c r="L96" s="29"/>
+      <c r="Q96" s="29"/>
+      <c r="R96" s="7" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="96" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" s="6" t="s">
+      <c r="D97" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="G96" s="26"/>
-      <c r="L96" s="23"/>
-      <c r="M96" s="17"/>
-      <c r="N96" s="17"/>
-      <c r="O96" s="17"/>
-      <c r="P96" s="17"/>
-      <c r="Q96" s="23"/>
-      <c r="R96" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A97" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="B97" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="D97" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="6"/>
       <c r="G97" s="26"/>
       <c r="L97" s="23"/>
+      <c r="M97" s="17"/>
+      <c r="N97" s="17"/>
+      <c r="O97" s="17"/>
+      <c r="P97" s="17"/>
       <c r="Q97" s="23"/>
-    </row>
-    <row r="98" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A98" s="2" t="s">
+      <c r="R97" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A98" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B98" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="D98" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="6"/>
+      <c r="G98" s="26"/>
+      <c r="L98" s="23"/>
+      <c r="Q98" s="23"/>
+    </row>
+    <row r="99" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A99" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D98" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G98" s="23"/>
-      <c r="L98" s="23"/>
-      <c r="M98" s="17"/>
-      <c r="N98" s="17"/>
-      <c r="O98" s="17"/>
-      <c r="P98" s="17"/>
-      <c r="Q98" s="23"/>
-    </row>
-    <row r="99" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>201</v>
+        <v>103</v>
       </c>
       <c r="D99" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E99" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G99" s="23"/>
       <c r="L99" s="23"/>
@@ -4584,28 +4592,22 @@
       <c r="O99" s="17"/>
       <c r="P99" s="17"/>
       <c r="Q99" s="23"/>
-      <c r="R99" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="100" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="D100" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="G100" s="23"/>
       <c r="L100" s="23"/>
@@ -4615,91 +4617,95 @@
       <c r="P100" s="17"/>
       <c r="Q100" s="23"/>
       <c r="R100" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A101" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D101" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G101" s="23"/>
+      <c r="L101" s="23"/>
+      <c r="M101" s="17"/>
+      <c r="N101" s="17"/>
+      <c r="O101" s="17"/>
+      <c r="P101" s="17"/>
+      <c r="Q101" s="23"/>
+      <c r="R101" s="8" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="101" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A101" s="2" t="s">
+    <row r="102" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D101" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E101" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G101" s="23"/>
-      <c r="H101" s="17" t="s">
+      <c r="D102" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G102" s="23"/>
+      <c r="H102" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="I101" s="17" t="s">
+      <c r="I102" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="J101" s="17" t="s">
+      <c r="J102" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="K101" s="17" t="s">
+      <c r="K102" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="L101" s="23"/>
-      <c r="M101" s="17" t="s">
+      <c r="L102" s="23"/>
+      <c r="M102" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="N101" s="17" t="s">
+      <c r="N102" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="O101" s="17" t="s">
+      <c r="O102" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="P101" s="17" t="s">
+      <c r="P102" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="Q101" s="23"/>
-      <c r="R101" s="2" t="s">
+      <c r="Q102" s="23"/>
+      <c r="R102" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="102" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A102" s="7" t="s">
+    <row r="103" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A103" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B103" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C102" s="7" t="s">
+      <c r="C103" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="D102" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="G102" s="23"/>
-      <c r="L102" s="23"/>
-      <c r="Q102" s="23"/>
-      <c r="R102" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B103" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="D103" s="7" t="b">
         <v>1</v>
@@ -4714,91 +4720,73 @@
       <c r="L103" s="23"/>
       <c r="Q103" s="23"/>
       <c r="R103" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="104" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D104" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E104" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="G104" s="23"/>
       <c r="L104" s="23"/>
       <c r="Q104" s="23"/>
       <c r="R104" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D105" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G105" s="23"/>
+      <c r="L105" s="23"/>
+      <c r="Q105" s="23"/>
+      <c r="R105" s="7" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="105" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D105" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E105" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G105" s="23"/>
-      <c r="H105" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I105" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J105" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K105" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L105" s="23"/>
-      <c r="M105" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N105" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O105" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P105" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q105" s="23"/>
     </row>
     <row r="106" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>285</v>
+        <v>117</v>
       </c>
       <c r="D106" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106" s="2" t="b">
         <v>1</v>
@@ -4833,23 +4821,23 @@
     </row>
     <row r="107" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>120</v>
+        <v>285</v>
       </c>
       <c r="D107" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G107" s="23"/>
       <c r="H107" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I107" s="2" t="s">
         <v>4</v>
@@ -4862,7 +4850,7 @@
       </c>
       <c r="L107" s="23"/>
       <c r="M107" s="17" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N107" s="17" t="s">
         <v>4</v>
@@ -4875,178 +4863,177 @@
       </c>
       <c r="Q107" s="23"/>
     </row>
-    <row r="108" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="B108" s="28" t="s">
+    <row r="108" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C108" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="D108" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E108" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F108" s="28"/>
+      <c r="C108" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D108" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="G108" s="23"/>
-      <c r="H108" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I108" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J108" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K108" s="28" t="s">
+      <c r="H108" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K108" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L108" s="23"/>
-      <c r="M108" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N108" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O108" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P108" s="28" t="s">
+      <c r="M108" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N108" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O108" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P108" s="17" t="s">
         <v>4</v>
       </c>
       <c r="Q108" s="23"/>
-      <c r="R108" s="28" t="s">
-        <v>286</v>
-      </c>
     </row>
     <row r="109" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="28" t="s">
-        <v>341</v>
+        <v>149</v>
       </c>
       <c r="B109" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C109" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D109" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E109" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" s="28"/>
+      <c r="G109" s="23"/>
+      <c r="H109" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I109" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J109" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K109" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L109" s="23"/>
+      <c r="M109" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N109" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O109" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P109" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q109" s="23"/>
+      <c r="R109" s="28" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="B110" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="28" t="s">
         <v>342</v>
       </c>
-      <c r="D109" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E109" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F109" s="28"/>
-      <c r="G109" s="29"/>
-      <c r="H109" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I109" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J109" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K109" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L109" s="29"/>
-      <c r="M109" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N109" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O109" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P109" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q109" s="29"/>
-      <c r="R109" s="28" t="s">
+      <c r="D110" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" s="28"/>
+      <c r="G110" s="29"/>
+      <c r="H110" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I110" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J110" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K110" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L110" s="29"/>
+      <c r="M110" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N110" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O110" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P110" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q110" s="29"/>
+      <c r="R110" s="28" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A110" t="s">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A111" t="s">
         <v>121</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>122</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>123</v>
       </c>
-      <c r="D110" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" t="b">
-        <v>0</v>
-      </c>
-      <c r="H110" s="16" t="s">
+      <c r="D111" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" t="b">
+        <v>0</v>
+      </c>
+      <c r="H111" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="I110" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J110" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K110" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L110" s="23"/>
-      <c r="M110" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="N110" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O110" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P110" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q110" s="23"/>
-      <c r="R110"/>
-    </row>
-    <row r="111" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D111" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G111" s="23"/>
-      <c r="H111" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K111" s="2" t="s">
+      <c r="I111" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J111" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K111" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L111" s="23"/>
       <c r="M111" s="17" t="s">
-        <v>14</v>
+        <v>287</v>
       </c>
       <c r="N111" s="17" t="s">
         <v>4</v>
@@ -5058,19 +5045,17 @@
         <v>4</v>
       </c>
       <c r="Q111" s="23"/>
-      <c r="R111" s="2" t="s">
-        <v>202</v>
-      </c>
+      <c r="R111"/>
     </row>
     <row r="112" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
-        <v>258</v>
+        <v>124</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D112" s="2" t="b">
         <v>1</v>
@@ -5105,147 +5090,191 @@
         <v>4</v>
       </c>
       <c r="Q112" s="23"/>
+      <c r="R112" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="113" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
-        <v>127</v>
+        <v>258</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D113" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E113" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G113" s="23"/>
-      <c r="H113" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="I113" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="J113" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="K113" s="17" t="s">
-        <v>272</v>
+      <c r="H113" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K113" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L113" s="23"/>
       <c r="M113" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N113" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O113" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P113" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q113" s="23"/>
+    </row>
+    <row r="114" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D114" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G114" s="23"/>
+      <c r="H114" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="N113" s="17" t="s">
+      <c r="I114" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="O113" s="17" t="s">
+      <c r="J114" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="P113" s="17" t="s">
+      <c r="K114" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="Q113" s="23"/>
-    </row>
-    <row r="114" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="43" t="s">
+      <c r="L114" s="23"/>
+      <c r="M114" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="N114" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="O114" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="P114" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q114" s="23"/>
+    </row>
+    <row r="115" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="43" t="s">
         <v>356</v>
       </c>
-      <c r="B114" s="43" t="s">
+      <c r="B115" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C114" s="43" t="s">
+      <c r="C115" s="43" t="s">
         <v>357</v>
       </c>
-      <c r="D114" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E114" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="G114" s="29"/>
-      <c r="H114" s="43" t="s">
+      <c r="D115" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G115" s="29"/>
+      <c r="H115" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="I114" s="43" t="s">
+      <c r="I115" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="J114" s="43" t="s">
+      <c r="J115" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="K114" s="43" t="s">
+      <c r="K115" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="L114" s="29"/>
-      <c r="M114" s="43" t="s">
+      <c r="L115" s="29"/>
+      <c r="M115" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="N114" s="43" t="s">
+      <c r="N115" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="O114" s="43" t="s">
+      <c r="O115" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="P114" s="43" t="s">
+      <c r="P115" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="Q114" s="29"/>
-    </row>
-    <row r="115" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A115" s="30" t="s">
+      <c r="Q115" s="29"/>
+    </row>
+    <row r="116" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A116" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="B115" s="30" t="s">
+      <c r="B116" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C115" s="30" t="s">
+      <c r="C116" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="D115" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F115" s="30" t="s">
+      <c r="D116" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G115" s="29"/>
-      <c r="L115" s="29"/>
-      <c r="Q115" s="29"/>
-    </row>
-    <row r="116" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A116" s="2" t="s">
+      <c r="G116" s="29"/>
+      <c r="L116" s="29"/>
+      <c r="Q116" s="29"/>
+    </row>
+    <row r="117" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A117" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B117" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D116" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F116" s="2" t="s">
+      <c r="D117" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F117" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G116" s="23"/>
-      <c r="L116" s="23"/>
-      <c r="M116" s="17"/>
-      <c r="N116" s="17"/>
-      <c r="O116" s="17"/>
-      <c r="P116" s="17"/>
-      <c r="Q116" s="23"/>
-    </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R117"/>
+      <c r="G117" s="23"/>
+      <c r="L117" s="23"/>
+      <c r="M117" s="17"/>
+      <c r="N117" s="17"/>
+      <c r="O117" s="17"/>
+      <c r="P117" s="17"/>
+      <c r="Q117" s="23"/>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R118"/>
@@ -5309,6 +5338,9 @@
     </row>
     <row r="138" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R138"/>
+    </row>
+    <row r="139" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R139"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Introductie nieuwe CLI createmimformat en mimformatname
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="366">
   <si>
     <t>Name</t>
   </si>
@@ -1111,6 +1111,18 @@
   </si>
   <si>
     <t>Yes if scalar types may be entered without reference to a UML datatype</t>
+  </si>
+  <si>
+    <t>mimformatname</t>
+  </si>
+  <si>
+    <t>The name of the MIM format file generated</t>
+  </si>
+  <si>
+    <t>createmimformat</t>
+  </si>
+  <si>
+    <t>Yes if MIM format must be generated</t>
   </si>
 </sst>
 </file>
@@ -1276,7 +1288,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1376,6 +1388,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1691,13 +1706,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R139"/>
+  <dimension ref="A1:R141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A74" sqref="A74:XFD74"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1908,16 +1923,16 @@
       <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="46" t="b">
+      <c r="D7" s="47" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1935,10 +1950,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
       <c r="G8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
@@ -2670,111 +2685,135 @@
         <v>324</v>
       </c>
     </row>
-    <row r="32" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="46" t="s">
+        <v>365</v>
+      </c>
+      <c r="D32" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="29"/>
+      <c r="H32" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="29"/>
+      <c r="M32" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="N32" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="O32" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="P32" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q32" s="29"/>
+    </row>
+    <row r="33" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" s="23"/>
-      <c r="H32" s="2" t="s">
+      <c r="D33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="23"/>
+      <c r="H33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I32" s="40" t="s">
+      <c r="I33" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="J32" s="40" t="s">
+      <c r="J33" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="40" t="s">
+      <c r="K33" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="L32" s="23"/>
-      <c r="M32" s="17" t="s">
+      <c r="L33" s="23"/>
+      <c r="M33" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N32" s="40" t="s">
+      <c r="N33" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="O32" s="40" t="s">
+      <c r="O33" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="P32" s="40" t="s">
+      <c r="P33" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="2" t="s">
+      <c r="Q33" s="23"/>
+      <c r="R33" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="33" spans="1:18" s="33" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A33" s="33" t="s">
+    <row r="34" spans="1:18" s="33" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A34" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B34" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="C33" s="33" t="s">
+      <c r="C34" s="33" t="s">
         <v>333</v>
       </c>
-      <c r="D33" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E33" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="G33" s="29"/>
-      <c r="I33" s="33" t="s">
+      <c r="D34" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" s="29"/>
+      <c r="I34" s="33" t="s">
         <v>334</v>
       </c>
-      <c r="J33" s="39" t="s">
+      <c r="J34" s="39" t="s">
         <v>334</v>
       </c>
-      <c r="K33" s="39" t="s">
+      <c r="K34" s="39" t="s">
         <v>334</v>
       </c>
-      <c r="L33" s="29"/>
-      <c r="Q33" s="29"/>
-    </row>
-    <row r="34" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A34" s="34" t="s">
+      <c r="L34" s="29"/>
+      <c r="Q34" s="29"/>
+    </row>
+    <row r="35" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A35" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B35" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C35" s="34" t="s">
         <v>167</v>
-      </c>
-      <c r="D34" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="G34" s="35"/>
-      <c r="L34" s="35"/>
-      <c r="Q34" s="35"/>
-    </row>
-    <row r="35" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>170</v>
       </c>
       <c r="D35" s="34" t="b">
         <v>0</v>
@@ -2788,22 +2827,19 @@
     </row>
     <row r="36" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="34" t="s">
-        <v>35</v>
+        <v>168</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>5</v>
+        <v>169</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="D36" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E36" s="34" t="b">
         <v>1</v>
-      </c>
-      <c r="F36" s="34" t="s">
-        <v>14</v>
       </c>
       <c r="G36" s="35"/>
       <c r="L36" s="35"/>
@@ -2811,13 +2847,13 @@
     </row>
     <row r="37" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="34" t="s">
-        <v>335</v>
+        <v>35</v>
       </c>
       <c r="B37" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>336</v>
+        <v>36</v>
       </c>
       <c r="D37" s="34" t="b">
         <v>0</v>
@@ -2829,241 +2865,251 @@
         <v>14</v>
       </c>
       <c r="G37" s="35"/>
-      <c r="H37" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="I37" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="J37" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="K37" s="34" t="s">
-        <v>4</v>
-      </c>
       <c r="L37" s="35"/>
       <c r="Q37" s="35"/>
     </row>
-    <row r="38" spans="1:18" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A38" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="36" t="s">
+    <row r="38" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="B38" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="36" t="s">
+      <c r="C38" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="D38" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="35"/>
+      <c r="H38" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="J38" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="K38" s="34" t="s">
+        <v>4</v>
+      </c>
       <c r="L38" s="35"/>
       <c r="Q38" s="35"/>
     </row>
-    <row r="39" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A39" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="34" t="s">
+    <row r="39" spans="1:18" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A39" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="F39" s="34" t="s">
+      <c r="C39" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="36" t="s">
         <v>14</v>
       </c>
       <c r="G39" s="35"/>
       <c r="L39" s="35"/>
       <c r="Q39" s="35"/>
     </row>
-    <row r="40" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="36" t="s">
+    <row r="40" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A40" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="36" t="b">
-        <v>1</v>
+      <c r="C40" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>14</v>
       </c>
       <c r="G40" s="35"/>
-      <c r="H40" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="K40" s="36" t="s">
-        <v>14</v>
-      </c>
       <c r="L40" s="35"/>
-      <c r="M40" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="N40" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="O40" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="P40" s="36" t="s">
-        <v>4</v>
-      </c>
       <c r="Q40" s="35"/>
     </row>
     <row r="41" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="35"/>
+      <c r="H41" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L41" s="35"/>
+      <c r="M41" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="N41" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="O41" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="P41" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q41" s="35"/>
+    </row>
+    <row r="42" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="36" t="s">
         <v>325</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="B42" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C42" s="36" t="s">
         <v>326</v>
       </c>
-      <c r="D41" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="36" t="s">
+      <c r="D42" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" s="36" t="s">
         <v>329</v>
-      </c>
-      <c r="G41" s="35"/>
-      <c r="L41" s="35"/>
-      <c r="Q41" s="35"/>
-    </row>
-    <row r="42" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="D42" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" s="34" t="s">
-        <v>14</v>
       </c>
       <c r="G42" s="35"/>
       <c r="L42" s="35"/>
       <c r="Q42" s="35"/>
     </row>
-    <row r="43" spans="1:18" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A43" s="37" t="s">
+    <row r="43" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D43" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="Q43" s="35"/>
+    </row>
+    <row r="44" spans="1:18" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A44" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B44" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="37" t="s">
+      <c r="C44" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D43" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="F43" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" s="38"/>
-      <c r="L43" s="38"/>
-      <c r="Q43" s="38"/>
-      <c r="R43" s="37" t="s">
+      <c r="D44" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="38"/>
+      <c r="L44" s="38"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="37" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="44" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A44" s="7" t="s">
+    <row r="45" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B45" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C45" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F44" s="7" t="s">
+      <c r="D45" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="G44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="7" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G45" s="23"/>
       <c r="L45" s="23"/>
-      <c r="M45" s="17"/>
-      <c r="N45" s="17"/>
-      <c r="O45" s="17"/>
-      <c r="P45" s="17"/>
       <c r="Q45" s="23"/>
+      <c r="R45" s="7" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
+      <c r="A46" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G46" s="23"/>
       <c r="L46" s="23"/>
       <c r="M46" s="17"/>
@@ -3072,22 +3118,11 @@
       <c r="P46" s="17"/>
       <c r="Q46" s="23"/>
     </row>
-    <row r="47" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A47" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D47" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="47"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
       <c r="G47" s="23"/>
       <c r="L47" s="23"/>
       <c r="M47" s="17"/>
@@ -3096,21 +3131,21 @@
       <c r="P47" s="17"/>
       <c r="Q47" s="23"/>
     </row>
-    <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
-        <v>50</v>
+        <v>173</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>51</v>
+        <v>175</v>
       </c>
       <c r="D48" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" s="23"/>
       <c r="L48" s="23"/>
@@ -3120,15 +3155,15 @@
       <c r="P48" s="17"/>
       <c r="Q48" s="23"/>
     </row>
-    <row r="49" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D49" s="2" t="b">
         <v>0</v>
@@ -3136,95 +3171,95 @@
       <c r="E49" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F49" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="G49" s="26"/>
+      <c r="G49" s="23"/>
       <c r="L49" s="23"/>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
       <c r="O49" s="17"/>
       <c r="P49" s="17"/>
       <c r="Q49" s="23"/>
-      <c r="R49" s="2" t="s">
+    </row>
+    <row r="50" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G50" s="26"/>
+      <c r="L50" s="23"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+      <c r="Q50" s="23"/>
+      <c r="R50" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E50" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F50" s="6"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="17" t="s">
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="I50" s="17" t="s">
+      <c r="I51" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="J50" s="17" t="s">
+      <c r="J51" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="K50" s="17" t="s">
+      <c r="K51" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="L50" s="23"/>
-      <c r="M50" s="17" t="s">
+      <c r="L51" s="23"/>
+      <c r="M51" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="N50" s="17" t="s">
+      <c r="N51" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="O50" s="17" t="s">
+      <c r="O51" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="P50" s="17" t="s">
+      <c r="P51" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="Q50" s="23"/>
-    </row>
-    <row r="51" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="7" t="s">
+      <c r="Q51" s="23"/>
+    </row>
+    <row r="52" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B52" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C52" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D51" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G51" s="23"/>
-      <c r="L51" s="23"/>
-      <c r="Q51" s="23"/>
-      <c r="R51"/>
-    </row>
-    <row r="52" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A52" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="D52" s="7" t="b">
         <v>0</v>
       </c>
@@ -3232,77 +3267,78 @@
         <v>1</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>224</v>
+        <v>4</v>
       </c>
       <c r="G52" s="23"/>
       <c r="L52" s="23"/>
       <c r="Q52" s="23"/>
-    </row>
-    <row r="53" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D53" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>14</v>
+      <c r="R52"/>
+    </row>
+    <row r="53" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A53" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D53" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="G53" s="23"/>
       <c r="L53" s="23"/>
-      <c r="M53" s="17"/>
-      <c r="N53" s="17"/>
-      <c r="O53" s="17"/>
-      <c r="P53" s="17"/>
       <c r="Q53" s="23"/>
     </row>
-    <row r="54" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="7" t="s">
+    <row r="54" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D54" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F54" s="7" t="s">
+      <c r="C54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G54" s="23"/>
       <c r="L54" s="23"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="17"/>
+      <c r="P54" s="17"/>
       <c r="Q54" s="23"/>
     </row>
-    <row r="55" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A55" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D55" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E55" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>14</v>
@@ -3310,25 +3346,22 @@
       <c r="G55" s="23"/>
       <c r="L55" s="23"/>
       <c r="Q55" s="23"/>
-      <c r="R55" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="56" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A56" s="7" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>182</v>
+        <v>60</v>
       </c>
       <c r="D56" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E56" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>14</v>
@@ -3336,390 +3369,386 @@
       <c r="G56" s="23"/>
       <c r="L56" s="23"/>
       <c r="Q56" s="23"/>
-    </row>
-    <row r="57" spans="1:18" s="28" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A57" s="15" t="s">
+      <c r="R56" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D57" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G57" s="23"/>
+      <c r="L57" s="23"/>
+      <c r="Q57" s="23"/>
+    </row>
+    <row r="58" spans="1:18" s="28" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A58" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B58" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C58" s="14" t="s">
         <v>344</v>
       </c>
-      <c r="D57" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="15" t="s">
+      <c r="D58" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="G57" s="24"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="24"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
-      <c r="P57" s="15"/>
-      <c r="Q57" s="24"/>
-      <c r="R57" s="15"/>
-    </row>
-    <row r="58" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="7" t="s">
+      <c r="G58" s="24"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15"/>
+      <c r="O58" s="15"/>
+      <c r="P58" s="15"/>
+      <c r="Q58" s="24"/>
+      <c r="R58" s="15"/>
+    </row>
+    <row r="59" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="D58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="7" t="s">
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="G58" s="23"/>
-      <c r="L58" s="23"/>
-      <c r="Q58" s="23"/>
-    </row>
-    <row r="59" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A59" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="18" t="s">
-        <v>347</v>
-      </c>
       <c r="G59" s="23"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="18"/>
       <c r="L59" s="23"/>
-      <c r="M59" s="18"/>
-      <c r="N59" s="18"/>
-      <c r="O59" s="18"/>
-      <c r="P59" s="18"/>
       <c r="Q59" s="23"/>
     </row>
     <row r="60" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="G60" s="23"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="23"/>
+      <c r="M60" s="18"/>
+      <c r="N60" s="18"/>
+      <c r="O60" s="18"/>
+      <c r="P60" s="18"/>
+      <c r="Q60" s="23"/>
+    </row>
+    <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B61" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C61" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="7" t="s">
+      <c r="D61" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="G60" s="23"/>
-      <c r="L60" s="23"/>
-      <c r="Q60" s="23"/>
-    </row>
-    <row r="61" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="15" t="s">
+      <c r="G61" s="23"/>
+      <c r="L61" s="23"/>
+      <c r="Q61" s="23"/>
+    </row>
+    <row r="62" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B62" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C62" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="D61" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="15" t="s">
+      <c r="D62" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="G61" s="24"/>
-      <c r="H61" s="15"/>
-      <c r="I61" s="15"/>
-      <c r="J61" s="15"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="24"/>
-      <c r="M61" s="15"/>
-      <c r="N61" s="15"/>
-      <c r="O61" s="15"/>
-      <c r="P61" s="15"/>
-      <c r="Q61" s="24"/>
-      <c r="R61" s="15" t="s">
+      <c r="G62" s="24"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="24"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15"/>
+      <c r="O62" s="15"/>
+      <c r="P62" s="15"/>
+      <c r="Q62" s="24"/>
+      <c r="R62" s="15" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="62" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="7" t="s">
+    <row r="63" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B63" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C63" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D62" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" s="7" t="s">
+      <c r="D63" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="G62" s="23"/>
-      <c r="L62" s="23"/>
-      <c r="Q62" s="23"/>
-      <c r="R62" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D63" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="G63" s="23"/>
       <c r="L63" s="23"/>
       <c r="Q63" s="23"/>
       <c r="R63" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D64" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G64" s="23"/>
+      <c r="L64" s="23"/>
+      <c r="Q64" s="23"/>
+      <c r="R64" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="64" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A64" s="31" t="s">
+    <row r="65" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A65" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="B64" s="31" t="s">
+      <c r="B65" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C64" s="31" t="s">
+      <c r="C65" s="31" t="s">
         <v>319</v>
       </c>
-      <c r="D64" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G64" s="29"/>
-      <c r="H64" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="I64" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="J64" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="K64" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="L64" s="29"/>
-      <c r="M64" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="N64" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="O64" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="P64" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q64" s="29"/>
-    </row>
-    <row r="65" spans="1:18" s="42" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="42" t="s">
+      <c r="D65" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G65" s="29"/>
+      <c r="H65" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I65" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="J65" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K65" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L65" s="29"/>
+      <c r="M65" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="N65" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="O65" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P65" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q65" s="29"/>
+    </row>
+    <row r="66" spans="1:18" s="42" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="B66" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="42" t="s">
+      <c r="C66" s="42" t="s">
         <v>353</v>
       </c>
-      <c r="D65" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" s="42" t="s">
+      <c r="D66" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="G65" s="29"/>
-      <c r="L65" s="29"/>
-      <c r="Q65" s="29"/>
-    </row>
-    <row r="66" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" s="7" t="s">
+      <c r="G66" s="29"/>
+      <c r="L66" s="29"/>
+      <c r="Q66" s="29"/>
+    </row>
+    <row r="67" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B67" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C67" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="7" t="s">
+      <c r="D67" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E67" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G66" s="23"/>
-      <c r="L66" s="23"/>
-      <c r="Q66" s="23"/>
-      <c r="R66" s="7" t="s">
+      <c r="G67" s="23"/>
+      <c r="L67" s="23"/>
+      <c r="Q67" s="23"/>
+      <c r="R67" s="7" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="67" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G67" s="23"/>
-      <c r="H67" s="2" t="s">
+      <c r="D68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" s="23"/>
+      <c r="H68" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="I67" s="17" t="s">
+      <c r="I68" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="J67" s="17" t="s">
+      <c r="J68" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="K67" s="17" t="s">
+      <c r="K68" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="L67" s="23"/>
-      <c r="M67" s="17" t="s">
+      <c r="L68" s="23"/>
+      <c r="M68" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="N67" s="17" t="s">
+      <c r="N68" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="O67" s="17" t="s">
+      <c r="O68" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="P67" s="17" t="s">
+      <c r="P68" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="Q67" s="23"/>
-      <c r="R67" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A68" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="G68" s="23"/>
-      <c r="L68" s="23"/>
-      <c r="M68" s="17"/>
-      <c r="N68" s="17"/>
-      <c r="O68" s="17"/>
-      <c r="P68" s="17"/>
       <c r="Q68" s="23"/>
       <c r="R68" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>189</v>
+        <v>10</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
       <c r="D69" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E69" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>213</v>
+        <v>278</v>
       </c>
       <c r="G69" s="23"/>
       <c r="L69" s="23"/>
@@ -3728,252 +3757,234 @@
       <c r="O69" s="17"/>
       <c r="P69" s="17"/>
       <c r="Q69" s="23"/>
-    </row>
-    <row r="70" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" s="27" t="s">
-        <v>310</v>
-      </c>
-      <c r="B70" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="27" t="s">
-        <v>311</v>
-      </c>
-      <c r="D70" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="27" t="s">
-        <v>312</v>
+      <c r="R69" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A70" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="G70" s="23"/>
       <c r="L70" s="23"/>
+      <c r="M70" s="17"/>
+      <c r="N70" s="17"/>
+      <c r="O70" s="17"/>
+      <c r="P70" s="17"/>
       <c r="Q70" s="23"/>
-      <c r="R70" s="27" t="s">
+    </row>
+    <row r="71" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A71" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B71" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="D71" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="G71" s="23"/>
+      <c r="L71" s="23"/>
+      <c r="Q71" s="23"/>
+      <c r="R71" s="27" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="71" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D71" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G71" s="23"/>
-      <c r="H71" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="I71" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="J71" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="K71" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="L71" s="23"/>
-      <c r="M71" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="N71" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="O71" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="P71" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q71" s="23"/>
-    </row>
-    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D72" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" s="23"/>
+      <c r="H72" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="I72" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="J72" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="K72" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="L72" s="23"/>
+      <c r="M72" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="N72" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="O72" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="P72" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q72" s="23"/>
+    </row>
+    <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="D72" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G72" s="23"/>
-      <c r="L72" s="23"/>
-      <c r="M72" s="17"/>
-      <c r="N72" s="17"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="17"/>
-      <c r="Q72" s="23"/>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A73" t="s">
-        <v>72</v>
-      </c>
-      <c r="B73" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" t="s">
-        <v>73</v>
-      </c>
-      <c r="D73" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" t="s">
-        <v>4</v>
-      </c>
-      <c r="R73"/>
-    </row>
-    <row r="74" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A74" s="34" t="s">
-        <v>360</v>
-      </c>
-      <c r="B74" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="34" t="s">
-        <v>361</v>
-      </c>
-      <c r="D74" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="45" t="s">
-        <v>4</v>
+      <c r="D73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G73" s="23"/>
+      <c r="L73" s="23"/>
+      <c r="M73" s="17"/>
+      <c r="N73" s="17"/>
+      <c r="O73" s="17"/>
+      <c r="P73" s="17"/>
+      <c r="Q73" s="23"/>
+    </row>
+    <row r="74" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="46" t="s">
+        <v>362</v>
+      </c>
+      <c r="B74" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="46" t="s">
+        <v>363</v>
+      </c>
+      <c r="D74" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="46" t="s">
+        <v>242</v>
       </c>
       <c r="G74" s="29"/>
       <c r="L74" s="29"/>
       <c r="Q74" s="29"/>
     </row>
-    <row r="75" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A75" s="2" t="s">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>73</v>
+      </c>
+      <c r="D75" t="b">
+        <v>1</v>
+      </c>
+      <c r="E75" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>4</v>
+      </c>
+      <c r="R75"/>
+    </row>
+    <row r="76" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A76" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="B76" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="34" t="s">
+        <v>361</v>
+      </c>
+      <c r="D76" s="45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" s="29"/>
+      <c r="L76" s="29"/>
+      <c r="Q76" s="29"/>
+    </row>
+    <row r="77" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D75" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G75" s="23"/>
-      <c r="L75" s="23"/>
-      <c r="M75" s="17"/>
-      <c r="N75" s="17"/>
-      <c r="O75" s="17"/>
-      <c r="P75" s="17"/>
-      <c r="Q75" s="23"/>
-    </row>
-    <row r="76" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A76" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G76" s="23"/>
-      <c r="L76" s="23"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="17"/>
-      <c r="Q76" s="23"/>
-    </row>
-    <row r="77" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="D77" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F77" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G77" s="23"/>
-      <c r="H77" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="I77" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="J77" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="K77" s="17" t="s">
-        <v>279</v>
-      </c>
       <c r="L77" s="23"/>
-      <c r="M77" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="N77" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="O77" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="P77" s="17" t="s">
-        <v>280</v>
-      </c>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
+      <c r="P77" s="17"/>
       <c r="Q77" s="23"/>
     </row>
     <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D78" s="2" t="b">
         <v>0</v>
@@ -3982,7 +3993,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>349</v>
+        <v>4</v>
       </c>
       <c r="G78" s="23"/>
       <c r="L78" s="23"/>
@@ -3992,41 +4003,59 @@
       <c r="P78" s="17"/>
       <c r="Q78" s="23"/>
     </row>
-    <row r="79" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B79" s="7" t="s">
+    <row r="79" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D79" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>272</v>
+      <c r="C79" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D79" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G79" s="23"/>
+      <c r="H79" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="I79" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="J79" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="K79" s="17" t="s">
+        <v>279</v>
+      </c>
       <c r="L79" s="23"/>
+      <c r="M79" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="N79" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="O79" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="P79" s="17" t="s">
+        <v>280</v>
+      </c>
       <c r="Q79" s="23"/>
-      <c r="R79" s="7" t="s">
-        <v>248</v>
-      </c>
     </row>
     <row r="80" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
-        <v>192</v>
+        <v>78</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>193</v>
+        <v>79</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>194</v>
+        <v>80</v>
       </c>
       <c r="D80" s="2" t="b">
         <v>0</v>
@@ -4035,453 +4064,453 @@
         <v>0</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>281</v>
+        <v>349</v>
       </c>
       <c r="G80" s="23"/>
-      <c r="H80" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="L80" s="23"/>
-      <c r="M80" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="N80" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="O80" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="P80" s="17" t="s">
-        <v>17</v>
-      </c>
+      <c r="M80" s="17"/>
+      <c r="N80" s="17"/>
+      <c r="O80" s="17"/>
+      <c r="P80" s="17"/>
       <c r="Q80" s="23"/>
     </row>
-    <row r="81" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="7" t="s">
-        <v>195</v>
+        <v>81</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>174</v>
+        <v>10</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>196</v>
+        <v>82</v>
       </c>
       <c r="D81" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
       <c r="G81" s="23"/>
       <c r="L81" s="23"/>
       <c r="Q81" s="23"/>
-      <c r="R81" s="8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R81" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
-        <v>83</v>
+        <v>192</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>10</v>
+        <v>193</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>84</v>
+        <v>194</v>
       </c>
       <c r="D82" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F82" s="2" t="s">
+        <v>281</v>
+      </c>
       <c r="G82" s="23"/>
-      <c r="H82" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="I82" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="J82" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="K82" s="17" t="s">
-        <v>282</v>
+      <c r="H82" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="L82" s="23"/>
       <c r="M82" s="17" t="s">
-        <v>283</v>
+        <v>17</v>
       </c>
       <c r="N82" s="17" t="s">
-        <v>283</v>
+        <v>17</v>
       </c>
       <c r="O82" s="17" t="s">
-        <v>283</v>
+        <v>17</v>
       </c>
       <c r="P82" s="17" t="s">
-        <v>283</v>
+        <v>17</v>
       </c>
       <c r="Q82" s="23"/>
     </row>
-    <row r="83" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D83" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E83" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>86</v>
+    <row r="83" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A83" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D83" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="G83" s="23"/>
       <c r="L83" s="23"/>
-      <c r="M83" s="17"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
-      <c r="P83" s="17"/>
       <c r="Q83" s="23"/>
-    </row>
-    <row r="84" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A84" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D84" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>90</v>
+      <c r="R83" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G84" s="23"/>
+      <c r="H84" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="I84" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="J84" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="K84" s="17" t="s">
+        <v>282</v>
+      </c>
       <c r="L84" s="23"/>
+      <c r="M84" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="N84" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="O84" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="P84" s="17" t="s">
+        <v>283</v>
+      </c>
       <c r="Q84" s="23"/>
-      <c r="R84" s="8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A85" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D85" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E85" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>14</v>
+    </row>
+    <row r="85" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="G85" s="23"/>
       <c r="L85" s="23"/>
+      <c r="M85" s="17"/>
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="17"/>
       <c r="Q85" s="23"/>
-      <c r="R85" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>94</v>
+    </row>
+    <row r="86" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A86" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D86" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="G86" s="23"/>
       <c r="L86" s="23"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
       <c r="Q86" s="23"/>
-    </row>
-    <row r="87" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A87" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="B87" s="17" t="s">
+      <c r="R86" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A87" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C87" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="D87" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="17" t="s">
-        <v>4</v>
+      <c r="C87" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D87" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G87" s="23"/>
       <c r="L87" s="23"/>
       <c r="Q87" s="23"/>
-    </row>
-    <row r="88" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="7" t="b">
-        <v>1</v>
+      <c r="R87" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A88" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D88" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G88" s="23"/>
-      <c r="H88" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I88" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J88" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K88" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="L88" s="23"/>
-      <c r="M88" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N88" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O88" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P88" s="7" t="s">
-        <v>4</v>
-      </c>
+      <c r="M88" s="17"/>
+      <c r="N88" s="17"/>
+      <c r="O88" s="17"/>
+      <c r="P88" s="17"/>
       <c r="Q88" s="23"/>
     </row>
-    <row r="89" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A89" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="B89" s="20" t="s">
+    <row r="89" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A89" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="B89" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="D89" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="7" t="b">
-        <v>1</v>
+        <v>291</v>
+      </c>
+      <c r="D89" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="17" t="s">
+        <v>4</v>
       </c>
       <c r="G89" s="23"/>
       <c r="L89" s="23"/>
       <c r="Q89" s="23"/>
     </row>
-    <row r="90" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A90" s="2" t="s">
+    <row r="90" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G90" s="23"/>
+      <c r="H90" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I90" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J90" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K90" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L90" s="23"/>
+      <c r="M90" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N90" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O90" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P90" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q90" s="23"/>
+    </row>
+    <row r="91" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A91" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="B91" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="D91" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G91" s="23"/>
+      <c r="L91" s="23"/>
+      <c r="Q91" s="23"/>
+    </row>
+    <row r="92" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D90" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G90" s="23"/>
-      <c r="L90" s="23"/>
-      <c r="M90" s="17"/>
-      <c r="N90" s="17"/>
-      <c r="O90" s="17"/>
-      <c r="P90" s="17"/>
-      <c r="Q90" s="23"/>
-      <c r="R90" s="8" t="s">
+      <c r="D92" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G92" s="23"/>
+      <c r="L92" s="23"/>
+      <c r="M92" s="17"/>
+      <c r="N92" s="17"/>
+      <c r="O92" s="17"/>
+      <c r="P92" s="17"/>
+      <c r="Q92" s="23"/>
+      <c r="R92" s="8" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="91" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
+    <row r="93" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F91" s="2" t="s">
+      <c r="D93" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="G91" s="23"/>
-      <c r="H91" s="17"/>
-      <c r="I91" s="17"/>
-      <c r="J91" s="17"/>
-      <c r="K91" s="17"/>
-      <c r="L91" s="23"/>
-      <c r="M91" s="17"/>
-      <c r="N91" s="17"/>
-      <c r="O91" s="17"/>
-      <c r="P91" s="17"/>
-      <c r="Q91" s="23"/>
-      <c r="R91" s="8" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A92" t="s">
-        <v>197</v>
-      </c>
-      <c r="B92" t="s">
-        <v>198</v>
-      </c>
-      <c r="C92" t="s">
-        <v>199</v>
-      </c>
-      <c r="D92" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" t="b">
-        <v>1</v>
-      </c>
-      <c r="M92" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="N92" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="O92" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="P92" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="R92"/>
-    </row>
-    <row r="93" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A93" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="B93" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="C93" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="D93" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="G93" s="26"/>
+      <c r="G93" s="23"/>
+      <c r="H93" s="17"/>
+      <c r="I93" s="17"/>
+      <c r="J93" s="17"/>
+      <c r="K93" s="17"/>
       <c r="L93" s="23"/>
       <c r="M93" s="17"/>
       <c r="N93" s="17"/>
       <c r="O93" s="17"/>
       <c r="P93" s="17"/>
       <c r="Q93" s="23"/>
-    </row>
-    <row r="94" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="B94" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C94" s="28" t="s">
-        <v>340</v>
-      </c>
-      <c r="D94" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="28" t="s">
-        <v>272</v>
-      </c>
-      <c r="G94" s="23"/>
-      <c r="L94" s="23"/>
-      <c r="Q94" s="23"/>
-      <c r="R94" s="7" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D95" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G95" s="23"/>
+      <c r="R93" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
+        <v>197</v>
+      </c>
+      <c r="B94" t="s">
+        <v>198</v>
+      </c>
+      <c r="C94" t="s">
+        <v>199</v>
+      </c>
+      <c r="D94" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" t="b">
+        <v>1</v>
+      </c>
+      <c r="M94" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="N94" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="O94" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="P94" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="R94"/>
+    </row>
+    <row r="95" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A95" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="D95" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="G95" s="26"/>
       <c r="L95" s="23"/>
       <c r="M95" s="17"/>
       <c r="N95" s="17"/>
@@ -4491,13 +4520,13 @@
     </row>
     <row r="96" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="28" t="s">
-        <v>337</v>
+        <v>235</v>
       </c>
       <c r="B96" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D96" s="28" t="b">
         <v>1</v>
@@ -4508,22 +4537,22 @@
       <c r="F96" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="G96" s="29"/>
-      <c r="L96" s="29"/>
-      <c r="Q96" s="29"/>
+      <c r="G96" s="23"/>
+      <c r="L96" s="23"/>
+      <c r="Q96" s="23"/>
       <c r="R96" s="7" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D97" s="2" t="b">
         <v>0</v>
@@ -4531,50 +4560,52 @@
       <c r="E97" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F97" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="G97" s="26"/>
+      <c r="F97" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G97" s="23"/>
       <c r="L97" s="23"/>
       <c r="M97" s="17"/>
       <c r="N97" s="17"/>
       <c r="O97" s="17"/>
       <c r="P97" s="17"/>
       <c r="Q97" s="23"/>
-      <c r="R97" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A98" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="B98" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="D98" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" s="6"/>
-      <c r="G98" s="26"/>
-      <c r="L98" s="23"/>
-      <c r="Q98" s="23"/>
-    </row>
-    <row r="99" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="98" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="B98" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="D98" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="G98" s="29"/>
+      <c r="L98" s="29"/>
+      <c r="Q98" s="29"/>
+      <c r="R98" s="7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D99" s="2" t="b">
         <v>0</v>
@@ -4582,62 +4613,59 @@
       <c r="E99" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F99" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G99" s="23"/>
+      <c r="F99" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="G99" s="26"/>
       <c r="L99" s="23"/>
       <c r="M99" s="17"/>
       <c r="N99" s="17"/>
       <c r="O99" s="17"/>
       <c r="P99" s="17"/>
       <c r="Q99" s="23"/>
-    </row>
-    <row r="100" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B100" s="2" t="s">
+      <c r="R99" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A100" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B100" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D100" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G100" s="23"/>
+      <c r="C100" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="D100" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" s="6"/>
+      <c r="G100" s="26"/>
       <c r="L100" s="23"/>
-      <c r="M100" s="17"/>
-      <c r="N100" s="17"/>
-      <c r="O100" s="17"/>
-      <c r="P100" s="17"/>
       <c r="Q100" s="23"/>
-      <c r="R100" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="101" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D101" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="G101" s="23"/>
       <c r="L101" s="23"/>
@@ -4646,232 +4674,198 @@
       <c r="O101" s="17"/>
       <c r="P101" s="17"/>
       <c r="Q101" s="23"/>
-      <c r="R101" s="8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="102" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
-        <v>108</v>
+        <v>200</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>109</v>
+        <v>201</v>
       </c>
       <c r="D102" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G102" s="23"/>
-      <c r="H102" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="I102" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="J102" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="K102" s="17" t="s">
-        <v>279</v>
-      </c>
       <c r="L102" s="23"/>
-      <c r="M102" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="N102" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="O102" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="P102" s="17" t="s">
-        <v>280</v>
-      </c>
+      <c r="M102" s="17"/>
+      <c r="N102" s="17"/>
+      <c r="O102" s="17"/>
+      <c r="P102" s="17"/>
       <c r="Q102" s="23"/>
-      <c r="R102" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A103" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B103" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D103" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F103" s="7" t="s">
-        <v>233</v>
+      <c r="R102" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D103" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="G103" s="23"/>
       <c r="L103" s="23"/>
+      <c r="M103" s="17"/>
+      <c r="N103" s="17"/>
+      <c r="O103" s="17"/>
+      <c r="P103" s="17"/>
       <c r="Q103" s="23"/>
-      <c r="R103" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D104" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E104" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F104" s="7" t="s">
+      <c r="R103" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A104" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D104" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G104" s="23"/>
+      <c r="H104" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="I104" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="J104" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="K104" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="L104" s="23"/>
+      <c r="M104" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="N104" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="O104" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="P104" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q104" s="23"/>
+      <c r="R104" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A105" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D105" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="G104" s="23"/>
-      <c r="L104" s="23"/>
-      <c r="Q104" s="23"/>
-      <c r="R104" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D105" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E105" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F105" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="G105" s="23"/>
       <c r="L105" s="23"/>
       <c r="Q105" s="23"/>
       <c r="R105" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D106" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="G106" s="23"/>
+      <c r="L106" s="23"/>
+      <c r="Q106" s="23"/>
+      <c r="R106" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D107" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G107" s="23"/>
+      <c r="L107" s="23"/>
+      <c r="Q107" s="23"/>
+      <c r="R107" s="7" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="106" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D106" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E106" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G106" s="23"/>
-      <c r="H106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L106" s="23"/>
-      <c r="M106" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N106" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O106" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P106" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q106" s="23"/>
-    </row>
-    <row r="107" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G107" s="23"/>
-      <c r="H107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L107" s="23"/>
-      <c r="M107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q107" s="23"/>
     </row>
     <row r="108" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D108" s="2" t="b">
         <v>0</v>
@@ -4881,7 +4875,7 @@
       </c>
       <c r="G108" s="23"/>
       <c r="H108" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I108" s="2" t="s">
         <v>4</v>
@@ -4894,7 +4888,7 @@
       </c>
       <c r="L108" s="23"/>
       <c r="M108" s="17" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N108" s="17" t="s">
         <v>4</v>
@@ -4907,225 +4901,221 @@
       </c>
       <c r="Q108" s="23"/>
     </row>
-    <row r="109" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="28" t="s">
+    <row r="109" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G109" s="23"/>
+      <c r="H109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L109" s="23"/>
+      <c r="M109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q109" s="23"/>
+    </row>
+    <row r="110" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D110" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G110" s="23"/>
+      <c r="H110" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L110" s="23"/>
+      <c r="M110" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N110" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O110" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P110" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q110" s="23"/>
+    </row>
+    <row r="111" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="B109" s="28" t="s">
+      <c r="B111" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C109" s="28" t="s">
+      <c r="C111" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="D109" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E109" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F109" s="28"/>
-      <c r="G109" s="23"/>
-      <c r="H109" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I109" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J109" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K109" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L109" s="23"/>
-      <c r="M109" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N109" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O109" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P109" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q109" s="23"/>
-      <c r="R109" s="28" t="s">
+      <c r="D111" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="28"/>
+      <c r="G111" s="23"/>
+      <c r="H111" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I111" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J111" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K111" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L111" s="23"/>
+      <c r="M111" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N111" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O111" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P111" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q111" s="23"/>
+      <c r="R111" s="28" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="110" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="28" t="s">
+    <row r="112" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="28" t="s">
         <v>341</v>
       </c>
-      <c r="B110" s="28" t="s">
+      <c r="B112" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C110" s="28" t="s">
+      <c r="C112" s="28" t="s">
         <v>342</v>
       </c>
-      <c r="D110" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E110" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" s="28"/>
-      <c r="G110" s="29"/>
-      <c r="H110" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I110" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J110" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K110" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L110" s="29"/>
-      <c r="M110" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N110" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O110" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P110" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q110" s="29"/>
-      <c r="R110" s="28" t="s">
+      <c r="D112" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E112" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" s="28"/>
+      <c r="G112" s="29"/>
+      <c r="H112" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I112" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J112" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K112" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L112" s="29"/>
+      <c r="M112" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N112" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O112" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P112" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q112" s="29"/>
+      <c r="R112" s="28" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A113" t="s">
         <v>121</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B113" t="s">
         <v>122</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C113" t="s">
         <v>123</v>
       </c>
-      <c r="D111" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" t="b">
-        <v>0</v>
-      </c>
-      <c r="H111" s="16" t="s">
+      <c r="D113" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" t="b">
+        <v>0</v>
+      </c>
+      <c r="H113" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="I111" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J111" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K111" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L111" s="23"/>
-      <c r="M111" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="N111" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O111" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P111" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q111" s="23"/>
-      <c r="R111"/>
-    </row>
-    <row r="112" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D112" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G112" s="23"/>
-      <c r="H112" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I112" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J112" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K112" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L112" s="23"/>
-      <c r="M112" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N112" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O112" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P112" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q112" s="23"/>
-      <c r="R112" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="113" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D113" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G113" s="23"/>
-      <c r="H113" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K113" s="2" t="s">
+      <c r="I113" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J113" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K113" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L113" s="23"/>
       <c r="M113" s="17" t="s">
-        <v>14</v>
+        <v>287</v>
       </c>
       <c r="N113" s="17" t="s">
         <v>4</v>
@@ -5137,150 +5127,236 @@
         <v>4</v>
       </c>
       <c r="Q113" s="23"/>
+      <c r="R113"/>
     </row>
     <row r="114" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D114" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E114" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G114" s="23"/>
-      <c r="H114" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="I114" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="J114" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="K114" s="17" t="s">
-        <v>272</v>
+      <c r="H114" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K114" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L114" s="23"/>
       <c r="M114" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N114" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O114" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P114" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q114" s="23"/>
+      <c r="R114" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D115" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G115" s="23"/>
+      <c r="H115" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L115" s="23"/>
+      <c r="M115" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N115" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O115" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P115" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q115" s="23"/>
+    </row>
+    <row r="116" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A116" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D116" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G116" s="23"/>
+      <c r="H116" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="N114" s="17" t="s">
+      <c r="I116" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="O114" s="17" t="s">
+      <c r="J116" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="P114" s="17" t="s">
+      <c r="K116" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="Q114" s="23"/>
-    </row>
-    <row r="115" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="43" t="s">
+      <c r="L116" s="23"/>
+      <c r="M116" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="N116" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="O116" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="P116" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q116" s="23"/>
+    </row>
+    <row r="117" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="43" t="s">
         <v>356</v>
       </c>
-      <c r="B115" s="43" t="s">
+      <c r="B117" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C115" s="43" t="s">
+      <c r="C117" s="43" t="s">
         <v>357</v>
       </c>
-      <c r="D115" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="G115" s="29"/>
-      <c r="H115" s="43" t="s">
+      <c r="D117" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G117" s="29"/>
+      <c r="H117" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="I115" s="43" t="s">
+      <c r="I117" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="J115" s="43" t="s">
+      <c r="J117" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="K115" s="43" t="s">
+      <c r="K117" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="L115" s="29"/>
-      <c r="M115" s="43" t="s">
+      <c r="L117" s="29"/>
+      <c r="M117" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="N115" s="43" t="s">
+      <c r="N117" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="O115" s="43" t="s">
+      <c r="O117" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="P115" s="43" t="s">
+      <c r="P117" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="Q115" s="29"/>
-    </row>
-    <row r="116" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A116" s="30" t="s">
+      <c r="Q117" s="29"/>
+    </row>
+    <row r="118" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A118" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="B116" s="30" t="s">
+      <c r="B118" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C116" s="30" t="s">
+      <c r="C118" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="D116" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F116" s="30" t="s">
+      <c r="D118" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F118" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G116" s="29"/>
-      <c r="L116" s="29"/>
-      <c r="Q116" s="29"/>
-    </row>
-    <row r="117" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A117" s="2" t="s">
+      <c r="G118" s="29"/>
+      <c r="L118" s="29"/>
+      <c r="Q118" s="29"/>
+    </row>
+    <row r="119" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A119" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D117" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F117" s="2" t="s">
+      <c r="D119" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G117" s="23"/>
-      <c r="L117" s="23"/>
-      <c r="M117" s="17"/>
-      <c r="N117" s="17"/>
-      <c r="O117" s="17"/>
-      <c r="P117" s="17"/>
-      <c r="Q117" s="23"/>
-    </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R118"/>
-    </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R119"/>
+      <c r="G119" s="23"/>
+      <c r="L119" s="23"/>
+      <c r="M119" s="17"/>
+      <c r="N119" s="17"/>
+      <c r="O119" s="17"/>
+      <c r="P119" s="17"/>
+      <c r="Q119" s="23"/>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R120"/>
@@ -5341,6 +5417,12 @@
     </row>
     <row r="139" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R139"/>
+    </row>
+    <row r="140" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R140"/>
+    </row>
+    <row r="141" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R141"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5348,15 +5430,15 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1"/>
     <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="F59" r:id="rId3"/>
+    <hyperlink ref="F60" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
[BRO] Standaard properties opgenomen in configuratie van BRO
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="371">
   <si>
     <t>Name</t>
   </si>
@@ -1123,6 +1123,21 @@
   </si>
   <si>
     <t>Yes if MIM format must be generated</t>
+  </si>
+  <si>
+    <t>createstccsv</t>
+  </si>
+  <si>
+    <t>Yes if Stelselcatalogus CSV must be generated</t>
+  </si>
+  <si>
+    <t>stccsvname</t>
+  </si>
+  <si>
+    <t>[model-abbreviation]-stelselcatalogus</t>
+  </si>
+  <si>
+    <t>The name of the Stelselcatalogus CSV file generated</t>
   </si>
 </sst>
 </file>
@@ -1288,7 +1303,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1388,6 +1403,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1706,13 +1724,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R141"/>
+  <dimension ref="A1:R143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1722,7 +1740,7 @@
     <col min="3" max="3" width="50.69140625" customWidth="1"/>
     <col min="4" max="4" width="13.23046875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="30.53515625" customWidth="1"/>
+    <col min="6" max="6" width="33.4609375" customWidth="1"/>
     <col min="7" max="7" width="3.921875" style="25" customWidth="1"/>
     <col min="8" max="8" width="18.4609375" customWidth="1"/>
     <col min="9" max="9" width="17.61328125" bestFit="1" customWidth="1"/>
@@ -1923,16 +1941,16 @@
       <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="47" t="b">
+      <c r="D7" s="48" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1950,10 +1968,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
       <c r="G8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
@@ -2870,13 +2888,13 @@
     </row>
     <row r="38" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="34" t="s">
-        <v>335</v>
+        <v>366</v>
       </c>
       <c r="B38" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>336</v>
+        <v>367</v>
       </c>
       <c r="D38" s="34" t="b">
         <v>0</v>
@@ -2903,226 +2921,248 @@
       <c r="L38" s="35"/>
       <c r="Q38" s="35"/>
     </row>
-    <row r="39" spans="1:18" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A39" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="36" t="s">
+    <row r="39" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="B39" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" s="36" t="s">
+      <c r="C39" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="D39" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G39" s="35"/>
+      <c r="H39" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" s="34" t="s">
+        <v>4</v>
+      </c>
       <c r="L39" s="35"/>
       <c r="Q39" s="35"/>
     </row>
-    <row r="40" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A40" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="34" t="s">
+    <row r="40" spans="1:18" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A40" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="F40" s="34" t="s">
+      <c r="C40" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" s="36" t="s">
         <v>14</v>
       </c>
       <c r="G40" s="35"/>
       <c r="L40" s="35"/>
       <c r="Q40" s="35"/>
     </row>
-    <row r="41" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="36" t="s">
+    <row r="41" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A41" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="36" t="b">
-        <v>1</v>
+      <c r="C41" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" s="34" t="s">
+        <v>14</v>
       </c>
       <c r="G41" s="35"/>
-      <c r="H41" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="I41" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J41" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="K41" s="36" t="s">
-        <v>14</v>
-      </c>
       <c r="L41" s="35"/>
-      <c r="M41" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="N41" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="O41" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="P41" s="36" t="s">
-        <v>4</v>
-      </c>
       <c r="Q41" s="35"/>
     </row>
     <row r="42" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" s="35"/>
+      <c r="H42" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="K42" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L42" s="35"/>
+      <c r="M42" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="N42" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="O42" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="P42" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q42" s="35"/>
+    </row>
+    <row r="43" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="36" t="s">
         <v>325</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="B43" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C43" s="36" t="s">
         <v>326</v>
       </c>
-      <c r="D42" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" s="36" t="s">
+      <c r="D43" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="36" t="s">
         <v>329</v>
-      </c>
-      <c r="G42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="Q42" s="35"/>
-    </row>
-    <row r="43" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="B43" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="D43" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43" s="34" t="s">
-        <v>14</v>
       </c>
       <c r="G43" s="35"/>
       <c r="L43" s="35"/>
       <c r="Q43" s="35"/>
     </row>
-    <row r="44" spans="1:18" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A44" s="37" t="s">
+    <row r="44" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="Q44" s="35"/>
+    </row>
+    <row r="45" spans="1:18" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A45" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B45" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C45" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="F44" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G44" s="38"/>
-      <c r="L44" s="38"/>
-      <c r="Q44" s="38"/>
-      <c r="R44" s="37" t="s">
+      <c r="D45" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="38"/>
+      <c r="L45" s="38"/>
+      <c r="Q45" s="38"/>
+      <c r="R45" s="37" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="45" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A45" s="7" t="s">
+    <row r="46" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A46" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B46" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C46" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D45" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F45" s="7" t="s">
+      <c r="D46" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="G45" s="23"/>
-      <c r="L45" s="23"/>
-      <c r="Q45" s="23"/>
-      <c r="R45" s="7" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="D46" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G46" s="23"/>
       <c r="L46" s="23"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="17"/>
-      <c r="O46" s="17"/>
-      <c r="P46" s="17"/>
       <c r="Q46" s="23"/>
+      <c r="R46" s="7" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="47"/>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
+      <c r="A47" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G47" s="23"/>
       <c r="L47" s="23"/>
       <c r="M47" s="17"/>
@@ -3131,22 +3171,11 @@
       <c r="P47" s="17"/>
       <c r="Q47" s="23"/>
     </row>
-    <row r="48" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A48" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D48" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="48"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
       <c r="G48" s="23"/>
       <c r="L48" s="23"/>
       <c r="M48" s="17"/>
@@ -3155,21 +3184,21 @@
       <c r="P48" s="17"/>
       <c r="Q48" s="23"/>
     </row>
-    <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
-        <v>50</v>
+        <v>173</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>51</v>
+        <v>175</v>
       </c>
       <c r="D49" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E49" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" s="23"/>
       <c r="L49" s="23"/>
@@ -3179,15 +3208,15 @@
       <c r="P49" s="17"/>
       <c r="Q49" s="23"/>
     </row>
-    <row r="50" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D50" s="2" t="b">
         <v>0</v>
@@ -3195,95 +3224,95 @@
       <c r="E50" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F50" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="G50" s="26"/>
+      <c r="G50" s="23"/>
       <c r="L50" s="23"/>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
       <c r="O50" s="17"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="23"/>
-      <c r="R50" s="2" t="s">
+    </row>
+    <row r="51" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A51" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G51" s="26"/>
+      <c r="L51" s="23"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="23"/>
+      <c r="R51" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E51" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="17" t="s">
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E52" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F52" s="6"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="I51" s="17" t="s">
+      <c r="I52" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="J51" s="17" t="s">
+      <c r="J52" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="K51" s="17" t="s">
+      <c r="K52" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="L51" s="23"/>
-      <c r="M51" s="17" t="s">
+      <c r="L52" s="23"/>
+      <c r="M52" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="N51" s="17" t="s">
+      <c r="N52" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="O51" s="17" t="s">
+      <c r="O52" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="P51" s="17" t="s">
+      <c r="P52" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="Q51" s="23"/>
-    </row>
-    <row r="52" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="7" t="s">
+      <c r="Q52" s="23"/>
+    </row>
+    <row r="53" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B53" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C53" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D52" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G52" s="23"/>
-      <c r="L52" s="23"/>
-      <c r="Q52" s="23"/>
-      <c r="R52"/>
-    </row>
-    <row r="53" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A53" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="D53" s="7" t="b">
         <v>0</v>
       </c>
@@ -3291,77 +3320,78 @@
         <v>1</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>224</v>
+        <v>4</v>
       </c>
       <c r="G53" s="23"/>
       <c r="L53" s="23"/>
       <c r="Q53" s="23"/>
-    </row>
-    <row r="54" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>14</v>
+      <c r="R53"/>
+    </row>
+    <row r="54" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A54" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D54" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="G54" s="23"/>
       <c r="L54" s="23"/>
-      <c r="M54" s="17"/>
-      <c r="N54" s="17"/>
-      <c r="O54" s="17"/>
-      <c r="P54" s="17"/>
       <c r="Q54" s="23"/>
     </row>
-    <row r="55" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55" s="7" t="s">
+    <row r="55" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D55" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="7" t="s">
+      <c r="C55" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G55" s="23"/>
       <c r="L55" s="23"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
+      <c r="P55" s="17"/>
       <c r="Q55" s="23"/>
     </row>
-    <row r="56" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D56" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E56" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>14</v>
@@ -3369,25 +3399,22 @@
       <c r="G56" s="23"/>
       <c r="L56" s="23"/>
       <c r="Q56" s="23"/>
-      <c r="R56" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="57" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A57" s="7" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>182</v>
+        <v>60</v>
       </c>
       <c r="D57" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E57" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>14</v>
@@ -3395,390 +3422,386 @@
       <c r="G57" s="23"/>
       <c r="L57" s="23"/>
       <c r="Q57" s="23"/>
-    </row>
-    <row r="58" spans="1:18" s="28" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A58" s="15" t="s">
+      <c r="R57" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58" s="23"/>
+      <c r="L58" s="23"/>
+      <c r="Q58" s="23"/>
+    </row>
+    <row r="59" spans="1:18" s="28" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A59" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B59" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C59" s="14" t="s">
         <v>344</v>
       </c>
-      <c r="D58" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="15" t="s">
+      <c r="D59" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="G58" s="24"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="24"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
-      <c r="O58" s="15"/>
-      <c r="P58" s="15"/>
-      <c r="Q58" s="24"/>
-      <c r="R58" s="15"/>
-    </row>
-    <row r="59" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="7" t="s">
+      <c r="G59" s="24"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="24"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15"/>
+      <c r="O59" s="15"/>
+      <c r="P59" s="15"/>
+      <c r="Q59" s="24"/>
+      <c r="R59" s="15"/>
+    </row>
+    <row r="60" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="7" t="s">
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="G59" s="23"/>
-      <c r="L59" s="23"/>
-      <c r="Q59" s="23"/>
-    </row>
-    <row r="60" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A60" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="18" t="s">
-        <v>347</v>
-      </c>
       <c r="G60" s="23"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
-      <c r="J60" s="18"/>
-      <c r="K60" s="18"/>
       <c r="L60" s="23"/>
-      <c r="M60" s="18"/>
-      <c r="N60" s="18"/>
-      <c r="O60" s="18"/>
-      <c r="P60" s="18"/>
       <c r="Q60" s="23"/>
     </row>
     <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D61" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="G61" s="23"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="18"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="18"/>
+      <c r="Q61" s="23"/>
+    </row>
+    <row r="62" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C62" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="7" t="s">
+      <c r="D62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="G61" s="23"/>
-      <c r="L61" s="23"/>
-      <c r="Q61" s="23"/>
-    </row>
-    <row r="62" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="15" t="s">
+      <c r="G62" s="23"/>
+      <c r="L62" s="23"/>
+      <c r="Q62" s="23"/>
+    </row>
+    <row r="63" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B63" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C63" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="D62" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="15" t="s">
+      <c r="D63" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="G62" s="24"/>
-      <c r="H62" s="15"/>
-      <c r="I62" s="15"/>
-      <c r="J62" s="15"/>
-      <c r="K62" s="15"/>
-      <c r="L62" s="24"/>
-      <c r="M62" s="15"/>
-      <c r="N62" s="15"/>
-      <c r="O62" s="15"/>
-      <c r="P62" s="15"/>
-      <c r="Q62" s="24"/>
-      <c r="R62" s="15" t="s">
+      <c r="G63" s="24"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="24"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="15"/>
+      <c r="Q63" s="24"/>
+      <c r="R63" s="15" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="63" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" s="7" t="s">
+    <row r="64" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A64" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B64" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C64" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D63" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" s="7" t="s">
+      <c r="D64" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F64" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="G63" s="23"/>
-      <c r="L63" s="23"/>
-      <c r="Q63" s="23"/>
-      <c r="R63" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D64" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="G64" s="23"/>
       <c r="L64" s="23"/>
       <c r="Q64" s="23"/>
       <c r="R64" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D65" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G65" s="23"/>
+      <c r="L65" s="23"/>
+      <c r="Q65" s="23"/>
+      <c r="R65" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="65" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A65" s="31" t="s">
+    <row r="66" spans="1:18" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A66" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="B65" s="31" t="s">
+      <c r="B66" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="31" t="s">
+      <c r="C66" s="31" t="s">
         <v>319</v>
       </c>
-      <c r="D65" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G65" s="29"/>
-      <c r="H65" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="I65" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="J65" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="K65" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="L65" s="29"/>
-      <c r="M65" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="N65" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="O65" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="P65" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q65" s="29"/>
-    </row>
-    <row r="66" spans="1:18" s="42" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="42" t="s">
+      <c r="D66" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G66" s="29"/>
+      <c r="H66" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I66" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="J66" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K66" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L66" s="29"/>
+      <c r="M66" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="N66" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="O66" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P66" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q66" s="29"/>
+    </row>
+    <row r="67" spans="1:18" s="42" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="B67" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C66" s="42" t="s">
+      <c r="C67" s="42" t="s">
         <v>353</v>
       </c>
-      <c r="D66" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="42" t="s">
+      <c r="D67" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="G66" s="29"/>
-      <c r="L66" s="29"/>
-      <c r="Q66" s="29"/>
-    </row>
-    <row r="67" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" s="7" t="s">
+      <c r="G67" s="29"/>
+      <c r="L67" s="29"/>
+      <c r="Q67" s="29"/>
+    </row>
+    <row r="68" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A68" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B68" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C68" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D67" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="7" t="s">
+      <c r="D68" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E68" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G67" s="23"/>
-      <c r="L67" s="23"/>
-      <c r="Q67" s="23"/>
-      <c r="R67" s="7" t="s">
+      <c r="G68" s="23"/>
+      <c r="L68" s="23"/>
+      <c r="Q68" s="23"/>
+      <c r="R68" s="7" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G68" s="23"/>
-      <c r="H68" s="2" t="s">
+      <c r="D69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" s="23"/>
+      <c r="H69" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="I68" s="17" t="s">
+      <c r="I69" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="J68" s="17" t="s">
+      <c r="J69" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="K68" s="17" t="s">
+      <c r="K69" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="L68" s="23"/>
-      <c r="M68" s="17" t="s">
+      <c r="L69" s="23"/>
+      <c r="M69" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="N68" s="17" t="s">
+      <c r="N69" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="O68" s="17" t="s">
+      <c r="O69" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="P68" s="17" t="s">
+      <c r="P69" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="Q68" s="23"/>
-      <c r="R68" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A69" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="G69" s="23"/>
-      <c r="L69" s="23"/>
-      <c r="M69" s="17"/>
-      <c r="N69" s="17"/>
-      <c r="O69" s="17"/>
-      <c r="P69" s="17"/>
       <c r="Q69" s="23"/>
       <c r="R69" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>189</v>
+        <v>10</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
       <c r="D70" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E70" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>213</v>
+        <v>278</v>
       </c>
       <c r="G70" s="23"/>
       <c r="L70" s="23"/>
@@ -3787,213 +3810,216 @@
       <c r="O70" s="17"/>
       <c r="P70" s="17"/>
       <c r="Q70" s="23"/>
-    </row>
-    <row r="71" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A71" s="27" t="s">
-        <v>310</v>
-      </c>
-      <c r="B71" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="27" t="s">
-        <v>311</v>
-      </c>
-      <c r="D71" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="27" t="s">
-        <v>312</v>
+      <c r="R70" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="G71" s="23"/>
       <c r="L71" s="23"/>
+      <c r="M71" s="17"/>
+      <c r="N71" s="17"/>
+      <c r="O71" s="17"/>
+      <c r="P71" s="17"/>
       <c r="Q71" s="23"/>
-      <c r="R71" s="27" t="s">
+    </row>
+    <row r="72" spans="1:18" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A72" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B72" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="D72" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="G72" s="23"/>
+      <c r="L72" s="23"/>
+      <c r="Q72" s="23"/>
+      <c r="R72" s="27" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="72" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="2" t="s">
+    <row r="73" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D72" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G72" s="23"/>
-      <c r="H72" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="I72" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="J72" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="K72" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="L72" s="23"/>
-      <c r="M72" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="N72" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="O72" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="P72" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q72" s="23"/>
-    </row>
-    <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" s="23"/>
+      <c r="H73" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="I73" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="J73" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="K73" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="L73" s="23"/>
+      <c r="M73" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="N73" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="O73" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="P73" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q73" s="23"/>
+    </row>
+    <row r="74" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A74" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="D73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G73" s="23"/>
-      <c r="L73" s="23"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
-      <c r="Q73" s="23"/>
-    </row>
-    <row r="74" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="46" t="s">
+      <c r="D74" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G74" s="23"/>
+      <c r="L74" s="23"/>
+      <c r="M74" s="17"/>
+      <c r="N74" s="17"/>
+      <c r="O74" s="17"/>
+      <c r="P74" s="17"/>
+      <c r="Q74" s="23"/>
+    </row>
+    <row r="75" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="46" t="s">
         <v>362</v>
       </c>
-      <c r="B74" s="46" t="s">
+      <c r="B75" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="46" t="s">
+      <c r="C75" s="46" t="s">
         <v>363</v>
       </c>
-      <c r="D74" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="46" t="s">
+      <c r="D75" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="G74" s="29"/>
-      <c r="L74" s="29"/>
-      <c r="Q74" s="29"/>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A75" t="s">
+      <c r="G75" s="29"/>
+      <c r="L75" s="29"/>
+      <c r="Q75" s="29"/>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
         <v>72</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>5</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>73</v>
       </c>
-      <c r="D75" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" t="s">
-        <v>4</v>
-      </c>
-      <c r="R75"/>
-    </row>
-    <row r="76" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A76" s="34" t="s">
+      <c r="D76" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" t="s">
+        <v>4</v>
+      </c>
+      <c r="R76"/>
+    </row>
+    <row r="77" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A77" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="B76" s="34" t="s">
+      <c r="B77" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C76" s="34" t="s">
+      <c r="C77" s="34" t="s">
         <v>361</v>
       </c>
-      <c r="D76" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="G76" s="29"/>
-      <c r="L76" s="29"/>
-      <c r="Q76" s="29"/>
-    </row>
-    <row r="77" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A77" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D77" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G77" s="23"/>
-      <c r="L77" s="23"/>
-      <c r="M77" s="17"/>
-      <c r="N77" s="17"/>
-      <c r="O77" s="17"/>
-      <c r="P77" s="17"/>
-      <c r="Q77" s="23"/>
+      <c r="D77" s="45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G77" s="29"/>
+      <c r="L77" s="29"/>
+      <c r="Q77" s="29"/>
     </row>
     <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
-        <v>74</v>
+        <v>232</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>75</v>
+        <v>246</v>
       </c>
       <c r="D78" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G78" s="23"/>
       <c r="L78" s="23"/>
@@ -4003,454 +4029,447 @@
       <c r="P78" s="17"/>
       <c r="Q78" s="23"/>
     </row>
-    <row r="79" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G79" s="23"/>
+      <c r="L79" s="23"/>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="17"/>
+      <c r="Q79" s="23"/>
+    </row>
+    <row r="80" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D79" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G79" s="23"/>
-      <c r="H79" s="17" t="s">
+      <c r="D80" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G80" s="23"/>
+      <c r="H80" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="I79" s="17" t="s">
+      <c r="I80" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="J79" s="17" t="s">
+      <c r="J80" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="K79" s="17" t="s">
+      <c r="K80" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="L79" s="23"/>
-      <c r="M79" s="17" t="s">
+      <c r="L80" s="23"/>
+      <c r="M80" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="N79" s="17" t="s">
+      <c r="N80" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="O79" s="17" t="s">
+      <c r="O80" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="P79" s="17" t="s">
+      <c r="P80" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="Q79" s="23"/>
-    </row>
-    <row r="80" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A80" s="2" t="s">
+      <c r="Q80" s="23"/>
+    </row>
+    <row r="81" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A81" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F80" s="2" t="s">
+      <c r="D81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="G80" s="23"/>
-      <c r="L80" s="23"/>
-      <c r="M80" s="17"/>
-      <c r="N80" s="17"/>
-      <c r="O80" s="17"/>
-      <c r="P80" s="17"/>
-      <c r="Q80" s="23"/>
-    </row>
-    <row r="81" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D81" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>272</v>
       </c>
       <c r="G81" s="23"/>
       <c r="L81" s="23"/>
+      <c r="M81" s="17"/>
+      <c r="N81" s="17"/>
+      <c r="O81" s="17"/>
+      <c r="P81" s="17"/>
       <c r="Q81" s="23"/>
-      <c r="R81" s="7" t="s">
+    </row>
+    <row r="82" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D82" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="G82" s="23"/>
+      <c r="L82" s="23"/>
+      <c r="Q82" s="23"/>
+      <c r="R82" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="82" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A82" s="2" t="s">
+    <row r="83" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A83" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82" s="2" t="s">
+      <c r="D83" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="G82" s="23"/>
-      <c r="H82" s="2" t="s">
+      <c r="G83" s="23"/>
+      <c r="H83" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L82" s="23"/>
-      <c r="M82" s="17" t="s">
+      <c r="L83" s="23"/>
+      <c r="M83" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N82" s="17" t="s">
+      <c r="N83" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O82" s="17" t="s">
+      <c r="O83" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P82" s="17" t="s">
+      <c r="P83" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q82" s="23"/>
-    </row>
-    <row r="83" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A83" s="7" t="s">
+      <c r="Q83" s="23"/>
+    </row>
+    <row r="84" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A84" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B84" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="C84" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D83" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="7" t="s">
+      <c r="D84" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="G83" s="23"/>
-      <c r="L83" s="23"/>
-      <c r="Q83" s="23"/>
-      <c r="R83" s="8" t="s">
+      <c r="G84" s="23"/>
+      <c r="L84" s="23"/>
+      <c r="Q84" s="23"/>
+      <c r="R84" s="8" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G84" s="23"/>
-      <c r="H84" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="I84" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="J84" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="K84" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="L84" s="23"/>
-      <c r="M84" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="N84" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="O84" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="P84" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q84" s="23"/>
     </row>
     <row r="85" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G85" s="23"/>
+      <c r="H85" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="I85" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="J85" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="K85" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="L85" s="23"/>
+      <c r="M85" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="N85" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="O85" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="P85" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q85" s="23"/>
+    </row>
+    <row r="86" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="2" t="s">
+      <c r="D86" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G85" s="23"/>
-      <c r="L85" s="23"/>
-      <c r="M85" s="17"/>
-      <c r="N85" s="17"/>
-      <c r="O85" s="17"/>
-      <c r="P85" s="17"/>
-      <c r="Q85" s="23"/>
-    </row>
-    <row r="86" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A86" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D86" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="G86" s="23"/>
       <c r="L86" s="23"/>
+      <c r="M86" s="17"/>
+      <c r="N86" s="17"/>
+      <c r="O86" s="17"/>
+      <c r="P86" s="17"/>
       <c r="Q86" s="23"/>
-      <c r="R86" s="8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="87" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A87" s="7" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="D87" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E87" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="G87" s="23"/>
       <c r="L87" s="23"/>
       <c r="Q87" s="23"/>
-      <c r="R87" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>94</v>
+      <c r="R87" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A88" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D88" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G88" s="23"/>
       <c r="L88" s="23"/>
-      <c r="M88" s="17"/>
-      <c r="N88" s="17"/>
-      <c r="O88" s="17"/>
-      <c r="P88" s="17"/>
       <c r="Q88" s="23"/>
-    </row>
-    <row r="89" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A89" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="B89" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="D89" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="17" t="s">
-        <v>4</v>
+      <c r="R88" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G89" s="23"/>
       <c r="L89" s="23"/>
+      <c r="M89" s="17"/>
+      <c r="N89" s="17"/>
+      <c r="O89" s="17"/>
+      <c r="P89" s="17"/>
       <c r="Q89" s="23"/>
     </row>
-    <row r="90" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="7" t="s">
+    <row r="90" spans="1:18" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A90" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="B90" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="D90" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G90" s="23"/>
+      <c r="L90" s="23"/>
+      <c r="Q90" s="23"/>
+    </row>
+    <row r="91" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="B90" s="19"/>
-      <c r="C90" s="19"/>
-      <c r="D90" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G90" s="23"/>
-      <c r="H90" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I90" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J90" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K90" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L90" s="23"/>
-      <c r="M90" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N90" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O90" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P90" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q90" s="23"/>
-    </row>
-    <row r="91" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A91" s="20" t="s">
+      <c r="B91" s="19"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G91" s="23"/>
+      <c r="H91" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I91" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J91" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K91" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L91" s="23"/>
+      <c r="M91" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N91" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O91" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P91" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q91" s="23"/>
+    </row>
+    <row r="92" spans="1:18" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A92" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="B91" s="20" t="s">
+      <c r="B92" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C91" s="20" t="s">
+      <c r="C92" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="D91" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G91" s="23"/>
-      <c r="L91" s="23"/>
-      <c r="Q91" s="23"/>
-    </row>
-    <row r="92" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A92" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D92" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>4</v>
+      <c r="D92" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G92" s="23"/>
       <c r="L92" s="23"/>
-      <c r="M92" s="17"/>
-      <c r="N92" s="17"/>
-      <c r="O92" s="17"/>
-      <c r="P92" s="17"/>
       <c r="Q92" s="23"/>
-      <c r="R92" s="8" t="s">
-        <v>217</v>
-      </c>
     </row>
     <row r="93" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D93" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>328</v>
+        <v>4</v>
       </c>
       <c r="G93" s="23"/>
-      <c r="H93" s="17"/>
-      <c r="I93" s="17"/>
-      <c r="J93" s="17"/>
-      <c r="K93" s="17"/>
       <c r="L93" s="23"/>
       <c r="M93" s="17"/>
       <c r="N93" s="17"/>
@@ -4458,268 +4477,271 @@
       <c r="P93" s="17"/>
       <c r="Q93" s="23"/>
       <c r="R93" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G94" s="23"/>
+      <c r="H94" s="17"/>
+      <c r="I94" s="17"/>
+      <c r="J94" s="17"/>
+      <c r="K94" s="17"/>
+      <c r="L94" s="23"/>
+      <c r="M94" s="17"/>
+      <c r="N94" s="17"/>
+      <c r="O94" s="17"/>
+      <c r="P94" s="17"/>
+      <c r="Q94" s="23"/>
+      <c r="R94" s="8" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A94" t="s">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
         <v>197</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>198</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C95" t="s">
         <v>199</v>
       </c>
-      <c r="D94" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" t="b">
-        <v>1</v>
-      </c>
-      <c r="M94" s="28" t="s">
+      <c r="D95" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" t="b">
+        <v>1</v>
+      </c>
+      <c r="M95" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="N94" s="28" t="s">
+      <c r="N95" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="O94" s="28" t="s">
+      <c r="O95" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="P94" s="28" t="s">
+      <c r="P95" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="R94"/>
-    </row>
-    <row r="95" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A95" s="13" t="s">
+      <c r="R95"/>
+    </row>
+    <row r="96" spans="1:18" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A96" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="B95" s="13" t="s">
+      <c r="B96" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="C95" s="13" t="s">
+      <c r="C96" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="D95" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E95" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="6" t="s">
+      <c r="D96" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="G95" s="26"/>
-      <c r="L95" s="23"/>
-      <c r="M95" s="17"/>
-      <c r="N95" s="17"/>
-      <c r="O95" s="17"/>
-      <c r="P95" s="17"/>
-      <c r="Q95" s="23"/>
-    </row>
-    <row r="96" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="28" t="s">
+      <c r="G96" s="26"/>
+      <c r="L96" s="23"/>
+      <c r="M96" s="17"/>
+      <c r="N96" s="17"/>
+      <c r="O96" s="17"/>
+      <c r="P96" s="17"/>
+      <c r="Q96" s="23"/>
+    </row>
+    <row r="97" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="B96" s="28" t="s">
+      <c r="B97" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C96" s="28" t="s">
+      <c r="C97" s="28" t="s">
         <v>340</v>
       </c>
-      <c r="D96" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E96" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" s="28" t="s">
+      <c r="D97" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="28" t="s">
         <v>272</v>
-      </c>
-      <c r="G96" s="23"/>
-      <c r="L96" s="23"/>
-      <c r="Q96" s="23"/>
-      <c r="R96" s="7" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D97" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G97" s="23"/>
       <c r="L97" s="23"/>
-      <c r="M97" s="17"/>
-      <c r="N97" s="17"/>
-      <c r="O97" s="17"/>
-      <c r="P97" s="17"/>
       <c r="Q97" s="23"/>
-    </row>
-    <row r="98" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="28" t="s">
+      <c r="R97" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D98" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G98" s="23"/>
+      <c r="L98" s="23"/>
+      <c r="M98" s="17"/>
+      <c r="N98" s="17"/>
+      <c r="O98" s="17"/>
+      <c r="P98" s="17"/>
+      <c r="Q98" s="23"/>
+    </row>
+    <row r="99" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="28" t="s">
         <v>337</v>
       </c>
-      <c r="B98" s="28" t="s">
+      <c r="B99" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C98" s="28" t="s">
+      <c r="C99" s="28" t="s">
         <v>339</v>
       </c>
-      <c r="D98" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" s="28" t="s">
+      <c r="D99" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="G98" s="29"/>
-      <c r="L98" s="29"/>
-      <c r="Q98" s="29"/>
-      <c r="R98" s="7" t="s">
+      <c r="G99" s="29"/>
+      <c r="L99" s="29"/>
+      <c r="Q99" s="29"/>
+      <c r="R99" s="7" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="99" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:18" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A100" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D99" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" s="6" t="s">
+      <c r="D100" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="G99" s="26"/>
-      <c r="L99" s="23"/>
-      <c r="M99" s="17"/>
-      <c r="N99" s="17"/>
-      <c r="O99" s="17"/>
-      <c r="P99" s="17"/>
-      <c r="Q99" s="23"/>
-      <c r="R99" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A100" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="B100" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="D100" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E100" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F100" s="6"/>
       <c r="G100" s="26"/>
       <c r="L100" s="23"/>
+      <c r="M100" s="17"/>
+      <c r="N100" s="17"/>
+      <c r="O100" s="17"/>
+      <c r="P100" s="17"/>
       <c r="Q100" s="23"/>
-    </row>
-    <row r="101" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A101" s="2" t="s">
+      <c r="R100" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="47" t="s">
+        <v>368</v>
+      </c>
+      <c r="B101" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" s="47" t="s">
+        <v>370</v>
+      </c>
+      <c r="D101" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="G101" s="26"/>
+      <c r="L101" s="29"/>
+      <c r="Q101" s="29"/>
+    </row>
+    <row r="102" spans="1:18" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A102" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B102" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="D102" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" s="6"/>
+      <c r="G102" s="26"/>
+      <c r="L102" s="23"/>
+      <c r="Q102" s="23"/>
+    </row>
+    <row r="103" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D101" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G101" s="23"/>
-      <c r="L101" s="23"/>
-      <c r="M101" s="17"/>
-      <c r="N101" s="17"/>
-      <c r="O101" s="17"/>
-      <c r="P101" s="17"/>
-      <c r="Q101" s="23"/>
-    </row>
-    <row r="102" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G102" s="23"/>
-      <c r="L102" s="23"/>
-      <c r="M102" s="17"/>
-      <c r="N102" s="17"/>
-      <c r="O102" s="17"/>
-      <c r="P102" s="17"/>
-      <c r="Q102" s="23"/>
-      <c r="R102" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
-      <c r="A103" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="D103" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="G103" s="23"/>
       <c r="L103" s="23"/>
@@ -4728,232 +4750,198 @@
       <c r="O103" s="17"/>
       <c r="P103" s="17"/>
       <c r="Q103" s="23"/>
-      <c r="R103" s="8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="104" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>108</v>
+        <v>200</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>109</v>
+        <v>201</v>
       </c>
       <c r="D104" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G104" s="23"/>
-      <c r="H104" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="I104" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="J104" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="K104" s="17" t="s">
-        <v>279</v>
-      </c>
       <c r="L104" s="23"/>
-      <c r="M104" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="N104" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="O104" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="P104" s="17" t="s">
-        <v>280</v>
-      </c>
+      <c r="M104" s="17"/>
+      <c r="N104" s="17"/>
+      <c r="O104" s="17"/>
+      <c r="P104" s="17"/>
       <c r="Q104" s="23"/>
-      <c r="R104" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A105" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D105" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E105" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F105" s="7" t="s">
-        <v>233</v>
+      <c r="R104" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A105" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D105" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="G105" s="23"/>
       <c r="L105" s="23"/>
+      <c r="M105" s="17"/>
+      <c r="N105" s="17"/>
+      <c r="O105" s="17"/>
+      <c r="P105" s="17"/>
       <c r="Q105" s="23"/>
-      <c r="R105" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B106" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D106" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F106" s="7" t="s">
+      <c r="R105" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A106" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D106" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G106" s="23"/>
+      <c r="H106" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="I106" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="J106" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="K106" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="L106" s="23"/>
+      <c r="M106" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="N106" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="O106" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="P106" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q106" s="23"/>
+      <c r="R106" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A107" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D107" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="G106" s="23"/>
-      <c r="L106" s="23"/>
-      <c r="Q106" s="23"/>
-      <c r="R106" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D107" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F107" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="G107" s="23"/>
       <c r="L107" s="23"/>
       <c r="Q107" s="23"/>
       <c r="R107" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D108" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="G108" s="23"/>
+      <c r="L108" s="23"/>
+      <c r="Q108" s="23"/>
+      <c r="R108" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D109" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G109" s="23"/>
+      <c r="L109" s="23"/>
+      <c r="Q109" s="23"/>
+      <c r="R109" s="7" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="108" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D108" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E108" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G108" s="23"/>
-      <c r="H108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L108" s="23"/>
-      <c r="M108" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N108" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O108" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P108" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q108" s="23"/>
-    </row>
-    <row r="109" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G109" s="23"/>
-      <c r="H109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L109" s="23"/>
-      <c r="M109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q109" s="23"/>
     </row>
     <row r="110" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D110" s="2" t="b">
         <v>0</v>
@@ -4963,7 +4951,7 @@
       </c>
       <c r="G110" s="23"/>
       <c r="H110" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I110" s="2" t="s">
         <v>4</v>
@@ -4976,7 +4964,7 @@
       </c>
       <c r="L110" s="23"/>
       <c r="M110" s="17" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N110" s="17" t="s">
         <v>4</v>
@@ -4989,225 +4977,221 @@
       </c>
       <c r="Q110" s="23"/>
     </row>
-    <row r="111" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="28" t="s">
+    <row r="111" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G111" s="23"/>
+      <c r="H111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L111" s="23"/>
+      <c r="M111" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N111" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O111" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P111" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q111" s="23"/>
+    </row>
+    <row r="112" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D112" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E112" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G112" s="23"/>
+      <c r="H112" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L112" s="23"/>
+      <c r="M112" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q112" s="23"/>
+    </row>
+    <row r="113" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="B111" s="28" t="s">
+      <c r="B113" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C111" s="28" t="s">
+      <c r="C113" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="D111" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E111" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" s="28"/>
-      <c r="G111" s="23"/>
-      <c r="H111" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I111" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J111" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K111" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L111" s="23"/>
-      <c r="M111" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N111" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O111" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P111" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q111" s="23"/>
-      <c r="R111" s="28" t="s">
+      <c r="D113" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E113" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F113" s="28"/>
+      <c r="G113" s="23"/>
+      <c r="H113" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I113" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J113" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K113" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L113" s="23"/>
+      <c r="M113" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N113" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O113" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P113" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q113" s="23"/>
+      <c r="R113" s="28" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="112" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="28" t="s">
+    <row r="114" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="28" t="s">
         <v>341</v>
       </c>
-      <c r="B112" s="28" t="s">
+      <c r="B114" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C112" s="28" t="s">
+      <c r="C114" s="28" t="s">
         <v>342</v>
       </c>
-      <c r="D112" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E112" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F112" s="28"/>
-      <c r="G112" s="29"/>
-      <c r="H112" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I112" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J112" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K112" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L112" s="29"/>
-      <c r="M112" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N112" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O112" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P112" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q112" s="29"/>
-      <c r="R112" s="28" t="s">
+      <c r="D114" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E114" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F114" s="28"/>
+      <c r="G114" s="29"/>
+      <c r="H114" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I114" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J114" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K114" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L114" s="29"/>
+      <c r="M114" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N114" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O114" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P114" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q114" s="29"/>
+      <c r="R114" s="28" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A113" t="s">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A115" t="s">
         <v>121</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B115" t="s">
         <v>122</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C115" t="s">
         <v>123</v>
       </c>
-      <c r="D113" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" t="b">
-        <v>0</v>
-      </c>
-      <c r="H113" s="16" t="s">
+      <c r="D115" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" t="b">
+        <v>0</v>
+      </c>
+      <c r="H115" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="I113" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J113" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K113" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L113" s="23"/>
-      <c r="M113" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="N113" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O113" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P113" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q113" s="23"/>
-      <c r="R113"/>
-    </row>
-    <row r="114" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D114" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E114" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G114" s="23"/>
-      <c r="H114" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L114" s="23"/>
-      <c r="M114" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="N114" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O114" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P114" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q114" s="23"/>
-      <c r="R114" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="115" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D115" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G115" s="23"/>
-      <c r="H115" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K115" s="2" t="s">
+      <c r="I115" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J115" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K115" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L115" s="23"/>
       <c r="M115" s="17" t="s">
-        <v>14</v>
+        <v>287</v>
       </c>
       <c r="N115" s="17" t="s">
         <v>4</v>
@@ -5219,150 +5203,236 @@
         <v>4</v>
       </c>
       <c r="Q115" s="23"/>
+      <c r="R115"/>
     </row>
     <row r="116" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D116" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E116" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G116" s="23"/>
-      <c r="H116" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="I116" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="J116" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="K116" s="17" t="s">
-        <v>272</v>
+      <c r="H116" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L116" s="23"/>
       <c r="M116" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N116" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O116" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P116" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q116" s="23"/>
+      <c r="R116" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D117" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G117" s="23"/>
+      <c r="H117" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L117" s="23"/>
+      <c r="M117" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N117" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O117" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P117" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q117" s="23"/>
+    </row>
+    <row r="118" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A118" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D118" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G118" s="23"/>
+      <c r="H118" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="N116" s="17" t="s">
+      <c r="I118" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="O116" s="17" t="s">
+      <c r="J118" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="P116" s="17" t="s">
+      <c r="K118" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="Q116" s="23"/>
-    </row>
-    <row r="117" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="43" t="s">
+      <c r="L118" s="23"/>
+      <c r="M118" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="N118" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="O118" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="P118" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q118" s="23"/>
+    </row>
+    <row r="119" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A119" s="43" t="s">
         <v>356</v>
       </c>
-      <c r="B117" s="43" t="s">
+      <c r="B119" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C117" s="43" t="s">
+      <c r="C119" s="43" t="s">
         <v>357</v>
       </c>
-      <c r="D117" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="G117" s="29"/>
-      <c r="H117" s="43" t="s">
+      <c r="D119" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G119" s="29"/>
+      <c r="H119" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="I117" s="43" t="s">
+      <c r="I119" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="J117" s="43" t="s">
+      <c r="J119" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="K117" s="43" t="s">
+      <c r="K119" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="L117" s="29"/>
-      <c r="M117" s="43" t="s">
+      <c r="L119" s="29"/>
+      <c r="M119" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="N117" s="43" t="s">
+      <c r="N119" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="O117" s="43" t="s">
+      <c r="O119" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="P117" s="43" t="s">
+      <c r="P119" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="Q117" s="29"/>
-    </row>
-    <row r="118" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A118" s="30" t="s">
+      <c r="Q119" s="29"/>
+    </row>
+    <row r="120" spans="1:18" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A120" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="B118" s="30" t="s">
+      <c r="B120" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C118" s="30" t="s">
+      <c r="C120" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="D118" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E118" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F118" s="30" t="s">
+      <c r="D120" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F120" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G118" s="29"/>
-      <c r="L118" s="29"/>
-      <c r="Q118" s="29"/>
-    </row>
-    <row r="119" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A119" s="2" t="s">
+      <c r="G120" s="29"/>
+      <c r="L120" s="29"/>
+      <c r="Q120" s="29"/>
+    </row>
+    <row r="121" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A121" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D119" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E119" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F119" s="2" t="s">
+      <c r="D121" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F121" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G119" s="23"/>
-      <c r="L119" s="23"/>
-      <c r="M119" s="17"/>
-      <c r="N119" s="17"/>
-      <c r="O119" s="17"/>
-      <c r="P119" s="17"/>
-      <c r="Q119" s="23"/>
-    </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R120"/>
-    </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R121"/>
+      <c r="G121" s="23"/>
+      <c r="L121" s="23"/>
+      <c r="M121" s="17"/>
+      <c r="N121" s="17"/>
+      <c r="O121" s="17"/>
+      <c r="P121" s="17"/>
+      <c r="Q121" s="23"/>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R122"/>
@@ -5423,6 +5493,12 @@
     </row>
     <row r="141" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R141"/>
+    </row>
+    <row r="142" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R142"/>
+    </row>
+    <row r="143" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R143"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5430,15 +5506,15 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1"/>
     <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="F60" r:id="rId3"/>
+    <hyperlink ref="F61" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
[bro] correctie: MIM serialisatie niet op logische modellen
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -1303,7 +1303,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1403,6 +1403,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1727,10 +1730,10 @@
   <dimension ref="A1:R143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C102" sqref="C102"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1941,16 +1944,16 @@
       <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="48" t="b">
+      <c r="D7" s="49" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1968,10 +1971,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
       <c r="G8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
@@ -2736,14 +2739,14 @@
       <c r="M32" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="N32" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="O32" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="P32" s="46" t="s">
-        <v>4</v>
+      <c r="N32" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="O32" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="P32" s="48" t="s">
+        <v>14</v>
       </c>
       <c r="Q32" s="29"/>
     </row>
@@ -3145,16 +3148,16 @@
       </c>
     </row>
     <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="48" t="s">
+      <c r="A47" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="48" t="s">
+      <c r="B47" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="48" t="s">
+      <c r="C47" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="48" t="b">
+      <c r="D47" s="49" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="2" t="b">
@@ -3172,10 +3175,10 @@
       <c r="Q47" s="23"/>
     </row>
     <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="48"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
+      <c r="A48" s="49"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
       <c r="G48" s="23"/>
       <c r="L48" s="23"/>
       <c r="M48" s="17"/>

</xml_diff>

<commit_message>
[BRO] SKOS export verbeterd
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -1730,10 +1730,10 @@
   <dimension ref="A1:R143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B104" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5090,7 +5090,7 @@
         <v>14</v>
       </c>
       <c r="I113" s="28" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="J113" s="28" t="s">
         <v>4</v>
@@ -5103,7 +5103,7 @@
         <v>14</v>
       </c>
       <c r="N113" s="28" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="O113" s="28" t="s">
         <v>4</v>
@@ -5138,7 +5138,7 @@
         <v>14</v>
       </c>
       <c r="I114" s="28" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="J114" s="28" t="s">
         <v>4</v>
@@ -5151,7 +5151,7 @@
         <v>14</v>
       </c>
       <c r="N114" s="28" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="O114" s="28" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
[BRO] nativescalars yes voor LM, no voor CM
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="371">
   <si>
     <t>Name</t>
   </si>
@@ -1303,7 +1303,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1403,6 +1403,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1730,10 +1733,10 @@
   <dimension ref="A1:R143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B104" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A115" sqref="A115"/>
+      <selection pane="bottomRight" activeCell="I77" sqref="I77:K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1944,16 +1947,16 @@
       <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="49" t="b">
+      <c r="D7" s="50" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1971,10 +1974,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="49"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
       <c r="G8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
@@ -3148,16 +3151,16 @@
       </c>
     </row>
     <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="49" t="s">
+      <c r="B47" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="49" t="s">
+      <c r="C47" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="49" t="b">
+      <c r="D47" s="50" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="2" t="b">
@@ -3175,10 +3178,10 @@
       <c r="Q47" s="23"/>
     </row>
     <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="49"/>
-      <c r="B48" s="49"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
+      <c r="A48" s="50"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
       <c r="G48" s="23"/>
       <c r="L48" s="23"/>
       <c r="M48" s="17"/>
@@ -3998,11 +4001,32 @@
       <c r="E77" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="F77" s="45" t="s">
-        <v>4</v>
-      </c>
       <c r="G77" s="29"/>
+      <c r="H77" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="I77" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="J77" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="K77" s="49" t="s">
+        <v>14</v>
+      </c>
       <c r="L77" s="29"/>
+      <c r="M77" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="N77" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="O77" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="P77" s="49" t="s">
+        <v>4</v>
+      </c>
       <c r="Q77" s="29"/>
     </row>
     <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
[BRO] Overstap naar MIM 1.1.1 en NEN3610:2022
BRO volgt voor conceptuele modellen MIM 1.1.1, voor logische modellen
NEN3610:2022.

Minor?
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -1748,10 +1748,10 @@
   <dimension ref="A1:T144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R89" sqref="H89:R89"/>
+      <selection pane="bottomRight" activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Omzetting van conceptuele schema's.
Nieuwe stap in #247 - alle conceptuele schemas zijn onder een owner
opgenomen, en de configuratie is klaar om getest te worden op basis van
aangeleverde regressietestgevallen.

De configuraties zijn ook opgetild naar NEN3610-2022 en MIM111. Hierdoor
kunnen major verschillen ontstaan.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="378">
   <si>
     <t>Name</t>
   </si>
@@ -1150,6 +1150,15 @@
   </si>
   <si>
     <t>Should a regression test be performed on the results of this run?</t>
+  </si>
+  <si>
+    <t>xlinkversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Version of the xlinks specification</t>
+  </si>
+  <si>
+    <t>BROPROFILE</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1324,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1415,6 +1424,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1745,13 +1757,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T144"/>
+  <dimension ref="A1:T145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C73" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H73" sqref="H73"/>
+      <selection pane="bottomRight" activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1982,16 +1994,16 @@
       <c r="S6" s="23"/>
     </row>
     <row r="7" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="51" t="b">
+      <c r="D7" s="52" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -2011,10 +2023,10 @@
       </c>
     </row>
     <row r="8" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
       <c r="G8" s="23"/>
       <c r="L8" s="50"/>
       <c r="M8" s="23"/>
@@ -3284,16 +3296,16 @@
       </c>
     </row>
     <row r="47" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="51" t="s">
+      <c r="A47" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="51" t="s">
+      <c r="B47" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="51" t="s">
+      <c r="C47" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="51" t="b">
+      <c r="D47" s="52" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="2" t="b">
@@ -3313,10 +3325,10 @@
       <c r="S47" s="23"/>
     </row>
     <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="51"/>
-      <c r="B48" s="51"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
+      <c r="A48" s="52"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
       <c r="G48" s="23"/>
       <c r="L48" s="50"/>
       <c r="M48" s="23"/>
@@ -5760,64 +5772,85 @@
       </c>
       <c r="S120" s="29"/>
     </row>
-    <row r="121" spans="1:20" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A121" s="30" t="s">
+    <row r="121" spans="1:20" s="51" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="51" t="s">
+        <v>375</v>
+      </c>
+      <c r="B121" s="51" t="s">
+        <v>271</v>
+      </c>
+      <c r="C121" s="51" t="s">
+        <v>376</v>
+      </c>
+      <c r="D121" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="F121" s="51" t="s">
+        <v>377</v>
+      </c>
+      <c r="G121" s="29"/>
+      <c r="M121" s="29"/>
+      <c r="S121" s="29"/>
+    </row>
+    <row r="122" spans="1:20" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A122" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="B121" s="30" t="s">
+      <c r="B122" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C121" s="30" t="s">
+      <c r="C122" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="D121" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E121" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F121" s="30" t="s">
+      <c r="D122" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E122" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F122" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G121" s="29"/>
-      <c r="L121" s="50"/>
-      <c r="M121" s="29"/>
-      <c r="R121" s="50"/>
-      <c r="S121" s="29"/>
-    </row>
-    <row r="122" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A122" s="2" t="s">
+      <c r="G122" s="29"/>
+      <c r="L122" s="50"/>
+      <c r="M122" s="29"/>
+      <c r="R122" s="50"/>
+      <c r="S122" s="29"/>
+    </row>
+    <row r="123" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A123" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B123" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D122" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E122" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F122" s="2" t="s">
+      <c r="D123" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E123" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F123" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G122" s="23"/>
-      <c r="L122" s="50"/>
-      <c r="M122" s="23"/>
-      <c r="N122" s="17"/>
-      <c r="O122" s="17"/>
-      <c r="P122" s="17"/>
-      <c r="Q122" s="17"/>
-      <c r="R122" s="50"/>
-      <c r="S122" s="23"/>
-    </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T123"/>
+      <c r="G123" s="23"/>
+      <c r="L123" s="50"/>
+      <c r="M123" s="23"/>
+      <c r="N123" s="17"/>
+      <c r="O123" s="17"/>
+      <c r="P123" s="17"/>
+      <c r="Q123" s="17"/>
+      <c r="R123" s="50"/>
+      <c r="S123" s="23"/>
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A124" s="51"/>
       <c r="T124"/>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.4">
@@ -5879,6 +5912,9 @@
     </row>
     <row r="144" spans="20:20" x14ac:dyDescent="0.4">
       <c r="T144"/>
+    </row>
+    <row r="145" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T145"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
properties aanpassingen mbt gitcfg voor BRO en IHW
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\BRO\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1977B04-1ECB-479B-892C-31F07D8A43F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12060"/>
+    <workbookView xWindow="48430" yWindow="6110" windowWidth="24690" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BRO" sheetId="3" r:id="rId1"/>
@@ -1164,7 +1165,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1324,7 +1325,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1352,22 +1353,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1392,25 +1381,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="6" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1429,54 +1399,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
-    <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
-    <cellStyle name="Good" xfId="6" builtinId="26"/>
+    <cellStyle name="Controlecel" xfId="2" builtinId="23"/>
+    <cellStyle name="Goed" xfId="6" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
+    <cellStyle name="Ongeldig" xfId="3" builtinId="27"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Verklarende tekst" xfId="4" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1753,17 +1684,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:T145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F121" sqref="F121"/>
+      <selection pane="bottomRight" activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1774,19 +1705,19 @@
     <col min="4" max="4" width="13.23046875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="33.4609375" customWidth="1"/>
-    <col min="7" max="7" width="3.921875" style="25" customWidth="1"/>
+    <col min="7" max="7" width="3.921875" style="21" customWidth="1"/>
     <col min="8" max="8" width="18.4609375" customWidth="1"/>
     <col min="9" max="9" width="17.61328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.3046875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.84375" customWidth="1"/>
-    <col min="12" max="12" width="17.61328125" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.61328125" style="25" customWidth="1"/>
+    <col min="12" max="12" width="17.61328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.61328125" style="21" customWidth="1"/>
     <col min="14" max="14" width="18.4609375" customWidth="1"/>
     <col min="15" max="15" width="17.61328125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.3046875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.84375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.61328125" style="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.15234375" style="25" customWidth="1"/>
+    <col min="18" max="18" width="17.61328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.15234375" style="21" customWidth="1"/>
     <col min="20" max="20" width="27.3046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1809,7 +1740,7 @@
       <c r="F1" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="G1" s="21"/>
+      <c r="G1" s="17"/>
       <c r="H1" s="4" t="s">
         <v>300</v>
       </c>
@@ -1825,7 +1756,7 @@
       <c r="L1" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="M1" s="21"/>
+      <c r="M1" s="17"/>
       <c r="N1" s="4" t="s">
         <v>300</v>
       </c>
@@ -1841,14 +1772,14 @@
       <c r="R1" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="S1" s="21"/>
+      <c r="S1" s="17"/>
       <c r="T1" s="3" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
-      <c r="G2" s="22"/>
+      <c r="G2" s="18"/>
       <c r="H2" s="3" t="s">
         <v>302</v>
       </c>
@@ -1864,7 +1795,7 @@
       <c r="L2" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="M2" s="22"/>
+      <c r="M2" s="18"/>
       <c r="N2" s="3" t="s">
         <v>306</v>
       </c>
@@ -1880,7 +1811,7 @@
       <c r="R2" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="S2" s="22"/>
+      <c r="S2" s="18"/>
       <c r="T2" s="5"/>
     </row>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
@@ -1899,15 +1830,9 @@
       <c r="E3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="23"/>
+      <c r="G3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="S3" s="19"/>
     </row>
     <row r="4" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
@@ -1928,15 +1853,9 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="23"/>
+      <c r="G4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="S4" s="19"/>
       <c r="T4" s="8" t="s">
         <v>222</v>
       </c>
@@ -1960,15 +1879,9 @@
       <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="23"/>
+      <c r="G5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="S5" s="19"/>
       <c r="T5" s="8" t="s">
         <v>223</v>
       </c>
@@ -1989,53 +1902,41 @@
       <c r="E6" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="S6" s="23"/>
+      <c r="G6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="S6" s="19"/>
     </row>
     <row r="7" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="52" t="b">
+      <c r="D7" s="28" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="50"/>
-      <c r="S7" s="23"/>
+      <c r="G7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="S7" s="19"/>
       <c r="T7" s="2" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="G8" s="23"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="23"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="G8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="S8" s="19"/>
     </row>
     <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
@@ -2056,9 +1957,9 @@
       <c r="F9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="S9" s="23"/>
+      <c r="G9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="S9" s="19"/>
     </row>
     <row r="10" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
@@ -2076,9 +1977,9 @@
       <c r="E10" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="S10" s="23"/>
+      <c r="G10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="S10" s="19"/>
     </row>
     <row r="11" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
@@ -2099,52 +2000,45 @@
       <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="23"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="23"/>
+      <c r="G11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="S11" s="19"/>
       <c r="T11" s="7"/>
     </row>
-    <row r="12" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D12" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="23"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="12" t="s">
+      <c r="D12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="O12" s="17" t="s">
+      <c r="O12" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="P12" s="17" t="s">
+      <c r="P12" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="Q12" s="17" t="s">
+      <c r="Q12" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="R12" s="50" t="s">
+      <c r="R12" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="S12" s="23"/>
+      <c r="S12" s="19"/>
       <c r="T12" t="s">
         <v>289</v>
       </c>
@@ -2168,9 +2062,9 @@
       <c r="F13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="S13" s="23"/>
+      <c r="G13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="S13" s="19"/>
     </row>
     <row r="14" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
@@ -2188,7 +2082,7 @@
       <c r="E14" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G14" s="23"/>
+      <c r="G14" s="19"/>
       <c r="H14" s="2" t="s">
         <v>17</v>
       </c>
@@ -2201,26 +2095,26 @@
       <c r="K14" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="L14" s="50" t="s">
+      <c r="L14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="23"/>
-      <c r="N14" s="17" t="s">
+      <c r="M14" s="19"/>
+      <c r="N14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O14" s="17" t="s">
+      <c r="O14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P14" s="17" t="s">
+      <c r="P14" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="Q14" s="17" t="s">
+      <c r="Q14" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="R14" s="50" t="s">
+      <c r="R14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S14" s="23"/>
+      <c r="S14" s="19"/>
       <c r="T14" s="2" t="s">
         <v>249</v>
       </c>
@@ -2244,15 +2138,9 @@
       <c r="F15" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="G15" s="23"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="50"/>
-      <c r="S15" s="23"/>
+      <c r="G15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="S15" s="19"/>
     </row>
     <row r="16" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
@@ -2273,15 +2161,9 @@
       <c r="F16" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="G16" s="23"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="50"/>
-      <c r="S16" s="23"/>
+      <c r="G16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="S16" s="19"/>
     </row>
     <row r="17" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
@@ -2298,18 +2180,9 @@
       <c r="F17" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="G17" s="23"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="50"/>
-      <c r="S17" s="23"/>
+      <c r="G17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="S17" s="19"/>
     </row>
     <row r="18" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
@@ -2327,15 +2200,9 @@
       <c r="E18" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G18" s="23"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="50"/>
-      <c r="S18" s="23"/>
+      <c r="G18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="S18" s="19"/>
     </row>
     <row r="19" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
@@ -2353,18 +2220,12 @@
       <c r="E19" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="G19" s="23"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="50"/>
-      <c r="S19" s="23"/>
+      <c r="G19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="S19" s="19"/>
     </row>
     <row r="20" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
@@ -2382,18 +2243,12 @@
       <c r="E20" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="G20" s="23"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="50"/>
-      <c r="S20" s="23"/>
+      <c r="G20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="S20" s="19"/>
     </row>
     <row r="21" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
@@ -2411,7 +2266,7 @@
       <c r="E21" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G21" s="23"/>
+      <c r="G21" s="19"/>
       <c r="H21" s="2" t="s">
         <v>14</v>
       </c>
@@ -2424,26 +2279,26 @@
       <c r="K21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L21" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M21" s="23"/>
-      <c r="N21" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O21" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P21" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q21" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R21" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S21" s="23"/>
+      <c r="L21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" s="19"/>
+      <c r="N21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S21" s="19"/>
     </row>
     <row r="22" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
@@ -2464,9 +2319,9 @@
       <c r="F22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="S22" s="23"/>
+      <c r="G22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="S22" s="19"/>
     </row>
     <row r="23" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
@@ -2484,9 +2339,9 @@
       <c r="E23" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="S23" s="23"/>
+      <c r="G23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="S23" s="19"/>
     </row>
     <row r="24" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
@@ -2504,7 +2359,7 @@
       <c r="E24" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G24" s="23"/>
+      <c r="G24" s="19"/>
       <c r="H24" s="2" t="s">
         <v>14</v>
       </c>
@@ -2517,26 +2372,26 @@
       <c r="K24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L24" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="M24" s="23"/>
-      <c r="N24" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O24" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="P24" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q24" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R24" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="S24" s="23"/>
+      <c r="L24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" s="19"/>
+      <c r="N24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S24" s="19"/>
     </row>
     <row r="25" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
@@ -2554,7 +2409,7 @@
       <c r="E25" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G25" s="23"/>
+      <c r="G25" s="19"/>
       <c r="H25" s="2" t="s">
         <v>14</v>
       </c>
@@ -2567,76 +2422,76 @@
       <c r="K25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L25" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M25" s="23"/>
-      <c r="N25" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O25" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P25" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q25" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R25" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S25" s="23"/>
-    </row>
-    <row r="26" spans="1:20" s="44" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="44" t="s">
+      <c r="L25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" s="19"/>
+      <c r="N25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S25" s="19"/>
+    </row>
+    <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="D26" s="44" t="b">
-        <v>0</v>
-      </c>
-      <c r="E26" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" s="29"/>
-      <c r="H26" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="K26" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M26" s="29"/>
-      <c r="N26" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="O26" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="P26" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q26" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="R26" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S26" s="29"/>
+      <c r="D26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" s="19"/>
+      <c r="N26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S26" s="19"/>
     </row>
     <row r="27" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
@@ -2657,15 +2512,9 @@
       <c r="F27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="23"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="23"/>
+      <c r="G27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="S27" s="19"/>
       <c r="T27" s="8" t="s">
         <v>275</v>
       </c>
@@ -2686,7 +2535,7 @@
       <c r="E28" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G28" s="23"/>
+      <c r="G28" s="19"/>
       <c r="H28" s="2" t="s">
         <v>14</v>
       </c>
@@ -2699,182 +2548,178 @@
       <c r="K28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L28" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M28" s="23"/>
-      <c r="N28" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O28" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P28" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q28" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R28" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S28" s="23"/>
-    </row>
-    <row r="29" spans="1:20" s="41" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="41" t="s">
+      <c r="L28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M28" s="19"/>
+      <c r="N28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S28" s="19"/>
+    </row>
+    <row r="29" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D29" s="41" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="41" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="29"/>
-      <c r="H29" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="L29" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M29" s="29"/>
-      <c r="N29" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="O29" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="P29" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q29" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="R29" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="S29" s="29"/>
-    </row>
-    <row r="30" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="32" t="s">
+      <c r="D29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="19"/>
+      <c r="H29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M29" s="19"/>
+      <c r="N29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S29" s="19"/>
+    </row>
+    <row r="30" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D30" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="29"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="29"/>
-      <c r="R30" s="50"/>
-      <c r="S30" s="29"/>
-      <c r="T30" s="32" t="s">
+      <c r="D30" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="32" t="s">
+    <row r="31" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D31" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="32" t="s">
+      <c r="D31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="G31" s="29"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="29"/>
-      <c r="R31" s="50"/>
-      <c r="S31" s="29"/>
-      <c r="T31" s="32" t="s">
+      <c r="G31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="46" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="46" t="s">
+    <row r="32" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="46" t="s">
+      <c r="C32" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="D32" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" s="29"/>
-      <c r="H32" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="K32" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="L32" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="M32" s="29"/>
-      <c r="N32" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="O32" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="P32" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q32" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="R32" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="S32" s="29"/>
+      <c r="D32" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="19"/>
+      <c r="H32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32" s="19"/>
+      <c r="N32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S32" s="19"/>
     </row>
     <row r="33" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
@@ -2892,380 +2737,379 @@
       <c r="E33" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G33" s="23"/>
+      <c r="G33" s="19"/>
       <c r="H33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="40" t="s">
+      <c r="I33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J33" s="40" t="s">
+      <c r="J33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="40" t="s">
+      <c r="K33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L33" s="50" t="s">
+      <c r="L33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M33" s="23"/>
-      <c r="N33" s="17" t="s">
+      <c r="M33" s="19"/>
+      <c r="N33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O33" s="40" t="s">
+      <c r="O33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P33" s="40" t="s">
+      <c r="P33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="40" t="s">
+      <c r="Q33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R33" s="50" t="s">
+      <c r="R33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S33" s="23"/>
+      <c r="S33" s="19"/>
       <c r="T33" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="33" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A34" s="33" t="s">
+    <row r="34" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D34" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="G34" s="29"/>
-      <c r="I34" s="33" t="s">
+      <c r="D34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" s="19"/>
+      <c r="I34" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="J34" s="39" t="s">
+      <c r="J34" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="K34" s="39" t="s">
+      <c r="K34" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="L34" s="50" t="s">
+      <c r="L34" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="M34" s="29"/>
-      <c r="R34" s="50"/>
-      <c r="S34" s="29"/>
-    </row>
-    <row r="35" spans="1:20" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A35" s="34" t="s">
+      <c r="M34" s="19"/>
+      <c r="S34" s="19"/>
+    </row>
+    <row r="35" spans="1:20" s="23" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A35" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D35" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35" s="35"/>
-      <c r="M35" s="35"/>
-      <c r="S35" s="35"/>
-    </row>
-    <row r="36" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="34" t="s">
+      <c r="D35" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="S35" s="24"/>
+    </row>
+    <row r="36" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D36" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" s="35"/>
-      <c r="M36" s="35"/>
-      <c r="S36" s="35"/>
-    </row>
-    <row r="37" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="34" t="s">
+      <c r="D36" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="S36" s="24"/>
+    </row>
+    <row r="37" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C37" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="35"/>
-      <c r="M37" s="35"/>
-      <c r="S37" s="35"/>
-    </row>
-    <row r="38" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="34" t="s">
+      <c r="D37" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="S37" s="24"/>
+    </row>
+    <row r="38" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="23" t="s">
         <v>367</v>
       </c>
-      <c r="D38" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="35"/>
-      <c r="H38" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="J38" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="K38" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="L38" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="M38" s="35"/>
-      <c r="S38" s="35"/>
-    </row>
-    <row r="39" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="34" t="s">
+      <c r="D38" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="24"/>
+      <c r="H38" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J38" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K38" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L38" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M38" s="24"/>
+      <c r="S38" s="24"/>
+    </row>
+    <row r="39" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="23" t="s">
         <v>336</v>
       </c>
-      <c r="D39" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="35"/>
-      <c r="H39" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="I39" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="J39" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="K39" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="L39" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="M39" s="35"/>
-      <c r="S39" s="35"/>
-    </row>
-    <row r="40" spans="1:20" s="36" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A40" s="36" t="s">
+      <c r="D39" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="24"/>
+      <c r="H39" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L39" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M39" s="24"/>
+      <c r="S39" s="24"/>
+    </row>
+    <row r="40" spans="1:20" s="25" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A40" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" s="35"/>
-      <c r="M40" s="35"/>
-      <c r="S40" s="35"/>
-    </row>
-    <row r="41" spans="1:20" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A41" s="34" t="s">
+      <c r="D40" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="24"/>
+      <c r="M40" s="24"/>
+      <c r="S40" s="24"/>
+    </row>
+    <row r="41" spans="1:20" s="23" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A41" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="F41" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="35"/>
-      <c r="M41" s="35"/>
-      <c r="S41" s="35"/>
-    </row>
-    <row r="42" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="36" t="s">
+      <c r="D41" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="S41" s="24"/>
+    </row>
+    <row r="42" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="G42" s="35"/>
-      <c r="H42" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="I42" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J42" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="K42" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="L42" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="M42" s="35"/>
-      <c r="N42" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="O42" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="P42" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q42" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="R42" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="S42" s="35"/>
-    </row>
-    <row r="43" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="36" t="s">
+      <c r="D42" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" s="24"/>
+      <c r="H42" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K42" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="L42" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="M42" s="24"/>
+      <c r="N42" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="O42" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P42" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q42" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="R42" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="S42" s="24"/>
+    </row>
+    <row r="43" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="25" t="s">
         <v>325</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="C43" s="25" t="s">
         <v>326</v>
       </c>
-      <c r="D43" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43" s="36" t="s">
+      <c r="D43" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="25" t="s">
         <v>329</v>
       </c>
-      <c r="G43" s="35"/>
-      <c r="M43" s="35"/>
-      <c r="S43" s="35"/>
-    </row>
-    <row r="44" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="34" t="s">
+      <c r="G43" s="24"/>
+      <c r="M43" s="24"/>
+      <c r="S43" s="24"/>
+    </row>
+    <row r="44" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="D44" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G44" s="35"/>
-      <c r="M44" s="35"/>
-      <c r="S44" s="35"/>
-    </row>
-    <row r="45" spans="1:20" s="37" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A45" s="37" t="s">
+      <c r="D44" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="24"/>
+      <c r="M44" s="24"/>
+      <c r="S44" s="24"/>
+    </row>
+    <row r="45" spans="1:20" s="26" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="37" t="s">
+      <c r="C45" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="F45" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G45" s="38"/>
-      <c r="M45" s="38"/>
-      <c r="S45" s="38"/>
-      <c r="T45" s="37" t="s">
+      <c r="D45" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="S45" s="27"/>
+      <c r="T45" s="26" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3288,24 +3132,24 @@
       <c r="F46" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G46" s="23"/>
-      <c r="M46" s="23"/>
-      <c r="S46" s="23"/>
+      <c r="G46" s="19"/>
+      <c r="M46" s="19"/>
+      <c r="S46" s="19"/>
       <c r="T46" s="7" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="52" t="s">
+      <c r="A47" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="52" t="s">
+      <c r="B47" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="52" t="s">
+      <c r="C47" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="52" t="b">
+      <c r="D47" s="28" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="2" t="b">
@@ -3314,30 +3158,18 @@
       <c r="F47" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="23"/>
-      <c r="L47" s="50"/>
-      <c r="M47" s="23"/>
-      <c r="N47" s="17"/>
-      <c r="O47" s="17"/>
-      <c r="P47" s="17"/>
-      <c r="Q47" s="17"/>
-      <c r="R47" s="50"/>
-      <c r="S47" s="23"/>
+      <c r="G47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="S47" s="19"/>
     </row>
     <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="52"/>
-      <c r="B48" s="52"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="G48" s="23"/>
-      <c r="L48" s="50"/>
-      <c r="M48" s="23"/>
-      <c r="N48" s="17"/>
-      <c r="O48" s="17"/>
-      <c r="P48" s="17"/>
-      <c r="Q48" s="17"/>
-      <c r="R48" s="50"/>
-      <c r="S48" s="23"/>
+      <c r="A48" s="28"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="G48" s="19"/>
+      <c r="M48" s="19"/>
+      <c r="S48" s="19"/>
     </row>
     <row r="49" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
@@ -3355,15 +3187,9 @@
       <c r="E49" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G49" s="23"/>
-      <c r="L49" s="50"/>
-      <c r="M49" s="23"/>
-      <c r="N49" s="17"/>
-      <c r="O49" s="17"/>
-      <c r="P49" s="17"/>
-      <c r="Q49" s="17"/>
-      <c r="R49" s="50"/>
-      <c r="S49" s="23"/>
+      <c r="G49" s="19"/>
+      <c r="M49" s="19"/>
+      <c r="S49" s="19"/>
     </row>
     <row r="50" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
@@ -3381,15 +3207,9 @@
       <c r="E50" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G50" s="23"/>
-      <c r="L50" s="50"/>
-      <c r="M50" s="23"/>
-      <c r="N50" s="17"/>
-      <c r="O50" s="17"/>
-      <c r="P50" s="17"/>
-      <c r="Q50" s="17"/>
-      <c r="R50" s="50"/>
-      <c r="S50" s="23"/>
+      <c r="G50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="S50" s="19"/>
     </row>
     <row r="51" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
@@ -3410,15 +3230,9 @@
       <c r="F51" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="G51" s="26"/>
-      <c r="L51" s="50"/>
-      <c r="M51" s="23"/>
-      <c r="N51" s="17"/>
-      <c r="O51" s="17"/>
-      <c r="P51" s="17"/>
-      <c r="Q51" s="17"/>
-      <c r="R51" s="50"/>
-      <c r="S51" s="23"/>
+      <c r="G51" s="22"/>
+      <c r="M51" s="19"/>
+      <c r="S51" s="19"/>
       <c r="T51" s="2" t="s">
         <v>205</v>
       </c>
@@ -3436,39 +3250,39 @@
         <v>0</v>
       </c>
       <c r="F52" s="6"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="17" t="s">
+      <c r="G52" s="22"/>
+      <c r="H52" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="I52" s="17" t="s">
+      <c r="I52" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="J52" s="17" t="s">
+      <c r="J52" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="K52" s="17" t="s">
+      <c r="K52" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="L52" s="50" t="s">
+      <c r="L52" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="M52" s="23"/>
-      <c r="N52" s="17" t="s">
+      <c r="M52" s="19"/>
+      <c r="N52" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="O52" s="17" t="s">
+      <c r="O52" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="P52" s="17" t="s">
+      <c r="P52" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="Q52" s="17" t="s">
+      <c r="Q52" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="R52" s="50" t="s">
+      <c r="R52" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="S52" s="23"/>
+      <c r="S52" s="19"/>
     </row>
     <row r="53" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="7" t="s">
@@ -3489,9 +3303,9 @@
       <c r="F53" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G53" s="23"/>
-      <c r="M53" s="23"/>
-      <c r="S53" s="23"/>
+      <c r="G53" s="19"/>
+      <c r="M53" s="19"/>
+      <c r="S53" s="19"/>
       <c r="T53"/>
     </row>
     <row r="54" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3513,9 +3327,9 @@
       <c r="F54" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="G54" s="23"/>
-      <c r="M54" s="23"/>
-      <c r="S54" s="23"/>
+      <c r="G54" s="19"/>
+      <c r="M54" s="19"/>
+      <c r="S54" s="19"/>
     </row>
     <row r="55" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
@@ -3536,15 +3350,9 @@
       <c r="F55" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G55" s="23"/>
-      <c r="L55" s="50"/>
-      <c r="M55" s="23"/>
-      <c r="N55" s="17"/>
-      <c r="O55" s="17"/>
-      <c r="P55" s="17"/>
-      <c r="Q55" s="17"/>
-      <c r="R55" s="50"/>
-      <c r="S55" s="23"/>
+      <c r="G55" s="19"/>
+      <c r="M55" s="19"/>
+      <c r="S55" s="19"/>
     </row>
     <row r="56" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="7" t="s">
@@ -3565,9 +3373,9 @@
       <c r="F56" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G56" s="23"/>
-      <c r="M56" s="23"/>
-      <c r="S56" s="23"/>
+      <c r="G56" s="19"/>
+      <c r="M56" s="19"/>
+      <c r="S56" s="19"/>
     </row>
     <row r="57" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A57" s="7" t="s">
@@ -3588,9 +3396,9 @@
       <c r="F57" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G57" s="23"/>
-      <c r="M57" s="23"/>
-      <c r="S57" s="23"/>
+      <c r="G57" s="19"/>
+      <c r="M57" s="19"/>
+      <c r="S57" s="19"/>
       <c r="T57" s="7" t="s">
         <v>207</v>
       </c>
@@ -3614,43 +3422,43 @@
       <c r="F58" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G58" s="23"/>
-      <c r="M58" s="23"/>
-      <c r="S58" s="23"/>
-    </row>
-    <row r="59" spans="1:20" s="28" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A59" s="15" t="s">
+      <c r="G58" s="19"/>
+      <c r="M58" s="19"/>
+      <c r="S58" s="19"/>
+    </row>
+    <row r="59" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A59" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="D59" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="15" t="s">
+      <c r="D59" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="G59" s="24"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="15"/>
-      <c r="L59" s="15"/>
-      <c r="M59" s="24"/>
-      <c r="N59" s="15"/>
-      <c r="O59" s="15"/>
-      <c r="P59" s="15"/>
-      <c r="Q59" s="15"/>
-      <c r="R59" s="15"/>
-      <c r="S59" s="24"/>
-      <c r="T59" s="15"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
+      <c r="M59" s="20"/>
+      <c r="N59" s="13"/>
+      <c r="O59" s="13"/>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="R59" s="13"/>
+      <c r="S59" s="20"/>
+      <c r="T59" s="13"/>
     </row>
     <row r="60" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
@@ -3671,9 +3479,9 @@
       <c r="F60" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="G60" s="23"/>
-      <c r="M60" s="23"/>
-      <c r="S60" s="23"/>
+      <c r="G60" s="19"/>
+      <c r="M60" s="19"/>
+      <c r="S60" s="19"/>
     </row>
     <row r="61" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
@@ -3691,22 +3499,22 @@
       <c r="E61" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F61" s="18" t="s">
+      <c r="F61" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="G61" s="23"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
-      <c r="J61" s="18"/>
-      <c r="K61" s="18"/>
-      <c r="L61" s="18"/>
-      <c r="M61" s="23"/>
-      <c r="N61" s="18"/>
-      <c r="O61" s="18"/>
-      <c r="P61" s="18"/>
-      <c r="Q61" s="18"/>
-      <c r="R61" s="18"/>
-      <c r="S61" s="23"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="19"/>
+      <c r="N61" s="14"/>
+      <c r="O61" s="14"/>
+      <c r="P61" s="14"/>
+      <c r="Q61" s="14"/>
+      <c r="R61" s="14"/>
+      <c r="S61" s="19"/>
     </row>
     <row r="62" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A62" s="7" t="s">
@@ -3727,43 +3535,43 @@
       <c r="F62" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="G62" s="23"/>
-      <c r="M62" s="23"/>
-      <c r="S62" s="23"/>
+      <c r="G62" s="19"/>
+      <c r="M62" s="19"/>
+      <c r="S62" s="19"/>
     </row>
     <row r="63" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" s="15" t="s">
+      <c r="A63" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C63" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="D63" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="15" t="s">
+      <c r="D63" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="G63" s="24"/>
-      <c r="H63" s="15"/>
-      <c r="I63" s="15"/>
-      <c r="J63" s="15"/>
-      <c r="K63" s="15"/>
-      <c r="L63" s="15"/>
-      <c r="M63" s="24"/>
-      <c r="N63" s="15"/>
-      <c r="O63" s="15"/>
-      <c r="P63" s="15"/>
-      <c r="Q63" s="15"/>
-      <c r="R63" s="15"/>
-      <c r="S63" s="24"/>
-      <c r="T63" s="15" t="s">
+      <c r="G63" s="20"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
+      <c r="M63" s="20"/>
+      <c r="N63" s="13"/>
+      <c r="O63" s="13"/>
+      <c r="P63" s="13"/>
+      <c r="Q63" s="13"/>
+      <c r="R63" s="13"/>
+      <c r="S63" s="20"/>
+      <c r="T63" s="13" t="s">
         <v>263</v>
       </c>
     </row>
@@ -3786,9 +3594,9 @@
       <c r="F64" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G64" s="23"/>
-      <c r="M64" s="23"/>
-      <c r="S64" s="23"/>
+      <c r="G64" s="19"/>
+      <c r="M64" s="19"/>
+      <c r="S64" s="19"/>
       <c r="T64" s="7" t="s">
         <v>208</v>
       </c>
@@ -3812,87 +3620,85 @@
       <c r="F65" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="G65" s="23"/>
-      <c r="M65" s="23"/>
-      <c r="S65" s="23"/>
+      <c r="G65" s="19"/>
+      <c r="M65" s="19"/>
+      <c r="S65" s="19"/>
       <c r="T65" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="1:20" s="31" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A66" s="31" t="s">
+    <row r="66" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A66" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B66" s="31" t="s">
+      <c r="B66" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="31" t="s">
+      <c r="C66" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D66" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G66" s="29"/>
-      <c r="H66" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="I66" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="J66" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="K66" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="L66" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M66" s="29"/>
-      <c r="N66" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="O66" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="P66" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q66" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="R66" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S66" s="29"/>
-    </row>
-    <row r="67" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="42" t="s">
+      <c r="D66" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G66" s="19"/>
+      <c r="H66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M66" s="19"/>
+      <c r="N66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S66" s="19"/>
+    </row>
+    <row r="67" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="42" t="s">
+      <c r="C67" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="D67" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="42" t="s">
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="G67" s="29"/>
-      <c r="L67" s="50"/>
-      <c r="M67" s="29"/>
-      <c r="R67" s="50"/>
-      <c r="S67" s="29"/>
+      <c r="G67" s="19"/>
+      <c r="M67" s="19"/>
+      <c r="S67" s="19"/>
     </row>
     <row r="68" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="7" t="s">
@@ -3913,9 +3719,9 @@
       <c r="F68" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G68" s="23"/>
-      <c r="M68" s="23"/>
-      <c r="S68" s="23"/>
+      <c r="G68" s="19"/>
+      <c r="M68" s="19"/>
+      <c r="S68" s="19"/>
       <c r="T68" s="7" t="s">
         <v>247</v>
       </c>
@@ -3936,39 +3742,39 @@
       <c r="E69" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G69" s="23"/>
+      <c r="G69" s="19"/>
       <c r="H69" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="I69" s="17" t="s">
+      <c r="I69" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="J69" s="17" t="s">
+      <c r="J69" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="K69" s="17" t="s">
+      <c r="K69" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L69" s="50" t="s">
+      <c r="L69" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="M69" s="23"/>
-      <c r="N69" s="17" t="s">
+      <c r="M69" s="19"/>
+      <c r="N69" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="O69" s="17" t="s">
+      <c r="O69" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="P69" s="17" t="s">
+      <c r="P69" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="Q69" s="17" t="s">
+      <c r="Q69" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="R69" s="50" t="s">
+      <c r="R69" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="S69" s="23"/>
+      <c r="S69" s="19"/>
       <c r="T69" s="2" t="s">
         <v>211</v>
       </c>
@@ -3992,15 +3798,9 @@
       <c r="F70" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="G70" s="23"/>
-      <c r="L70" s="50"/>
-      <c r="M70" s="23"/>
-      <c r="N70" s="17"/>
-      <c r="O70" s="17"/>
-      <c r="P70" s="17"/>
-      <c r="Q70" s="17"/>
-      <c r="R70" s="50"/>
-      <c r="S70" s="23"/>
+      <c r="G70" s="19"/>
+      <c r="M70" s="19"/>
+      <c r="S70" s="19"/>
       <c r="T70" s="2" t="s">
         <v>212</v>
       </c>
@@ -4024,41 +3824,33 @@
       <c r="F71" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="G71" s="23"/>
-      <c r="L71" s="50"/>
-      <c r="M71" s="23"/>
-      <c r="N71" s="17"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="17"/>
-      <c r="Q71" s="17"/>
-      <c r="R71" s="50"/>
-      <c r="S71" s="23"/>
-    </row>
-    <row r="72" spans="1:20" s="27" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" s="27" t="s">
+      <c r="G71" s="19"/>
+      <c r="M71" s="19"/>
+      <c r="S71" s="19"/>
+    </row>
+    <row r="72" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B72" s="27" t="s">
+      <c r="B72" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="27" t="s">
+      <c r="C72" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="D72" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="27" t="s">
+      <c r="D72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="G72" s="23"/>
-      <c r="L72" s="50"/>
-      <c r="M72" s="23"/>
-      <c r="R72" s="50"/>
-      <c r="S72" s="23"/>
-      <c r="T72" s="27" t="s">
+      <c r="G72" s="19"/>
+      <c r="M72" s="19"/>
+      <c r="S72" s="19"/>
+      <c r="T72" s="2" t="s">
         <v>313</v>
       </c>
     </row>
@@ -4078,39 +3870,39 @@
       <c r="E73" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G73" s="23"/>
-      <c r="H73" s="17" t="s">
+      <c r="G73" s="19"/>
+      <c r="H73" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="I73" s="17" t="s">
+      <c r="I73" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="J73" s="17" t="s">
+      <c r="J73" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="K73" s="17" t="s">
+      <c r="K73" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="L73" s="50" t="s">
+      <c r="L73" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="M73" s="23"/>
-      <c r="N73" s="17" t="s">
+      <c r="M73" s="19"/>
+      <c r="N73" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="O73" s="17" t="s">
+      <c r="O73" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="P73" s="17" t="s">
+      <c r="P73" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="Q73" s="17" t="s">
+      <c r="Q73" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="R73" s="50" t="s">
+      <c r="R73" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="S73" s="23"/>
+      <c r="S73" s="19"/>
     </row>
     <row r="74" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
@@ -4128,40 +3920,32 @@
       <c r="E74" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G74" s="23"/>
-      <c r="L74" s="50"/>
-      <c r="M74" s="23"/>
-      <c r="N74" s="17"/>
-      <c r="O74" s="17"/>
-      <c r="P74" s="17"/>
-      <c r="Q74" s="17"/>
-      <c r="R74" s="50"/>
-      <c r="S74" s="23"/>
-    </row>
-    <row r="75" spans="1:20" s="46" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="46" t="s">
+      <c r="G74" s="19"/>
+      <c r="M74" s="19"/>
+      <c r="S74" s="19"/>
+    </row>
+    <row r="75" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B75" s="46" t="s">
+      <c r="B75" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="46" t="s">
+      <c r="C75" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="D75" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" s="46" t="s">
+      <c r="D75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G75" s="29"/>
-      <c r="L75" s="50"/>
-      <c r="M75" s="29"/>
-      <c r="R75" s="50"/>
-      <c r="S75" s="29"/>
+      <c r="G75" s="19"/>
+      <c r="M75" s="19"/>
+      <c r="S75" s="19"/>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
@@ -4185,54 +3969,54 @@
       <c r="T76"/>
     </row>
     <row r="77" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A77" s="34" t="s">
+      <c r="A77" s="23" t="s">
         <v>360</v>
       </c>
-      <c r="B77" s="34" t="s">
+      <c r="B77" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="34" t="s">
+      <c r="C77" s="23" t="s">
         <v>361</v>
       </c>
-      <c r="D77" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="G77" s="29"/>
-      <c r="H77" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="I77" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="J77" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="K77" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="L77" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="M77" s="29"/>
-      <c r="N77" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="O77" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="P77" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q77" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="R77" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S77" s="29"/>
+      <c r="D77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G77" s="19"/>
+      <c r="H77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M77" s="19"/>
+      <c r="N77" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O77" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P77" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q77" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R77" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S77" s="19"/>
     </row>
     <row r="78" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
@@ -4253,15 +4037,9 @@
       <c r="F78" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G78" s="23"/>
-      <c r="L78" s="50"/>
-      <c r="M78" s="23"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="17"/>
-      <c r="P78" s="17"/>
-      <c r="Q78" s="17"/>
-      <c r="R78" s="50"/>
-      <c r="S78" s="23"/>
+      <c r="G78" s="19"/>
+      <c r="M78" s="19"/>
+      <c r="S78" s="19"/>
     </row>
     <row r="79" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
@@ -4282,15 +4060,9 @@
       <c r="F79" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G79" s="23"/>
-      <c r="L79" s="50"/>
-      <c r="M79" s="23"/>
-      <c r="N79" s="17"/>
-      <c r="O79" s="17"/>
-      <c r="P79" s="17"/>
-      <c r="Q79" s="17"/>
-      <c r="R79" s="50"/>
-      <c r="S79" s="23"/>
+      <c r="G79" s="19"/>
+      <c r="M79" s="19"/>
+      <c r="S79" s="19"/>
     </row>
     <row r="80" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
@@ -4308,39 +4080,39 @@
       <c r="E80" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G80" s="23"/>
-      <c r="H80" s="17" t="s">
+      <c r="G80" s="19"/>
+      <c r="H80" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="I80" s="17" t="s">
+      <c r="I80" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="J80" s="17" t="s">
+      <c r="J80" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="K80" s="17" t="s">
+      <c r="K80" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="L80" s="50" t="s">
+      <c r="L80" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="M80" s="23"/>
-      <c r="N80" s="17" t="s">
+      <c r="M80" s="19"/>
+      <c r="N80" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="O80" s="17" t="s">
+      <c r="O80" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="P80" s="17" t="s">
+      <c r="P80" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="Q80" s="17" t="s">
+      <c r="Q80" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="R80" s="50" t="s">
+      <c r="R80" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="S80" s="23"/>
+      <c r="S80" s="19"/>
     </row>
     <row r="81" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
@@ -4361,15 +4133,9 @@
       <c r="F81" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="G81" s="23"/>
-      <c r="L81" s="50"/>
-      <c r="M81" s="23"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
-      <c r="Q81" s="17"/>
-      <c r="R81" s="50"/>
-      <c r="S81" s="23"/>
+      <c r="G81" s="19"/>
+      <c r="M81" s="19"/>
+      <c r="S81" s="19"/>
     </row>
     <row r="82" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="7" t="s">
@@ -4390,9 +4156,9 @@
       <c r="F82" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="G82" s="23"/>
-      <c r="M82" s="23"/>
-      <c r="S82" s="23"/>
+      <c r="G82" s="19"/>
+      <c r="M82" s="19"/>
+      <c r="S82" s="19"/>
       <c r="T82" s="7" t="s">
         <v>248</v>
       </c>
@@ -4416,7 +4182,7 @@
       <c r="F83" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G83" s="23"/>
+      <c r="G83" s="19"/>
       <c r="I83" s="2" t="s">
         <v>281</v>
       </c>
@@ -4426,14 +4192,8 @@
       <c r="K83" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="L83" s="50"/>
-      <c r="M83" s="23"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
-      <c r="P83" s="17"/>
-      <c r="Q83" s="17"/>
-      <c r="R83" s="50"/>
-      <c r="S83" s="23"/>
+      <c r="M83" s="19"/>
+      <c r="S83" s="19"/>
     </row>
     <row r="84" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A84" s="7" t="s">
@@ -4454,9 +4214,9 @@
       <c r="F84" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="G84" s="23"/>
-      <c r="M84" s="23"/>
-      <c r="S84" s="23"/>
+      <c r="G84" s="19"/>
+      <c r="M84" s="19"/>
+      <c r="S84" s="19"/>
       <c r="T84" s="8" t="s">
         <v>214</v>
       </c>
@@ -4477,39 +4237,39 @@
       <c r="E85" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G85" s="23"/>
-      <c r="H85" s="17" t="s">
+      <c r="G85" s="19"/>
+      <c r="H85" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="I85" s="17" t="s">
+      <c r="I85" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="J85" s="17" t="s">
+      <c r="J85" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="K85" s="17" t="s">
+      <c r="K85" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="L85" s="50" t="s">
+      <c r="L85" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="M85" s="23"/>
-      <c r="N85" s="17" t="s">
+      <c r="M85" s="19"/>
+      <c r="N85" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="O85" s="17" t="s">
+      <c r="O85" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="P85" s="17" t="s">
+      <c r="P85" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="Q85" s="17" t="s">
+      <c r="Q85" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="R85" s="50" t="s">
+      <c r="R85" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="S85" s="23"/>
+      <c r="S85" s="19"/>
     </row>
     <row r="86" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
@@ -4530,15 +4290,9 @@
       <c r="F86" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G86" s="23"/>
-      <c r="L86" s="50"/>
-      <c r="M86" s="23"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
-      <c r="Q86" s="17"/>
-      <c r="R86" s="50"/>
-      <c r="S86" s="23"/>
+      <c r="G86" s="19"/>
+      <c r="M86" s="19"/>
+      <c r="S86" s="19"/>
     </row>
     <row r="87" spans="1:20" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A87" s="7" t="s">
@@ -4559,9 +4313,9 @@
       <c r="F87" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G87" s="23"/>
-      <c r="M87" s="23"/>
-      <c r="S87" s="23"/>
+      <c r="G87" s="19"/>
+      <c r="M87" s="19"/>
+      <c r="S87" s="19"/>
       <c r="T87" s="8" t="s">
         <v>215</v>
       </c>
@@ -4585,49 +4339,49 @@
       <c r="F88" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G88" s="23"/>
-      <c r="M88" s="23"/>
-      <c r="S88" s="23"/>
+      <c r="G88" s="19"/>
+      <c r="M88" s="19"/>
+      <c r="S88" s="19"/>
       <c r="T88" s="7" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="89" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="34" t="s">
+      <c r="A89" s="23" t="s">
         <v>373</v>
       </c>
-      <c r="B89" s="34" t="s">
+      <c r="B89" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C89" s="34" t="s">
+      <c r="C89" s="23" t="s">
         <v>374</v>
       </c>
-      <c r="D89" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G89" s="29"/>
-      <c r="H89" s="34"/>
-      <c r="I89" s="34"/>
-      <c r="J89" s="34"/>
-      <c r="K89" s="34"/>
-      <c r="L89" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="M89" s="35"/>
-      <c r="N89" s="34"/>
-      <c r="O89" s="34"/>
-      <c r="P89" s="34"/>
-      <c r="Q89" s="34"/>
-      <c r="R89" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="S89" s="29"/>
+      <c r="D89" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G89" s="19"/>
+      <c r="H89" s="23"/>
+      <c r="I89" s="23"/>
+      <c r="J89" s="23"/>
+      <c r="K89" s="23"/>
+      <c r="L89" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M89" s="24"/>
+      <c r="N89" s="23"/>
+      <c r="O89" s="23"/>
+      <c r="P89" s="23"/>
+      <c r="Q89" s="23"/>
+      <c r="R89" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S89" s="19"/>
     </row>
     <row r="90" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
@@ -4648,54 +4402,46 @@
       <c r="F90" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G90" s="23"/>
-      <c r="L90" s="50"/>
-      <c r="M90" s="23"/>
-      <c r="N90" s="17"/>
-      <c r="O90" s="17"/>
-      <c r="P90" s="17"/>
-      <c r="Q90" s="17"/>
-      <c r="R90" s="50"/>
-      <c r="S90" s="23"/>
-    </row>
-    <row r="91" spans="1:20" s="17" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A91" s="17" t="s">
+      <c r="G90" s="19"/>
+      <c r="M90" s="19"/>
+      <c r="S90" s="19"/>
+    </row>
+    <row r="91" spans="1:20" s="2" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C91" s="20" t="s">
+      <c r="C91" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="D91" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G91" s="23"/>
-      <c r="L91" s="50"/>
-      <c r="M91" s="23"/>
-      <c r="R91" s="50"/>
-      <c r="S91" s="23"/>
+      <c r="D91" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G91" s="19"/>
+      <c r="M91" s="19"/>
+      <c r="S91" s="19"/>
     </row>
     <row r="92" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="B92" s="19"/>
-      <c r="C92" s="19"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="15"/>
       <c r="D92" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E92" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G92" s="23"/>
+      <c r="G92" s="19"/>
       <c r="H92" s="7" t="s">
         <v>14</v>
       </c>
@@ -4711,7 +4457,7 @@
       <c r="L92" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M92" s="23"/>
+      <c r="M92" s="19"/>
       <c r="N92" s="7" t="s">
         <v>14</v>
       </c>
@@ -4727,16 +4473,16 @@
       <c r="R92" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S92" s="23"/>
+      <c r="S92" s="19"/>
     </row>
     <row r="93" spans="1:20" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A93" s="20" t="s">
+      <c r="A93" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="B93" s="20" t="s">
+      <c r="B93" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C93" s="20" t="s">
+      <c r="C93" s="16" t="s">
         <v>292</v>
       </c>
       <c r="D93" s="7" t="b">
@@ -4745,9 +4491,9 @@
       <c r="E93" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G93" s="23"/>
-      <c r="M93" s="23"/>
-      <c r="S93" s="23"/>
+      <c r="G93" s="19"/>
+      <c r="M93" s="19"/>
+      <c r="S93" s="19"/>
     </row>
     <row r="94" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
@@ -4768,15 +4514,9 @@
       <c r="F94" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G94" s="23"/>
-      <c r="L94" s="50"/>
-      <c r="M94" s="23"/>
-      <c r="N94" s="17"/>
-      <c r="O94" s="17"/>
-      <c r="P94" s="17"/>
-      <c r="Q94" s="17"/>
-      <c r="R94" s="50"/>
-      <c r="S94" s="23"/>
+      <c r="G94" s="19"/>
+      <c r="M94" s="19"/>
+      <c r="S94" s="19"/>
       <c r="T94" s="8" t="s">
         <v>217</v>
       </c>
@@ -4800,19 +4540,9 @@
       <c r="F95" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="G95" s="23"/>
-      <c r="H95" s="17"/>
-      <c r="I95" s="17"/>
-      <c r="J95" s="17"/>
-      <c r="K95" s="17"/>
-      <c r="L95" s="50"/>
-      <c r="M95" s="23"/>
-      <c r="N95" s="17"/>
-      <c r="O95" s="17"/>
-      <c r="P95" s="17"/>
-      <c r="Q95" s="17"/>
-      <c r="R95" s="50"/>
-      <c r="S95" s="23"/>
+      <c r="G95" s="19"/>
+      <c r="M95" s="19"/>
+      <c r="S95" s="19"/>
       <c r="T95" s="8" t="s">
         <v>327</v>
       </c>
@@ -4833,74 +4563,68 @@
       <c r="E96" t="b">
         <v>1</v>
       </c>
-      <c r="N96" s="28" t="s">
+      <c r="N96" t="s">
         <v>317</v>
       </c>
-      <c r="O96" s="28" t="s">
+      <c r="O96" t="s">
         <v>317</v>
       </c>
-      <c r="P96" s="28" t="s">
+      <c r="P96" t="s">
         <v>317</v>
       </c>
-      <c r="Q96" s="28" t="s">
+      <c r="Q96" t="s">
         <v>317</v>
       </c>
-      <c r="R96" s="28" t="s">
+      <c r="R96" t="s">
         <v>317</v>
       </c>
       <c r="T96"/>
     </row>
-    <row r="97" spans="1:20" s="13" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A97" s="13" t="s">
+    <row r="97" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A97" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B97" s="13" t="s">
+      <c r="B97" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C97" s="13" t="s">
+      <c r="C97" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D97" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="13" t="b">
+      <c r="D97" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F97" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="G97" s="26"/>
-      <c r="L97" s="50"/>
-      <c r="M97" s="23"/>
-      <c r="N97" s="17"/>
-      <c r="O97" s="17"/>
-      <c r="P97" s="17"/>
-      <c r="Q97" s="17"/>
-      <c r="R97" s="50"/>
-      <c r="S97" s="23"/>
+      <c r="G97" s="22"/>
+      <c r="M97" s="19"/>
+      <c r="S97" s="19"/>
     </row>
     <row r="98" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="28" t="s">
+      <c r="A98" t="s">
         <v>235</v>
       </c>
-      <c r="B98" s="28" t="s">
+      <c r="B98" t="s">
         <v>10</v>
       </c>
-      <c r="C98" s="28" t="s">
+      <c r="C98" t="s">
         <v>340</v>
       </c>
-      <c r="D98" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" s="28" t="s">
+      <c r="D98" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" t="s">
         <v>272</v>
       </c>
-      <c r="G98" s="23"/>
-      <c r="M98" s="23"/>
-      <c r="S98" s="23"/>
+      <c r="G98" s="19"/>
+      <c r="M98" s="19"/>
+      <c r="S98" s="19"/>
       <c r="T98" s="7" t="s">
         <v>286</v>
       </c>
@@ -4924,38 +4648,32 @@
       <c r="F99" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G99" s="23"/>
-      <c r="L99" s="50"/>
-      <c r="M99" s="23"/>
-      <c r="N99" s="17"/>
-      <c r="O99" s="17"/>
-      <c r="P99" s="17"/>
-      <c r="Q99" s="17"/>
-      <c r="R99" s="50"/>
-      <c r="S99" s="23"/>
+      <c r="G99" s="19"/>
+      <c r="M99" s="19"/>
+      <c r="S99" s="19"/>
     </row>
     <row r="100" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="28" t="s">
+      <c r="A100" t="s">
         <v>337</v>
       </c>
-      <c r="B100" s="28" t="s">
+      <c r="B100" t="s">
         <v>10</v>
       </c>
-      <c r="C100" s="28" t="s">
+      <c r="C100" t="s">
         <v>339</v>
       </c>
-      <c r="D100" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F100" s="28" t="s">
+      <c r="D100" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" t="s">
         <v>272</v>
       </c>
-      <c r="G100" s="29"/>
-      <c r="M100" s="29"/>
-      <c r="S100" s="29"/>
+      <c r="G100" s="19"/>
+      <c r="M100" s="19"/>
+      <c r="S100" s="19"/>
       <c r="T100" s="7" t="s">
         <v>338</v>
       </c>
@@ -4979,66 +4697,56 @@
       <c r="F101" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="G101" s="26"/>
-      <c r="L101" s="50"/>
-      <c r="M101" s="23"/>
-      <c r="N101" s="17"/>
-      <c r="O101" s="17"/>
-      <c r="P101" s="17"/>
-      <c r="Q101" s="17"/>
-      <c r="R101" s="50"/>
-      <c r="S101" s="23"/>
+      <c r="G101" s="22"/>
+      <c r="M101" s="19"/>
+      <c r="S101" s="19"/>
       <c r="T101" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="102" spans="1:20" s="47" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="47" t="s">
+    <row r="102" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B102" s="47" t="s">
+      <c r="B102" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C102" s="47" t="s">
+      <c r="C102" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="D102" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" s="47" t="b">
+      <c r="D102" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="G102" s="26"/>
-      <c r="L102" s="50"/>
-      <c r="M102" s="29"/>
-      <c r="R102" s="50"/>
-      <c r="S102" s="29"/>
-    </row>
-    <row r="103" spans="1:20" s="17" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A103" s="17" t="s">
+      <c r="G102" s="22"/>
+      <c r="M102" s="19"/>
+      <c r="S102" s="19"/>
+    </row>
+    <row r="103" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B103" s="17" t="s">
+      <c r="B103" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="17" t="s">
+      <c r="C103" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="D103" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E103" s="17" t="b">
+      <c r="D103" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F103" s="6"/>
-      <c r="G103" s="26"/>
-      <c r="L103" s="50"/>
-      <c r="M103" s="23"/>
-      <c r="R103" s="50"/>
-      <c r="S103" s="23"/>
+      <c r="G103" s="22"/>
+      <c r="M103" s="19"/>
+      <c r="S103" s="19"/>
     </row>
     <row r="104" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
@@ -5059,15 +4767,9 @@
       <c r="F104" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G104" s="23"/>
-      <c r="L104" s="50"/>
-      <c r="M104" s="23"/>
-      <c r="N104" s="17"/>
-      <c r="O104" s="17"/>
-      <c r="P104" s="17"/>
-      <c r="Q104" s="17"/>
-      <c r="R104" s="50"/>
-      <c r="S104" s="23"/>
+      <c r="G104" s="19"/>
+      <c r="M104" s="19"/>
+      <c r="S104" s="19"/>
     </row>
     <row r="105" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
@@ -5085,15 +4787,9 @@
       <c r="E105" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G105" s="23"/>
-      <c r="L105" s="50"/>
-      <c r="M105" s="23"/>
-      <c r="N105" s="17"/>
-      <c r="O105" s="17"/>
-      <c r="P105" s="17"/>
-      <c r="Q105" s="17"/>
-      <c r="R105" s="50"/>
-      <c r="S105" s="23"/>
+      <c r="G105" s="19"/>
+      <c r="M105" s="19"/>
+      <c r="S105" s="19"/>
       <c r="T105" s="8" t="s">
         <v>219</v>
       </c>
@@ -5117,15 +4813,9 @@
       <c r="F106" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G106" s="23"/>
-      <c r="L106" s="50"/>
-      <c r="M106" s="23"/>
-      <c r="N106" s="17"/>
-      <c r="O106" s="17"/>
-      <c r="P106" s="17"/>
-      <c r="Q106" s="17"/>
-      <c r="R106" s="50"/>
-      <c r="S106" s="23"/>
+      <c r="G106" s="19"/>
+      <c r="M106" s="19"/>
+      <c r="S106" s="19"/>
       <c r="T106" s="8" t="s">
         <v>240</v>
       </c>
@@ -5146,39 +4836,39 @@
       <c r="E107" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G107" s="23"/>
-      <c r="H107" s="17" t="s">
+      <c r="G107" s="19"/>
+      <c r="H107" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="I107" s="17" t="s">
+      <c r="I107" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="J107" s="17" t="s">
+      <c r="J107" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="K107" s="17" t="s">
+      <c r="K107" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="L107" s="50" t="s">
+      <c r="L107" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="M107" s="23"/>
-      <c r="N107" s="17" t="s">
+      <c r="M107" s="19"/>
+      <c r="N107" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="O107" s="17" t="s">
+      <c r="O107" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="P107" s="17" t="s">
+      <c r="P107" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="Q107" s="17" t="s">
+      <c r="Q107" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="R107" s="50" t="s">
+      <c r="R107" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="S107" s="23"/>
+      <c r="S107" s="19"/>
       <c r="T107" s="2" t="s">
         <v>211</v>
       </c>
@@ -5202,9 +4892,9 @@
       <c r="F108" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G108" s="23"/>
-      <c r="M108" s="23"/>
-      <c r="S108" s="23"/>
+      <c r="G108" s="19"/>
+      <c r="M108" s="19"/>
+      <c r="S108" s="19"/>
       <c r="T108" s="7" t="s">
         <v>216</v>
       </c>
@@ -5228,9 +4918,9 @@
       <c r="F109" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G109" s="23"/>
-      <c r="M109" s="23"/>
-      <c r="S109" s="23"/>
+      <c r="G109" s="19"/>
+      <c r="M109" s="19"/>
+      <c r="S109" s="19"/>
       <c r="T109" s="7" t="s">
         <v>220</v>
       </c>
@@ -5254,9 +4944,9 @@
       <c r="F110" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G110" s="23"/>
-      <c r="M110" s="23"/>
-      <c r="S110" s="23"/>
+      <c r="G110" s="19"/>
+      <c r="M110" s="19"/>
+      <c r="S110" s="19"/>
       <c r="T110" s="7" t="s">
         <v>221</v>
       </c>
@@ -5277,7 +4967,7 @@
       <c r="E111" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G111" s="23"/>
+      <c r="G111" s="19"/>
       <c r="H111" s="2" t="s">
         <v>4</v>
       </c>
@@ -5290,26 +4980,26 @@
       <c r="K111" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L111" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M111" s="23"/>
-      <c r="N111" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O111" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P111" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q111" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R111" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S111" s="23"/>
+      <c r="L111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M111" s="19"/>
+      <c r="N111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S111" s="19"/>
     </row>
     <row r="112" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
@@ -5327,7 +5017,7 @@
       <c r="E112" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G112" s="23"/>
+      <c r="G112" s="19"/>
       <c r="H112" s="2" t="s">
         <v>4</v>
       </c>
@@ -5340,26 +5030,26 @@
       <c r="K112" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L112" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M112" s="23"/>
-      <c r="N112" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O112" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P112" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q112" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R112" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S112" s="23"/>
+      <c r="L112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M112" s="19"/>
+      <c r="N112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S112" s="19"/>
     </row>
     <row r="113" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
@@ -5377,7 +5067,7 @@
       <c r="E113" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G113" s="23"/>
+      <c r="G113" s="19"/>
       <c r="H113" s="2" t="s">
         <v>14</v>
       </c>
@@ -5390,132 +5080,132 @@
       <c r="K113" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L113" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M113" s="23"/>
-      <c r="N113" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O113" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P113" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q113" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R113" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S113" s="23"/>
+      <c r="L113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M113" s="19"/>
+      <c r="N113" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S113" s="19"/>
     </row>
     <row r="114" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="28" t="s">
+      <c r="A114" t="s">
         <v>149</v>
       </c>
-      <c r="B114" s="28" t="s">
+      <c r="B114" t="s">
         <v>5</v>
       </c>
-      <c r="C114" s="28" t="s">
+      <c r="C114" t="s">
         <v>150</v>
       </c>
-      <c r="D114" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E114" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F114" s="28"/>
-      <c r="G114" s="23"/>
-      <c r="H114" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I114" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="J114" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K114" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L114" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="M114" s="23"/>
-      <c r="N114" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O114" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P114" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q114" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="R114" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="S114" s="23"/>
-      <c r="T114" s="28" t="s">
+      <c r="D114" t="b">
+        <v>0</v>
+      </c>
+      <c r="E114" t="b">
+        <v>1</v>
+      </c>
+      <c r="F114"/>
+      <c r="G114" s="19"/>
+      <c r="H114" t="s">
+        <v>14</v>
+      </c>
+      <c r="I114" t="s">
+        <v>4</v>
+      </c>
+      <c r="J114" t="s">
+        <v>4</v>
+      </c>
+      <c r="K114" t="s">
+        <v>4</v>
+      </c>
+      <c r="L114" t="s">
+        <v>4</v>
+      </c>
+      <c r="M114" s="19"/>
+      <c r="N114" t="s">
+        <v>14</v>
+      </c>
+      <c r="O114" t="s">
+        <v>4</v>
+      </c>
+      <c r="P114" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>4</v>
+      </c>
+      <c r="R114" t="s">
+        <v>4</v>
+      </c>
+      <c r="S114" s="19"/>
+      <c r="T114" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="115" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="28" t="s">
+      <c r="A115" t="s">
         <v>341</v>
       </c>
-      <c r="B115" s="28" t="s">
+      <c r="B115" t="s">
         <v>5</v>
       </c>
-      <c r="C115" s="28" t="s">
+      <c r="C115" t="s">
         <v>342</v>
       </c>
-      <c r="D115" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E115" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F115" s="28"/>
-      <c r="G115" s="29"/>
-      <c r="H115" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I115" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="J115" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K115" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L115" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="M115" s="29"/>
-      <c r="N115" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O115" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P115" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q115" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="R115" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="S115" s="29"/>
-      <c r="T115" s="28" t="s">
+      <c r="D115" t="b">
+        <v>0</v>
+      </c>
+      <c r="E115" t="b">
+        <v>1</v>
+      </c>
+      <c r="F115"/>
+      <c r="G115" s="19"/>
+      <c r="H115" t="s">
+        <v>14</v>
+      </c>
+      <c r="I115" t="s">
+        <v>4</v>
+      </c>
+      <c r="J115" t="s">
+        <v>4</v>
+      </c>
+      <c r="K115" t="s">
+        <v>4</v>
+      </c>
+      <c r="L115" t="s">
+        <v>4</v>
+      </c>
+      <c r="M115" s="19"/>
+      <c r="N115" t="s">
+        <v>14</v>
+      </c>
+      <c r="O115" t="s">
+        <v>4</v>
+      </c>
+      <c r="P115" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>4</v>
+      </c>
+      <c r="R115" t="s">
+        <v>4</v>
+      </c>
+      <c r="S115" s="19"/>
+      <c r="T115" t="s">
         <v>338</v>
       </c>
     </row>
@@ -5535,38 +5225,38 @@
       <c r="E116" t="b">
         <v>0</v>
       </c>
-      <c r="H116" s="16" t="s">
+      <c r="H116" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="I116" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J116" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K116" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L116" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M116" s="23"/>
-      <c r="N116" s="17" t="s">
+      <c r="I116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M116" s="19"/>
+      <c r="N116" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="O116" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P116" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q116" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R116" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S116" s="23"/>
+      <c r="O116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S116" s="19"/>
       <c r="T116"/>
     </row>
     <row r="117" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -5585,7 +5275,7 @@
       <c r="E117" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G117" s="23"/>
+      <c r="G117" s="19"/>
       <c r="H117" s="2" t="s">
         <v>14</v>
       </c>
@@ -5598,26 +5288,26 @@
       <c r="K117" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L117" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M117" s="23"/>
-      <c r="N117" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O117" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P117" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q117" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R117" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S117" s="23"/>
+      <c r="L117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M117" s="19"/>
+      <c r="N117" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S117" s="19"/>
       <c r="T117" s="2" t="s">
         <v>202</v>
       </c>
@@ -5638,7 +5328,7 @@
       <c r="E118" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G118" s="23"/>
+      <c r="G118" s="19"/>
       <c r="H118" s="2" t="s">
         <v>14</v>
       </c>
@@ -5651,26 +5341,26 @@
       <c r="K118" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L118" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="M118" s="23"/>
-      <c r="N118" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O118" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P118" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q118" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R118" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="S118" s="23"/>
+      <c r="L118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M118" s="19"/>
+      <c r="N118" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S118" s="19"/>
     </row>
     <row r="119" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
@@ -5688,137 +5378,135 @@
       <c r="E119" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G119" s="23"/>
-      <c r="H119" s="17" t="s">
+      <c r="G119" s="19"/>
+      <c r="H119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="I119" s="17" t="s">
+      <c r="I119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="J119" s="17" t="s">
+      <c r="J119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="K119" s="17" t="s">
+      <c r="K119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="L119" s="50" t="s">
+      <c r="L119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="M119" s="23"/>
-      <c r="N119" s="17" t="s">
+      <c r="M119" s="19"/>
+      <c r="N119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="O119" s="17" t="s">
+      <c r="O119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="P119" s="17" t="s">
+      <c r="P119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="Q119" s="17" t="s">
+      <c r="Q119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="R119" s="50" t="s">
+      <c r="R119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="S119" s="23"/>
-    </row>
-    <row r="120" spans="1:20" s="43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A120" s="43" t="s">
+      <c r="S119" s="19"/>
+    </row>
+    <row r="120" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A120" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B120" s="43" t="s">
+      <c r="B120" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C120" s="43" t="s">
+      <c r="C120" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="D120" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E120" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="G120" s="29"/>
-      <c r="H120" s="43" t="s">
+      <c r="D120" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G120" s="19"/>
+      <c r="H120" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="I120" s="43" t="s">
+      <c r="I120" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="J120" s="43" t="s">
+      <c r="J120" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="K120" s="43" t="s">
+      <c r="K120" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="L120" s="50" t="s">
+      <c r="L120" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="M120" s="29"/>
-      <c r="N120" s="43" t="s">
+      <c r="M120" s="19"/>
+      <c r="N120" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="O120" s="43" t="s">
+      <c r="O120" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="P120" s="43" t="s">
+      <c r="P120" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="Q120" s="43" t="s">
+      <c r="Q120" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="R120" s="50" t="s">
+      <c r="R120" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="S120" s="29"/>
-    </row>
-    <row r="121" spans="1:20" s="51" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A121" s="51" t="s">
+      <c r="S120" s="19"/>
+    </row>
+    <row r="121" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B121" s="51" t="s">
+      <c r="B121" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C121" s="51" t="s">
+      <c r="C121" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="D121" s="51" t="b">
-        <v>1</v>
-      </c>
-      <c r="E121" s="51" t="b">
-        <v>1</v>
-      </c>
-      <c r="F121" s="51" t="s">
+      <c r="D121" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F121" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="G121" s="29"/>
-      <c r="M121" s="29"/>
-      <c r="S121" s="29"/>
-    </row>
-    <row r="122" spans="1:20" s="30" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A122" s="30" t="s">
+      <c r="G121" s="19"/>
+      <c r="M121" s="19"/>
+      <c r="S121" s="19"/>
+    </row>
+    <row r="122" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A122" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B122" s="30" t="s">
+      <c r="B122" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C122" s="30" t="s">
+      <c r="C122" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D122" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E122" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F122" s="30" t="s">
+      <c r="D122" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E122" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F122" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="G122" s="29"/>
-      <c r="L122" s="50"/>
-      <c r="M122" s="29"/>
-      <c r="R122" s="50"/>
-      <c r="S122" s="29"/>
+      <c r="G122" s="19"/>
+      <c r="M122" s="19"/>
+      <c r="S122" s="19"/>
     </row>
     <row r="123" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A123" s="2" t="s">
@@ -5839,18 +5527,12 @@
       <c r="F123" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G123" s="23"/>
-      <c r="L123" s="50"/>
-      <c r="M123" s="23"/>
-      <c r="N123" s="17"/>
-      <c r="O123" s="17"/>
-      <c r="P123" s="17"/>
-      <c r="Q123" s="17"/>
-      <c r="R123" s="50"/>
-      <c r="S123" s="23"/>
+      <c r="G123" s="19"/>
+      <c r="M123" s="19"/>
+      <c r="S123" s="19"/>
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A124" s="51"/>
+      <c r="A124" s="2"/>
       <c r="T124"/>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.4">
@@ -5928,9 +5610,9 @@
     <mergeCell ref="D47:D48"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F19" r:id="rId1"/>
-    <hyperlink ref="F20" r:id="rId2"/>
-    <hyperlink ref="F61" r:id="rId3"/>
+    <hyperlink ref="F19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F61" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>
@@ -5938,7 +5620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
BRO: includemodelinfo gezet op "no"
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BRO/props/BRO.xlsx
+++ b/src/main/resources/input/BRO/props/BRO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\BRO\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E4C1FC-1D6A-4E2C-8972-8178A12C09A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3124F50-7524-4279-8254-788E4FA19634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BRO" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="387">
   <si>
     <t>Name</t>
   </si>
@@ -1184,6 +1184,9 @@
   </si>
   <si>
     <t>LOGICAL</t>
+  </si>
+  <si>
+    <t>includemodelinfo</t>
   </si>
 </sst>
 </file>
@@ -1712,13 +1715,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T148"/>
+  <dimension ref="A1:T149"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E46" sqref="A46:XFD46"/>
+      <selection pane="bottomRight" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3677,13 +3680,10 @@
     </row>
     <row r="66" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
-        <v>348</v>
+        <v>386</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>349</v>
+        <v>5</v>
       </c>
       <c r="D66" s="2" t="b">
         <v>0</v>
@@ -3692,149 +3692,149 @@
         <v>1</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>350</v>
+        <v>14</v>
       </c>
       <c r="G66" s="19"/>
       <c r="M66" s="19"/>
       <c r="S66" s="19"/>
     </row>
-    <row r="67" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D67" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>230</v>
+    <row r="67" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>350</v>
       </c>
       <c r="G67" s="19"/>
       <c r="M67" s="19"/>
       <c r="S67" s="19"/>
-      <c r="T67" s="7" t="s">
+    </row>
+    <row r="68" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A68" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D68" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E68" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="G68" s="19"/>
+      <c r="M68" s="19"/>
+      <c r="S68" s="19"/>
+      <c r="T68" s="7" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="68" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G68" s="19"/>
-      <c r="H68" s="2" t="s">
+      <c r="D69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" s="19"/>
+      <c r="H69" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="I69" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="J69" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K68" s="2" t="s">
+      <c r="K69" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="L68" s="2" t="s">
+      <c r="L69" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="M68" s="19"/>
-      <c r="N68" s="2" t="s">
+      <c r="M69" s="19"/>
+      <c r="N69" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="O68" s="2" t="s">
+      <c r="O69" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="P68" s="2" t="s">
+      <c r="P69" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="Q68" s="2" t="s">
+      <c r="Q69" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="R68" s="2" t="s">
+      <c r="R69" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="S68" s="19"/>
-      <c r="T68" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A69" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="G69" s="19"/>
-      <c r="M69" s="19"/>
       <c r="S69" s="19"/>
       <c r="T69" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
-        <v>185</v>
+        <v>65</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>187</v>
+        <v>66</v>
       </c>
       <c r="D70" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E70" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>210</v>
+        <v>274</v>
       </c>
       <c r="G70" s="19"/>
       <c r="M70" s="19"/>
       <c r="S70" s="19"/>
+      <c r="T70" s="2" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="71" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
-        <v>306</v>
+        <v>185</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>5</v>
+        <v>186</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>307</v>
+        <v>187</v>
       </c>
       <c r="D71" s="2" t="b">
         <v>0</v>
@@ -3843,68 +3843,67 @@
         <v>1</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>308</v>
+        <v>210</v>
       </c>
       <c r="G71" s="19"/>
       <c r="M71" s="19"/>
       <c r="S71" s="19"/>
-      <c r="T71" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="72" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
-        <v>67</v>
+        <v>306</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>68</v>
+        <v>307</v>
       </c>
       <c r="D72" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>308</v>
       </c>
       <c r="G72" s="19"/>
       <c r="M72" s="19"/>
       <c r="S72" s="19"/>
-    </row>
-    <row r="73" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T72" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
-        <v>374</v>
+        <v>67</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>375</v>
+        <v>68</v>
       </c>
       <c r="D73" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>376</v>
+        <v>0</v>
       </c>
       <c r="G73" s="19"/>
       <c r="M73" s="19"/>
       <c r="S73" s="19"/>
-      <c r="T73"/>
     </row>
     <row r="74" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>256</v>
+        <v>10</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D74" s="2" t="b">
         <v>0</v>
@@ -3913,7 +3912,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G74" s="19"/>
       <c r="M74" s="19"/>
@@ -3922,13 +3921,13 @@
     </row>
     <row r="75" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>10</v>
+        <v>256</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>0</v>
@@ -3936,50 +3935,23 @@
       <c r="E75" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F75" s="2" t="s">
+        <v>379</v>
+      </c>
       <c r="G75" s="19"/>
-      <c r="H75" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="L75" s="2" t="s">
-        <v>384</v>
-      </c>
       <c r="M75" s="19"/>
-      <c r="N75" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="O75" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="P75" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="Q75" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="R75" s="2" t="s">
-        <v>385</v>
-      </c>
       <c r="S75" s="19"/>
       <c r="T75"/>
     </row>
     <row r="76" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>256</v>
+        <v>10</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D76" s="2" t="b">
         <v>0</v>
@@ -3988,19 +3960,49 @@
         <v>1</v>
       </c>
       <c r="G76" s="19"/>
+      <c r="H76" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>384</v>
+      </c>
       <c r="M76" s="19"/>
+      <c r="N76" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="O76" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="P76" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q76" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="R76" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="S76" s="19"/>
       <c r="T76"/>
     </row>
     <row r="77" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
-        <v>188</v>
+        <v>382</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>10</v>
+        <v>256</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>351</v>
+        <v>383</v>
       </c>
       <c r="D77" s="2" t="b">
         <v>0</v>
@@ -4011,796 +4013,791 @@
       <c r="G77" s="19"/>
       <c r="M77" s="19"/>
       <c r="S77" s="19"/>
-    </row>
-    <row r="78" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T77"/>
+    </row>
+    <row r="78" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
-        <v>358</v>
+        <v>188</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D78" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E78" s="2" t="b">
         <v>1</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="G78" s="19"/>
       <c r="M78" s="19"/>
       <c r="S78" s="19"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A79" t="s">
+    <row r="79" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G79" s="19"/>
+      <c r="M79" s="19"/>
+      <c r="S79" s="19"/>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
         <v>69</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>5</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>70</v>
       </c>
-      <c r="D79" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" t="s">
-        <v>4</v>
-      </c>
-      <c r="T79"/>
-    </row>
-    <row r="80" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A80" s="23" t="s">
+      <c r="D80" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>4</v>
+      </c>
+      <c r="T80"/>
+    </row>
+    <row r="81" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A81" s="23" t="s">
         <v>356</v>
       </c>
-      <c r="B80" s="23" t="s">
+      <c r="B81" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="23" t="s">
+      <c r="C81" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="D80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G80" s="19"/>
-      <c r="H80" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J80" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K80" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L80" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M80" s="19"/>
-      <c r="N80" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O80" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P80" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q80" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R80" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S80" s="19"/>
-    </row>
-    <row r="81" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="D81" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G81" s="19"/>
+      <c r="H81" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="M81" s="19"/>
+      <c r="N81" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O81" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P81" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q81" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R81" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="S81" s="19"/>
     </row>
     <row r="82" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
-        <v>71</v>
+        <v>229</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>72</v>
+        <v>243</v>
       </c>
       <c r="D82" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G82" s="19"/>
       <c r="M82" s="19"/>
       <c r="S82" s="19"/>
     </row>
-    <row r="83" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D83" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G83" s="19"/>
+      <c r="M83" s="19"/>
+      <c r="S83" s="19"/>
+    </row>
+    <row r="84" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D83" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G83" s="19"/>
-      <c r="H83" s="2" t="s">
+      <c r="D84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G84" s="19"/>
+      <c r="H84" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="I84" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="J83" s="2" t="s">
+      <c r="J84" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="K83" s="2" t="s">
+      <c r="K84" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="L83" s="2" t="s">
+      <c r="L84" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="M83" s="19"/>
-      <c r="N83" s="2" t="s">
+      <c r="M84" s="19"/>
+      <c r="N84" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="O83" s="2" t="s">
+      <c r="O84" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="P83" s="2" t="s">
+      <c r="P84" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="Q83" s="2" t="s">
+      <c r="Q84" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="R83" s="2" t="s">
+      <c r="R84" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="S83" s="19"/>
-    </row>
-    <row r="84" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
+      <c r="S84" s="19"/>
+    </row>
+    <row r="85" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F84" s="2" t="s">
+      <c r="D85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="G84" s="19"/>
-      <c r="M84" s="19"/>
-      <c r="S84" s="19"/>
-    </row>
-    <row r="85" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>268</v>
       </c>
       <c r="G85" s="19"/>
       <c r="M85" s="19"/>
       <c r="S85" s="19"/>
-      <c r="T85" s="7" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="86" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>17</v>
+    </row>
+    <row r="86" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D86" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="G86" s="19"/>
-      <c r="I86" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="J86" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="M86" s="19"/>
       <c r="S86" s="19"/>
-    </row>
-    <row r="87" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A87" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D87" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>223</v>
+      <c r="T86" s="7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="G87" s="19"/>
+      <c r="I87" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>277</v>
+      </c>
       <c r="M87" s="19"/>
       <c r="S87" s="19"/>
-      <c r="T87" s="8" t="s">
+    </row>
+    <row r="88" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A88" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D88" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="G88" s="19"/>
+      <c r="M88" s="19"/>
+      <c r="S88" s="19"/>
+      <c r="T88" s="8" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="88" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G88" s="19"/>
-      <c r="H88" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="J88" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="K88" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="L88" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="M88" s="19"/>
-      <c r="N88" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="O88" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="P88" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q88" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="R88" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="S88" s="19"/>
     </row>
     <row r="89" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G89" s="19"/>
+      <c r="H89" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="M89" s="19"/>
+      <c r="N89" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="O89" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="P89" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q89" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="R89" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="S89" s="19"/>
+    </row>
+    <row r="90" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="2" t="s">
+      <c r="D90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="G89" s="19"/>
-      <c r="M89" s="19"/>
-      <c r="S89" s="19"/>
-    </row>
-    <row r="90" spans="1:20" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A90" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D90" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="G90" s="19"/>
       <c r="M90" s="19"/>
       <c r="S90" s="19"/>
-      <c r="T90" s="8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="91" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="91" spans="1:20" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A91" s="7" t="s">
-        <v>142</v>
+        <v>86</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
       <c r="D91" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E91" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="G91" s="19"/>
       <c r="M91" s="19"/>
       <c r="S91" s="19"/>
-      <c r="T91" s="7" t="s">
+      <c r="T91" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A92" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D92" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G92" s="19"/>
+      <c r="M92" s="19"/>
+      <c r="S92" s="19"/>
+      <c r="T92" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="92" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A92" s="23" t="s">
+    <row r="93" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="B92" s="23" t="s">
+      <c r="B93" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C92" s="23" t="s">
+      <c r="C93" s="23" t="s">
         <v>370</v>
       </c>
-      <c r="D92" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G92" s="19"/>
-      <c r="H92" s="23"/>
-      <c r="I92" s="23"/>
-      <c r="J92" s="23"/>
-      <c r="K92" s="23"/>
-      <c r="L92" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="M92" s="24"/>
-      <c r="N92" s="23"/>
-      <c r="O92" s="23"/>
-      <c r="P92" s="23"/>
-      <c r="Q92" s="23"/>
-      <c r="R92" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="S92" s="19"/>
-    </row>
-    <row r="93" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
+      <c r="D93" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93" s="19"/>
+      <c r="H93" s="23"/>
+      <c r="I93" s="23"/>
+      <c r="J93" s="23"/>
+      <c r="K93" s="23"/>
+      <c r="L93" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M93" s="24"/>
+      <c r="N93" s="23"/>
+      <c r="O93" s="23"/>
+      <c r="P93" s="23"/>
+      <c r="Q93" s="23"/>
+      <c r="R93" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S93" s="19"/>
+    </row>
+    <row r="94" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F93" s="2" t="s">
+      <c r="D94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F94" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="G93" s="19"/>
-      <c r="M93" s="19"/>
-      <c r="S93" s="19"/>
-    </row>
-    <row r="94" spans="1:20" s="2" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A94" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="D94" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="G94" s="19"/>
       <c r="M94" s="19"/>
       <c r="S94" s="19"/>
     </row>
-    <row r="95" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="7" t="s">
+    <row r="95" spans="1:20" s="2" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="D95" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G95" s="19"/>
+      <c r="M95" s="19"/>
+      <c r="S95" s="19"/>
+    </row>
+    <row r="96" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B95" s="15"/>
-      <c r="C95" s="15"/>
-      <c r="D95" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G95" s="19"/>
-      <c r="H95" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I95" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J95" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K95" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L95" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M95" s="19"/>
-      <c r="N95" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O95" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P95" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q95" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="R95" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="S95" s="19"/>
-    </row>
-    <row r="96" spans="1:20" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
-      <c r="A96" s="16" t="s">
+      <c r="B96" s="15"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G96" s="19"/>
+      <c r="H96" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I96" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J96" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K96" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L96" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M96" s="19"/>
+      <c r="N96" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O96" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P96" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q96" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="R96" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="S96" s="19"/>
+    </row>
+    <row r="97" spans="1:20" s="7" customFormat="1" ht="28.3" x14ac:dyDescent="0.4">
+      <c r="A97" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="B96" s="16" t="s">
+      <c r="B97" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C96" s="16" t="s">
+      <c r="C97" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="D96" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G96" s="19"/>
-      <c r="M96" s="19"/>
-      <c r="S96" s="19"/>
-    </row>
-    <row r="97" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A97" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D97" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>4</v>
+      <c r="D97" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G97" s="19"/>
       <c r="M97" s="19"/>
       <c r="S97" s="19"/>
-      <c r="T97" s="8" t="s">
-        <v>214</v>
-      </c>
     </row>
     <row r="98" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="D98" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>324</v>
+        <v>4</v>
       </c>
       <c r="G98" s="19"/>
       <c r="M98" s="19"/>
       <c r="S98" s="19"/>
       <c r="T98" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A99" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G99" s="19"/>
+      <c r="M99" s="19"/>
+      <c r="S99" s="19"/>
+      <c r="T99" s="8" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A99" t="s">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
         <v>194</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>195</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>196</v>
       </c>
-      <c r="D99" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" t="b">
-        <v>1</v>
-      </c>
-      <c r="N99" t="s">
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" t="b">
+        <v>1</v>
+      </c>
+      <c r="N100" t="s">
         <v>313</v>
       </c>
-      <c r="O99" t="s">
+      <c r="O100" t="s">
         <v>313</v>
       </c>
-      <c r="P99" t="s">
+      <c r="P100" t="s">
         <v>313</v>
       </c>
-      <c r="Q99" t="s">
+      <c r="Q100" t="s">
         <v>313</v>
       </c>
-      <c r="R99" t="s">
+      <c r="R100" t="s">
         <v>313</v>
       </c>
-      <c r="T99"/>
-    </row>
-    <row r="100" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A100" s="2" t="s">
+      <c r="T100"/>
+    </row>
+    <row r="101" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A101" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D100" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F100" s="6" t="s">
+      <c r="D101" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="G100" s="22"/>
-      <c r="M100" s="19"/>
-      <c r="S100" s="19"/>
-    </row>
-    <row r="101" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A101" t="s">
-        <v>232</v>
-      </c>
-      <c r="B101" t="s">
-        <v>10</v>
-      </c>
-      <c r="C101" t="s">
-        <v>336</v>
-      </c>
-      <c r="D101" t="b">
-        <v>1</v>
-      </c>
-      <c r="E101" t="b">
-        <v>1</v>
-      </c>
-      <c r="F101" t="s">
-        <v>268</v>
-      </c>
-      <c r="G101" s="19"/>
+      <c r="G101" s="22"/>
       <c r="M101" s="19"/>
       <c r="S101" s="19"/>
-      <c r="T101" s="7" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="102" spans="1:20" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>14</v>
+    </row>
+    <row r="102" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
+        <v>232</v>
+      </c>
+      <c r="B102" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" t="s">
+        <v>336</v>
+      </c>
+      <c r="D102" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" t="s">
+        <v>268</v>
       </c>
       <c r="G102" s="19"/>
       <c r="M102" s="19"/>
       <c r="S102" s="19"/>
-    </row>
-    <row r="103" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A103" t="s">
-        <v>333</v>
-      </c>
-      <c r="B103" t="s">
-        <v>10</v>
-      </c>
-      <c r="C103" t="s">
-        <v>335</v>
-      </c>
-      <c r="D103" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" t="b">
-        <v>1</v>
-      </c>
-      <c r="F103" t="s">
-        <v>268</v>
+      <c r="T102" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D103" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G103" s="19"/>
       <c r="M103" s="19"/>
       <c r="S103" s="19"/>
-      <c r="T103" s="7" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="104" spans="1:20" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A104" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D104" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E104" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G104" s="22"/>
+    </row>
+    <row r="104" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A104" t="s">
+        <v>333</v>
+      </c>
+      <c r="B104" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104" t="s">
+        <v>335</v>
+      </c>
+      <c r="D104" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" t="s">
+        <v>268</v>
+      </c>
+      <c r="G104" s="19"/>
       <c r="M104" s="19"/>
       <c r="S104" s="19"/>
-      <c r="T104" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="105" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T104" s="7" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
-        <v>364</v>
+        <v>97</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>366</v>
+        <v>98</v>
       </c>
       <c r="D105" s="2" t="b">
         <v>0</v>
@@ -4809,21 +4806,24 @@
         <v>1</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>365</v>
+        <v>280</v>
       </c>
       <c r="G105" s="22"/>
       <c r="M105" s="19"/>
       <c r="S105" s="19"/>
-    </row>
-    <row r="106" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T105" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
-        <v>289</v>
+        <v>364</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>290</v>
+        <v>366</v>
       </c>
       <c r="D106" s="2" t="b">
         <v>0</v>
@@ -4831,20 +4831,22 @@
       <c r="E106" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F106" s="6"/>
+      <c r="F106" s="6" t="s">
+        <v>365</v>
+      </c>
       <c r="G106" s="22"/>
       <c r="M106" s="19"/>
       <c r="S106" s="19"/>
     </row>
     <row r="107" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
-        <v>99</v>
+        <v>289</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>100</v>
+        <v>290</v>
       </c>
       <c r="D107" s="2" t="b">
         <v>0</v>
@@ -4852,150 +4854,145 @@
       <c r="E107" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F107" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G107" s="19"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="22"/>
       <c r="M107" s="19"/>
       <c r="S107" s="19"/>
     </row>
-    <row r="108" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>197</v>
+        <v>99</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>198</v>
+        <v>100</v>
       </c>
       <c r="D108" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E108" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G108" s="19"/>
       <c r="M108" s="19"/>
       <c r="S108" s="19"/>
-      <c r="T108" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="109" spans="1:20" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="109" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>104</v>
+        <v>198</v>
       </c>
       <c r="D109" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E109" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="G109" s="19"/>
       <c r="M109" s="19"/>
       <c r="S109" s="19"/>
       <c r="T109" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A110" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G110" s="19"/>
+      <c r="M110" s="19"/>
+      <c r="S110" s="19"/>
+      <c r="T110" s="8" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="110" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A110" s="2" t="s">
+    <row r="111" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A111" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D110" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G110" s="19"/>
-      <c r="H110" s="2" t="s">
+      <c r="D111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G111" s="19"/>
+      <c r="H111" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="I110" s="2" t="s">
+      <c r="I111" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="J110" s="2" t="s">
+      <c r="J111" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="K110" s="2" t="s">
+      <c r="K111" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="L110" s="2" t="s">
+      <c r="L111" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="M110" s="19"/>
-      <c r="N110" s="2" t="s">
+      <c r="M111" s="19"/>
+      <c r="N111" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="O110" s="2" t="s">
+      <c r="O111" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="P110" s="2" t="s">
+      <c r="P111" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="Q110" s="2" t="s">
+      <c r="Q111" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="R110" s="2" t="s">
+      <c r="R111" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="S110" s="19"/>
-      <c r="T110" s="2" t="s">
+      <c r="S111" s="19"/>
+      <c r="T111" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="111" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A111" s="7" t="s">
+    <row r="112" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A112" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B111" s="7" t="s">
+      <c r="B112" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="C112" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="D111" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F111" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="G111" s="19"/>
-      <c r="M111" s="19"/>
-      <c r="S111" s="19"/>
-      <c r="T111" s="7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="112" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B112" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="D112" s="7" t="b">
         <v>1</v>
@@ -5010,97 +5007,73 @@
       <c r="M112" s="19"/>
       <c r="S112" s="19"/>
       <c r="T112" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="113" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D113" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E113" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>14</v>
+        <v>230</v>
       </c>
       <c r="G113" s="19"/>
       <c r="M113" s="19"/>
       <c r="S113" s="19"/>
       <c r="T113" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D114" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G114" s="19"/>
+      <c r="M114" s="19"/>
+      <c r="S114" s="19"/>
+      <c r="T114" s="7" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="114" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D114" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E114" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G114" s="19"/>
-      <c r="H114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M114" s="19"/>
-      <c r="N114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S114" s="19"/>
     </row>
     <row r="115" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>281</v>
+        <v>114</v>
       </c>
       <c r="D115" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E115" s="2" t="b">
         <v>1</v>
@@ -5141,23 +5114,23 @@
     </row>
     <row r="116" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>117</v>
+        <v>281</v>
       </c>
       <c r="D116" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E116" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G116" s="19"/>
       <c r="H116" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>4</v>
@@ -5173,7 +5146,7 @@
       </c>
       <c r="M116" s="19"/>
       <c r="N116" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="O116" s="2" t="s">
         <v>4</v>
@@ -5189,69 +5162,65 @@
       </c>
       <c r="S116" s="19"/>
     </row>
-    <row r="117" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A117" t="s">
-        <v>146</v>
-      </c>
-      <c r="B117" t="s">
+    <row r="117" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C117" t="s">
-        <v>147</v>
-      </c>
-      <c r="D117" t="b">
-        <v>0</v>
-      </c>
-      <c r="E117" t="b">
-        <v>1</v>
-      </c>
-      <c r="F117"/>
+      <c r="C117" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D117" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E117" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="G117" s="19"/>
-      <c r="H117" t="s">
-        <v>14</v>
-      </c>
-      <c r="I117" t="s">
-        <v>4</v>
-      </c>
-      <c r="J117" t="s">
-        <v>4</v>
-      </c>
-      <c r="K117" t="s">
-        <v>4</v>
-      </c>
-      <c r="L117" t="s">
+      <c r="H117" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L117" s="2" t="s">
         <v>4</v>
       </c>
       <c r="M117" s="19"/>
-      <c r="N117" t="s">
-        <v>14</v>
-      </c>
-      <c r="O117" t="s">
-        <v>4</v>
-      </c>
-      <c r="P117" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q117" t="s">
-        <v>4</v>
-      </c>
-      <c r="R117" t="s">
+      <c r="N117" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R117" s="2" t="s">
         <v>4</v>
       </c>
       <c r="S117" s="19"/>
-      <c r="T117" t="s">
-        <v>282</v>
-      </c>
     </row>
     <row r="118" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
-        <v>337</v>
+        <v>146</v>
       </c>
       <c r="B118" t="s">
         <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>338</v>
+        <v>147</v>
       </c>
       <c r="D118" t="b">
         <v>0</v>
@@ -5294,78 +5263,81 @@
       </c>
       <c r="S118" s="19"/>
       <c r="T118" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A119" t="s">
+        <v>337</v>
+      </c>
+      <c r="B119" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" t="s">
+        <v>338</v>
+      </c>
+      <c r="D119" t="b">
+        <v>0</v>
+      </c>
+      <c r="E119" t="b">
+        <v>1</v>
+      </c>
+      <c r="F119"/>
+      <c r="G119" s="19"/>
+      <c r="H119" t="s">
+        <v>14</v>
+      </c>
+      <c r="I119" t="s">
+        <v>4</v>
+      </c>
+      <c r="J119" t="s">
+        <v>4</v>
+      </c>
+      <c r="K119" t="s">
+        <v>4</v>
+      </c>
+      <c r="L119" t="s">
+        <v>4</v>
+      </c>
+      <c r="M119" s="19"/>
+      <c r="N119" t="s">
+        <v>14</v>
+      </c>
+      <c r="O119" t="s">
+        <v>4</v>
+      </c>
+      <c r="P119" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>4</v>
+      </c>
+      <c r="R119" t="s">
+        <v>4</v>
+      </c>
+      <c r="S119" s="19"/>
+      <c r="T119" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A119" t="s">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A120" t="s">
         <v>118</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B120" t="s">
         <v>119</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C120" t="s">
         <v>120</v>
       </c>
-      <c r="D119" t="b">
-        <v>1</v>
-      </c>
-      <c r="E119" t="b">
-        <v>0</v>
-      </c>
-      <c r="H119" s="2" t="s">
+      <c r="D120" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" t="b">
+        <v>0</v>
+      </c>
+      <c r="H120" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="I119" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J119" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K119" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L119" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M119" s="19"/>
-      <c r="N119" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="O119" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P119" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q119" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R119" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S119" s="19"/>
-      <c r="T119"/>
-    </row>
-    <row r="120" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A120" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D120" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E120" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G120" s="19"/>
-      <c r="H120" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>4</v>
@@ -5381,7 +5353,7 @@
       </c>
       <c r="M120" s="19"/>
       <c r="N120" s="2" t="s">
-        <v>14</v>
+        <v>283</v>
       </c>
       <c r="O120" s="2" t="s">
         <v>4</v>
@@ -5396,19 +5368,17 @@
         <v>4</v>
       </c>
       <c r="S120" s="19"/>
-      <c r="T120" s="2" t="s">
-        <v>199</v>
-      </c>
+      <c r="T120"/>
     </row>
     <row r="121" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A121" s="2" t="s">
-        <v>254</v>
+        <v>121</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D121" s="2" t="b">
         <v>1</v>
@@ -5449,181 +5419,231 @@
         <v>4</v>
       </c>
       <c r="S121" s="19"/>
+      <c r="T121" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="122" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A122" s="2" t="s">
-        <v>124</v>
+        <v>254</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D122" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E122" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G122" s="19"/>
       <c r="H122" s="2" t="s">
-        <v>268</v>
+        <v>14</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>268</v>
+        <v>4</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>268</v>
+        <v>4</v>
       </c>
       <c r="K122" s="2" t="s">
-        <v>268</v>
+        <v>4</v>
       </c>
       <c r="L122" s="2" t="s">
-        <v>268</v>
+        <v>4</v>
       </c>
       <c r="M122" s="19"/>
       <c r="N122" s="2" t="s">
-        <v>268</v>
+        <v>14</v>
       </c>
       <c r="O122" s="2" t="s">
-        <v>268</v>
+        <v>4</v>
       </c>
       <c r="P122" s="2" t="s">
-        <v>268</v>
+        <v>4</v>
       </c>
       <c r="Q122" s="2" t="s">
-        <v>268</v>
+        <v>4</v>
       </c>
       <c r="R122" s="2" t="s">
-        <v>268</v>
+        <v>4</v>
       </c>
       <c r="S122" s="19"/>
     </row>
     <row r="123" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A123" s="2" t="s">
-        <v>352</v>
+        <v>124</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>353</v>
+        <v>125</v>
       </c>
       <c r="D123" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E123" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G123" s="19"/>
       <c r="H123" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="J123" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="K123" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="L123" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="M123" s="19"/>
       <c r="N123" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="O123" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="P123" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="Q123" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="R123" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="S123" s="19"/>
     </row>
     <row r="124" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A124" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D124" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E124" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G124" s="19"/>
+      <c r="H124" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I124" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="J124" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K124" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="L124" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="M124" s="19"/>
+      <c r="N124" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="O124" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="P124" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q124" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="R124" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="S124" s="19"/>
+    </row>
+    <row r="125" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A125" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B125" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C125" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="D124" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E124" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F124" s="2" t="s">
+      <c r="D125" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E125" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F125" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="G124" s="19"/>
-      <c r="M124" s="19"/>
-      <c r="S124" s="19"/>
-    </row>
-    <row r="125" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A125" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D125" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E125" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>312</v>
       </c>
       <c r="G125" s="19"/>
       <c r="M125" s="19"/>
       <c r="S125" s="19"/>
     </row>
-    <row r="126" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A126" s="2" t="s">
-        <v>126</v>
+        <v>310</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>128</v>
+        <v>311</v>
       </c>
       <c r="D126" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E126" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>239</v>
+        <v>312</v>
       </c>
       <c r="G126" s="19"/>
       <c r="M126" s="19"/>
       <c r="S126" s="19"/>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A127" s="2"/>
-      <c r="T127"/>
+    <row r="127" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A127" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D127" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E127" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G127" s="19"/>
+      <c r="M127" s="19"/>
+      <c r="S127" s="19"/>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A128" s="2"/>
       <c r="T128"/>
     </row>
     <row r="129" spans="20:20" x14ac:dyDescent="0.4">
@@ -5685,6 +5705,9 @@
     </row>
     <row r="148" spans="20:20" x14ac:dyDescent="0.4">
       <c r="T148"/>
+    </row>
+    <row r="149" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T149"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>